<commit_message>
Power test added to github, readme updated, data sheet updated for 6 tanks in wetlab not 4
</commit_message>
<xml_diff>
--- a/data/raw.xlsx
+++ b/data/raw.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Amelia\github\Ritger-Corynactis-urchin-deterrence\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D98357E1-139A-48F5-A799-5D951E90C76E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A84760D6-7A3D-43BC-9B45-3D49ADEA12F5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15" yWindow="-17520" windowWidth="24900" windowHeight="12525" activeTab="1" xr2:uid="{58E670A5-634C-427F-960F-9DA76C64E810}"/>
+    <workbookView xWindow="15" yWindow="-17520" windowWidth="26535" windowHeight="16380" xr2:uid="{58E670A5-634C-427F-960F-9DA76C64E810}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="3" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="71">
   <si>
     <t>Day</t>
   </si>
@@ -116,22 +116,7 @@
     <t>Day of the week</t>
   </si>
   <si>
-    <t>1-4 (boatyard), 5-12 (balcony)</t>
-  </si>
-  <si>
-    <t>1-X</t>
-  </si>
-  <si>
-    <t>NSEW</t>
-  </si>
-  <si>
     <t>Treatment</t>
-  </si>
-  <si>
-    <t>Control, R, O, P</t>
-  </si>
-  <si>
-    <t>1,2,3,4</t>
   </si>
   <si>
     <t>test size</t>
@@ -150,9 +135,6 @@
   </si>
   <si>
     <t>% cover of Corynactis on tile</t>
-  </si>
-  <si>
-    <t>1-10 (red), 11-20 (orange), 21-30 (pink)</t>
   </si>
   <si>
     <t>Area of kelp before trial</t>
@@ -236,16 +218,34 @@
     <t>Pink</t>
   </si>
   <si>
-    <t>E</t>
-  </si>
-  <si>
     <t>N</t>
   </si>
   <si>
     <t>S</t>
   </si>
   <si>
-    <t>W</t>
+    <t>tiles needing a home</t>
+  </si>
+  <si>
+    <t>1-6 (boatyard), 5-14 (balcony)</t>
+  </si>
+  <si>
+    <t>tiles needing a video</t>
+  </si>
+  <si>
+    <t>North (N/E) or South (S/W) in tank</t>
+  </si>
+  <si>
+    <t>1-10 (red), 11-20 (orange), 21-30 (pink), 0 (control)</t>
+  </si>
+  <si>
+    <t>1 (Contol),2 (Red), 3 (Orange), 4 (Pink)</t>
+  </si>
+  <si>
+    <t>Control, Red, Orange, Pink</t>
+  </si>
+  <si>
+    <t>1 through 76 (60 treatments, 16 controls)</t>
   </si>
 </sst>
 </file>
@@ -295,7 +295,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -303,6 +303,11 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -619,8 +624,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{168F7463-EB05-46FE-9A95-7790352FDB02}">
   <dimension ref="A1:B16244"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -631,12 +636,12 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="B3" s="4"/>
     </row>
@@ -653,15 +658,15 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>27</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B6" t="s">
-        <v>28</v>
+      <c r="B6" s="9" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -669,15 +674,15 @@
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>29</v>
+        <v>66</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B8" t="s">
-        <v>31</v>
+        <v>69</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -685,7 +690,7 @@
         <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>32</v>
+        <v>68</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
@@ -693,7 +698,7 @@
         <v>5</v>
       </c>
       <c r="B10" t="s">
-        <v>39</v>
+        <v>67</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -701,7 +706,7 @@
         <v>6</v>
       </c>
       <c r="B11" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
@@ -709,7 +714,7 @@
         <v>22</v>
       </c>
       <c r="B12" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
@@ -717,7 +722,7 @@
         <v>7</v>
       </c>
       <c r="B13" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
@@ -725,7 +730,7 @@
         <v>8</v>
       </c>
       <c r="B14" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
@@ -733,7 +738,7 @@
         <v>9</v>
       </c>
       <c r="B15" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
@@ -741,7 +746,7 @@
         <v>10</v>
       </c>
       <c r="B16" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
@@ -749,7 +754,7 @@
         <v>11</v>
       </c>
       <c r="B17" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
@@ -757,7 +762,7 @@
         <v>12</v>
       </c>
       <c r="B18" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
@@ -765,7 +770,7 @@
         <v>13</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
@@ -773,7 +778,7 @@
         <v>14</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
@@ -781,7 +786,7 @@
         <v>25</v>
       </c>
       <c r="B21" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
@@ -789,7 +794,7 @@
         <v>24</v>
       </c>
       <c r="B22" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
@@ -797,7 +802,7 @@
         <v>23</v>
       </c>
       <c r="B23" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
@@ -805,7 +810,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="B25" s="4"/>
     </row>
@@ -814,15 +819,15 @@
         <v>15</v>
       </c>
       <c r="B26" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="B27" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
@@ -830,7 +835,7 @@
         <v>16</v>
       </c>
       <c r="B28" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
@@ -838,7 +843,7 @@
         <v>17</v>
       </c>
       <c r="B29" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
@@ -846,7 +851,7 @@
         <v>18</v>
       </c>
       <c r="B30" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
@@ -854,7 +859,7 @@
         <v>19</v>
       </c>
       <c r="B31" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
@@ -862,15 +867,15 @@
         <v>20</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
@@ -878,7 +883,7 @@
         <v>21</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
@@ -886,7 +891,7 @@
         <v>23</v>
       </c>
       <c r="B35" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
@@ -49527,10 +49532,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD5E687B-43EE-4B00-8604-7EB9984510DD}">
-  <dimension ref="A1:U81"/>
+  <dimension ref="A1:U77"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -49543,7 +49549,7 @@
     <col min="6" max="6" width="12.44140625" customWidth="1"/>
     <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17.77734375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.109375" style="6" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="7.88671875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="15.77734375" customWidth="1"/>
     <col min="12" max="12" width="16" bestFit="1" customWidth="1"/>
@@ -49563,10 +49569,10 @@
         <v>2</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>24</v>
@@ -49578,12 +49584,12 @@
         <v>3</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="7" t="s">
         <v>5</v>
       </c>
       <c r="J1" s="2" t="s">
@@ -49637,14 +49643,18 @@
         <v>1</v>
       </c>
       <c r="F2" t="s">
-        <v>67</v>
-      </c>
-      <c r="G2" t="s">
-        <v>63</v>
+        <v>62</v>
+      </c>
+      <c r="G2" t="str">
+        <f>IF(I2&lt;=0, "Control", IF(I2&lt;=10, "Red", IF(I2&gt;=21, "Pink", "Orange")))</f>
+        <v>Orange</v>
       </c>
       <c r="H2">
-        <f t="shared" ref="H2:H33" si="0">IF(G2="Control", 1, IF(G2="Red", 2, IF(G2="Orange", 3, 4)))</f>
-        <v>1</v>
+        <f>IF(G2="Control", 1, IF(G2="Red", 2, IF(G2="Orange", 3, 4)))</f>
+        <v>3</v>
+      </c>
+      <c r="I2" s="8">
+        <v>11</v>
       </c>
       <c r="M2">
         <f>C2-236</f>
@@ -49665,20 +49675,22 @@
         <v>2</v>
       </c>
       <c r="F3" t="s">
-        <v>67</v>
-      </c>
-      <c r="G3" t="s">
-        <v>64</v>
+        <v>61</v>
+      </c>
+      <c r="G3" t="str">
+        <f t="shared" ref="G3:G66" si="0">IF(I3&lt;=0, "Control", IF(I3&lt;=10, "Red", IF(I3&gt;=21, "Pink", "Orange")))</f>
+        <v>Orange</v>
       </c>
       <c r="H3">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="I3">
-        <v>6</v>
-      </c>
+        <f t="shared" ref="H3:H66" si="1">IF(G3="Control", 1, IF(G3="Red", 2, IF(G3="Orange", 3, 4)))</f>
+        <v>3</v>
+      </c>
+      <c r="I3" s="8">
+        <v>20</v>
+      </c>
+      <c r="K3" s="6"/>
       <c r="M3">
-        <f>C3-236</f>
+        <f t="shared" ref="M3:M51" si="2">C3-236</f>
         <v>7</v>
       </c>
     </row>
@@ -49696,20 +49708,22 @@
         <v>3</v>
       </c>
       <c r="F4" t="s">
-        <v>68</v>
-      </c>
-      <c r="G4" t="s">
-        <v>65</v>
+        <v>62</v>
+      </c>
+      <c r="G4" t="str">
+        <f t="shared" si="0"/>
+        <v>Control</v>
       </c>
       <c r="H4">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="I4">
-        <v>16</v>
-      </c>
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I4" s="8">
+        <v>0</v>
+      </c>
+      <c r="K4" s="6"/>
       <c r="M4">
-        <f>C4-236</f>
+        <f t="shared" si="2"/>
         <v>7</v>
       </c>
     </row>
@@ -49727,20 +49741,22 @@
         <v>4</v>
       </c>
       <c r="F5" t="s">
-        <v>67</v>
-      </c>
-      <c r="G5" t="s">
-        <v>66</v>
+        <v>61</v>
+      </c>
+      <c r="G5" t="str">
+        <f t="shared" si="0"/>
+        <v>Red</v>
       </c>
       <c r="H5">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="I5">
-        <v>29</v>
-      </c>
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="I5" s="8">
+        <v>7</v>
+      </c>
+      <c r="K5" s="6"/>
       <c r="M5">
-        <f>C5-236</f>
+        <f t="shared" si="2"/>
         <v>7</v>
       </c>
     </row>
@@ -49758,17 +49774,22 @@
         <v>5</v>
       </c>
       <c r="F6" t="s">
-        <v>68</v>
-      </c>
-      <c r="G6" t="s">
-        <v>63</v>
+        <v>61</v>
+      </c>
+      <c r="G6" t="str">
+        <f t="shared" si="0"/>
+        <v>Pink</v>
       </c>
       <c r="H6">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="I6" s="8">
+        <v>21</v>
+      </c>
+      <c r="K6" s="6"/>
       <c r="M6">
-        <f>C6-236</f>
+        <f t="shared" si="2"/>
         <v>7</v>
       </c>
     </row>
@@ -49786,20 +49807,22 @@
         <v>6</v>
       </c>
       <c r="F7" t="s">
-        <v>69</v>
-      </c>
-      <c r="G7" t="s">
-        <v>64</v>
+        <v>61</v>
+      </c>
+      <c r="G7" t="str">
+        <f t="shared" si="0"/>
+        <v>Orange</v>
       </c>
       <c r="H7">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="I7">
-        <v>7</v>
-      </c>
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="I7" s="8">
+        <v>19</v>
+      </c>
+      <c r="K7" s="6"/>
       <c r="M7">
-        <f>C7-236</f>
+        <f t="shared" si="2"/>
         <v>7</v>
       </c>
     </row>
@@ -49817,20 +49840,21 @@
         <v>7</v>
       </c>
       <c r="F8" t="s">
-        <v>67</v>
-      </c>
-      <c r="G8" t="s">
-        <v>65</v>
+        <v>61</v>
+      </c>
+      <c r="G8" t="str">
+        <f t="shared" si="0"/>
+        <v>Orange</v>
       </c>
       <c r="H8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="I8">
-        <v>17</v>
+      <c r="I8" s="6">
+        <v>15</v>
       </c>
       <c r="M8">
-        <f>C8-236</f>
+        <f t="shared" si="2"/>
         <v>7</v>
       </c>
     </row>
@@ -49848,20 +49872,21 @@
         <v>8</v>
       </c>
       <c r="F9" t="s">
-        <v>67</v>
-      </c>
-      <c r="G9" t="s">
-        <v>64</v>
+        <v>62</v>
+      </c>
+      <c r="G9" t="str">
+        <f t="shared" si="0"/>
+        <v>Pink</v>
       </c>
       <c r="H9">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="I9">
-        <v>8</v>
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="I9" s="8">
+        <v>30</v>
       </c>
       <c r="M9">
-        <f>C9-236</f>
+        <f t="shared" si="2"/>
         <v>7</v>
       </c>
     </row>
@@ -49879,20 +49904,21 @@
         <v>9</v>
       </c>
       <c r="F10" t="s">
-        <v>68</v>
-      </c>
-      <c r="G10" t="s">
-        <v>65</v>
+        <v>61</v>
+      </c>
+      <c r="G10" t="str">
+        <f t="shared" si="0"/>
+        <v>Red</v>
       </c>
       <c r="H10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="I10" s="6">
         <v>3</v>
       </c>
-      <c r="I10">
-        <v>12</v>
-      </c>
       <c r="M10">
-        <f>C10-236</f>
+        <f t="shared" si="2"/>
         <v>7</v>
       </c>
     </row>
@@ -49910,20 +49936,21 @@
         <v>10</v>
       </c>
       <c r="F11" t="s">
-        <v>70</v>
-      </c>
-      <c r="G11" t="s">
-        <v>66</v>
+        <v>62</v>
+      </c>
+      <c r="G11" t="str">
+        <f t="shared" si="0"/>
+        <v>Red</v>
       </c>
       <c r="H11">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="I11">
-        <v>22</v>
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="I11" s="6">
+        <v>8</v>
       </c>
       <c r="M11">
-        <f>C11-236</f>
+        <f t="shared" si="2"/>
         <v>7</v>
       </c>
     </row>
@@ -49941,17 +49968,21 @@
         <v>11</v>
       </c>
       <c r="F12" t="s">
-        <v>67</v>
-      </c>
-      <c r="G12" t="s">
-        <v>63</v>
+        <v>61</v>
+      </c>
+      <c r="G12" t="str">
+        <f t="shared" si="0"/>
+        <v>Control</v>
       </c>
       <c r="H12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
+      <c r="I12" s="6">
+        <v>0</v>
+      </c>
       <c r="M12">
-        <f>C12-236</f>
+        <f t="shared" si="2"/>
         <v>7</v>
       </c>
     </row>
@@ -49969,20 +50000,21 @@
         <v>12</v>
       </c>
       <c r="F13" t="s">
-        <v>67</v>
-      </c>
-      <c r="G13" t="s">
-        <v>66</v>
+        <v>61</v>
+      </c>
+      <c r="G13" t="str">
+        <f t="shared" si="0"/>
+        <v>Orange</v>
       </c>
       <c r="H13">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="I13">
-        <v>25</v>
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="I13" s="6">
+        <v>16</v>
       </c>
       <c r="M13">
-        <f>C13-236</f>
+        <f t="shared" si="2"/>
         <v>7</v>
       </c>
     </row>
@@ -49991,30 +50023,31 @@
         <v>13</v>
       </c>
       <c r="B14" s="3">
-        <v>43709</v>
+        <v>43708</v>
       </c>
       <c r="C14">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E14">
+        <v>13</v>
+      </c>
+      <c r="F14" t="s">
+        <v>62</v>
+      </c>
+      <c r="G14" t="str">
+        <f t="shared" si="0"/>
+        <v>Control</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="F14" t="s">
-        <v>69</v>
-      </c>
-      <c r="G14" t="s">
-        <v>64</v>
-      </c>
-      <c r="H14">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="I14">
-        <v>6</v>
+      <c r="I14" s="6">
+        <v>0</v>
       </c>
       <c r="M14">
-        <f>C14-236</f>
-        <v>8</v>
+        <f t="shared" si="2"/>
+        <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.3">
@@ -50022,27 +50055,31 @@
         <v>14</v>
       </c>
       <c r="B15" s="3">
-        <v>43709</v>
+        <v>43708</v>
       </c>
       <c r="C15">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E15">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="F15" t="s">
-        <v>70</v>
-      </c>
-      <c r="G15" t="s">
-        <v>63</v>
+        <v>62</v>
+      </c>
+      <c r="G15" t="str">
+        <f t="shared" si="0"/>
+        <v>Pink</v>
       </c>
       <c r="H15">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="I15" s="6">
+        <v>25</v>
       </c>
       <c r="M15">
-        <f>C15-236</f>
-        <v>8</v>
+        <f t="shared" si="2"/>
+        <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.3">
@@ -50056,23 +50093,26 @@
         <v>244</v>
       </c>
       <c r="E16">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F16" t="s">
-        <v>68</v>
-      </c>
-      <c r="G16" t="s">
-        <v>65</v>
+        <v>61</v>
+      </c>
+      <c r="G16" t="str">
+        <f t="shared" si="0"/>
+        <v>Red</v>
       </c>
       <c r="H16">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="I16">
-        <v>16</v>
-      </c>
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="I16" s="8">
+        <v>8</v>
+      </c>
+      <c r="K16" s="7"/>
+      <c r="L16" s="5"/>
       <c r="M16">
-        <f>C16-236</f>
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
     </row>
@@ -50087,23 +50127,25 @@
         <v>244</v>
       </c>
       <c r="E17">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F17" t="s">
-        <v>68</v>
-      </c>
-      <c r="G17" t="s">
-        <v>66</v>
+        <v>62</v>
+      </c>
+      <c r="G17" t="str">
+        <f t="shared" si="0"/>
+        <v>Orange</v>
       </c>
       <c r="H17">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="I17">
-        <v>26</v>
-      </c>
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="I17" s="8">
+        <v>12</v>
+      </c>
+      <c r="K17" s="8"/>
       <c r="M17">
-        <f>C17-236</f>
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
     </row>
@@ -50118,20 +50160,25 @@
         <v>244</v>
       </c>
       <c r="E18">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F18" t="s">
-        <v>70</v>
-      </c>
-      <c r="G18" t="s">
-        <v>63</v>
+        <v>61</v>
+      </c>
+      <c r="G18" t="str">
+        <f t="shared" si="0"/>
+        <v>Orange</v>
       </c>
       <c r="H18">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="I18" s="8">
+        <v>16</v>
+      </c>
+      <c r="K18" s="8"/>
       <c r="M18">
-        <f>C18-236</f>
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
     </row>
@@ -50146,23 +50193,25 @@
         <v>244</v>
       </c>
       <c r="E19">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F19" t="s">
-        <v>67</v>
-      </c>
-      <c r="G19" t="s">
-        <v>64</v>
+        <v>62</v>
+      </c>
+      <c r="G19" t="str">
+        <f t="shared" si="0"/>
+        <v>Control</v>
       </c>
       <c r="H19">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="I19">
-        <v>2</v>
-      </c>
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I19" s="8">
+        <v>0</v>
+      </c>
+      <c r="K19" s="8"/>
       <c r="M19">
-        <f>C19-236</f>
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
     </row>
@@ -50177,23 +50226,25 @@
         <v>244</v>
       </c>
       <c r="E20">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F20" t="s">
-        <v>70</v>
-      </c>
-      <c r="G20" t="s">
-        <v>66</v>
+        <v>61</v>
+      </c>
+      <c r="G20" t="str">
+        <f t="shared" si="0"/>
+        <v>Pink</v>
       </c>
       <c r="H20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="I20">
-        <v>22</v>
-      </c>
+      <c r="I20" s="8">
+        <v>25</v>
+      </c>
+      <c r="K20" s="8"/>
       <c r="M20">
-        <f>C20-236</f>
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
     </row>
@@ -50208,23 +50259,26 @@
         <v>244</v>
       </c>
       <c r="E21">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F21" t="s">
-        <v>69</v>
-      </c>
-      <c r="G21" t="s">
-        <v>64</v>
+        <v>61</v>
+      </c>
+      <c r="G21" t="str">
+        <f t="shared" si="0"/>
+        <v>Red</v>
       </c>
       <c r="H21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="I21">
-        <v>7</v>
-      </c>
+      <c r="I21" s="8">
+        <v>9</v>
+      </c>
+      <c r="K21" s="8"/>
+      <c r="L21" s="5"/>
       <c r="M21">
-        <f>C21-236</f>
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
     </row>
@@ -50239,23 +50293,24 @@
         <v>244</v>
       </c>
       <c r="E22">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F22" t="s">
-        <v>70</v>
-      </c>
-      <c r="G22" t="s">
-        <v>65</v>
+        <v>61</v>
+      </c>
+      <c r="G22" t="str">
+        <f t="shared" si="0"/>
+        <v>Pink</v>
       </c>
       <c r="H22">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="I22">
-        <v>13</v>
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="I22" s="8">
+        <v>21</v>
       </c>
       <c r="M22">
-        <f>C22-236</f>
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
     </row>
@@ -50270,23 +50325,24 @@
         <v>244</v>
       </c>
       <c r="E23">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F23" t="s">
-        <v>67</v>
-      </c>
-      <c r="G23" t="s">
-        <v>65</v>
+        <v>62</v>
+      </c>
+      <c r="G23" t="str">
+        <f t="shared" si="0"/>
+        <v>Red</v>
       </c>
       <c r="H23">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="I23">
-        <v>11</v>
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="I23" s="8">
+        <v>5</v>
       </c>
       <c r="M23">
-        <f>C23-236</f>
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
     </row>
@@ -50301,23 +50357,24 @@
         <v>244</v>
       </c>
       <c r="E24">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F24" t="s">
-        <v>69</v>
-      </c>
-      <c r="G24" t="s">
-        <v>66</v>
+        <v>61</v>
+      </c>
+      <c r="G24" t="str">
+        <f t="shared" si="0"/>
+        <v>Red</v>
       </c>
       <c r="H24">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="I24">
-        <v>23</v>
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="I24" s="8">
+        <v>7</v>
       </c>
       <c r="M24">
-        <f>C24-236</f>
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
     </row>
@@ -50332,20 +50389,24 @@
         <v>244</v>
       </c>
       <c r="E25">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F25" t="s">
-        <v>67</v>
-      </c>
-      <c r="G25" t="s">
-        <v>63</v>
+        <v>61</v>
+      </c>
+      <c r="G25" t="str">
+        <f t="shared" si="0"/>
+        <v>Red</v>
       </c>
       <c r="H25">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="I25" s="8">
+        <v>4</v>
       </c>
       <c r="M25">
-        <f>C25-236</f>
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
     </row>
@@ -50354,27 +50415,31 @@
         <v>25</v>
       </c>
       <c r="B26" s="3">
-        <v>43710</v>
+        <v>43709</v>
       </c>
       <c r="C26">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E26">
+        <v>11</v>
+      </c>
+      <c r="F26" t="s">
+        <v>62</v>
+      </c>
+      <c r="G26" t="str">
+        <f t="shared" si="0"/>
+        <v>Control</v>
+      </c>
+      <c r="H26">
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="F26" t="s">
-        <v>69</v>
-      </c>
-      <c r="G26" t="s">
-        <v>63</v>
-      </c>
-      <c r="H26">
-        <f t="shared" si="0"/>
-        <v>1</v>
+      <c r="I26" s="8">
+        <v>0</v>
       </c>
       <c r="M26">
-        <f>C26-236</f>
-        <v>9</v>
+        <f t="shared" si="2"/>
+        <v>8</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.3">
@@ -50382,30 +50447,31 @@
         <v>26</v>
       </c>
       <c r="B27" s="3">
-        <v>43710</v>
+        <v>43709</v>
       </c>
       <c r="C27">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E27">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="F27" t="s">
-        <v>69</v>
-      </c>
-      <c r="G27" t="s">
-        <v>64</v>
+        <v>61</v>
+      </c>
+      <c r="G27" t="str">
+        <f t="shared" si="0"/>
+        <v>Pink</v>
       </c>
       <c r="H27">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="I27">
-        <v>3</v>
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="I27" s="8">
+        <v>24</v>
       </c>
       <c r="M27">
-        <f>C27-236</f>
-        <v>9</v>
+        <f t="shared" si="2"/>
+        <v>8</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.3">
@@ -50413,30 +50479,31 @@
         <v>27</v>
       </c>
       <c r="B28" s="3">
-        <v>43710</v>
+        <v>43709</v>
       </c>
       <c r="C28">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E28">
+        <v>13</v>
+      </c>
+      <c r="F28" t="s">
+        <v>61</v>
+      </c>
+      <c r="G28" t="str">
+        <f t="shared" si="0"/>
+        <v>Orange</v>
+      </c>
+      <c r="H28">
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="F28" t="s">
-        <v>69</v>
-      </c>
-      <c r="G28" t="s">
-        <v>65</v>
-      </c>
-      <c r="H28">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="I28">
-        <v>14</v>
+      <c r="I28" s="8">
+        <v>13</v>
       </c>
       <c r="M28">
-        <f>C28-236</f>
-        <v>9</v>
+        <f t="shared" si="2"/>
+        <v>8</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.3">
@@ -50444,30 +50511,31 @@
         <v>28</v>
       </c>
       <c r="B29" s="3">
-        <v>43710</v>
+        <v>43709</v>
       </c>
       <c r="C29">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E29">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="F29" t="s">
-        <v>70</v>
-      </c>
-      <c r="G29" t="s">
-        <v>66</v>
+        <v>62</v>
+      </c>
+      <c r="G29" t="str">
+        <f t="shared" si="0"/>
+        <v>Control</v>
       </c>
       <c r="H29">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="I29">
-        <v>25</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I29" s="8">
+        <v>0</v>
       </c>
       <c r="M29">
-        <f>C29-236</f>
-        <v>9</v>
+        <f t="shared" si="2"/>
+        <v>8</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.3">
@@ -50481,20 +50549,26 @@
         <v>245</v>
       </c>
       <c r="E30">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F30" t="s">
-        <v>70</v>
-      </c>
-      <c r="G30" t="s">
-        <v>63</v>
+        <v>62</v>
+      </c>
+      <c r="G30" t="str">
+        <f t="shared" si="0"/>
+        <v>Control</v>
       </c>
       <c r="H30">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
+      <c r="I30" s="8">
+        <v>0</v>
+      </c>
+      <c r="K30" s="8"/>
+      <c r="L30" s="5"/>
       <c r="M30">
-        <f>C30-236</f>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
     </row>
@@ -50509,23 +50583,25 @@
         <v>245</v>
       </c>
       <c r="E31">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F31" t="s">
-        <v>67</v>
-      </c>
-      <c r="G31" t="s">
-        <v>64</v>
+        <v>62</v>
+      </c>
+      <c r="G31" t="str">
+        <f t="shared" si="0"/>
+        <v>Pink</v>
       </c>
       <c r="H31">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="I31">
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
+      <c r="I31" s="8">
+        <v>23</v>
+      </c>
+      <c r="K31" s="8"/>
       <c r="M31">
-        <f>C31-236</f>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
     </row>
@@ -50540,23 +50616,25 @@
         <v>245</v>
       </c>
       <c r="E32">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="F32" t="s">
-        <v>67</v>
-      </c>
-      <c r="G32" t="s">
-        <v>66</v>
+        <v>62</v>
+      </c>
+      <c r="G32" t="str">
+        <f t="shared" si="0"/>
+        <v>Red</v>
       </c>
       <c r="H32">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="I32">
-        <v>30</v>
-      </c>
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="I32" s="8">
+        <v>2</v>
+      </c>
+      <c r="K32" s="8"/>
       <c r="M32">
-        <f>C32-236</f>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
     </row>
@@ -50571,23 +50649,26 @@
         <v>245</v>
       </c>
       <c r="E33">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F33" t="s">
-        <v>68</v>
-      </c>
-      <c r="G33" t="s">
-        <v>65</v>
+        <v>62</v>
+      </c>
+      <c r="G33" t="str">
+        <f t="shared" si="0"/>
+        <v>Orange</v>
       </c>
       <c r="H33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="I33">
-        <v>15</v>
-      </c>
+      <c r="I33" s="8">
+        <v>14</v>
+      </c>
+      <c r="K33" s="6"/>
+      <c r="L33" s="5"/>
       <c r="M33">
-        <f>C33-236</f>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
     </row>
@@ -50602,23 +50683,25 @@
         <v>245</v>
       </c>
       <c r="E34">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="F34" t="s">
-        <v>68</v>
-      </c>
-      <c r="G34" t="s">
-        <v>66</v>
+        <v>61</v>
+      </c>
+      <c r="G34" t="str">
+        <f t="shared" si="0"/>
+        <v>Orange</v>
       </c>
       <c r="H34">
-        <f t="shared" ref="H34:H65" si="1">IF(G34="Control", 1, IF(G34="Red", 2, IF(G34="Orange", 3, 4)))</f>
-        <v>4</v>
-      </c>
-      <c r="I34">
-        <v>27</v>
-      </c>
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="I34" s="8">
+        <v>15</v>
+      </c>
+      <c r="K34" s="8"/>
       <c r="M34">
-        <f>C34-236</f>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
     </row>
@@ -50633,23 +50716,25 @@
         <v>245</v>
       </c>
       <c r="E35">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F35" t="s">
-        <v>70</v>
-      </c>
-      <c r="G35" t="s">
-        <v>65</v>
+        <v>61</v>
+      </c>
+      <c r="G35" t="str">
+        <f t="shared" si="0"/>
+        <v>Red</v>
       </c>
       <c r="H35">
         <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="I35">
-        <v>12</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="I35" s="8">
+        <v>1</v>
+      </c>
+      <c r="K35" s="8"/>
       <c r="M35">
-        <f>C35-236</f>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
     </row>
@@ -50664,20 +50749,24 @@
         <v>245</v>
       </c>
       <c r="E36">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="F36" t="s">
-        <v>67</v>
-      </c>
-      <c r="G36" t="s">
-        <v>63</v>
+        <v>62</v>
+      </c>
+      <c r="G36" t="str">
+        <f t="shared" si="0"/>
+        <v>Control</v>
       </c>
       <c r="H36">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
+      <c r="I36" s="8">
+        <v>0</v>
+      </c>
       <c r="M36">
-        <f>C36-236</f>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
     </row>
@@ -50692,23 +50781,24 @@
         <v>245</v>
       </c>
       <c r="E37">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F37" t="s">
-        <v>68</v>
-      </c>
-      <c r="G37" t="s">
-        <v>64</v>
+        <v>62</v>
+      </c>
+      <c r="G37" t="str">
+        <f t="shared" si="0"/>
+        <v>Control</v>
       </c>
       <c r="H37">
         <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="I37">
         <v>1</v>
       </c>
+      <c r="I37" s="8">
+        <v>0</v>
+      </c>
       <c r="M37">
-        <f>C37-236</f>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
     </row>
@@ -50717,30 +50807,31 @@
         <v>37</v>
       </c>
       <c r="B38" s="3">
-        <v>43711</v>
+        <v>43710</v>
       </c>
       <c r="C38">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E38">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="F38" t="s">
-        <v>68</v>
-      </c>
-      <c r="G38" t="s">
-        <v>64</v>
+        <v>62</v>
+      </c>
+      <c r="G38" t="str">
+        <f t="shared" si="0"/>
+        <v>Orange</v>
       </c>
       <c r="H38">
         <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="I38">
+        <v>3</v>
+      </c>
+      <c r="I38" s="8">
+        <v>19</v>
+      </c>
+      <c r="M38">
+        <f t="shared" si="2"/>
         <v>9</v>
-      </c>
-      <c r="M38">
-        <f>C38-236</f>
-        <v>10</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.3">
@@ -50748,30 +50839,31 @@
         <v>38</v>
       </c>
       <c r="B39" s="3">
-        <v>43711</v>
+        <v>43710</v>
       </c>
       <c r="C39">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E39">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="F39" t="s">
-        <v>69</v>
-      </c>
-      <c r="G39" t="s">
-        <v>66</v>
+        <v>62</v>
+      </c>
+      <c r="G39" t="str">
+        <f t="shared" si="0"/>
+        <v>Orange</v>
       </c>
       <c r="H39">
         <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="I39">
-        <v>24</v>
+        <v>3</v>
+      </c>
+      <c r="I39" s="8">
+        <v>11</v>
       </c>
       <c r="M39">
-        <f>C39-236</f>
-        <v>10</v>
+        <f t="shared" si="2"/>
+        <v>9</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.3">
@@ -50779,30 +50871,31 @@
         <v>39</v>
       </c>
       <c r="B40" s="3">
-        <v>43711</v>
+        <v>43710</v>
       </c>
       <c r="C40">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E40">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="F40" t="s">
-        <v>68</v>
-      </c>
-      <c r="G40" t="s">
-        <v>65</v>
+        <v>61</v>
+      </c>
+      <c r="G40" t="str">
+        <f t="shared" si="0"/>
+        <v>Pink</v>
       </c>
       <c r="H40">
         <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="I40">
-        <v>17</v>
+        <v>4</v>
+      </c>
+      <c r="I40" s="8">
+        <v>22</v>
       </c>
       <c r="M40">
-        <f>C40-236</f>
-        <v>10</v>
+        <f t="shared" si="2"/>
+        <v>9</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.3">
@@ -50810,27 +50903,31 @@
         <v>40</v>
       </c>
       <c r="B41" s="3">
-        <v>43711</v>
+        <v>43710</v>
       </c>
       <c r="C41">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E41">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="F41" t="s">
-        <v>70</v>
-      </c>
-      <c r="G41" t="s">
-        <v>63</v>
+        <v>61</v>
+      </c>
+      <c r="G41" t="str">
+        <f t="shared" si="0"/>
+        <v>Red</v>
       </c>
       <c r="H41">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="I41" s="8">
+        <v>6</v>
       </c>
       <c r="M41">
-        <f>C41-236</f>
-        <v>10</v>
+        <f t="shared" si="2"/>
+        <v>9</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.3">
@@ -50838,27 +50935,31 @@
         <v>41</v>
       </c>
       <c r="B42" s="3">
-        <v>43711</v>
+        <v>43710</v>
       </c>
       <c r="C42">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E42">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="F42" t="s">
-        <v>68</v>
-      </c>
-      <c r="G42" t="s">
-        <v>63</v>
+        <v>62</v>
+      </c>
+      <c r="G42" t="str">
+        <f t="shared" si="0"/>
+        <v>Pink</v>
       </c>
       <c r="H42">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>4</v>
+      </c>
+      <c r="I42" s="8">
+        <v>27</v>
       </c>
       <c r="M42">
-        <f>C42-236</f>
-        <v>10</v>
+        <f t="shared" si="2"/>
+        <v>9</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.3">
@@ -50866,30 +50967,31 @@
         <v>42</v>
       </c>
       <c r="B43" s="3">
-        <v>43711</v>
+        <v>43710</v>
       </c>
       <c r="C43">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E43">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="F43" t="s">
-        <v>67</v>
-      </c>
-      <c r="G43" t="s">
-        <v>66</v>
+        <v>61</v>
+      </c>
+      <c r="G43" t="str">
+        <f t="shared" si="0"/>
+        <v>Orange</v>
       </c>
       <c r="H43">
         <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="I43">
-        <v>23</v>
+        <v>3</v>
+      </c>
+      <c r="I43" s="8">
+        <v>20</v>
       </c>
       <c r="M43">
-        <f>C43-236</f>
-        <v>10</v>
+        <f t="shared" si="2"/>
+        <v>9</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.3">
@@ -50903,23 +51005,24 @@
         <v>246</v>
       </c>
       <c r="E44">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="F44" t="s">
-        <v>70</v>
-      </c>
-      <c r="G44" t="s">
-        <v>64</v>
+        <v>62</v>
+      </c>
+      <c r="G44" t="str">
+        <f t="shared" si="0"/>
+        <v>Red</v>
       </c>
       <c r="H44">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="I44">
-        <v>2</v>
+      <c r="I44" s="8">
+        <v>5</v>
       </c>
       <c r="M44">
-        <f>C44-236</f>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
     </row>
@@ -50934,23 +51037,25 @@
         <v>246</v>
       </c>
       <c r="E45">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="F45" t="s">
-        <v>69</v>
-      </c>
-      <c r="G45" t="s">
-        <v>65</v>
+        <v>61</v>
+      </c>
+      <c r="G45" t="str">
+        <f t="shared" si="0"/>
+        <v>Pink</v>
       </c>
       <c r="H45">
         <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="I45">
-        <v>13</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="I45" s="8">
+        <v>29</v>
+      </c>
+      <c r="K45" s="8"/>
       <c r="M45">
-        <f>C45-236</f>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
     </row>
@@ -50965,20 +51070,25 @@
         <v>246</v>
       </c>
       <c r="E46">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="F46" t="s">
-        <v>69</v>
-      </c>
-      <c r="G46" t="s">
-        <v>63</v>
+        <v>61</v>
+      </c>
+      <c r="G46" t="str">
+        <f t="shared" si="0"/>
+        <v>Red</v>
       </c>
       <c r="H46">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="I46" s="8">
+        <v>3</v>
+      </c>
+      <c r="K46" s="8"/>
       <c r="M46">
-        <f>C46-236</f>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
     </row>
@@ -50993,23 +51103,26 @@
         <v>246</v>
       </c>
       <c r="E47">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="F47" t="s">
-        <v>67</v>
-      </c>
-      <c r="G47" t="s">
-        <v>64</v>
+        <v>62</v>
+      </c>
+      <c r="G47" t="str">
+        <f t="shared" si="0"/>
+        <v>Orange</v>
       </c>
       <c r="H47">
         <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="I47">
-        <v>9</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="I47" s="8">
+        <v>18</v>
+      </c>
+      <c r="K47" s="8"/>
+      <c r="L47" s="5"/>
       <c r="M47">
-        <f>C47-236</f>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
     </row>
@@ -51024,23 +51137,25 @@
         <v>246</v>
       </c>
       <c r="E48">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="F48" t="s">
-        <v>68</v>
-      </c>
-      <c r="G48" t="s">
-        <v>65</v>
+        <v>61</v>
+      </c>
+      <c r="G48" t="str">
+        <f t="shared" si="0"/>
+        <v>Control</v>
       </c>
       <c r="H48">
         <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="I48">
-        <v>19</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="I48" s="8">
+        <v>0</v>
+      </c>
+      <c r="K48" s="8"/>
       <c r="M48">
-        <f>C48-236</f>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
     </row>
@@ -51055,23 +51170,24 @@
         <v>246</v>
       </c>
       <c r="E49">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="F49" t="s">
-        <v>67</v>
-      </c>
-      <c r="G49" t="s">
-        <v>66</v>
+        <v>61</v>
+      </c>
+      <c r="G49" t="str">
+        <f t="shared" si="0"/>
+        <v>Pink</v>
       </c>
       <c r="H49">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="I49">
-        <v>21</v>
+      <c r="I49" s="8">
+        <v>27</v>
       </c>
       <c r="M49">
-        <f>C49-236</f>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
     </row>
@@ -51080,27 +51196,31 @@
         <v>49</v>
       </c>
       <c r="B50" s="3">
-        <v>43712</v>
+        <v>43711</v>
       </c>
       <c r="C50">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E50">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F50" t="s">
-        <v>70</v>
-      </c>
-      <c r="G50" t="s">
-        <v>63</v>
+        <v>61</v>
+      </c>
+      <c r="G50" t="str">
+        <f t="shared" si="0"/>
+        <v>Pink</v>
       </c>
       <c r="H50">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>4</v>
+      </c>
+      <c r="I50" s="8">
+        <v>28</v>
       </c>
       <c r="M50">
-        <f>C50-236</f>
-        <v>11</v>
+        <f t="shared" si="2"/>
+        <v>10</v>
       </c>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.3">
@@ -51108,30 +51228,31 @@
         <v>50</v>
       </c>
       <c r="B51" s="3">
-        <v>43712</v>
+        <v>43711</v>
       </c>
       <c r="C51">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E51">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="F51" t="s">
-        <v>68</v>
-      </c>
-      <c r="G51" t="s">
-        <v>65</v>
+        <v>62</v>
+      </c>
+      <c r="G51" t="str">
+        <f t="shared" si="0"/>
+        <v>Pink</v>
       </c>
       <c r="H51">
         <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="I51">
-        <v>11</v>
+        <v>4</v>
+      </c>
+      <c r="I51" s="8">
+        <v>26</v>
       </c>
       <c r="M51">
-        <f>C51-236</f>
-        <v>11</v>
+        <f t="shared" si="2"/>
+        <v>10</v>
       </c>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.3">
@@ -51139,30 +51260,31 @@
         <v>51</v>
       </c>
       <c r="B52" s="3">
-        <v>43712</v>
+        <v>43711</v>
       </c>
       <c r="C52">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E52">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="F52" t="s">
-        <v>69</v>
-      </c>
-      <c r="G52" t="s">
-        <v>64</v>
+        <v>61</v>
+      </c>
+      <c r="G52" t="str">
+        <f t="shared" si="0"/>
+        <v>Orange</v>
       </c>
       <c r="H52">
         <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="I52">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="I52" s="8">
+        <v>14</v>
       </c>
       <c r="M52">
         <f>C52-239</f>
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.3">
@@ -51170,30 +51292,31 @@
         <v>52</v>
       </c>
       <c r="B53" s="3">
-        <v>43712</v>
+        <v>43711</v>
       </c>
       <c r="C53">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E53">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="F53" t="s">
-        <v>67</v>
-      </c>
-      <c r="G53" t="s">
-        <v>66</v>
+        <v>62</v>
+      </c>
+      <c r="G53" t="str">
+        <f t="shared" si="0"/>
+        <v>Orange</v>
       </c>
       <c r="H53">
         <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="I53">
-        <v>24</v>
+        <v>3</v>
+      </c>
+      <c r="I53" s="8">
+        <v>17</v>
       </c>
       <c r="M53">
-        <f>C53-239</f>
-        <v>8</v>
+        <f t="shared" ref="M53:M77" si="3">C53-239</f>
+        <v>7</v>
       </c>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.3">
@@ -51201,30 +51324,31 @@
         <v>53</v>
       </c>
       <c r="B54" s="3">
-        <v>43712</v>
+        <v>43711</v>
       </c>
       <c r="C54">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E54">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="F54" t="s">
-        <v>68</v>
-      </c>
-      <c r="G54" t="s">
-        <v>64</v>
+        <v>61</v>
+      </c>
+      <c r="G54" t="str">
+        <f t="shared" si="0"/>
+        <v>Pink</v>
       </c>
       <c r="H54">
         <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="I54">
-        <v>5</v>
+        <v>4</v>
+      </c>
+      <c r="I54" s="8">
+        <v>23</v>
       </c>
       <c r="M54">
-        <f>C54-239</f>
-        <v>8</v>
+        <f t="shared" si="3"/>
+        <v>7</v>
       </c>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.3">
@@ -51232,27 +51356,31 @@
         <v>54</v>
       </c>
       <c r="B55" s="3">
-        <v>43712</v>
+        <v>43711</v>
       </c>
       <c r="C55">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E55">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="F55" t="s">
-        <v>67</v>
-      </c>
-      <c r="G55" t="s">
-        <v>63</v>
+        <v>61</v>
+      </c>
+      <c r="G55" t="str">
+        <f t="shared" si="0"/>
+        <v>Control</v>
       </c>
       <c r="H55">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
+      <c r="I55" s="8">
+        <v>0</v>
+      </c>
       <c r="M55">
-        <f>C55-239</f>
-        <v>8</v>
+        <f t="shared" si="3"/>
+        <v>7</v>
       </c>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.3">
@@ -51260,30 +51388,31 @@
         <v>55</v>
       </c>
       <c r="B56" s="3">
-        <v>43712</v>
+        <v>43711</v>
       </c>
       <c r="C56">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E56">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="F56" t="s">
-        <v>68</v>
-      </c>
-      <c r="G56" t="s">
-        <v>64</v>
+        <v>61</v>
+      </c>
+      <c r="G56" t="str">
+        <f t="shared" si="0"/>
+        <v>Control</v>
       </c>
       <c r="H56">
         <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="I56">
-        <v>10</v>
+        <v>1</v>
+      </c>
+      <c r="I56" s="8">
+        <v>0</v>
       </c>
       <c r="M56">
-        <f>C56-239</f>
-        <v>8</v>
+        <f t="shared" si="3"/>
+        <v>7</v>
       </c>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.3">
@@ -51291,27 +51420,31 @@
         <v>56</v>
       </c>
       <c r="B57" s="3">
-        <v>43712</v>
+        <v>43711</v>
       </c>
       <c r="C57">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E57">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="F57" t="s">
-        <v>69</v>
-      </c>
-      <c r="G57" t="s">
-        <v>63</v>
+        <v>61</v>
+      </c>
+      <c r="G57" t="str">
+        <f t="shared" si="0"/>
+        <v>Red</v>
       </c>
       <c r="H57">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="I57" s="8">
+        <v>10</v>
       </c>
       <c r="M57">
-        <f>C57-239</f>
-        <v>8</v>
+        <f t="shared" si="3"/>
+        <v>7</v>
       </c>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.3">
@@ -51319,30 +51452,32 @@
         <v>57</v>
       </c>
       <c r="B58" s="3">
-        <v>43712</v>
+        <v>43716</v>
       </c>
       <c r="C58">
-        <v>247</v>
+        <v>251</v>
       </c>
       <c r="E58">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="F58" t="s">
-        <v>67</v>
-      </c>
-      <c r="G58" t="s">
-        <v>65</v>
+        <v>61</v>
+      </c>
+      <c r="G58" t="str">
+        <f t="shared" si="0"/>
+        <v>Control</v>
       </c>
       <c r="H58">
         <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="I58">
-        <v>20</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="I58" s="8">
+        <v>0</v>
+      </c>
+      <c r="K58" s="8"/>
       <c r="M58">
-        <f>C58-239</f>
-        <v>8</v>
+        <f t="shared" si="3"/>
+        <v>12</v>
       </c>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.3">
@@ -51350,30 +51485,32 @@
         <v>58</v>
       </c>
       <c r="B59" s="3">
-        <v>43712</v>
+        <v>43716</v>
       </c>
       <c r="C59">
-        <v>247</v>
+        <v>251</v>
       </c>
       <c r="E59">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="F59" t="s">
-        <v>67</v>
-      </c>
-      <c r="G59" t="s">
-        <v>66</v>
+        <v>61</v>
+      </c>
+      <c r="G59" t="str">
+        <f t="shared" si="0"/>
+        <v>Orange</v>
       </c>
       <c r="H59">
         <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="I59">
-        <v>30</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="I59" s="8">
+        <v>17</v>
+      </c>
+      <c r="K59" s="6"/>
       <c r="M59">
-        <f>C59-239</f>
-        <v>8</v>
+        <f t="shared" si="3"/>
+        <v>12</v>
       </c>
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.3">
@@ -51381,30 +51518,32 @@
         <v>59</v>
       </c>
       <c r="B60" s="3">
-        <v>43712</v>
+        <v>43716</v>
       </c>
       <c r="C60">
-        <v>247</v>
+        <v>251</v>
       </c>
       <c r="E60">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="F60" t="s">
-        <v>68</v>
-      </c>
-      <c r="G60" t="s">
-        <v>65</v>
+        <v>61</v>
+      </c>
+      <c r="G60" t="str">
+        <f t="shared" si="0"/>
+        <v>Pink</v>
       </c>
       <c r="H60">
         <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="I60">
-        <v>15</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="I60" s="8">
+        <v>24</v>
+      </c>
+      <c r="K60" s="6"/>
       <c r="M60">
-        <f>C60-239</f>
-        <v>8</v>
+        <f t="shared" si="3"/>
+        <v>12</v>
       </c>
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.3">
@@ -51412,30 +51551,32 @@
         <v>60</v>
       </c>
       <c r="B61" s="3">
-        <v>43712</v>
+        <v>43716</v>
       </c>
       <c r="C61">
-        <v>247</v>
+        <v>251</v>
       </c>
       <c r="E61">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="F61" t="s">
-        <v>69</v>
-      </c>
-      <c r="G61" t="s">
-        <v>66</v>
+        <v>62</v>
+      </c>
+      <c r="G61" t="str">
+        <f t="shared" si="0"/>
+        <v>Pink</v>
       </c>
       <c r="H61">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="I61">
-        <v>21</v>
-      </c>
+      <c r="I61" s="8">
+        <v>22</v>
+      </c>
+      <c r="K61" s="6"/>
       <c r="M61">
-        <f>C61-239</f>
-        <v>8</v>
+        <f t="shared" si="3"/>
+        <v>12</v>
       </c>
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.3">
@@ -51443,27 +51584,32 @@
         <v>61</v>
       </c>
       <c r="B62" s="3">
-        <v>43713</v>
+        <v>43716</v>
       </c>
       <c r="C62">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="E62">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F62" t="s">
-        <v>70</v>
-      </c>
-      <c r="G62" t="s">
-        <v>63</v>
+        <v>62</v>
+      </c>
+      <c r="G62" t="str">
+        <f t="shared" si="0"/>
+        <v>Pink</v>
       </c>
       <c r="H62">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="I62" s="8">
+        <v>28</v>
+      </c>
+      <c r="K62" s="6"/>
       <c r="M62">
-        <f>C62-239</f>
-        <v>9</v>
+        <f t="shared" si="3"/>
+        <v>12</v>
       </c>
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.3">
@@ -51471,30 +51617,32 @@
         <v>62</v>
       </c>
       <c r="B63" s="3">
-        <v>43713</v>
+        <v>43716</v>
       </c>
       <c r="C63">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="E63">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="F63" t="s">
-        <v>68</v>
-      </c>
-      <c r="G63" t="s">
-        <v>65</v>
+        <v>61</v>
+      </c>
+      <c r="G63" t="str">
+        <f t="shared" si="0"/>
+        <v>Red</v>
       </c>
       <c r="H63">
         <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="I63">
-        <v>18</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="I63" s="8">
+        <v>10</v>
+      </c>
+      <c r="K63" s="6"/>
       <c r="M63">
-        <f>C63-239</f>
-        <v>9</v>
+        <f t="shared" si="3"/>
+        <v>12</v>
       </c>
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.3">
@@ -51502,30 +51650,32 @@
         <v>63</v>
       </c>
       <c r="B64" s="3">
-        <v>43713</v>
+        <v>43716</v>
       </c>
       <c r="C64">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="E64">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="F64" t="s">
-        <v>69</v>
-      </c>
-      <c r="G64" t="s">
-        <v>64</v>
+        <v>62</v>
+      </c>
+      <c r="G64" t="str">
+        <f t="shared" si="0"/>
+        <v>Red</v>
       </c>
       <c r="H64">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="I64">
-        <v>8</v>
-      </c>
+      <c r="I64" s="8">
+        <v>2</v>
+      </c>
+      <c r="K64" s="6"/>
       <c r="M64">
-        <f>C64-239</f>
-        <v>9</v>
+        <f t="shared" si="3"/>
+        <v>12</v>
       </c>
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.3">
@@ -51533,30 +51683,32 @@
         <v>64</v>
       </c>
       <c r="B65" s="3">
-        <v>43713</v>
+        <v>43716</v>
       </c>
       <c r="C65">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="E65">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="F65" t="s">
-        <v>67</v>
-      </c>
-      <c r="G65" t="s">
-        <v>66</v>
+        <v>61</v>
+      </c>
+      <c r="G65" t="str">
+        <f t="shared" si="0"/>
+        <v>Control</v>
       </c>
       <c r="H65">
         <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="I65">
-        <v>29</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="I65" s="8">
+        <v>0</v>
+      </c>
+      <c r="K65" s="6"/>
       <c r="M65">
-        <f>C65-239</f>
-        <v>9</v>
+        <f t="shared" si="3"/>
+        <v>12</v>
       </c>
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.3">
@@ -51564,30 +51716,32 @@
         <v>65</v>
       </c>
       <c r="B66" s="3">
-        <v>43713</v>
+        <v>43716</v>
       </c>
       <c r="C66">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="E66">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="F66" t="s">
-        <v>69</v>
-      </c>
-      <c r="G66" t="s">
-        <v>64</v>
+        <v>62</v>
+      </c>
+      <c r="G66" t="str">
+        <f t="shared" si="0"/>
+        <v>Pink</v>
       </c>
       <c r="H66">
-        <f t="shared" ref="H66:H81" si="2">IF(G66="Control", 1, IF(G66="Red", 2, IF(G66="Orange", 3, 4)))</f>
-        <v>2</v>
-      </c>
-      <c r="I66">
-        <v>10</v>
-      </c>
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="I66" s="6">
+        <v>29</v>
+      </c>
+      <c r="K66" s="6"/>
       <c r="M66">
-        <f>C66-239</f>
-        <v>9</v>
+        <f t="shared" si="3"/>
+        <v>12</v>
       </c>
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.3">
@@ -51595,27 +51749,32 @@
         <v>66</v>
       </c>
       <c r="B67" s="3">
-        <v>43713</v>
+        <v>43716</v>
       </c>
       <c r="C67">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="E67">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="F67" t="s">
-        <v>68</v>
-      </c>
-      <c r="G67" t="s">
-        <v>63</v>
+        <v>61</v>
+      </c>
+      <c r="G67" t="str">
+        <f t="shared" ref="G67:G77" si="4">IF(I67&lt;=0, "Control", IF(I67&lt;=10, "Red", IF(I67&gt;=21, "Pink", "Orange")))</f>
+        <v>Red</v>
       </c>
       <c r="H67">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
+        <f t="shared" ref="H67:H77" si="5">IF(G67="Control", 1, IF(G67="Red", 2, IF(G67="Orange", 3, 4)))</f>
+        <v>2</v>
+      </c>
+      <c r="I67" s="6">
+        <v>9</v>
+      </c>
+      <c r="K67" s="6"/>
       <c r="M67">
-        <f>C67-239</f>
-        <v>9</v>
+        <f t="shared" si="3"/>
+        <v>12</v>
       </c>
     </row>
     <row r="68" spans="1:13" x14ac:dyDescent="0.3">
@@ -51623,30 +51782,32 @@
         <v>67</v>
       </c>
       <c r="B68" s="3">
-        <v>43713</v>
+        <v>43716</v>
       </c>
       <c r="C68">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="E68">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="F68" t="s">
-        <v>67</v>
-      </c>
-      <c r="G68" t="s">
-        <v>64</v>
+        <v>61</v>
+      </c>
+      <c r="G68" t="str">
+        <f t="shared" si="4"/>
+        <v>Orange</v>
       </c>
       <c r="H68">
-        <f t="shared" si="2"/>
-        <v>2</v>
-      </c>
-      <c r="I68">
-        <v>5</v>
-      </c>
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="I68" s="6">
+        <v>18</v>
+      </c>
+      <c r="K68" s="6"/>
       <c r="M68">
-        <f>C68-239</f>
-        <v>9</v>
+        <f t="shared" si="3"/>
+        <v>12</v>
       </c>
     </row>
     <row r="69" spans="1:13" x14ac:dyDescent="0.3">
@@ -51654,27 +51815,32 @@
         <v>68</v>
       </c>
       <c r="B69" s="3">
-        <v>43713</v>
+        <v>43716</v>
       </c>
       <c r="C69">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="E69">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="F69" t="s">
-        <v>69</v>
-      </c>
-      <c r="G69" t="s">
-        <v>63</v>
+        <v>62</v>
+      </c>
+      <c r="G69" t="str">
+        <f t="shared" si="4"/>
+        <v>Orange</v>
       </c>
       <c r="H69">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="I69" s="6">
+        <v>12</v>
+      </c>
+      <c r="K69" s="6"/>
       <c r="M69">
-        <f>C69-239</f>
-        <v>9</v>
+        <f t="shared" si="3"/>
+        <v>12</v>
       </c>
     </row>
     <row r="70" spans="1:13" x14ac:dyDescent="0.3">
@@ -51682,30 +51848,32 @@
         <v>69</v>
       </c>
       <c r="B70" s="3">
-        <v>43713</v>
+        <v>43716</v>
       </c>
       <c r="C70">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="E70">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F70" t="s">
-        <v>68</v>
-      </c>
-      <c r="G70" t="s">
-        <v>65</v>
+        <v>61</v>
+      </c>
+      <c r="G70" t="str">
+        <f t="shared" si="4"/>
+        <v>Control</v>
       </c>
       <c r="H70">
-        <f t="shared" si="2"/>
-        <v>3</v>
-      </c>
-      <c r="I70">
-        <v>20</v>
-      </c>
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="I70" s="6">
+        <v>0</v>
+      </c>
+      <c r="K70" s="6"/>
       <c r="M70">
-        <f>C70-239</f>
-        <v>9</v>
+        <f t="shared" si="3"/>
+        <v>12</v>
       </c>
     </row>
     <row r="71" spans="1:13" x14ac:dyDescent="0.3">
@@ -51713,30 +51881,32 @@
         <v>70</v>
       </c>
       <c r="B71" s="3">
-        <v>43713</v>
+        <v>43716</v>
       </c>
       <c r="C71">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="E71">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="F71" t="s">
-        <v>67</v>
-      </c>
-      <c r="G71" t="s">
-        <v>66</v>
+        <v>61</v>
+      </c>
+      <c r="G71" t="str">
+        <f t="shared" si="4"/>
+        <v>Red</v>
       </c>
       <c r="H71">
-        <f t="shared" si="2"/>
-        <v>4</v>
-      </c>
-      <c r="I71">
-        <v>28</v>
-      </c>
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="I71" s="6">
+        <v>1</v>
+      </c>
+      <c r="K71" s="6"/>
       <c r="M71">
-        <f>C71-239</f>
-        <v>9</v>
+        <f t="shared" si="3"/>
+        <v>12</v>
       </c>
     </row>
     <row r="72" spans="1:13" x14ac:dyDescent="0.3">
@@ -51744,30 +51914,32 @@
         <v>71</v>
       </c>
       <c r="B72" s="3">
-        <v>43713</v>
+        <v>43717</v>
       </c>
       <c r="C72">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="E72">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="F72" t="s">
-        <v>69</v>
-      </c>
-      <c r="G72" t="s">
-        <v>65</v>
+        <v>61</v>
+      </c>
+      <c r="G72" t="str">
+        <f t="shared" si="4"/>
+        <v>Control</v>
       </c>
       <c r="H72">
-        <f t="shared" si="2"/>
-        <v>3</v>
-      </c>
-      <c r="I72">
-        <v>19</v>
-      </c>
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="I72" s="8">
+        <v>0</v>
+      </c>
+      <c r="K72" s="6"/>
       <c r="M72">
-        <f>C72-239</f>
-        <v>9</v>
+        <f t="shared" si="3"/>
+        <v>13</v>
       </c>
     </row>
     <row r="73" spans="1:13" x14ac:dyDescent="0.3">
@@ -51775,30 +51947,32 @@
         <v>72</v>
       </c>
       <c r="B73" s="3">
-        <v>43713</v>
+        <v>43717</v>
       </c>
       <c r="C73">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="E73">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="F73" t="s">
-        <v>67</v>
-      </c>
-      <c r="G73" t="s">
-        <v>66</v>
+        <v>62</v>
+      </c>
+      <c r="G73" t="str">
+        <f t="shared" si="4"/>
+        <v>Pink</v>
       </c>
       <c r="H73">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
-      <c r="I73">
-        <v>27</v>
-      </c>
+      <c r="I73" s="8">
+        <v>26</v>
+      </c>
+      <c r="K73" s="6"/>
       <c r="M73">
-        <f>C73-239</f>
-        <v>9</v>
+        <f t="shared" si="3"/>
+        <v>13</v>
       </c>
     </row>
     <row r="74" spans="1:13" x14ac:dyDescent="0.3">
@@ -51806,30 +51980,32 @@
         <v>73</v>
       </c>
       <c r="B74" s="3">
-        <v>43714</v>
+        <v>43717</v>
       </c>
       <c r="C74">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="E74">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F74" t="s">
-        <v>68</v>
-      </c>
-      <c r="G74" t="s">
-        <v>66</v>
+        <v>62</v>
+      </c>
+      <c r="G74" t="str">
+        <f t="shared" si="4"/>
+        <v>Orange</v>
       </c>
       <c r="H74">
-        <f t="shared" si="2"/>
-        <v>4</v>
-      </c>
-      <c r="I74">
-        <v>26</v>
-      </c>
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="I74" s="8">
+        <v>13</v>
+      </c>
+      <c r="K74" s="6"/>
       <c r="M74">
-        <f>C74-239</f>
-        <v>10</v>
+        <f t="shared" si="3"/>
+        <v>13</v>
       </c>
     </row>
     <row r="75" spans="1:13" x14ac:dyDescent="0.3">
@@ -51837,30 +52013,32 @@
         <v>74</v>
       </c>
       <c r="B75" s="3">
-        <v>43714</v>
+        <v>43717</v>
       </c>
       <c r="C75">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="E75">
+        <v>4</v>
+      </c>
+      <c r="F75" t="s">
+        <v>62</v>
+      </c>
+      <c r="G75" t="str">
+        <f t="shared" si="4"/>
+        <v>Red</v>
+      </c>
+      <c r="H75">
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
-      <c r="F75" t="s">
-        <v>70</v>
-      </c>
-      <c r="G75" t="s">
-        <v>65</v>
-      </c>
-      <c r="H75">
-        <f t="shared" si="2"/>
-        <v>3</v>
-      </c>
-      <c r="I75">
-        <v>18</v>
-      </c>
+      <c r="I75" s="8">
+        <v>4</v>
+      </c>
+      <c r="K75" s="6"/>
       <c r="M75">
-        <f>C75-239</f>
-        <v>10</v>
+        <f t="shared" si="3"/>
+        <v>13</v>
       </c>
     </row>
     <row r="76" spans="1:13" x14ac:dyDescent="0.3">
@@ -51868,27 +52046,32 @@
         <v>75</v>
       </c>
       <c r="B76" s="3">
-        <v>43714</v>
+        <v>43717</v>
       </c>
       <c r="C76">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="E76">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F76" t="s">
-        <v>69</v>
-      </c>
-      <c r="G76" t="s">
-        <v>63</v>
+        <v>61</v>
+      </c>
+      <c r="G76" t="str">
+        <f t="shared" si="4"/>
+        <v>Pink</v>
       </c>
       <c r="H76">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
+      <c r="I76" s="8">
+        <v>30</v>
+      </c>
+      <c r="K76" s="6"/>
       <c r="M76">
-        <f>C76-239</f>
-        <v>10</v>
+        <f t="shared" si="3"/>
+        <v>13</v>
       </c>
     </row>
     <row r="77" spans="1:13" x14ac:dyDescent="0.3">
@@ -51896,154 +52079,38 @@
         <v>76</v>
       </c>
       <c r="B77" s="3">
-        <v>43714</v>
+        <v>43717</v>
       </c>
       <c r="C77">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="E77">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F77" t="s">
-        <v>68</v>
-      </c>
-      <c r="G77" t="s">
-        <v>64</v>
+        <v>61</v>
+      </c>
+      <c r="G77" t="str">
+        <f t="shared" si="4"/>
+        <v>Red</v>
       </c>
       <c r="H77">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
-      <c r="I77">
-        <v>3</v>
-      </c>
+      <c r="I77" s="8">
+        <v>6</v>
+      </c>
+      <c r="K77" s="6"/>
       <c r="M77">
-        <f>C77-239</f>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A78">
-        <v>77</v>
-      </c>
-      <c r="B78" s="3">
-        <v>43714</v>
-      </c>
-      <c r="C78">
-        <v>249</v>
-      </c>
-      <c r="E78">
-        <v>5</v>
-      </c>
-      <c r="F78" t="s">
-        <v>69</v>
-      </c>
-      <c r="G78" t="s">
-        <v>63</v>
-      </c>
-      <c r="H78">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="M78">
-        <f>C78-239</f>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A79">
-        <v>78</v>
-      </c>
-      <c r="B79" s="3">
-        <v>43714</v>
-      </c>
-      <c r="C79">
-        <v>249</v>
-      </c>
-      <c r="E79">
-        <v>6</v>
-      </c>
-      <c r="F79" t="s">
-        <v>67</v>
-      </c>
-      <c r="G79" t="s">
-        <v>64</v>
-      </c>
-      <c r="H79">
-        <f t="shared" si="2"/>
-        <v>2</v>
-      </c>
-      <c r="I79">
-        <v>4</v>
-      </c>
-      <c r="M79">
-        <f>C79-239</f>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A80">
-        <v>79</v>
-      </c>
-      <c r="B80" s="3">
-        <v>43714</v>
-      </c>
-      <c r="C80">
-        <v>249</v>
-      </c>
-      <c r="E80">
-        <v>7</v>
-      </c>
-      <c r="F80" t="s">
-        <v>68</v>
-      </c>
-      <c r="G80" t="s">
-        <v>66</v>
-      </c>
-      <c r="H80">
-        <f t="shared" si="2"/>
-        <v>4</v>
-      </c>
-      <c r="I80">
-        <v>28</v>
-      </c>
-      <c r="M80">
-        <f>C80-239</f>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A81">
-        <v>80</v>
-      </c>
-      <c r="B81" s="3">
-        <v>43714</v>
-      </c>
-      <c r="C81">
-        <v>249</v>
-      </c>
-      <c r="E81">
-        <v>8</v>
-      </c>
-      <c r="F81" t="s">
-        <v>68</v>
-      </c>
-      <c r="G81" t="s">
-        <v>65</v>
-      </c>
-      <c r="H81">
-        <f t="shared" si="2"/>
-        <v>3</v>
-      </c>
-      <c r="I81">
-        <v>14</v>
-      </c>
-      <c r="M81">
-        <f>C81-239</f>
-        <v>10</v>
+        <f t="shared" si="3"/>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="K64:L71">
+    <sortCondition ref="K64"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -52051,10 +52118,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55F6BF2F-CBB2-4331-929A-D3F4AD694052}">
-  <dimension ref="A1:X22"/>
+  <dimension ref="A1:X27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F19" sqref="F19:J22"/>
+      <selection activeCell="L30" sqref="L30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -52086,7 +52153,7 @@
   <sheetData>
     <row r="1" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
@@ -52098,7 +52165,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>4</v>
@@ -52128,7 +52195,7 @@
         <v>15</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="P1" s="2" t="s">
         <v>16</v>
@@ -52146,7 +52213,7 @@
         <v>20</v>
       </c>
       <c r="U1" s="2" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="V1" s="2" t="s">
         <v>21</v>
@@ -52158,7 +52225,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="6:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="6:13" x14ac:dyDescent="0.3">
       <c r="F19">
         <v>9</v>
       </c>
@@ -52166,17 +52233,23 @@
         <v>81</v>
       </c>
       <c r="H19" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="I19" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="J19">
         <f>IF(I19="Control", 1, IF(I19="Red", 2, IF(I19="Orange", 3, 4)))</f>
         <v>3</v>
       </c>
-    </row>
-    <row r="20" spans="6:10" x14ac:dyDescent="0.3">
+      <c r="L19" t="s">
+        <v>63</v>
+      </c>
+      <c r="M19" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="20" spans="6:13" x14ac:dyDescent="0.3">
       <c r="F20">
         <v>10</v>
       </c>
@@ -52184,17 +52257,23 @@
         <v>82</v>
       </c>
       <c r="H20" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="I20" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="J20">
         <f>IF(I20="Control", 1, IF(I20="Red", 2, IF(I20="Orange", 3, 4)))</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="6:10" x14ac:dyDescent="0.3">
+      <c r="L20">
+        <v>26</v>
+      </c>
+      <c r="M20">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="6:13" x14ac:dyDescent="0.3">
       <c r="F21">
         <v>11</v>
       </c>
@@ -52202,17 +52281,23 @@
         <v>83</v>
       </c>
       <c r="H21" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="I21" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="J21">
         <f>IF(I21="Control", 1, IF(I21="Red", 2, IF(I21="Orange", 3, 4)))</f>
         <v>2</v>
       </c>
-    </row>
-    <row r="22" spans="6:10" x14ac:dyDescent="0.3">
+      <c r="L21">
+        <v>6</v>
+      </c>
+      <c r="M21">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="6:13" x14ac:dyDescent="0.3">
       <c r="F22">
         <v>12</v>
       </c>
@@ -52220,13 +52305,41 @@
         <v>84</v>
       </c>
       <c r="H22" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="I22" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="J22">
         <f>IF(I22="Control", 1, IF(I22="Red", 2, IF(I22="Orange", 3, 4)))</f>
+        <v>4</v>
+      </c>
+      <c r="L22">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="23" spans="6:13" x14ac:dyDescent="0.3">
+      <c r="L23">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="24" spans="6:13" x14ac:dyDescent="0.3">
+      <c r="L24">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="25" spans="6:13" x14ac:dyDescent="0.3">
+      <c r="L25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="6:13" x14ac:dyDescent="0.3">
+      <c r="L26">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="6:13" x14ac:dyDescent="0.3">
+      <c r="L27">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Readme updated, data sheet updated with starvation time
</commit_message>
<xml_diff>
--- a/data/raw.xlsx
+++ b/data/raw.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Amelia\github\Ritger-Corynactis-urchin-deterrence\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A84760D6-7A3D-43BC-9B45-3D49ADEA12F5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0F68F65-639B-4EF4-9CF2-6BBDC4D66E85}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15" yWindow="-17520" windowWidth="26535" windowHeight="16380" xr2:uid="{58E670A5-634C-427F-960F-9DA76C64E810}"/>
+    <workbookView xWindow="870" yWindow="-17160" windowWidth="26535" windowHeight="16380" activeTab="1" xr2:uid="{58E670A5-634C-427F-960F-9DA76C64E810}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="3" r:id="rId1"/>
@@ -300,14 +300,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -624,7 +624,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{168F7463-EB05-46FE-9A95-7790352FDB02}">
   <dimension ref="A1:B16244"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -640,10 +640,10 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="B3" s="4"/>
+      <c r="B3" s="9"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
@@ -665,7 +665,7 @@
       <c r="A6" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="8" t="s">
         <v>70</v>
       </c>
     </row>
@@ -809,10 +809,10 @@
       <c r="A24" s="2"/>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A25" s="4" t="s">
+      <c r="A25" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="B25" s="4"/>
+      <c r="B25" s="9"/>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
@@ -49532,11 +49532,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD5E687B-43EE-4B00-8604-7EB9984510DD}">
-  <dimension ref="A1:U77"/>
+  <dimension ref="A1:U78"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I4" sqref="I4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H63" sqref="H63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -49549,7 +49549,7 @@
     <col min="6" max="6" width="12.44140625" customWidth="1"/>
     <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17.77734375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.109375" style="5" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="7.88671875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="15.77734375" customWidth="1"/>
     <col min="12" max="12" width="16" bestFit="1" customWidth="1"/>
@@ -49589,7 +49589,7 @@
       <c r="H1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="I1" s="6" t="s">
         <v>5</v>
       </c>
       <c r="J1" s="2" t="s">
@@ -49653,13 +49653,19 @@
         <f>IF(G2="Control", 1, IF(G2="Red", 2, IF(G2="Orange", 3, 4)))</f>
         <v>3</v>
       </c>
-      <c r="I2" s="8">
+      <c r="I2" s="7">
         <v>11</v>
       </c>
       <c r="M2">
         <f>C2-236</f>
         <v>7</v>
       </c>
+      <c r="N2">
+        <v>1900</v>
+      </c>
+      <c r="O2">
+        <v>700</v>
+      </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A3">
@@ -49685,10 +49691,10 @@
         <f t="shared" ref="H3:H66" si="1">IF(G3="Control", 1, IF(G3="Red", 2, IF(G3="Orange", 3, 4)))</f>
         <v>3</v>
       </c>
-      <c r="I3" s="8">
+      <c r="I3" s="7">
         <v>20</v>
       </c>
-      <c r="K3" s="6"/>
+      <c r="K3" s="5"/>
       <c r="M3">
         <f t="shared" ref="M3:M51" si="2">C3-236</f>
         <v>7</v>
@@ -49718,10 +49724,10 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="I4" s="8">
+      <c r="I4" s="7">
         <v>0</v>
       </c>
-      <c r="K4" s="6"/>
+      <c r="K4" s="5"/>
       <c r="M4">
         <f t="shared" si="2"/>
         <v>7</v>
@@ -49751,10 +49757,10 @@
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="I5" s="8">
+      <c r="I5" s="7">
         <v>7</v>
       </c>
-      <c r="K5" s="6"/>
+      <c r="K5" s="5"/>
       <c r="M5">
         <f t="shared" si="2"/>
         <v>7</v>
@@ -49784,10 +49790,10 @@
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="I6" s="8">
+      <c r="I6" s="7">
         <v>21</v>
       </c>
-      <c r="K6" s="6"/>
+      <c r="K6" s="5"/>
       <c r="M6">
         <f t="shared" si="2"/>
         <v>7</v>
@@ -49817,10 +49823,10 @@
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="I7" s="8">
+      <c r="I7" s="7">
         <v>19</v>
       </c>
-      <c r="K7" s="6"/>
+      <c r="K7" s="5"/>
       <c r="M7">
         <f t="shared" si="2"/>
         <v>7</v>
@@ -49850,7 +49856,7 @@
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="I8" s="6">
+      <c r="I8" s="5">
         <v>15</v>
       </c>
       <c r="M8">
@@ -49882,7 +49888,7 @@
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="I9" s="8">
+      <c r="I9" s="7">
         <v>30</v>
       </c>
       <c r="M9">
@@ -49914,7 +49920,7 @@
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="I10" s="6">
+      <c r="I10" s="5">
         <v>3</v>
       </c>
       <c r="M10">
@@ -49946,7 +49952,7 @@
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="I11" s="6">
+      <c r="I11" s="5">
         <v>8</v>
       </c>
       <c r="M11">
@@ -49978,7 +49984,7 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="I12" s="6">
+      <c r="I12" s="5">
         <v>0</v>
       </c>
       <c r="M12">
@@ -50010,7 +50016,7 @@
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="I13" s="6">
+      <c r="I13" s="5">
         <v>16</v>
       </c>
       <c r="M13">
@@ -50042,7 +50048,7 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="I14" s="6">
+      <c r="I14" s="5">
         <v>0</v>
       </c>
       <c r="M14">
@@ -50074,7 +50080,7 @@
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="I15" s="6">
+      <c r="I15" s="5">
         <v>25</v>
       </c>
       <c r="M15">
@@ -50106,11 +50112,11 @@
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="I16" s="8">
+      <c r="I16" s="7">
         <v>8</v>
       </c>
-      <c r="K16" s="7"/>
-      <c r="L16" s="5"/>
+      <c r="K16" s="6"/>
+      <c r="L16" s="4"/>
       <c r="M16">
         <f t="shared" si="2"/>
         <v>8</v>
@@ -50140,10 +50146,10 @@
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="I17" s="8">
+      <c r="I17" s="7">
         <v>12</v>
       </c>
-      <c r="K17" s="8"/>
+      <c r="K17" s="7"/>
       <c r="M17">
         <f t="shared" si="2"/>
         <v>8</v>
@@ -50173,10 +50179,10 @@
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="I18" s="8">
+      <c r="I18" s="7">
         <v>16</v>
       </c>
-      <c r="K18" s="8"/>
+      <c r="K18" s="7"/>
       <c r="M18">
         <f t="shared" si="2"/>
         <v>8</v>
@@ -50206,10 +50212,10 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="I19" s="8">
+      <c r="I19" s="7">
         <v>0</v>
       </c>
-      <c r="K19" s="8"/>
+      <c r="K19" s="7"/>
       <c r="M19">
         <f t="shared" si="2"/>
         <v>8</v>
@@ -50239,10 +50245,10 @@
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="I20" s="8">
+      <c r="I20" s="7">
         <v>25</v>
       </c>
-      <c r="K20" s="8"/>
+      <c r="K20" s="7"/>
       <c r="M20">
         <f t="shared" si="2"/>
         <v>8</v>
@@ -50272,11 +50278,11 @@
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="I21" s="8">
+      <c r="I21" s="7">
         <v>9</v>
       </c>
-      <c r="K21" s="8"/>
-      <c r="L21" s="5"/>
+      <c r="K21" s="7"/>
+      <c r="L21" s="4"/>
       <c r="M21">
         <f t="shared" si="2"/>
         <v>8</v>
@@ -50306,7 +50312,7 @@
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="I22" s="8">
+      <c r="I22" s="7">
         <v>21</v>
       </c>
       <c r="M22">
@@ -50338,7 +50344,7 @@
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="I23" s="8">
+      <c r="I23" s="7">
         <v>5</v>
       </c>
       <c r="M23">
@@ -50370,7 +50376,7 @@
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="I24" s="8">
+      <c r="I24" s="7">
         <v>7</v>
       </c>
       <c r="M24">
@@ -50402,7 +50408,7 @@
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="I25" s="8">
+      <c r="I25" s="7">
         <v>4</v>
       </c>
       <c r="M25">
@@ -50434,7 +50440,7 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="I26" s="8">
+      <c r="I26" s="7">
         <v>0</v>
       </c>
       <c r="M26">
@@ -50466,7 +50472,7 @@
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="I27" s="8">
+      <c r="I27" s="7">
         <v>24</v>
       </c>
       <c r="M27">
@@ -50498,7 +50504,7 @@
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="I28" s="8">
+      <c r="I28" s="7">
         <v>13</v>
       </c>
       <c r="M28">
@@ -50530,7 +50536,7 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="I29" s="8">
+      <c r="I29" s="7">
         <v>0</v>
       </c>
       <c r="M29">
@@ -50562,11 +50568,11 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="I30" s="8">
+      <c r="I30" s="7">
         <v>0</v>
       </c>
-      <c r="K30" s="8"/>
-      <c r="L30" s="5"/>
+      <c r="K30" s="7"/>
+      <c r="L30" s="4"/>
       <c r="M30">
         <f t="shared" si="2"/>
         <v>9</v>
@@ -50596,10 +50602,10 @@
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="I31" s="8">
+      <c r="I31" s="7">
         <v>23</v>
       </c>
-      <c r="K31" s="8"/>
+      <c r="K31" s="7"/>
       <c r="M31">
         <f t="shared" si="2"/>
         <v>9</v>
@@ -50629,10 +50635,10 @@
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="I32" s="8">
+      <c r="I32" s="7">
         <v>2</v>
       </c>
-      <c r="K32" s="8"/>
+      <c r="K32" s="7"/>
       <c r="M32">
         <f t="shared" si="2"/>
         <v>9</v>
@@ -50662,11 +50668,11 @@
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="I33" s="8">
+      <c r="I33" s="7">
         <v>14</v>
       </c>
-      <c r="K33" s="6"/>
-      <c r="L33" s="5"/>
+      <c r="K33" s="5"/>
+      <c r="L33" s="4"/>
       <c r="M33">
         <f t="shared" si="2"/>
         <v>9</v>
@@ -50696,10 +50702,10 @@
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="I34" s="8">
+      <c r="I34" s="7">
         <v>15</v>
       </c>
-      <c r="K34" s="8"/>
+      <c r="K34" s="7"/>
       <c r="M34">
         <f t="shared" si="2"/>
         <v>9</v>
@@ -50729,10 +50735,10 @@
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="I35" s="8">
+      <c r="I35" s="7">
         <v>1</v>
       </c>
-      <c r="K35" s="8"/>
+      <c r="K35" s="7"/>
       <c r="M35">
         <f t="shared" si="2"/>
         <v>9</v>
@@ -50762,7 +50768,7 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="I36" s="8">
+      <c r="I36" s="7">
         <v>0</v>
       </c>
       <c r="M36">
@@ -50794,7 +50800,7 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="I37" s="8">
+      <c r="I37" s="7">
         <v>0</v>
       </c>
       <c r="M37">
@@ -50826,7 +50832,7 @@
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="I38" s="8">
+      <c r="I38" s="7">
         <v>19</v>
       </c>
       <c r="M38">
@@ -50858,7 +50864,7 @@
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="I39" s="8">
+      <c r="I39" s="7">
         <v>11</v>
       </c>
       <c r="M39">
@@ -50890,7 +50896,7 @@
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="I40" s="8">
+      <c r="I40" s="7">
         <v>22</v>
       </c>
       <c r="M40">
@@ -50922,7 +50928,7 @@
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="I41" s="8">
+      <c r="I41" s="7">
         <v>6</v>
       </c>
       <c r="M41">
@@ -50954,7 +50960,7 @@
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="I42" s="8">
+      <c r="I42" s="7">
         <v>27</v>
       </c>
       <c r="M42">
@@ -50986,7 +50992,7 @@
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="I43" s="8">
+      <c r="I43" s="7">
         <v>20</v>
       </c>
       <c r="M43">
@@ -51018,7 +51024,7 @@
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="I44" s="8">
+      <c r="I44" s="7">
         <v>5</v>
       </c>
       <c r="M44">
@@ -51050,10 +51056,10 @@
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="I45" s="8">
+      <c r="I45" s="7">
         <v>29</v>
       </c>
-      <c r="K45" s="8"/>
+      <c r="K45" s="7"/>
       <c r="M45">
         <f t="shared" si="2"/>
         <v>10</v>
@@ -51083,10 +51089,10 @@
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="I46" s="8">
+      <c r="I46" s="7">
         <v>3</v>
       </c>
-      <c r="K46" s="8"/>
+      <c r="K46" s="7"/>
       <c r="M46">
         <f t="shared" si="2"/>
         <v>10</v>
@@ -51116,11 +51122,11 @@
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="I47" s="8">
+      <c r="I47" s="7">
         <v>18</v>
       </c>
-      <c r="K47" s="8"/>
-      <c r="L47" s="5"/>
+      <c r="K47" s="7"/>
+      <c r="L47" s="4"/>
       <c r="M47">
         <f t="shared" si="2"/>
         <v>10</v>
@@ -51150,10 +51156,10 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="I48" s="8">
+      <c r="I48" s="7">
         <v>0</v>
       </c>
-      <c r="K48" s="8"/>
+      <c r="K48" s="7"/>
       <c r="M48">
         <f t="shared" si="2"/>
         <v>10</v>
@@ -51183,7 +51189,7 @@
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="I49" s="8">
+      <c r="I49" s="7">
         <v>27</v>
       </c>
       <c r="M49">
@@ -51215,7 +51221,7 @@
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="I50" s="8">
+      <c r="I50" s="7">
         <v>28</v>
       </c>
       <c r="M50">
@@ -51247,7 +51253,7 @@
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="I51" s="8">
+      <c r="I51" s="7">
         <v>26</v>
       </c>
       <c r="M51">
@@ -51279,7 +51285,7 @@
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="I52" s="8">
+      <c r="I52" s="7">
         <v>14</v>
       </c>
       <c r="M52">
@@ -51311,7 +51317,7 @@
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="I53" s="8">
+      <c r="I53" s="7">
         <v>17</v>
       </c>
       <c r="M53">
@@ -51343,7 +51349,7 @@
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="I54" s="8">
+      <c r="I54" s="7">
         <v>23</v>
       </c>
       <c r="M54">
@@ -51375,7 +51381,7 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="I55" s="8">
+      <c r="I55" s="7">
         <v>0</v>
       </c>
       <c r="M55">
@@ -51407,7 +51413,7 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="I56" s="8">
+      <c r="I56" s="7">
         <v>0</v>
       </c>
       <c r="M56">
@@ -51439,7 +51445,7 @@
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="I57" s="8">
+      <c r="I57" s="7">
         <v>10</v>
       </c>
       <c r="M57">
@@ -51452,10 +51458,10 @@
         <v>57</v>
       </c>
       <c r="B58" s="3">
-        <v>43716</v>
+        <v>43713</v>
       </c>
       <c r="C58">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="E58">
         <v>1</v>
@@ -51471,13 +51477,13 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="I58" s="8">
+      <c r="I58" s="7">
         <v>0</v>
       </c>
-      <c r="K58" s="8"/>
+      <c r="K58" s="7"/>
       <c r="M58">
         <f t="shared" si="3"/>
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.3">
@@ -51485,10 +51491,10 @@
         <v>58</v>
       </c>
       <c r="B59" s="3">
-        <v>43716</v>
+        <v>43713</v>
       </c>
       <c r="C59">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="E59">
         <v>2</v>
@@ -51504,13 +51510,13 @@
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="I59" s="8">
+      <c r="I59" s="7">
         <v>17</v>
       </c>
-      <c r="K59" s="6"/>
+      <c r="K59" s="5"/>
       <c r="M59">
         <f t="shared" si="3"/>
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.3">
@@ -51518,10 +51524,10 @@
         <v>59</v>
       </c>
       <c r="B60" s="3">
-        <v>43716</v>
+        <v>43713</v>
       </c>
       <c r="C60">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="E60">
         <v>3</v>
@@ -51537,13 +51543,13 @@
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="I60" s="8">
+      <c r="I60" s="7">
         <v>24</v>
       </c>
-      <c r="K60" s="6"/>
+      <c r="K60" s="5"/>
       <c r="M60">
         <f t="shared" si="3"/>
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.3">
@@ -51551,10 +51557,10 @@
         <v>60</v>
       </c>
       <c r="B61" s="3">
-        <v>43716</v>
+        <v>43713</v>
       </c>
       <c r="C61">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="E61">
         <v>4</v>
@@ -51570,13 +51576,13 @@
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="I61" s="8">
+      <c r="I61" s="7">
         <v>22</v>
       </c>
-      <c r="K61" s="6"/>
+      <c r="K61" s="5"/>
       <c r="M61">
         <f t="shared" si="3"/>
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.3">
@@ -51584,10 +51590,10 @@
         <v>61</v>
       </c>
       <c r="B62" s="3">
-        <v>43716</v>
+        <v>43713</v>
       </c>
       <c r="C62">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="E62">
         <v>5</v>
@@ -51603,13 +51609,13 @@
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="I62" s="8">
+      <c r="I62" s="7">
         <v>28</v>
       </c>
-      <c r="K62" s="6"/>
+      <c r="K62" s="5"/>
       <c r="M62">
         <f t="shared" si="3"/>
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.3">
@@ -51617,10 +51623,10 @@
         <v>62</v>
       </c>
       <c r="B63" s="3">
-        <v>43716</v>
+        <v>43713</v>
       </c>
       <c r="C63">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="E63">
         <v>6</v>
@@ -51636,13 +51642,13 @@
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="I63" s="8">
+      <c r="I63" s="7">
         <v>10</v>
       </c>
-      <c r="K63" s="6"/>
+      <c r="K63" s="5"/>
       <c r="M63">
         <f t="shared" si="3"/>
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.3">
@@ -51650,10 +51656,10 @@
         <v>63</v>
       </c>
       <c r="B64" s="3">
-        <v>43716</v>
+        <v>43713</v>
       </c>
       <c r="C64">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="E64">
         <v>7</v>
@@ -51669,13 +51675,13 @@
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="I64" s="8">
+      <c r="I64" s="7">
         <v>2</v>
       </c>
-      <c r="K64" s="6"/>
+      <c r="K64" s="5"/>
       <c r="M64">
         <f t="shared" si="3"/>
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.3">
@@ -51683,10 +51689,10 @@
         <v>64</v>
       </c>
       <c r="B65" s="3">
-        <v>43716</v>
+        <v>43713</v>
       </c>
       <c r="C65">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="E65">
         <v>8</v>
@@ -51702,13 +51708,13 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="I65" s="8">
+      <c r="I65" s="7">
         <v>0</v>
       </c>
-      <c r="K65" s="6"/>
+      <c r="K65" s="5"/>
       <c r="M65">
         <f t="shared" si="3"/>
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.3">
@@ -51716,10 +51722,10 @@
         <v>65</v>
       </c>
       <c r="B66" s="3">
-        <v>43716</v>
+        <v>43713</v>
       </c>
       <c r="C66">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="E66">
         <v>9</v>
@@ -51735,13 +51741,13 @@
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="I66" s="6">
+      <c r="I66" s="5">
         <v>29</v>
       </c>
-      <c r="K66" s="6"/>
+      <c r="K66" s="5"/>
       <c r="M66">
         <f t="shared" si="3"/>
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.3">
@@ -51749,10 +51755,10 @@
         <v>66</v>
       </c>
       <c r="B67" s="3">
-        <v>43716</v>
+        <v>43713</v>
       </c>
       <c r="C67">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="E67">
         <v>10</v>
@@ -51768,13 +51774,13 @@
         <f t="shared" ref="H67:H77" si="5">IF(G67="Control", 1, IF(G67="Red", 2, IF(G67="Orange", 3, 4)))</f>
         <v>2</v>
       </c>
-      <c r="I67" s="6">
+      <c r="I67" s="5">
         <v>9</v>
       </c>
-      <c r="K67" s="6"/>
+      <c r="K67" s="5"/>
       <c r="M67">
         <f t="shared" si="3"/>
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="68" spans="1:13" x14ac:dyDescent="0.3">
@@ -51782,10 +51788,10 @@
         <v>67</v>
       </c>
       <c r="B68" s="3">
-        <v>43716</v>
+        <v>43713</v>
       </c>
       <c r="C68">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="E68">
         <v>11</v>
@@ -51801,13 +51807,13 @@
         <f t="shared" si="5"/>
         <v>3</v>
       </c>
-      <c r="I68" s="6">
+      <c r="I68" s="5">
         <v>18</v>
       </c>
-      <c r="K68" s="6"/>
+      <c r="K68" s="5"/>
       <c r="M68">
         <f t="shared" si="3"/>
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="69" spans="1:13" x14ac:dyDescent="0.3">
@@ -51815,10 +51821,10 @@
         <v>68</v>
       </c>
       <c r="B69" s="3">
-        <v>43716</v>
+        <v>43713</v>
       </c>
       <c r="C69">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="E69">
         <v>12</v>
@@ -51834,13 +51840,13 @@
         <f t="shared" si="5"/>
         <v>3</v>
       </c>
-      <c r="I69" s="6">
+      <c r="I69" s="5">
         <v>12</v>
       </c>
-      <c r="K69" s="6"/>
+      <c r="K69" s="5"/>
       <c r="M69">
         <f t="shared" si="3"/>
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="70" spans="1:13" x14ac:dyDescent="0.3">
@@ -51848,10 +51854,10 @@
         <v>69</v>
       </c>
       <c r="B70" s="3">
-        <v>43716</v>
+        <v>43713</v>
       </c>
       <c r="C70">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="E70">
         <v>13</v>
@@ -51867,13 +51873,13 @@
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-      <c r="I70" s="6">
+      <c r="I70" s="5">
         <v>0</v>
       </c>
-      <c r="K70" s="6"/>
+      <c r="K70" s="5"/>
       <c r="M70">
         <f t="shared" si="3"/>
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="71" spans="1:13" x14ac:dyDescent="0.3">
@@ -51881,10 +51887,10 @@
         <v>70</v>
       </c>
       <c r="B71" s="3">
-        <v>43716</v>
+        <v>43713</v>
       </c>
       <c r="C71">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="E71">
         <v>14</v>
@@ -51900,13 +51906,13 @@
         <f t="shared" si="5"/>
         <v>2</v>
       </c>
-      <c r="I71" s="6">
+      <c r="I71" s="5">
         <v>1</v>
       </c>
-      <c r="K71" s="6"/>
+      <c r="K71" s="5"/>
       <c r="M71">
         <f t="shared" si="3"/>
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="72" spans="1:13" x14ac:dyDescent="0.3">
@@ -51914,10 +51920,10 @@
         <v>71</v>
       </c>
       <c r="B72" s="3">
-        <v>43717</v>
+        <v>43714</v>
       </c>
       <c r="C72">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="E72">
         <v>1</v>
@@ -51933,13 +51939,13 @@
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-      <c r="I72" s="8">
+      <c r="I72" s="7">
         <v>0</v>
       </c>
-      <c r="K72" s="6"/>
+      <c r="K72" s="5"/>
       <c r="M72">
         <f t="shared" si="3"/>
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="73" spans="1:13" x14ac:dyDescent="0.3">
@@ -51947,10 +51953,10 @@
         <v>72</v>
       </c>
       <c r="B73" s="3">
-        <v>43717</v>
+        <v>43714</v>
       </c>
       <c r="C73">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="E73">
         <v>2</v>
@@ -51966,13 +51972,13 @@
         <f t="shared" si="5"/>
         <v>4</v>
       </c>
-      <c r="I73" s="8">
+      <c r="I73" s="7">
         <v>26</v>
       </c>
-      <c r="K73" s="6"/>
+      <c r="K73" s="5"/>
       <c r="M73">
         <f t="shared" si="3"/>
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="74" spans="1:13" x14ac:dyDescent="0.3">
@@ -51980,10 +51986,10 @@
         <v>73</v>
       </c>
       <c r="B74" s="3">
-        <v>43717</v>
+        <v>43714</v>
       </c>
       <c r="C74">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="E74">
         <v>3</v>
@@ -51999,13 +52005,13 @@
         <f t="shared" si="5"/>
         <v>3</v>
       </c>
-      <c r="I74" s="8">
+      <c r="I74" s="7">
         <v>13</v>
       </c>
-      <c r="K74" s="6"/>
+      <c r="K74" s="5"/>
       <c r="M74">
         <f t="shared" si="3"/>
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="75" spans="1:13" x14ac:dyDescent="0.3">
@@ -52013,10 +52019,10 @@
         <v>74</v>
       </c>
       <c r="B75" s="3">
-        <v>43717</v>
+        <v>43714</v>
       </c>
       <c r="C75">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="E75">
         <v>4</v>
@@ -52032,13 +52038,13 @@
         <f t="shared" si="5"/>
         <v>2</v>
       </c>
-      <c r="I75" s="8">
+      <c r="I75" s="7">
         <v>4</v>
       </c>
-      <c r="K75" s="6"/>
+      <c r="K75" s="5"/>
       <c r="M75">
         <f t="shared" si="3"/>
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="76" spans="1:13" x14ac:dyDescent="0.3">
@@ -52046,10 +52052,10 @@
         <v>75</v>
       </c>
       <c r="B76" s="3">
-        <v>43717</v>
+        <v>43714</v>
       </c>
       <c r="C76">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="E76">
         <v>5</v>
@@ -52065,13 +52071,13 @@
         <f t="shared" si="5"/>
         <v>4</v>
       </c>
-      <c r="I76" s="8">
+      <c r="I76" s="7">
         <v>30</v>
       </c>
-      <c r="K76" s="6"/>
+      <c r="K76" s="5"/>
       <c r="M76">
         <f t="shared" si="3"/>
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="77" spans="1:13" x14ac:dyDescent="0.3">
@@ -52079,10 +52085,10 @@
         <v>76</v>
       </c>
       <c r="B77" s="3">
-        <v>43717</v>
+        <v>43714</v>
       </c>
       <c r="C77">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="E77">
         <v>6</v>
@@ -52098,14 +52104,17 @@
         <f t="shared" si="5"/>
         <v>2</v>
       </c>
-      <c r="I77" s="8">
+      <c r="I77" s="7">
         <v>6</v>
       </c>
-      <c r="K77" s="6"/>
+      <c r="K77" s="5"/>
       <c r="M77">
         <f t="shared" si="3"/>
-        <v>13</v>
-      </c>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="78" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B78" s="3"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="K64:L71">

</xml_diff>

<commit_message>
data and readme updated before trial
</commit_message>
<xml_diff>
--- a/data/raw.xlsx
+++ b/data/raw.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Amelia\github\Ritger-Corynactis-urchin-deterrence\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0F68F65-639B-4EF4-9CF2-6BBDC4D66E85}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E492580C-E0CA-47C2-81C2-BF6B27DF8B50}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="870" yWindow="-17160" windowWidth="26535" windowHeight="16380" activeTab="1" xr2:uid="{58E670A5-634C-427F-960F-9DA76C64E810}"/>
+    <workbookView xWindow="0" yWindow="-16680" windowWidth="21600" windowHeight="12675" activeTab="1" xr2:uid="{58E670A5-634C-427F-960F-9DA76C64E810}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="3" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="70">
   <si>
     <t>Day</t>
   </si>
@@ -213,9 +213,6 @@
   </si>
   <si>
     <t>Orange</t>
-  </si>
-  <si>
-    <t>Pink</t>
   </si>
   <si>
     <t>N</t>
@@ -658,7 +655,7 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -666,7 +663,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -674,7 +671,7 @@
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -682,7 +679,7 @@
         <v>27</v>
       </c>
       <c r="B8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -690,7 +687,7 @@
         <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
@@ -698,7 +695,7 @@
         <v>5</v>
       </c>
       <c r="B10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -49532,11 +49529,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD5E687B-43EE-4B00-8604-7EB9984510DD}">
-  <dimension ref="A1:U78"/>
+  <dimension ref="A1:U77"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H63" sqref="H63"/>
+      <selection pane="bottomLeft" activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -49643,7 +49640,7 @@
         <v>1</v>
       </c>
       <c r="F2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G2" t="str">
         <f>IF(I2&lt;=0, "Control", IF(I2&lt;=10, "Red", IF(I2&gt;=21, "Pink", "Orange")))</f>
@@ -49681,14 +49678,14 @@
         <v>2</v>
       </c>
       <c r="F3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G3" t="str">
-        <f t="shared" ref="G3:G66" si="0">IF(I3&lt;=0, "Control", IF(I3&lt;=10, "Red", IF(I3&gt;=21, "Pink", "Orange")))</f>
+        <f t="shared" ref="G3:G57" si="0">IF(I3&lt;=0, "Control", IF(I3&lt;=10, "Red", IF(I3&gt;=21, "Pink", "Orange")))</f>
         <v>Orange</v>
       </c>
       <c r="H3">
-        <f t="shared" ref="H3:H66" si="1">IF(G3="Control", 1, IF(G3="Red", 2, IF(G3="Orange", 3, 4)))</f>
+        <f t="shared" ref="H3:H57" si="1">IF(G3="Control", 1, IF(G3="Red", 2, IF(G3="Orange", 3, 4)))</f>
         <v>3</v>
       </c>
       <c r="I3" s="7">
@@ -49714,7 +49711,7 @@
         <v>3</v>
       </c>
       <c r="F4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G4" t="str">
         <f t="shared" si="0"/>
@@ -49747,7 +49744,7 @@
         <v>4</v>
       </c>
       <c r="F5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G5" t="str">
         <f t="shared" si="0"/>
@@ -49780,7 +49777,7 @@
         <v>5</v>
       </c>
       <c r="F6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G6" t="str">
         <f t="shared" si="0"/>
@@ -49813,7 +49810,7 @@
         <v>6</v>
       </c>
       <c r="F7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G7" t="str">
         <f t="shared" si="0"/>
@@ -49846,7 +49843,7 @@
         <v>7</v>
       </c>
       <c r="F8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G8" t="str">
         <f t="shared" si="0"/>
@@ -49878,7 +49875,7 @@
         <v>8</v>
       </c>
       <c r="F9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G9" t="str">
         <f t="shared" si="0"/>
@@ -49910,7 +49907,7 @@
         <v>9</v>
       </c>
       <c r="F10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G10" t="str">
         <f t="shared" si="0"/>
@@ -49942,7 +49939,7 @@
         <v>10</v>
       </c>
       <c r="F11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G11" t="str">
         <f t="shared" si="0"/>
@@ -49974,7 +49971,7 @@
         <v>11</v>
       </c>
       <c r="F12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G12" t="str">
         <f t="shared" si="0"/>
@@ -50006,7 +50003,7 @@
         <v>12</v>
       </c>
       <c r="F13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G13" t="str">
         <f t="shared" si="0"/>
@@ -50038,7 +50035,7 @@
         <v>13</v>
       </c>
       <c r="F14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G14" t="str">
         <f t="shared" si="0"/>
@@ -50070,7 +50067,7 @@
         <v>14</v>
       </c>
       <c r="F15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G15" t="str">
         <f t="shared" si="0"/>
@@ -50102,7 +50099,7 @@
         <v>1</v>
       </c>
       <c r="F16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G16" t="str">
         <f t="shared" si="0"/>
@@ -50136,7 +50133,7 @@
         <v>2</v>
       </c>
       <c r="F17" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G17" t="str">
         <f t="shared" si="0"/>
@@ -50169,7 +50166,7 @@
         <v>3</v>
       </c>
       <c r="F18" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G18" t="str">
         <f t="shared" si="0"/>
@@ -50202,7 +50199,7 @@
         <v>4</v>
       </c>
       <c r="F19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G19" t="str">
         <f t="shared" si="0"/>
@@ -50235,7 +50232,7 @@
         <v>5</v>
       </c>
       <c r="F20" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G20" t="str">
         <f t="shared" si="0"/>
@@ -50268,7 +50265,7 @@
         <v>6</v>
       </c>
       <c r="F21" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G21" t="str">
         <f t="shared" si="0"/>
@@ -50302,7 +50299,7 @@
         <v>7</v>
       </c>
       <c r="F22" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G22" t="str">
         <f t="shared" si="0"/>
@@ -50334,7 +50331,7 @@
         <v>8</v>
       </c>
       <c r="F23" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G23" t="str">
         <f t="shared" si="0"/>
@@ -50366,7 +50363,7 @@
         <v>9</v>
       </c>
       <c r="F24" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G24" t="str">
         <f t="shared" si="0"/>
@@ -50398,7 +50395,7 @@
         <v>10</v>
       </c>
       <c r="F25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G25" t="str">
         <f t="shared" si="0"/>
@@ -50430,7 +50427,7 @@
         <v>11</v>
       </c>
       <c r="F26" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G26" t="str">
         <f t="shared" si="0"/>
@@ -50462,7 +50459,7 @@
         <v>12</v>
       </c>
       <c r="F27" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G27" t="str">
         <f t="shared" si="0"/>
@@ -50494,7 +50491,7 @@
         <v>13</v>
       </c>
       <c r="F28" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G28" t="str">
         <f t="shared" si="0"/>
@@ -50526,7 +50523,7 @@
         <v>14</v>
       </c>
       <c r="F29" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G29" t="str">
         <f t="shared" si="0"/>
@@ -50558,7 +50555,7 @@
         <v>1</v>
       </c>
       <c r="F30" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G30" t="str">
         <f t="shared" si="0"/>
@@ -50592,7 +50589,7 @@
         <v>2</v>
       </c>
       <c r="F31" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G31" t="str">
         <f t="shared" si="0"/>
@@ -50625,7 +50622,7 @@
         <v>3</v>
       </c>
       <c r="F32" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G32" t="str">
         <f t="shared" si="0"/>
@@ -50658,7 +50655,7 @@
         <v>4</v>
       </c>
       <c r="F33" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G33" t="str">
         <f t="shared" si="0"/>
@@ -50692,7 +50689,7 @@
         <v>5</v>
       </c>
       <c r="F34" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G34" t="str">
         <f t="shared" si="0"/>
@@ -50725,7 +50722,7 @@
         <v>6</v>
       </c>
       <c r="F35" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G35" t="str">
         <f t="shared" si="0"/>
@@ -50758,7 +50755,7 @@
         <v>7</v>
       </c>
       <c r="F36" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G36" t="str">
         <f t="shared" si="0"/>
@@ -50790,7 +50787,7 @@
         <v>8</v>
       </c>
       <c r="F37" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G37" t="str">
         <f t="shared" si="0"/>
@@ -50822,7 +50819,7 @@
         <v>9</v>
       </c>
       <c r="F38" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G38" t="str">
         <f t="shared" si="0"/>
@@ -50854,7 +50851,7 @@
         <v>10</v>
       </c>
       <c r="F39" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G39" t="str">
         <f t="shared" si="0"/>
@@ -50886,7 +50883,7 @@
         <v>11</v>
       </c>
       <c r="F40" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G40" t="str">
         <f t="shared" si="0"/>
@@ -50918,7 +50915,7 @@
         <v>12</v>
       </c>
       <c r="F41" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G41" t="str">
         <f t="shared" si="0"/>
@@ -50950,7 +50947,7 @@
         <v>13</v>
       </c>
       <c r="F42" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G42" t="str">
         <f t="shared" si="0"/>
@@ -50982,7 +50979,7 @@
         <v>14</v>
       </c>
       <c r="F43" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G43" t="str">
         <f t="shared" si="0"/>
@@ -51014,7 +51011,7 @@
         <v>1</v>
       </c>
       <c r="F44" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G44" t="str">
         <f t="shared" si="0"/>
@@ -51046,7 +51043,7 @@
         <v>2</v>
       </c>
       <c r="F45" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G45" t="str">
         <f t="shared" si="0"/>
@@ -51079,7 +51076,7 @@
         <v>3</v>
       </c>
       <c r="F46" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G46" t="str">
         <f t="shared" si="0"/>
@@ -51112,7 +51109,7 @@
         <v>4</v>
       </c>
       <c r="F47" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G47" t="str">
         <f t="shared" si="0"/>
@@ -51146,7 +51143,7 @@
         <v>5</v>
       </c>
       <c r="F48" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G48" t="str">
         <f t="shared" si="0"/>
@@ -51179,7 +51176,7 @@
         <v>6</v>
       </c>
       <c r="F49" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G49" t="str">
         <f t="shared" si="0"/>
@@ -51211,7 +51208,7 @@
         <v>7</v>
       </c>
       <c r="F50" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G50" t="str">
         <f t="shared" si="0"/>
@@ -51243,7 +51240,7 @@
         <v>8</v>
       </c>
       <c r="F51" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G51" t="str">
         <f t="shared" si="0"/>
@@ -51275,7 +51272,7 @@
         <v>9</v>
       </c>
       <c r="F52" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G52" t="str">
         <f t="shared" si="0"/>
@@ -51307,7 +51304,7 @@
         <v>10</v>
       </c>
       <c r="F53" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G53" t="str">
         <f t="shared" si="0"/>
@@ -51339,7 +51336,7 @@
         <v>11</v>
       </c>
       <c r="F54" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G54" t="str">
         <f t="shared" si="0"/>
@@ -51371,7 +51368,7 @@
         <v>12</v>
       </c>
       <c r="F55" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G55" t="str">
         <f t="shared" si="0"/>
@@ -51403,7 +51400,7 @@
         <v>13</v>
       </c>
       <c r="F56" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G56" t="str">
         <f t="shared" si="0"/>
@@ -51435,7 +51432,7 @@
         <v>14</v>
       </c>
       <c r="F57" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G57" t="str">
         <f t="shared" si="0"/>
@@ -51458,32 +51455,32 @@
         <v>57</v>
       </c>
       <c r="B58" s="3">
-        <v>43713</v>
+        <v>43712</v>
       </c>
       <c r="C58">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E58">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F58" t="s">
         <v>61</v>
       </c>
       <c r="G58" t="str">
-        <f t="shared" si="0"/>
-        <v>Control</v>
+        <f t="shared" ref="G58:G71" si="4">IF(I58&lt;=0, "Control", IF(I58&lt;=10, "Red", IF(I58&gt;=21, "Pink", "Orange")))</f>
+        <v>Red</v>
       </c>
       <c r="H58">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <f t="shared" ref="H58:H71" si="5">IF(G58="Control", 1, IF(G58="Red", 2, IF(G58="Orange", 3, 4)))</f>
+        <v>2</v>
       </c>
       <c r="I58" s="7">
-        <v>0</v>
-      </c>
-      <c r="K58" s="7"/>
+        <v>2</v>
+      </c>
+      <c r="K58" s="5"/>
       <c r="M58">
         <f t="shared" si="3"/>
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.3">
@@ -51491,32 +51488,32 @@
         <v>58</v>
       </c>
       <c r="B59" s="3">
-        <v>43713</v>
+        <v>43712</v>
       </c>
       <c r="C59">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E59">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="F59" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G59" t="str">
-        <f t="shared" si="0"/>
-        <v>Orange</v>
+        <f t="shared" si="4"/>
+        <v>Control</v>
       </c>
       <c r="H59">
-        <f t="shared" si="1"/>
-        <v>3</v>
+        <f t="shared" si="5"/>
+        <v>1</v>
       </c>
       <c r="I59" s="7">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="K59" s="5"/>
       <c r="M59">
         <f t="shared" si="3"/>
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.3">
@@ -51524,32 +51521,32 @@
         <v>59</v>
       </c>
       <c r="B60" s="3">
-        <v>43713</v>
+        <v>43712</v>
       </c>
       <c r="C60">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E60">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="F60" t="s">
         <v>61</v>
       </c>
       <c r="G60" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>Pink</v>
       </c>
       <c r="H60">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
-      <c r="I60" s="7">
-        <v>24</v>
+      <c r="I60" s="5">
+        <v>29</v>
       </c>
       <c r="K60" s="5"/>
       <c r="M60">
         <f t="shared" si="3"/>
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.3">
@@ -51557,32 +51554,32 @@
         <v>60</v>
       </c>
       <c r="B61" s="3">
-        <v>43713</v>
+        <v>43712</v>
       </c>
       <c r="C61">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E61">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="F61" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G61" t="str">
-        <f t="shared" si="0"/>
-        <v>Pink</v>
+        <f t="shared" si="4"/>
+        <v>Red</v>
       </c>
       <c r="H61">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="I61" s="7">
-        <v>22</v>
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="I61" s="5">
+        <v>9</v>
       </c>
       <c r="K61" s="5"/>
       <c r="M61">
         <f t="shared" si="3"/>
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.3">
@@ -51590,32 +51587,32 @@
         <v>61</v>
       </c>
       <c r="B62" s="3">
-        <v>43713</v>
+        <v>43712</v>
       </c>
       <c r="C62">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E62">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="F62" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G62" t="str">
-        <f t="shared" si="0"/>
-        <v>Pink</v>
+        <f t="shared" si="4"/>
+        <v>Orange</v>
       </c>
       <c r="H62">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="I62" s="7">
-        <v>28</v>
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="I62" s="5">
+        <v>18</v>
       </c>
       <c r="K62" s="5"/>
       <c r="M62">
         <f t="shared" si="3"/>
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.3">
@@ -51623,32 +51620,32 @@
         <v>62</v>
       </c>
       <c r="B63" s="3">
-        <v>43713</v>
+        <v>43712</v>
       </c>
       <c r="C63">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E63">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="F63" t="s">
         <v>61</v>
       </c>
       <c r="G63" t="str">
-        <f t="shared" si="0"/>
-        <v>Red</v>
+        <f t="shared" si="4"/>
+        <v>Orange</v>
       </c>
       <c r="H63">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="I63" s="7">
-        <v>10</v>
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="I63" s="5">
+        <v>12</v>
       </c>
       <c r="K63" s="5"/>
       <c r="M63">
         <f t="shared" si="3"/>
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.3">
@@ -51656,32 +51653,32 @@
         <v>63</v>
       </c>
       <c r="B64" s="3">
-        <v>43713</v>
+        <v>43712</v>
       </c>
       <c r="C64">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E64">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="F64" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G64" t="str">
-        <f t="shared" si="0"/>
-        <v>Red</v>
+        <f t="shared" si="4"/>
+        <v>Control</v>
       </c>
       <c r="H64">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="I64" s="7">
-        <v>2</v>
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="I64" s="5">
+        <v>0</v>
       </c>
       <c r="K64" s="5"/>
       <c r="M64">
         <f t="shared" si="3"/>
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.3">
@@ -51689,32 +51686,32 @@
         <v>64</v>
       </c>
       <c r="B65" s="3">
-        <v>43713</v>
+        <v>43712</v>
       </c>
       <c r="C65">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E65">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="F65" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G65" t="str">
-        <f t="shared" si="0"/>
-        <v>Control</v>
+        <f t="shared" si="4"/>
+        <v>Red</v>
       </c>
       <c r="H65">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="I65" s="5">
         <v>1</v>
-      </c>
-      <c r="I65" s="7">
-        <v>0</v>
       </c>
       <c r="K65" s="5"/>
       <c r="M65">
         <f t="shared" si="3"/>
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.3">
@@ -51728,23 +51725,23 @@
         <v>248</v>
       </c>
       <c r="E66">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="F66" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G66" t="str">
-        <f t="shared" si="0"/>
-        <v>Pink</v>
+        <f t="shared" si="4"/>
+        <v>Control</v>
       </c>
       <c r="H66">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="I66" s="5">
-        <v>29</v>
-      </c>
-      <c r="K66" s="5"/>
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="I66" s="7">
+        <v>0</v>
+      </c>
+      <c r="K66" s="7"/>
       <c r="M66">
         <f t="shared" si="3"/>
         <v>9</v>
@@ -51761,21 +51758,21 @@
         <v>248</v>
       </c>
       <c r="E67">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="F67" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G67" t="str">
-        <f t="shared" ref="G67:G77" si="4">IF(I67&lt;=0, "Control", IF(I67&lt;=10, "Red", IF(I67&gt;=21, "Pink", "Orange")))</f>
-        <v>Red</v>
+        <f t="shared" si="4"/>
+        <v>Orange</v>
       </c>
       <c r="H67">
-        <f t="shared" ref="H67:H77" si="5">IF(G67="Control", 1, IF(G67="Red", 2, IF(G67="Orange", 3, 4)))</f>
-        <v>2</v>
-      </c>
-      <c r="I67" s="5">
-        <v>9</v>
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="I67" s="7">
+        <v>17</v>
       </c>
       <c r="K67" s="5"/>
       <c r="M67">
@@ -51794,21 +51791,21 @@
         <v>248</v>
       </c>
       <c r="E68">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="F68" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G68" t="str">
         <f t="shared" si="4"/>
-        <v>Orange</v>
+        <v>Pink</v>
       </c>
       <c r="H68">
         <f t="shared" si="5"/>
-        <v>3</v>
-      </c>
-      <c r="I68" s="5">
-        <v>18</v>
+        <v>4</v>
+      </c>
+      <c r="I68" s="7">
+        <v>24</v>
       </c>
       <c r="K68" s="5"/>
       <c r="M68">
@@ -51827,21 +51824,21 @@
         <v>248</v>
       </c>
       <c r="E69">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="F69" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G69" t="str">
         <f t="shared" si="4"/>
-        <v>Orange</v>
+        <v>Pink</v>
       </c>
       <c r="H69">
         <f t="shared" si="5"/>
-        <v>3</v>
-      </c>
-      <c r="I69" s="5">
-        <v>12</v>
+        <v>4</v>
+      </c>
+      <c r="I69" s="7">
+        <v>22</v>
       </c>
       <c r="K69" s="5"/>
       <c r="M69">
@@ -51860,21 +51857,21 @@
         <v>248</v>
       </c>
       <c r="E70">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="F70" t="s">
         <v>61</v>
       </c>
       <c r="G70" t="str">
         <f t="shared" si="4"/>
-        <v>Control</v>
+        <v>Pink</v>
       </c>
       <c r="H70">
         <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-      <c r="I70" s="5">
-        <v>0</v>
+        <v>4</v>
+      </c>
+      <c r="I70" s="7">
+        <v>28</v>
       </c>
       <c r="K70" s="5"/>
       <c r="M70">
@@ -51893,10 +51890,10 @@
         <v>248</v>
       </c>
       <c r="E71">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="F71" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G71" t="str">
         <f t="shared" si="4"/>
@@ -51906,8 +51903,8 @@
         <f t="shared" si="5"/>
         <v>2</v>
       </c>
-      <c r="I71" s="5">
-        <v>1</v>
+      <c r="I71" s="7">
+        <v>10</v>
       </c>
       <c r="K71" s="5"/>
       <c r="M71">
@@ -51929,14 +51926,14 @@
         <v>1</v>
       </c>
       <c r="F72" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G72" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="G72:G77" si="6">IF(I72&lt;=0, "Control", IF(I72&lt;=10, "Red", IF(I72&gt;=21, "Pink", "Orange")))</f>
         <v>Control</v>
       </c>
       <c r="H72">
-        <f t="shared" si="5"/>
+        <f t="shared" ref="H72:H77" si="7">IF(G72="Control", 1, IF(G72="Red", 2, IF(G72="Orange", 3, 4)))</f>
         <v>1</v>
       </c>
       <c r="I72" s="7">
@@ -51962,14 +51959,14 @@
         <v>2</v>
       </c>
       <c r="F73" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G73" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>Pink</v>
       </c>
       <c r="H73">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="I73" s="7">
@@ -51995,14 +51992,14 @@
         <v>3</v>
       </c>
       <c r="F74" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G74" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>Orange</v>
       </c>
       <c r="H74">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>3</v>
       </c>
       <c r="I74" s="7">
@@ -52028,14 +52025,14 @@
         <v>4</v>
       </c>
       <c r="F75" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G75" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>Red</v>
       </c>
       <c r="H75">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
       <c r="I75" s="7">
@@ -52061,14 +52058,14 @@
         <v>5</v>
       </c>
       <c r="F76" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G76" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>Pink</v>
       </c>
       <c r="H76">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="I76" s="7">
@@ -52094,14 +52091,14 @@
         <v>6</v>
       </c>
       <c r="F77" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G77" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>Red</v>
       </c>
       <c r="H77">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
       <c r="I77" s="7">
@@ -52113,12 +52110,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B78" s="3"/>
-    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="K64:L71">
-    <sortCondition ref="K64"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="K58:L65">
+    <sortCondition ref="K58"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -52127,27 +52121,27 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55F6BF2F-CBB2-4331-929A-D3F4AD694052}">
-  <dimension ref="A1:X27"/>
+  <dimension ref="A1:X37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L30" sqref="L30"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="G36" sqref="G36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.88671875" customWidth="1"/>
+    <col min="1" max="1" width="11.88671875" customWidth="1"/>
+    <col min="2" max="2" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.21875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.44140625" customWidth="1"/>
     <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.77734375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.77734375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="26.77734375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="26.77734375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.5546875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="16.109375" bestFit="1" customWidth="1"/>
     <col min="15" max="16" width="19.33203125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="18.33203125" bestFit="1" customWidth="1"/>
@@ -52162,13 +52156,13 @@
   <sheetData>
     <row r="1" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>3</v>
@@ -52179,26 +52173,26 @@
       <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="6" t="s">
         <v>5</v>
       </c>
       <c r="H1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>10</v>
       </c>
       <c r="N1" s="2" t="s">
         <v>15</v>
@@ -52234,122 +52228,1834 @@
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="6:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3">
+        <v>43708</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E2" t="str">
+        <f>IF(G2&lt;=0, "Control", IF(G2&lt;=10, "Red", IF(G2&gt;=21, "Pink", "Orange")))</f>
+        <v>Orange</v>
+      </c>
+      <c r="F2">
+        <f>IF(E2="Control", 1, IF(E2="Red", 2, IF(E2="Orange", 3, 4)))</f>
+        <v>3</v>
+      </c>
+      <c r="G2" s="7">
+        <v>11</v>
+      </c>
+      <c r="H2">
+        <f>'Kelp consumption'!J2</f>
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <f>'Kelp consumption'!K2</f>
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <f>'Kelp consumption'!L2</f>
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <f>'Kelp consumption'!M2</f>
+        <v>7</v>
+      </c>
+      <c r="L2">
+        <f>'Kelp consumption'!N2</f>
+        <v>1900</v>
+      </c>
+      <c r="M2">
+        <f>'Kelp consumption'!O2</f>
+        <v>700</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3">
+        <v>43708</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E3" t="str">
+        <f t="shared" ref="E3:E26" si="0">IF(G3&lt;=0, "Control", IF(G3&lt;=10, "Red", IF(G3&gt;=21, "Pink", "Orange")))</f>
+        <v>Orange</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ref="F3:F26" si="1">IF(E3="Control", 1, IF(E3="Red", 2, IF(E3="Orange", 3, 4)))</f>
+        <v>3</v>
+      </c>
+      <c r="G3" s="7">
+        <v>20</v>
+      </c>
+      <c r="H3">
+        <f>'Kelp consumption'!J3</f>
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <f>'Kelp consumption'!K3</f>
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <f>'Kelp consumption'!L3</f>
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <f>'Kelp consumption'!M3</f>
+        <v>7</v>
+      </c>
+      <c r="L3">
+        <f>'Kelp consumption'!N3</f>
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <f>'Kelp consumption'!O3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3">
+        <v>43708</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4" t="s">
+        <v>61</v>
+      </c>
+      <c r="E4" t="str">
+        <f t="shared" si="0"/>
+        <v>Control</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="G4" s="7">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <f>'Kelp consumption'!J4</f>
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <f>'Kelp consumption'!K4</f>
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <f>'Kelp consumption'!L4</f>
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <f>'Kelp consumption'!M4</f>
+        <v>7</v>
+      </c>
+      <c r="L4">
+        <f>'Kelp consumption'!N4</f>
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <f>'Kelp consumption'!O4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3">
+        <v>43708</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="D5" t="s">
+        <v>60</v>
+      </c>
+      <c r="E5" t="str">
+        <f t="shared" si="0"/>
+        <v>Red</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="G5" s="7">
+        <v>7</v>
+      </c>
+      <c r="H5">
+        <f>'Kelp consumption'!J5</f>
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <f>'Kelp consumption'!K5</f>
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <f>'Kelp consumption'!L5</f>
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <f>'Kelp consumption'!M5</f>
+        <v>7</v>
+      </c>
+      <c r="L5">
+        <f>'Kelp consumption'!N5</f>
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <f>'Kelp consumption'!O5</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3">
+        <v>43708</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
+      </c>
+      <c r="D6" t="s">
+        <v>60</v>
+      </c>
+      <c r="E6" t="str">
+        <f t="shared" si="0"/>
+        <v>Pink</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="G6" s="7">
+        <v>21</v>
+      </c>
+      <c r="H6">
+        <f>'Kelp consumption'!J6</f>
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <f>'Kelp consumption'!K6</f>
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <f>'Kelp consumption'!L6</f>
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <f>'Kelp consumption'!M6</f>
+        <v>7</v>
+      </c>
+      <c r="L6">
+        <f>'Kelp consumption'!N6</f>
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <f>'Kelp consumption'!O6</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3">
+        <v>43708</v>
+      </c>
+      <c r="C7">
+        <v>6</v>
+      </c>
+      <c r="D7" t="s">
+        <v>60</v>
+      </c>
+      <c r="E7" t="str">
+        <f t="shared" si="0"/>
+        <v>Orange</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="G7" s="7">
+        <v>19</v>
+      </c>
+      <c r="H7">
+        <f>'Kelp consumption'!J7</f>
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <f>'Kelp consumption'!K7</f>
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <f>'Kelp consumption'!L7</f>
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <f>'Kelp consumption'!M7</f>
+        <v>7</v>
+      </c>
+      <c r="L7">
+        <f>'Kelp consumption'!N7</f>
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <f>'Kelp consumption'!O7</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>15</v>
+      </c>
+      <c r="B8" s="3">
+        <v>43709</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8" t="s">
+        <v>60</v>
+      </c>
+      <c r="E8" t="str">
+        <f t="shared" si="0"/>
+        <v>Red</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="G8" s="7">
+        <v>8</v>
+      </c>
+      <c r="H8">
+        <f>'Kelp consumption'!J16</f>
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <f>'Kelp consumption'!K16</f>
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <f>'Kelp consumption'!L16</f>
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <f>'Kelp consumption'!M16</f>
+        <v>8</v>
+      </c>
+      <c r="L8">
+        <f>'Kelp consumption'!N16</f>
+        <v>0</v>
+      </c>
+      <c r="M8">
+        <f>'Kelp consumption'!O16</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>16</v>
+      </c>
+      <c r="B9" s="3">
+        <v>43709</v>
+      </c>
+      <c r="C9">
+        <v>2</v>
+      </c>
+      <c r="D9" t="s">
+        <v>61</v>
+      </c>
+      <c r="E9" t="str">
+        <f t="shared" si="0"/>
+        <v>Orange</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="G9" s="7">
+        <v>12</v>
+      </c>
+      <c r="H9">
+        <f>'Kelp consumption'!J17</f>
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <f>'Kelp consumption'!K17</f>
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <f>'Kelp consumption'!L17</f>
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <f>'Kelp consumption'!M17</f>
+        <v>8</v>
+      </c>
+      <c r="L9">
+        <f>'Kelp consumption'!N17</f>
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <f>'Kelp consumption'!O17</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>17</v>
+      </c>
+      <c r="B10" s="3">
+        <v>43709</v>
+      </c>
+      <c r="C10">
+        <v>3</v>
+      </c>
+      <c r="D10" t="s">
+        <v>60</v>
+      </c>
+      <c r="E10" t="str">
+        <f t="shared" si="0"/>
+        <v>Orange</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="G10" s="7">
+        <v>16</v>
+      </c>
+      <c r="H10">
+        <f>'Kelp consumption'!J18</f>
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <f>'Kelp consumption'!K18</f>
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <f>'Kelp consumption'!L18</f>
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <f>'Kelp consumption'!M18</f>
+        <v>8</v>
+      </c>
+      <c r="L10">
+        <f>'Kelp consumption'!N18</f>
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <f>'Kelp consumption'!O18</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>18</v>
+      </c>
+      <c r="B11" s="3">
+        <v>43709</v>
+      </c>
+      <c r="C11">
+        <v>4</v>
+      </c>
+      <c r="D11" t="s">
+        <v>61</v>
+      </c>
+      <c r="E11" t="str">
+        <f t="shared" si="0"/>
+        <v>Control</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="G11" s="7">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <f>'Kelp consumption'!J19</f>
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <f>'Kelp consumption'!K19</f>
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <f>'Kelp consumption'!L19</f>
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <f>'Kelp consumption'!M19</f>
+        <v>8</v>
+      </c>
+      <c r="L11">
+        <f>'Kelp consumption'!N19</f>
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <f>'Kelp consumption'!O19</f>
+        <v>0</v>
+      </c>
+      <c r="O11">
+        <v>9</v>
+      </c>
+      <c r="P11">
+        <v>81</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>60</v>
+      </c>
+      <c r="R11" t="s">
+        <v>59</v>
+      </c>
+      <c r="S11">
+        <f>IF(R11="Control", 1, IF(R11="Red", 2, IF(R11="Orange", 3, 4)))</f>
+        <v>3</v>
+      </c>
+      <c r="U11" t="s">
+        <v>62</v>
+      </c>
+      <c r="V11" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>19</v>
+      </c>
+      <c r="B12" s="3">
+        <v>43709</v>
+      </c>
+      <c r="C12">
+        <v>5</v>
+      </c>
+      <c r="D12" t="s">
+        <v>60</v>
+      </c>
+      <c r="E12" t="str">
+        <f t="shared" si="0"/>
+        <v>Pink</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="G12" s="7">
+        <v>25</v>
+      </c>
+      <c r="H12">
+        <f>'Kelp consumption'!J20</f>
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <f>'Kelp consumption'!K20</f>
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <f>'Kelp consumption'!L20</f>
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <f>'Kelp consumption'!M20</f>
+        <v>8</v>
+      </c>
+      <c r="L12">
+        <f>'Kelp consumption'!N20</f>
+        <v>0</v>
+      </c>
+      <c r="M12">
+        <f>'Kelp consumption'!O20</f>
+        <v>0</v>
+      </c>
+      <c r="O12">
+        <v>10</v>
+      </c>
+      <c r="P12">
+        <v>82</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>60</v>
+      </c>
+      <c r="R12" t="s">
+        <v>57</v>
+      </c>
+      <c r="S12">
+        <f>IF(R12="Control", 1, IF(R12="Red", 2, IF(R12="Orange", 3, 4)))</f>
+        <v>1</v>
+      </c>
+      <c r="U12">
+        <v>26</v>
+      </c>
+      <c r="V12">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>20</v>
+      </c>
+      <c r="B13" s="3">
+        <v>43709</v>
+      </c>
+      <c r="C13">
+        <v>6</v>
+      </c>
+      <c r="D13" t="s">
+        <v>60</v>
+      </c>
+      <c r="E13" t="str">
+        <f t="shared" si="0"/>
+        <v>Red</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="G13" s="7">
+        <v>9</v>
+      </c>
+      <c r="H13">
+        <f>'Kelp consumption'!J21</f>
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <f>'Kelp consumption'!K21</f>
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <f>'Kelp consumption'!L21</f>
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <f>'Kelp consumption'!M21</f>
+        <v>8</v>
+      </c>
+      <c r="L13">
+        <f>'Kelp consumption'!N21</f>
+        <v>0</v>
+      </c>
+      <c r="M13">
+        <f>'Kelp consumption'!O21</f>
+        <v>0</v>
+      </c>
+      <c r="O13">
+        <v>11</v>
+      </c>
+      <c r="P13">
+        <v>83</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>60</v>
+      </c>
+      <c r="R13" t="s">
+        <v>58</v>
+      </c>
+      <c r="S13">
+        <f>IF(R13="Control", 1, IF(R13="Red", 2, IF(R13="Orange", 3, 4)))</f>
+        <v>2</v>
+      </c>
+      <c r="U13">
+        <v>6</v>
+      </c>
+      <c r="V13">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>29</v>
+      </c>
+      <c r="B14" s="3">
+        <v>43710</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14" t="s">
+        <v>61</v>
+      </c>
+      <c r="E14" t="str">
+        <f t="shared" si="0"/>
+        <v>Control</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="G14" s="7">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <f>'Kelp consumption'!J30</f>
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <f>'Kelp consumption'!K30</f>
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <f>'Kelp consumption'!L30</f>
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <f>'Kelp consumption'!M30</f>
+        <v>9</v>
+      </c>
+      <c r="L14">
+        <f>'Kelp consumption'!N30</f>
+        <v>0</v>
+      </c>
+      <c r="M14">
+        <f>'Kelp consumption'!O30</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>30</v>
+      </c>
+      <c r="B15" s="3">
+        <v>43710</v>
+      </c>
+      <c r="C15">
+        <v>2</v>
+      </c>
+      <c r="D15" t="s">
+        <v>61</v>
+      </c>
+      <c r="E15" t="str">
+        <f t="shared" si="0"/>
+        <v>Pink</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="G15" s="7">
+        <v>23</v>
+      </c>
+      <c r="H15">
+        <f>'Kelp consumption'!J31</f>
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <f>'Kelp consumption'!K31</f>
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <f>'Kelp consumption'!L31</f>
+        <v>0</v>
+      </c>
+      <c r="K15">
+        <f>'Kelp consumption'!M31</f>
+        <v>9</v>
+      </c>
+      <c r="L15">
+        <f>'Kelp consumption'!N31</f>
+        <v>0</v>
+      </c>
+      <c r="M15">
+        <f>'Kelp consumption'!O31</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>31</v>
+      </c>
+      <c r="B16" s="3">
+        <v>43710</v>
+      </c>
+      <c r="C16">
+        <v>3</v>
+      </c>
+      <c r="D16" t="s">
+        <v>61</v>
+      </c>
+      <c r="E16" t="str">
+        <f t="shared" si="0"/>
+        <v>Red</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="G16" s="7">
+        <v>2</v>
+      </c>
+      <c r="H16">
+        <f>'Kelp consumption'!J32</f>
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <f>'Kelp consumption'!K32</f>
+        <v>0</v>
+      </c>
+      <c r="J16">
+        <f>'Kelp consumption'!L32</f>
+        <v>0</v>
+      </c>
+      <c r="K16">
+        <f>'Kelp consumption'!M32</f>
+        <v>9</v>
+      </c>
+      <c r="L16">
+        <f>'Kelp consumption'!N32</f>
+        <v>0</v>
+      </c>
+      <c r="M16">
+        <f>'Kelp consumption'!O32</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>32</v>
+      </c>
+      <c r="B17" s="3">
+        <v>43710</v>
+      </c>
+      <c r="C17">
+        <v>4</v>
+      </c>
+      <c r="D17" t="s">
+        <v>61</v>
+      </c>
+      <c r="E17" t="str">
+        <f t="shared" si="0"/>
+        <v>Orange</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="G17" s="7">
+        <v>14</v>
+      </c>
+      <c r="H17">
+        <f>'Kelp consumption'!J33</f>
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <f>'Kelp consumption'!K33</f>
+        <v>0</v>
+      </c>
+      <c r="J17">
+        <f>'Kelp consumption'!L33</f>
+        <v>0</v>
+      </c>
+      <c r="K17">
+        <f>'Kelp consumption'!M33</f>
+        <v>9</v>
+      </c>
+      <c r="L17">
+        <f>'Kelp consumption'!N33</f>
+        <v>0</v>
+      </c>
+      <c r="M17">
+        <f>'Kelp consumption'!O33</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>33</v>
+      </c>
+      <c r="B18" s="3">
+        <v>43710</v>
+      </c>
+      <c r="C18">
+        <v>5</v>
+      </c>
+      <c r="D18" t="s">
+        <v>60</v>
+      </c>
+      <c r="E18" t="str">
+        <f t="shared" si="0"/>
+        <v>Orange</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="G18" s="7">
+        <v>15</v>
+      </c>
+      <c r="H18">
+        <f>'Kelp consumption'!J34</f>
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <f>'Kelp consumption'!K34</f>
+        <v>0</v>
+      </c>
+      <c r="J18">
+        <f>'Kelp consumption'!L34</f>
+        <v>0</v>
+      </c>
+      <c r="K18">
+        <f>'Kelp consumption'!M34</f>
+        <v>9</v>
+      </c>
+      <c r="L18">
+        <f>'Kelp consumption'!N34</f>
+        <v>0</v>
+      </c>
+      <c r="M18">
+        <f>'Kelp consumption'!O34</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>34</v>
+      </c>
+      <c r="B19" s="3">
+        <v>43710</v>
+      </c>
+      <c r="C19">
+        <v>6</v>
+      </c>
+      <c r="D19" t="s">
+        <v>60</v>
+      </c>
+      <c r="E19" t="str">
+        <f t="shared" si="0"/>
+        <v>Red</v>
+      </c>
       <c r="F19">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="G19" s="7">
+        <v>1</v>
+      </c>
+      <c r="H19">
+        <f>'Kelp consumption'!J35</f>
+        <v>0</v>
+      </c>
+      <c r="I19">
+        <f>'Kelp consumption'!K35</f>
+        <v>0</v>
+      </c>
+      <c r="J19">
+        <f>'Kelp consumption'!L35</f>
+        <v>0</v>
+      </c>
+      <c r="K19">
+        <f>'Kelp consumption'!M35</f>
         <v>9</v>
       </c>
-      <c r="G19">
-        <v>81</v>
-      </c>
-      <c r="H19" t="s">
+      <c r="L19">
+        <f>'Kelp consumption'!N35</f>
+        <v>0</v>
+      </c>
+      <c r="M19">
+        <f>'Kelp consumption'!O35</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>43</v>
+      </c>
+      <c r="B20" s="3">
+        <v>43711</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20" t="s">
         <v>61</v>
       </c>
-      <c r="I19" t="s">
-        <v>59</v>
-      </c>
-      <c r="J19">
-        <f>IF(I19="Control", 1, IF(I19="Red", 2, IF(I19="Orange", 3, 4)))</f>
+      <c r="E20" t="str">
+        <f t="shared" si="0"/>
+        <v>Red</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="G20" s="7">
+        <v>5</v>
+      </c>
+      <c r="H20">
+        <f>'Kelp consumption'!J44</f>
+        <v>0</v>
+      </c>
+      <c r="I20">
+        <f>'Kelp consumption'!K44</f>
+        <v>0</v>
+      </c>
+      <c r="J20">
+        <f>'Kelp consumption'!L44</f>
+        <v>0</v>
+      </c>
+      <c r="K20">
+        <f>'Kelp consumption'!M44</f>
+        <v>10</v>
+      </c>
+      <c r="L20">
+        <f>'Kelp consumption'!N44</f>
+        <v>0</v>
+      </c>
+      <c r="M20">
+        <f>'Kelp consumption'!O44</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>44</v>
+      </c>
+      <c r="B21" s="3">
+        <v>43711</v>
+      </c>
+      <c r="C21">
+        <v>2</v>
+      </c>
+      <c r="D21" t="s">
+        <v>60</v>
+      </c>
+      <c r="E21" t="str">
+        <f t="shared" si="0"/>
+        <v>Pink</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="G21" s="7">
+        <v>29</v>
+      </c>
+      <c r="H21">
+        <f>'Kelp consumption'!J45</f>
+        <v>0</v>
+      </c>
+      <c r="I21">
+        <f>'Kelp consumption'!K45</f>
+        <v>0</v>
+      </c>
+      <c r="J21">
+        <f>'Kelp consumption'!L45</f>
+        <v>0</v>
+      </c>
+      <c r="K21">
+        <f>'Kelp consumption'!M45</f>
+        <v>10</v>
+      </c>
+      <c r="L21">
+        <f>'Kelp consumption'!N45</f>
+        <v>0</v>
+      </c>
+      <c r="M21">
+        <f>'Kelp consumption'!O45</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>45</v>
+      </c>
+      <c r="B22" s="3">
+        <v>43711</v>
+      </c>
+      <c r="C22">
         <v>3</v>
       </c>
-      <c r="L19" t="s">
-        <v>63</v>
-      </c>
-      <c r="M19" t="s">
+      <c r="D22" t="s">
+        <v>60</v>
+      </c>
+      <c r="E22" t="str">
+        <f t="shared" si="0"/>
+        <v>Red</v>
+      </c>
+      <c r="F22">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="G22" s="7">
+        <v>3</v>
+      </c>
+      <c r="H22">
+        <f>'Kelp consumption'!J46</f>
+        <v>0</v>
+      </c>
+      <c r="I22">
+        <f>'Kelp consumption'!K46</f>
+        <v>0</v>
+      </c>
+      <c r="J22">
+        <f>'Kelp consumption'!L46</f>
+        <v>0</v>
+      </c>
+      <c r="K22">
+        <f>'Kelp consumption'!M46</f>
+        <v>10</v>
+      </c>
+      <c r="L22">
+        <f>'Kelp consumption'!N46</f>
+        <v>0</v>
+      </c>
+      <c r="M22">
+        <f>'Kelp consumption'!O46</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>46</v>
+      </c>
+      <c r="B23" s="3">
+        <v>43711</v>
+      </c>
+      <c r="C23">
+        <v>4</v>
+      </c>
+      <c r="D23" t="s">
+        <v>61</v>
+      </c>
+      <c r="E23" t="str">
+        <f t="shared" si="0"/>
+        <v>Orange</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="G23" s="7">
+        <v>18</v>
+      </c>
+      <c r="H23">
+        <f>'Kelp consumption'!J47</f>
+        <v>0</v>
+      </c>
+      <c r="I23">
+        <f>'Kelp consumption'!K47</f>
+        <v>0</v>
+      </c>
+      <c r="J23">
+        <f>'Kelp consumption'!L47</f>
+        <v>0</v>
+      </c>
+      <c r="K23">
+        <f>'Kelp consumption'!M47</f>
+        <v>10</v>
+      </c>
+      <c r="L23">
+        <f>'Kelp consumption'!N47</f>
+        <v>0</v>
+      </c>
+      <c r="M23">
+        <f>'Kelp consumption'!O47</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>47</v>
+      </c>
+      <c r="B24" s="3">
+        <v>43711</v>
+      </c>
+      <c r="C24">
+        <v>5</v>
+      </c>
+      <c r="D24" t="s">
+        <v>60</v>
+      </c>
+      <c r="E24" t="str">
+        <f t="shared" si="0"/>
+        <v>Control</v>
+      </c>
+      <c r="F24">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="G24" s="7">
+        <v>0</v>
+      </c>
+      <c r="H24">
+        <f>'Kelp consumption'!J48</f>
+        <v>0</v>
+      </c>
+      <c r="I24">
+        <f>'Kelp consumption'!K48</f>
+        <v>0</v>
+      </c>
+      <c r="J24">
+        <f>'Kelp consumption'!L48</f>
+        <v>0</v>
+      </c>
+      <c r="K24">
+        <f>'Kelp consumption'!M48</f>
+        <v>10</v>
+      </c>
+      <c r="L24">
+        <f>'Kelp consumption'!N48</f>
+        <v>0</v>
+      </c>
+      <c r="M24">
+        <f>'Kelp consumption'!O48</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>48</v>
+      </c>
+      <c r="B25" s="3">
+        <v>43711</v>
+      </c>
+      <c r="C25">
+        <v>6</v>
+      </c>
+      <c r="D25" t="s">
+        <v>60</v>
+      </c>
+      <c r="E25" t="str">
+        <f t="shared" si="0"/>
+        <v>Pink</v>
+      </c>
+      <c r="F25">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="G25" s="7">
+        <v>27</v>
+      </c>
+      <c r="H25">
+        <f>'Kelp consumption'!J49</f>
+        <v>0</v>
+      </c>
+      <c r="I25">
+        <f>'Kelp consumption'!K49</f>
+        <v>0</v>
+      </c>
+      <c r="J25">
+        <f>'Kelp consumption'!L49</f>
+        <v>0</v>
+      </c>
+      <c r="K25">
+        <f>'Kelp consumption'!M49</f>
+        <v>10</v>
+      </c>
+      <c r="L25">
+        <f>'Kelp consumption'!N49</f>
+        <v>0</v>
+      </c>
+      <c r="M25">
+        <f>'Kelp consumption'!O49</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A26">
         <v>65</v>
       </c>
-    </row>
-    <row r="20" spans="6:13" x14ac:dyDescent="0.3">
-      <c r="F20">
+      <c r="B26" s="3">
+        <v>43713</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="D26" t="s">
+        <v>60</v>
+      </c>
+      <c r="E26" t="str">
+        <f t="shared" si="0"/>
+        <v>Control</v>
+      </c>
+      <c r="F26">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="G26" s="7">
+        <v>0</v>
+      </c>
+      <c r="H26">
+        <f>'Kelp consumption'!J66</f>
+        <v>0</v>
+      </c>
+      <c r="I26">
+        <f>'Kelp consumption'!K66</f>
+        <v>0</v>
+      </c>
+      <c r="J26">
+        <f>'Kelp consumption'!L66</f>
+        <v>0</v>
+      </c>
+      <c r="K26">
+        <f>'Kelp consumption'!M66</f>
+        <v>9</v>
+      </c>
+      <c r="L26">
+        <f>'Kelp consumption'!N66</f>
+        <v>0</v>
+      </c>
+      <c r="M26">
+        <f>'Kelp consumption'!O66</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>66</v>
+      </c>
+      <c r="B27" s="3">
+        <v>43713</v>
+      </c>
+      <c r="C27">
+        <v>2</v>
+      </c>
+      <c r="D27" t="s">
+        <v>60</v>
+      </c>
+      <c r="E27" t="str">
+        <f t="shared" ref="E27:E40" si="2">IF(G27&lt;=0, "Control", IF(G27&lt;=10, "Red", IF(G27&gt;=21, "Pink", "Orange")))</f>
+        <v>Orange</v>
+      </c>
+      <c r="F27">
+        <f t="shared" ref="F27:F37" si="3">IF(E27="Control", 1, IF(E27="Red", 2, IF(E27="Orange", 3, 4)))</f>
+        <v>3</v>
+      </c>
+      <c r="G27" s="7">
+        <v>17</v>
+      </c>
+      <c r="H27">
+        <f>'Kelp consumption'!J67</f>
+        <v>0</v>
+      </c>
+      <c r="I27">
+        <f>'Kelp consumption'!K67</f>
+        <v>0</v>
+      </c>
+      <c r="J27">
+        <f>'Kelp consumption'!L67</f>
+        <v>0</v>
+      </c>
+      <c r="K27">
+        <f>'Kelp consumption'!M67</f>
+        <v>9</v>
+      </c>
+      <c r="L27">
+        <f>'Kelp consumption'!N67</f>
+        <v>0</v>
+      </c>
+      <c r="M27">
+        <f>'Kelp consumption'!O67</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>67</v>
+      </c>
+      <c r="B28" s="3">
+        <v>43713</v>
+      </c>
+      <c r="C28">
+        <v>3</v>
+      </c>
+      <c r="D28" t="s">
+        <v>60</v>
+      </c>
+      <c r="E28" t="str">
+        <f t="shared" si="2"/>
+        <v>Pink</v>
+      </c>
+      <c r="F28">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="G28" s="7">
+        <v>24</v>
+      </c>
+      <c r="H28">
+        <f>'Kelp consumption'!J68</f>
+        <v>0</v>
+      </c>
+      <c r="I28">
+        <f>'Kelp consumption'!K68</f>
+        <v>0</v>
+      </c>
+      <c r="J28">
+        <f>'Kelp consumption'!L68</f>
+        <v>0</v>
+      </c>
+      <c r="K28">
+        <f>'Kelp consumption'!M68</f>
+        <v>9</v>
+      </c>
+      <c r="L28">
+        <f>'Kelp consumption'!N68</f>
+        <v>0</v>
+      </c>
+      <c r="M28">
+        <f>'Kelp consumption'!O68</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>68</v>
+      </c>
+      <c r="B29" s="3">
+        <v>43713</v>
+      </c>
+      <c r="C29">
+        <v>4</v>
+      </c>
+      <c r="D29" t="s">
+        <v>61</v>
+      </c>
+      <c r="E29" t="str">
+        <f t="shared" si="2"/>
+        <v>Pink</v>
+      </c>
+      <c r="F29">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="G29" s="7">
+        <v>22</v>
+      </c>
+      <c r="H29">
+        <f>'Kelp consumption'!J69</f>
+        <v>0</v>
+      </c>
+      <c r="I29">
+        <f>'Kelp consumption'!K69</f>
+        <v>0</v>
+      </c>
+      <c r="J29">
+        <f>'Kelp consumption'!L69</f>
+        <v>0</v>
+      </c>
+      <c r="K29">
+        <f>'Kelp consumption'!M69</f>
+        <v>9</v>
+      </c>
+      <c r="L29">
+        <f>'Kelp consumption'!N69</f>
+        <v>0</v>
+      </c>
+      <c r="M29">
+        <f>'Kelp consumption'!O69</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>69</v>
+      </c>
+      <c r="B30" s="3">
+        <v>43713</v>
+      </c>
+      <c r="C30">
+        <v>5</v>
+      </c>
+      <c r="D30" t="s">
+        <v>61</v>
+      </c>
+      <c r="E30" t="str">
+        <f t="shared" si="2"/>
+        <v>Pink</v>
+      </c>
+      <c r="F30">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="G30" s="7">
+        <v>28</v>
+      </c>
+      <c r="H30">
+        <f>'Kelp consumption'!J70</f>
+        <v>0</v>
+      </c>
+      <c r="I30">
+        <f>'Kelp consumption'!K70</f>
+        <v>0</v>
+      </c>
+      <c r="J30">
+        <f>'Kelp consumption'!L70</f>
+        <v>0</v>
+      </c>
+      <c r="K30">
+        <f>'Kelp consumption'!M70</f>
+        <v>9</v>
+      </c>
+      <c r="L30">
+        <f>'Kelp consumption'!N70</f>
+        <v>0</v>
+      </c>
+      <c r="M30">
+        <f>'Kelp consumption'!O70</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>70</v>
+      </c>
+      <c r="B31" s="3">
+        <v>43713</v>
+      </c>
+      <c r="C31">
+        <v>6</v>
+      </c>
+      <c r="D31" t="s">
+        <v>60</v>
+      </c>
+      <c r="E31" t="str">
+        <f t="shared" si="2"/>
+        <v>Red</v>
+      </c>
+      <c r="F31">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="G31" s="7">
         <v>10</v>
       </c>
-      <c r="G20">
-        <v>82</v>
-      </c>
-      <c r="H20" t="s">
+      <c r="H31">
+        <f>'Kelp consumption'!J71</f>
+        <v>0</v>
+      </c>
+      <c r="I31">
+        <f>'Kelp consumption'!K71</f>
+        <v>0</v>
+      </c>
+      <c r="J31">
+        <f>'Kelp consumption'!L71</f>
+        <v>0</v>
+      </c>
+      <c r="K31">
+        <f>'Kelp consumption'!M71</f>
+        <v>9</v>
+      </c>
+      <c r="L31">
+        <f>'Kelp consumption'!N71</f>
+        <v>0</v>
+      </c>
+      <c r="M31">
+        <f>'Kelp consumption'!O71</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>71</v>
+      </c>
+      <c r="B32" s="3">
+        <v>43714</v>
+      </c>
+      <c r="C32">
+        <v>1</v>
+      </c>
+      <c r="D32" t="s">
+        <v>60</v>
+      </c>
+      <c r="E32" t="str">
+        <f t="shared" si="2"/>
+        <v>Control</v>
+      </c>
+      <c r="F32">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="G32" s="7">
+        <v>0</v>
+      </c>
+      <c r="H32">
+        <f>'Kelp consumption'!J72</f>
+        <v>0</v>
+      </c>
+      <c r="I32">
+        <f>'Kelp consumption'!K72</f>
+        <v>0</v>
+      </c>
+      <c r="J32">
+        <f>'Kelp consumption'!L72</f>
+        <v>0</v>
+      </c>
+      <c r="K32">
+        <f>'Kelp consumption'!M72</f>
+        <v>10</v>
+      </c>
+      <c r="L32">
+        <f>'Kelp consumption'!N72</f>
+        <v>0</v>
+      </c>
+      <c r="M32">
+        <f>'Kelp consumption'!O72</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>72</v>
+      </c>
+      <c r="B33" s="3">
+        <v>43714</v>
+      </c>
+      <c r="C33">
+        <v>2</v>
+      </c>
+      <c r="D33" t="s">
         <v>61</v>
       </c>
-      <c r="I20" t="s">
-        <v>57</v>
-      </c>
-      <c r="J20">
-        <f>IF(I20="Control", 1, IF(I20="Red", 2, IF(I20="Orange", 3, 4)))</f>
-        <v>1</v>
-      </c>
-      <c r="L20">
+      <c r="E33" t="str">
+        <f t="shared" si="2"/>
+        <v>Pink</v>
+      </c>
+      <c r="F33">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="G33" s="7">
         <v>26</v>
       </c>
-      <c r="M20">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="21" spans="6:13" x14ac:dyDescent="0.3">
-      <c r="F21">
-        <v>11</v>
-      </c>
-      <c r="G21">
-        <v>83</v>
-      </c>
-      <c r="H21" t="s">
+      <c r="H33">
+        <f>'Kelp consumption'!J73</f>
+        <v>0</v>
+      </c>
+      <c r="I33">
+        <f>'Kelp consumption'!K73</f>
+        <v>0</v>
+      </c>
+      <c r="J33">
+        <f>'Kelp consumption'!L73</f>
+        <v>0</v>
+      </c>
+      <c r="K33">
+        <f>'Kelp consumption'!M73</f>
+        <v>10</v>
+      </c>
+      <c r="L33">
+        <f>'Kelp consumption'!N73</f>
+        <v>0</v>
+      </c>
+      <c r="M33">
+        <f>'Kelp consumption'!O73</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>73</v>
+      </c>
+      <c r="B34" s="3">
+        <v>43714</v>
+      </c>
+      <c r="C34">
+        <v>3</v>
+      </c>
+      <c r="D34" t="s">
         <v>61</v>
       </c>
-      <c r="I21" t="s">
-        <v>58</v>
-      </c>
-      <c r="J21">
-        <f>IF(I21="Control", 1, IF(I21="Red", 2, IF(I21="Orange", 3, 4)))</f>
+      <c r="E34" t="str">
+        <f t="shared" si="2"/>
+        <v>Orange</v>
+      </c>
+      <c r="F34">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="G34" s="7">
+        <v>13</v>
+      </c>
+      <c r="H34">
+        <f>'Kelp consumption'!J74</f>
+        <v>0</v>
+      </c>
+      <c r="I34">
+        <f>'Kelp consumption'!K74</f>
+        <v>0</v>
+      </c>
+      <c r="J34">
+        <f>'Kelp consumption'!L74</f>
+        <v>0</v>
+      </c>
+      <c r="K34">
+        <f>'Kelp consumption'!M74</f>
+        <v>10</v>
+      </c>
+      <c r="L34">
+        <f>'Kelp consumption'!N74</f>
+        <v>0</v>
+      </c>
+      <c r="M34">
+        <f>'Kelp consumption'!O74</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>74</v>
+      </c>
+      <c r="B35" s="3">
+        <v>43714</v>
+      </c>
+      <c r="C35">
+        <v>4</v>
+      </c>
+      <c r="D35" t="s">
+        <v>61</v>
+      </c>
+      <c r="E35" t="str">
+        <f t="shared" si="2"/>
+        <v>Red</v>
+      </c>
+      <c r="F35">
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
-      <c r="L21">
+      <c r="G35" s="7">
+        <v>4</v>
+      </c>
+      <c r="H35">
+        <f>'Kelp consumption'!J75</f>
+        <v>0</v>
+      </c>
+      <c r="I35">
+        <f>'Kelp consumption'!K75</f>
+        <v>0</v>
+      </c>
+      <c r="J35">
+        <f>'Kelp consumption'!L75</f>
+        <v>0</v>
+      </c>
+      <c r="K35">
+        <f>'Kelp consumption'!M75</f>
+        <v>10</v>
+      </c>
+      <c r="L35">
+        <f>'Kelp consumption'!N75</f>
+        <v>0</v>
+      </c>
+      <c r="M35">
+        <f>'Kelp consumption'!O75</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>75</v>
+      </c>
+      <c r="B36" s="3">
+        <v>43714</v>
+      </c>
+      <c r="C36">
+        <v>5</v>
+      </c>
+      <c r="D36" t="s">
+        <v>60</v>
+      </c>
+      <c r="E36" t="str">
+        <f t="shared" si="2"/>
+        <v>Pink</v>
+      </c>
+      <c r="F36">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="G36" s="7">
+        <v>30</v>
+      </c>
+      <c r="H36">
+        <f>'Kelp consumption'!J76</f>
+        <v>0</v>
+      </c>
+      <c r="I36">
+        <f>'Kelp consumption'!K76</f>
+        <v>0</v>
+      </c>
+      <c r="J36">
+        <f>'Kelp consumption'!L76</f>
+        <v>0</v>
+      </c>
+      <c r="K36">
+        <f>'Kelp consumption'!M76</f>
+        <v>10</v>
+      </c>
+      <c r="L36">
+        <f>'Kelp consumption'!N76</f>
+        <v>0</v>
+      </c>
+      <c r="M36">
+        <f>'Kelp consumption'!O76</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>76</v>
+      </c>
+      <c r="B37" s="3">
+        <v>43714</v>
+      </c>
+      <c r="C37">
         <v>6</v>
       </c>
-      <c r="M21">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="22" spans="6:13" x14ac:dyDescent="0.3">
-      <c r="F22">
-        <v>12</v>
-      </c>
-      <c r="G22">
-        <v>84</v>
-      </c>
-      <c r="H22" t="s">
-        <v>61</v>
-      </c>
-      <c r="I22" t="s">
+      <c r="D37" t="s">
         <v>60</v>
       </c>
-      <c r="J22">
-        <f>IF(I22="Control", 1, IF(I22="Red", 2, IF(I22="Orange", 3, 4)))</f>
-        <v>4</v>
-      </c>
-      <c r="L22">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="23" spans="6:13" x14ac:dyDescent="0.3">
-      <c r="L23">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="24" spans="6:13" x14ac:dyDescent="0.3">
-      <c r="L24">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="25" spans="6:13" x14ac:dyDescent="0.3">
-      <c r="L25">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="26" spans="6:13" x14ac:dyDescent="0.3">
-      <c r="L26">
+      <c r="E37" t="str">
+        <f t="shared" si="2"/>
+        <v>Red</v>
+      </c>
+      <c r="F37">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="G37" s="7">
+        <v>6</v>
+      </c>
+      <c r="H37">
+        <f>'Kelp consumption'!J77</f>
+        <v>0</v>
+      </c>
+      <c r="I37">
+        <f>'Kelp consumption'!K77</f>
+        <v>0</v>
+      </c>
+      <c r="J37">
+        <f>'Kelp consumption'!L77</f>
+        <v>0</v>
+      </c>
+      <c r="K37">
+        <f>'Kelp consumption'!M77</f>
         <v>10</v>
       </c>
-    </row>
-    <row r="27" spans="6:13" x14ac:dyDescent="0.3">
-      <c r="L27">
-        <v>4</v>
+      <c r="L37">
+        <f>'Kelp consumption'!N77</f>
+        <v>0</v>
+      </c>
+      <c r="M37">
+        <f>'Kelp consumption'!O77</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Sept 2 afternoon update
</commit_message>
<xml_diff>
--- a/data/raw.xlsx
+++ b/data/raw.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Amelia\github\Ritger-Corynactis-urchin-deterrence\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B45F00F4-35D0-49E9-84C6-71421035C0C8}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B3D5BA7-FB85-4BEE-9E86-E411525BA150}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-16680" windowWidth="21600" windowHeight="12675" activeTab="1" xr2:uid="{58E670A5-634C-427F-960F-9DA76C64E810}"/>
+    <workbookView xWindow="204" yWindow="348" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{58E670A5-634C-427F-960F-9DA76C64E810}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="3" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="74">
   <si>
     <t>Day</t>
   </si>
@@ -252,6 +252,9 @@
   </si>
   <si>
     <t>GoPro didn't connect to BacPack</t>
+  </si>
+  <si>
+    <t>GoPro not connected to BacPack</t>
   </si>
 </sst>
 </file>
@@ -49540,9 +49543,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD5E687B-43EE-4B00-8604-7EB9984510DD}">
   <dimension ref="A1:V77"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="V5" sqref="V5"/>
+      <selection pane="bottomLeft" activeCell="N24" sqref="N24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -49732,6 +49735,9 @@
       <c r="P3">
         <v>730</v>
       </c>
+      <c r="T3">
+        <v>0</v>
+      </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A4">
@@ -49970,6 +49976,9 @@
       <c r="P8">
         <v>740</v>
       </c>
+      <c r="T8">
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A9">
@@ -50017,6 +50026,9 @@
       <c r="P9">
         <v>740</v>
       </c>
+      <c r="T9">
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A10">
@@ -50064,6 +50076,9 @@
       <c r="P10">
         <v>740</v>
       </c>
+      <c r="T10">
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A11">
@@ -50111,6 +50126,9 @@
       <c r="P11">
         <v>740</v>
       </c>
+      <c r="T11">
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A12">
@@ -50193,7 +50211,7 @@
         <v>42</v>
       </c>
       <c r="M13">
-        <v>42.5</v>
+        <v>43</v>
       </c>
       <c r="N13">
         <f t="shared" si="2"/>
@@ -50299,6 +50317,9 @@
       <c r="P15">
         <v>740</v>
       </c>
+      <c r="T15">
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A16">
@@ -50327,15 +50348,30 @@
       <c r="I16" s="7">
         <v>8</v>
       </c>
-      <c r="K16" s="6"/>
-      <c r="L16" s="4"/>
-      <c r="M16" s="4"/>
+      <c r="K16" s="4">
+        <v>45</v>
+      </c>
+      <c r="L16">
+        <v>45</v>
+      </c>
+      <c r="M16">
+        <v>45</v>
+      </c>
       <c r="N16">
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O16">
+        <v>1910</v>
+      </c>
+      <c r="P16">
+        <v>710</v>
+      </c>
+      <c r="T16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -50362,13 +50398,27 @@
       <c r="I17" s="7">
         <v>12</v>
       </c>
-      <c r="K17" s="7"/>
+      <c r="K17">
+        <v>43</v>
+      </c>
+      <c r="L17">
+        <v>50</v>
+      </c>
+      <c r="M17">
+        <v>41</v>
+      </c>
       <c r="N17">
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O17">
+        <v>1910</v>
+      </c>
+      <c r="P17">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -50395,13 +50445,30 @@
       <c r="I18" s="7">
         <v>16</v>
       </c>
-      <c r="K18" s="7"/>
+      <c r="K18">
+        <v>58</v>
+      </c>
+      <c r="L18">
+        <v>85</v>
+      </c>
+      <c r="M18">
+        <v>85</v>
+      </c>
       <c r="N18">
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O18">
+        <v>1910</v>
+      </c>
+      <c r="P18">
+        <v>710</v>
+      </c>
+      <c r="T18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -50428,13 +50495,30 @@
       <c r="I19" s="7">
         <v>0</v>
       </c>
-      <c r="K19" s="7"/>
+      <c r="K19">
+        <v>48</v>
+      </c>
+      <c r="L19">
+        <v>51</v>
+      </c>
+      <c r="M19">
+        <v>51</v>
+      </c>
       <c r="N19">
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O19">
+        <v>1910</v>
+      </c>
+      <c r="P19">
+        <v>710</v>
+      </c>
+      <c r="T19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -50461,13 +50545,27 @@
       <c r="I20" s="7">
         <v>25</v>
       </c>
-      <c r="K20" s="7"/>
+      <c r="K20">
+        <v>50</v>
+      </c>
+      <c r="L20">
+        <v>60</v>
+      </c>
+      <c r="M20">
+        <v>61</v>
+      </c>
       <c r="N20">
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O20">
+        <v>1910</v>
+      </c>
+      <c r="P20">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
@@ -50494,15 +50592,30 @@
       <c r="I21" s="7">
         <v>9</v>
       </c>
-      <c r="K21" s="7"/>
-      <c r="L21" s="4"/>
-      <c r="M21" s="4"/>
+      <c r="K21">
+        <v>49</v>
+      </c>
+      <c r="L21">
+        <v>46</v>
+      </c>
+      <c r="M21">
+        <v>45</v>
+      </c>
       <c r="N21">
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O21">
+        <v>1910</v>
+      </c>
+      <c r="P21">
+        <v>710</v>
+      </c>
+      <c r="T21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
@@ -50529,12 +50642,27 @@
       <c r="I22" s="7">
         <v>21</v>
       </c>
+      <c r="K22">
+        <v>48</v>
+      </c>
+      <c r="L22">
+        <v>54</v>
+      </c>
+      <c r="M22">
+        <v>53</v>
+      </c>
       <c r="N22">
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O22">
+        <v>1905</v>
+      </c>
+      <c r="P22">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
@@ -50561,12 +50689,30 @@
       <c r="I23" s="7">
         <v>5</v>
       </c>
+      <c r="K23">
+        <v>57</v>
+      </c>
+      <c r="L23">
+        <v>79</v>
+      </c>
+      <c r="M23">
+        <v>79</v>
+      </c>
       <c r="N23">
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O23">
+        <v>1905</v>
+      </c>
+      <c r="P23">
+        <v>705</v>
+      </c>
+      <c r="T23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
@@ -50593,12 +50739,30 @@
       <c r="I24" s="7">
         <v>7</v>
       </c>
+      <c r="K24">
+        <v>50</v>
+      </c>
+      <c r="L24">
+        <v>50</v>
+      </c>
+      <c r="M24">
+        <v>51</v>
+      </c>
       <c r="N24">
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O24">
+        <v>1905</v>
+      </c>
+      <c r="P24">
+        <v>705</v>
+      </c>
+      <c r="T24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
@@ -50625,12 +50789,30 @@
       <c r="I25" s="7">
         <v>4</v>
       </c>
+      <c r="K25">
+        <v>50</v>
+      </c>
+      <c r="L25">
+        <v>55</v>
+      </c>
+      <c r="M25">
+        <v>56</v>
+      </c>
       <c r="N25">
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O25">
+        <v>1905</v>
+      </c>
+      <c r="P25">
+        <v>705</v>
+      </c>
+      <c r="T25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>25</v>
       </c>
@@ -50657,12 +50839,27 @@
       <c r="I26" s="7">
         <v>0</v>
       </c>
+      <c r="K26">
+        <v>61</v>
+      </c>
+      <c r="L26">
+        <v>92</v>
+      </c>
+      <c r="M26">
+        <v>94</v>
+      </c>
       <c r="N26">
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O26">
+        <v>1905</v>
+      </c>
+      <c r="P26">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>26</v>
       </c>
@@ -50689,12 +50886,30 @@
       <c r="I27" s="7">
         <v>24</v>
       </c>
+      <c r="K27">
+        <v>44</v>
+      </c>
+      <c r="L27">
+        <v>34</v>
+      </c>
+      <c r="M27">
+        <v>35</v>
+      </c>
       <c r="N27">
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O27">
+        <v>1905</v>
+      </c>
+      <c r="P27">
+        <v>705</v>
+      </c>
+      <c r="T27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>27</v>
       </c>
@@ -50721,12 +50936,30 @@
       <c r="I28" s="7">
         <v>13</v>
       </c>
+      <c r="K28">
+        <v>45</v>
+      </c>
+      <c r="L28">
+        <v>44</v>
+      </c>
+      <c r="M28">
+        <v>45</v>
+      </c>
       <c r="N28">
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O28">
+        <v>1905</v>
+      </c>
+      <c r="P28">
+        <v>705</v>
+      </c>
+      <c r="T28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>28</v>
       </c>
@@ -50753,12 +50986,30 @@
       <c r="I29" s="7">
         <v>0</v>
       </c>
+      <c r="K29">
+        <v>47</v>
+      </c>
+      <c r="L29">
+        <v>40</v>
+      </c>
+      <c r="M29">
+        <v>41</v>
+      </c>
       <c r="N29">
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O29">
+        <v>1905</v>
+      </c>
+      <c r="P29">
+        <v>705</v>
+      </c>
+      <c r="T29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>29</v>
       </c>
@@ -50793,7 +51044,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>30</v>
       </c>
@@ -50826,7 +51077,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>31</v>
       </c>
@@ -52343,8 +52594,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55F6BF2F-CBB2-4331-929A-D3F4AD694052}">
   <dimension ref="A1:X37"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="G36" sqref="G36"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="R3" sqref="R3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -52496,6 +52747,9 @@
         <f>'Kelp consumption'!P2</f>
         <v>730</v>
       </c>
+      <c r="Q2">
+        <v>5</v>
+      </c>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A3">
@@ -52545,6 +52799,9 @@
         <f>'Kelp consumption'!P3</f>
         <v>730</v>
       </c>
+      <c r="Q3">
+        <v>0</v>
+      </c>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A4">
@@ -52594,6 +52851,12 @@
         <f>'Kelp consumption'!P4</f>
         <v>730</v>
       </c>
+      <c r="Q4">
+        <v>1</v>
+      </c>
+      <c r="X4" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A5">
@@ -52643,6 +52906,9 @@
         <f>'Kelp consumption'!P5</f>
         <v>730</v>
       </c>
+      <c r="Q5">
+        <v>1</v>
+      </c>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A6">
@@ -52692,6 +52958,9 @@
         <f>'Kelp consumption'!P6</f>
         <v>730</v>
       </c>
+      <c r="Q6">
+        <v>5</v>
+      </c>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A7">
@@ -52741,6 +53010,9 @@
         <f>'Kelp consumption'!P7</f>
         <v>730</v>
       </c>
+      <c r="Q7">
+        <v>8</v>
+      </c>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A8">
@@ -52772,11 +53044,11 @@
       </c>
       <c r="I8">
         <f>'Kelp consumption'!K16</f>
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="J8">
         <f>'Kelp consumption'!L16</f>
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="K8">
         <f>'Kelp consumption'!N16</f>
@@ -52784,11 +53056,11 @@
       </c>
       <c r="L8">
         <f>'Kelp consumption'!O16</f>
-        <v>0</v>
+        <v>1910</v>
       </c>
       <c r="M8">
         <f>'Kelp consumption'!P16</f>
-        <v>0</v>
+        <v>710</v>
       </c>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.3">
@@ -52821,11 +53093,11 @@
       </c>
       <c r="I9">
         <f>'Kelp consumption'!K17</f>
-        <v>0</v>
+        <v>43</v>
       </c>
       <c r="J9">
         <f>'Kelp consumption'!L17</f>
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="K9">
         <f>'Kelp consumption'!N17</f>
@@ -52833,11 +53105,11 @@
       </c>
       <c r="L9">
         <f>'Kelp consumption'!O17</f>
-        <v>0</v>
+        <v>1910</v>
       </c>
       <c r="M9">
         <f>'Kelp consumption'!P17</f>
-        <v>0</v>
+        <v>710</v>
       </c>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.3">
@@ -52870,11 +53142,11 @@
       </c>
       <c r="I10">
         <f>'Kelp consumption'!K18</f>
-        <v>0</v>
+        <v>58</v>
       </c>
       <c r="J10">
         <f>'Kelp consumption'!L18</f>
-        <v>0</v>
+        <v>85</v>
       </c>
       <c r="K10">
         <f>'Kelp consumption'!N18</f>
@@ -52882,11 +53154,11 @@
       </c>
       <c r="L10">
         <f>'Kelp consumption'!O18</f>
-        <v>0</v>
+        <v>1910</v>
       </c>
       <c r="M10">
         <f>'Kelp consumption'!P18</f>
-        <v>0</v>
+        <v>710</v>
       </c>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.3">
@@ -52919,11 +53191,11 @@
       </c>
       <c r="I11">
         <f>'Kelp consumption'!K19</f>
-        <v>0</v>
+        <v>48</v>
       </c>
       <c r="J11">
         <f>'Kelp consumption'!L19</f>
-        <v>0</v>
+        <v>51</v>
       </c>
       <c r="K11">
         <f>'Kelp consumption'!N19</f>
@@ -52931,11 +53203,11 @@
       </c>
       <c r="L11">
         <f>'Kelp consumption'!O19</f>
-        <v>0</v>
+        <v>1910</v>
       </c>
       <c r="M11">
         <f>'Kelp consumption'!P19</f>
-        <v>0</v>
+        <v>710</v>
       </c>
       <c r="O11">
         <v>9</v>
@@ -52990,11 +53262,11 @@
       </c>
       <c r="I12">
         <f>'Kelp consumption'!K20</f>
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="J12">
         <f>'Kelp consumption'!L20</f>
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="K12">
         <f>'Kelp consumption'!N20</f>
@@ -53002,11 +53274,11 @@
       </c>
       <c r="L12">
         <f>'Kelp consumption'!O20</f>
-        <v>0</v>
+        <v>1910</v>
       </c>
       <c r="M12">
         <f>'Kelp consumption'!P20</f>
-        <v>0</v>
+        <v>710</v>
       </c>
       <c r="O12">
         <v>10</v>
@@ -53061,11 +53333,11 @@
       </c>
       <c r="I13">
         <f>'Kelp consumption'!K21</f>
-        <v>0</v>
+        <v>49</v>
       </c>
       <c r="J13">
         <f>'Kelp consumption'!L21</f>
-        <v>0</v>
+        <v>46</v>
       </c>
       <c r="K13">
         <f>'Kelp consumption'!N21</f>
@@ -53073,11 +53345,11 @@
       </c>
       <c r="L13">
         <f>'Kelp consumption'!O21</f>
-        <v>0</v>
+        <v>1910</v>
       </c>
       <c r="M13">
         <f>'Kelp consumption'!P21</f>
-        <v>0</v>
+        <v>710</v>
       </c>
       <c r="O13">
         <v>11</v>

</xml_diff>

<commit_message>
Sept 3 morning update
</commit_message>
<xml_diff>
--- a/data/raw.xlsx
+++ b/data/raw.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/EcosystemRecoveryLab/Github/Ritger-Corynactis-urchin-deterrence/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3D53318-F657-3644-AC6A-2A15A1F1CED2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B94991D5-CA1A-5F40-8C1A-62FDA4FC2E3D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15080" yWindow="1880" windowWidth="17280" windowHeight="19820" activeTab="2" xr2:uid="{58E670A5-634C-427F-960F-9DA76C64E810}"/>
+    <workbookView xWindow="5900" yWindow="6800" windowWidth="20720" windowHeight="17400" activeTab="2" xr2:uid="{58E670A5-634C-427F-960F-9DA76C64E810}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="3" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="75">
   <si>
     <t>Day</t>
   </si>
@@ -49540,9 +49540,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD5E687B-43EE-4B00-8604-7EB9984510DD}">
   <dimension ref="A1:V77"/>
   <sheetViews>
-    <sheetView topLeftCell="N1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N24" sqref="N24"/>
+    <sheetView topLeftCell="I1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Q43" sqref="Q43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -51033,13 +51033,25 @@
       <c r="I30" s="7">
         <v>0</v>
       </c>
-      <c r="K30" s="7"/>
-      <c r="L30" s="4"/>
-      <c r="M30" s="4"/>
+      <c r="K30" s="7">
+        <v>59</v>
+      </c>
+      <c r="L30" s="4">
+        <v>96</v>
+      </c>
+      <c r="M30" s="4">
+        <v>98</v>
+      </c>
       <c r="N30">
         <f t="shared" si="2"/>
         <v>9</v>
       </c>
+      <c r="O30">
+        <v>1915</v>
+      </c>
+      <c r="P30">
+        <v>720</v>
+      </c>
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A31">
@@ -51068,11 +51080,25 @@
       <c r="I31" s="7">
         <v>23</v>
       </c>
-      <c r="K31" s="7"/>
+      <c r="K31" s="7">
+        <v>45</v>
+      </c>
+      <c r="L31" s="4">
+        <v>40</v>
+      </c>
+      <c r="M31" s="4">
+        <v>42</v>
+      </c>
       <c r="N31">
         <f t="shared" si="2"/>
         <v>9</v>
       </c>
+      <c r="O31">
+        <v>1915</v>
+      </c>
+      <c r="P31">
+        <v>720</v>
+      </c>
     </row>
     <row r="32" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A32">
@@ -51101,13 +51127,27 @@
       <c r="I32" s="7">
         <v>2</v>
       </c>
-      <c r="K32" s="7"/>
+      <c r="K32" s="7">
+        <v>49</v>
+      </c>
+      <c r="L32" s="4">
+        <v>62</v>
+      </c>
+      <c r="M32" s="4">
+        <v>63</v>
+      </c>
       <c r="N32">
         <f t="shared" si="2"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O32">
+        <v>1915</v>
+      </c>
+      <c r="P32">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>32</v>
       </c>
@@ -51134,15 +51174,27 @@
       <c r="I33" s="7">
         <v>14</v>
       </c>
-      <c r="K33" s="5"/>
-      <c r="L33" s="4"/>
-      <c r="M33" s="4"/>
+      <c r="K33" s="7">
+        <v>48</v>
+      </c>
+      <c r="L33" s="4">
+        <v>47</v>
+      </c>
+      <c r="M33" s="4">
+        <v>47</v>
+      </c>
       <c r="N33">
         <f t="shared" si="2"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O33">
+        <v>1915</v>
+      </c>
+      <c r="P33">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>33</v>
       </c>
@@ -51169,13 +51221,27 @@
       <c r="I34" s="7">
         <v>15</v>
       </c>
-      <c r="K34" s="7"/>
+      <c r="K34" s="7">
+        <v>53</v>
+      </c>
+      <c r="L34" s="4">
+        <v>76</v>
+      </c>
+      <c r="M34" s="4">
+        <v>75</v>
+      </c>
       <c r="N34">
         <f t="shared" si="2"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O34">
+        <v>1915</v>
+      </c>
+      <c r="P34">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>34</v>
       </c>
@@ -51202,13 +51268,27 @@
       <c r="I35" s="7">
         <v>1</v>
       </c>
-      <c r="K35" s="7"/>
+      <c r="K35" s="7">
+        <v>47</v>
+      </c>
+      <c r="L35" s="4">
+        <v>47</v>
+      </c>
+      <c r="M35" s="4">
+        <v>47</v>
+      </c>
       <c r="N35">
         <f t="shared" si="2"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O35">
+        <v>1915</v>
+      </c>
+      <c r="P35">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>35</v>
       </c>
@@ -51235,12 +51315,27 @@
       <c r="I36" s="7">
         <v>0</v>
       </c>
+      <c r="K36" s="7">
+        <v>52</v>
+      </c>
+      <c r="L36" s="4">
+        <v>63</v>
+      </c>
+      <c r="M36" s="4">
+        <v>63</v>
+      </c>
       <c r="N36">
         <f t="shared" si="2"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O36">
+        <v>1920</v>
+      </c>
+      <c r="P36">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>36</v>
       </c>
@@ -51267,12 +51362,27 @@
       <c r="I37" s="7">
         <v>0</v>
       </c>
+      <c r="K37" s="7">
+        <v>47</v>
+      </c>
+      <c r="L37" s="4">
+        <v>49</v>
+      </c>
+      <c r="M37" s="4">
+        <v>50</v>
+      </c>
       <c r="N37">
         <f t="shared" si="2"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O37">
+        <v>1920</v>
+      </c>
+      <c r="P37">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>37</v>
       </c>
@@ -51299,12 +51409,27 @@
       <c r="I38" s="7">
         <v>19</v>
       </c>
+      <c r="K38" s="7">
+        <v>45</v>
+      </c>
+      <c r="L38" s="4">
+        <v>46</v>
+      </c>
+      <c r="M38" s="4">
+        <v>47</v>
+      </c>
       <c r="N38">
         <f t="shared" si="2"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O38">
+        <v>1920</v>
+      </c>
+      <c r="P38">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>38</v>
       </c>
@@ -51331,12 +51456,27 @@
       <c r="I39" s="7">
         <v>11</v>
       </c>
+      <c r="K39" s="7">
+        <v>54</v>
+      </c>
+      <c r="L39" s="4">
+        <v>72</v>
+      </c>
+      <c r="M39" s="4">
+        <v>73</v>
+      </c>
       <c r="N39">
         <f t="shared" si="2"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O39">
+        <v>1920</v>
+      </c>
+      <c r="P39">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>39</v>
       </c>
@@ -51363,12 +51503,27 @@
       <c r="I40" s="7">
         <v>22</v>
       </c>
+      <c r="K40" s="7">
+        <v>53</v>
+      </c>
+      <c r="L40" s="4">
+        <v>68</v>
+      </c>
+      <c r="M40" s="4">
+        <v>70</v>
+      </c>
       <c r="N40">
         <f t="shared" si="2"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O40">
+        <v>1920</v>
+      </c>
+      <c r="P40">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>40</v>
       </c>
@@ -51395,12 +51550,27 @@
       <c r="I41" s="7">
         <v>6</v>
       </c>
+      <c r="K41" s="7">
+        <v>5</v>
+      </c>
+      <c r="L41" s="4">
+        <v>90</v>
+      </c>
+      <c r="M41" s="4">
+        <v>89</v>
+      </c>
       <c r="N41">
         <f t="shared" si="2"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O41">
+        <v>1920</v>
+      </c>
+      <c r="P41">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>41</v>
       </c>
@@ -51427,12 +51597,27 @@
       <c r="I42" s="7">
         <v>27</v>
       </c>
+      <c r="K42" s="7">
+        <v>59</v>
+      </c>
+      <c r="L42" s="4">
+        <v>83</v>
+      </c>
+      <c r="M42" s="4">
+        <v>83</v>
+      </c>
       <c r="N42">
         <f t="shared" si="2"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O42">
+        <v>1920</v>
+      </c>
+      <c r="P42">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>42</v>
       </c>
@@ -51459,12 +51644,27 @@
       <c r="I43" s="7">
         <v>20</v>
       </c>
+      <c r="K43" s="7">
+        <v>50</v>
+      </c>
+      <c r="L43" s="4">
+        <v>57</v>
+      </c>
+      <c r="M43" s="4">
+        <v>57</v>
+      </c>
       <c r="N43">
         <f t="shared" si="2"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O43">
+        <v>1920</v>
+      </c>
+      <c r="P43">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>43</v>
       </c>
@@ -51496,7 +51696,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>44</v>
       </c>
@@ -51529,7 +51729,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>45</v>
       </c>
@@ -51562,7 +51762,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>46</v>
       </c>
@@ -51597,7 +51797,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>47</v>
       </c>
@@ -52591,8 +52791,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55F6BF2F-CBB2-4331-929A-D3F4AD694052}">
   <dimension ref="A1:X45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q10" sqref="Q10"/>
+    <sheetView tabSelected="1" topLeftCell="E2" workbookViewId="0">
+      <selection activeCell="Q14" sqref="Q14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -53356,11 +53556,11 @@
       </c>
       <c r="I14">
         <f>'Kelp consumption'!K30</f>
-        <v>0</v>
+        <v>59</v>
       </c>
       <c r="J14">
         <f>'Kelp consumption'!L30</f>
-        <v>0</v>
+        <v>96</v>
       </c>
       <c r="K14">
         <f>'Kelp consumption'!N30</f>
@@ -53368,11 +53568,14 @@
       </c>
       <c r="L14">
         <f>'Kelp consumption'!O30</f>
-        <v>0</v>
+        <v>1915</v>
       </c>
       <c r="M14">
         <f>'Kelp consumption'!P30</f>
-        <v>0</v>
+        <v>720</v>
+      </c>
+      <c r="X14" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.2">
@@ -53405,11 +53608,11 @@
       </c>
       <c r="I15">
         <f>'Kelp consumption'!K31</f>
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="J15">
         <f>'Kelp consumption'!L31</f>
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="K15">
         <f>'Kelp consumption'!N31</f>
@@ -53417,11 +53620,11 @@
       </c>
       <c r="L15">
         <f>'Kelp consumption'!O31</f>
-        <v>0</v>
+        <v>1915</v>
       </c>
       <c r="M15">
         <f>'Kelp consumption'!P31</f>
-        <v>0</v>
+        <v>720</v>
       </c>
     </row>
     <row r="16" spans="1:24" x14ac:dyDescent="0.2">
@@ -53454,11 +53657,11 @@
       </c>
       <c r="I16">
         <f>'Kelp consumption'!K32</f>
-        <v>0</v>
+        <v>49</v>
       </c>
       <c r="J16">
         <f>'Kelp consumption'!L32</f>
-        <v>0</v>
+        <v>62</v>
       </c>
       <c r="K16">
         <f>'Kelp consumption'!N32</f>
@@ -53466,11 +53669,11 @@
       </c>
       <c r="L16">
         <f>'Kelp consumption'!O32</f>
-        <v>0</v>
+        <v>1915</v>
       </c>
       <c r="M16">
         <f>'Kelp consumption'!P32</f>
-        <v>0</v>
+        <v>720</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
@@ -53503,11 +53706,11 @@
       </c>
       <c r="I17">
         <f>'Kelp consumption'!K33</f>
-        <v>0</v>
+        <v>48</v>
       </c>
       <c r="J17">
         <f>'Kelp consumption'!L33</f>
-        <v>0</v>
+        <v>47</v>
       </c>
       <c r="K17">
         <f>'Kelp consumption'!N33</f>
@@ -53515,11 +53718,11 @@
       </c>
       <c r="L17">
         <f>'Kelp consumption'!O33</f>
-        <v>0</v>
+        <v>1915</v>
       </c>
       <c r="M17">
         <f>'Kelp consumption'!P33</f>
-        <v>0</v>
+        <v>720</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.2">
@@ -53552,11 +53755,11 @@
       </c>
       <c r="I18">
         <f>'Kelp consumption'!K34</f>
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="J18">
         <f>'Kelp consumption'!L34</f>
-        <v>0</v>
+        <v>76</v>
       </c>
       <c r="K18">
         <f>'Kelp consumption'!N34</f>
@@ -53564,11 +53767,11 @@
       </c>
       <c r="L18">
         <f>'Kelp consumption'!O34</f>
-        <v>0</v>
+        <v>1915</v>
       </c>
       <c r="M18">
         <f>'Kelp consumption'!P34</f>
-        <v>0</v>
+        <v>720</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
@@ -53601,11 +53804,11 @@
       </c>
       <c r="I19">
         <f>'Kelp consumption'!K35</f>
-        <v>0</v>
+        <v>47</v>
       </c>
       <c r="J19">
         <f>'Kelp consumption'!L35</f>
-        <v>0</v>
+        <v>47</v>
       </c>
       <c r="K19">
         <f>'Kelp consumption'!N35</f>
@@ -53613,11 +53816,11 @@
       </c>
       <c r="L19">
         <f>'Kelp consumption'!O35</f>
-        <v>0</v>
+        <v>1915</v>
       </c>
       <c r="M19">
         <f>'Kelp consumption'!P35</f>
-        <v>0</v>
+        <v>720</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Sept 4 morning update
</commit_message>
<xml_diff>
--- a/data/raw.xlsx
+++ b/data/raw.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/EcosystemRecoveryLab/Github/Ritger-Corynactis-urchin-deterrence/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B94991D5-CA1A-5F40-8C1A-62FDA4FC2E3D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{608B5E12-7104-8F42-A8BF-FAE3D0669640}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5900" yWindow="6800" windowWidth="20720" windowHeight="17400" activeTab="2" xr2:uid="{58E670A5-634C-427F-960F-9DA76C64E810}"/>
+    <workbookView xWindow="3840" yWindow="7500" windowWidth="33780" windowHeight="17400" activeTab="1" xr2:uid="{58E670A5-634C-427F-960F-9DA76C64E810}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="3" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="77">
   <si>
     <t>Day</t>
   </si>
@@ -252,6 +252,12 @@
   </si>
   <si>
     <t>Urchin never moved</t>
+  </si>
+  <si>
+    <t>No video</t>
+  </si>
+  <si>
+    <t>0?</t>
   </si>
 </sst>
 </file>
@@ -49540,9 +49546,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD5E687B-43EE-4B00-8604-7EB9984510DD}">
   <dimension ref="A1:V77"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q43" sqref="Q43"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="T52" sqref="T52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -51147,7 +51153,7 @@
         <v>720</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>32</v>
       </c>
@@ -51193,8 +51199,11 @@
       <c r="P33">
         <v>720</v>
       </c>
-    </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="T33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>33</v>
       </c>
@@ -51241,7 +51250,7 @@
         <v>720</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>34</v>
       </c>
@@ -51287,8 +51296,11 @@
       <c r="P35">
         <v>720</v>
       </c>
-    </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="T35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>35</v>
       </c>
@@ -51335,7 +51347,7 @@
         <v>720</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>36</v>
       </c>
@@ -51381,8 +51393,11 @@
       <c r="P37">
         <v>720</v>
       </c>
-    </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="T37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>37</v>
       </c>
@@ -51429,7 +51444,7 @@
         <v>720</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>38</v>
       </c>
@@ -51476,7 +51491,7 @@
         <v>720</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>39</v>
       </c>
@@ -51523,7 +51538,7 @@
         <v>720</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>40</v>
       </c>
@@ -51570,7 +51585,7 @@
         <v>720</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>41</v>
       </c>
@@ -51617,7 +51632,7 @@
         <v>720</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>42</v>
       </c>
@@ -51663,8 +51678,11 @@
       <c r="P43">
         <v>720</v>
       </c>
-    </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="T43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>43</v>
       </c>
@@ -51691,12 +51709,26 @@
       <c r="I44" s="7">
         <v>5</v>
       </c>
+      <c r="K44" s="7">
+        <v>60</v>
+      </c>
+      <c r="L44" s="4">
+        <v>93</v>
+      </c>
+      <c r="M44" s="4">
+        <v>93</v>
+      </c>
       <c r="N44">
-        <f t="shared" si="2"/>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+      <c r="O44">
+        <v>1930</v>
+      </c>
+      <c r="P44">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="45" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>44</v>
       </c>
@@ -51723,13 +51755,26 @@
       <c r="I45" s="7">
         <v>29</v>
       </c>
-      <c r="K45" s="7"/>
+      <c r="K45" s="7">
+        <v>53</v>
+      </c>
+      <c r="L45" s="4">
+        <v>69</v>
+      </c>
+      <c r="M45" s="4">
+        <v>69</v>
+      </c>
       <c r="N45">
-        <f t="shared" si="2"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="O45">
+        <v>1930</v>
+      </c>
+      <c r="P45">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="46" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>45</v>
       </c>
@@ -51756,13 +51801,29 @@
       <c r="I46" s="7">
         <v>3</v>
       </c>
-      <c r="K46" s="7"/>
+      <c r="K46" s="7">
+        <v>43</v>
+      </c>
+      <c r="L46" s="4">
+        <v>35</v>
+      </c>
+      <c r="M46" s="4">
+        <v>35</v>
+      </c>
       <c r="N46">
-        <f t="shared" si="2"/>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+      <c r="O46">
+        <v>1930</v>
+      </c>
+      <c r="P46">
+        <v>720</v>
+      </c>
+      <c r="T46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>46</v>
       </c>
@@ -51789,15 +51850,29 @@
       <c r="I47" s="7">
         <v>18</v>
       </c>
-      <c r="K47" s="7"/>
-      <c r="L47" s="4"/>
-      <c r="M47" s="4"/>
+      <c r="K47" s="7">
+        <v>60</v>
+      </c>
+      <c r="L47" s="4">
+        <v>92</v>
+      </c>
+      <c r="M47" s="4">
+        <v>91</v>
+      </c>
       <c r="N47">
-        <f t="shared" si="2"/>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+      <c r="O47">
+        <v>1930</v>
+      </c>
+      <c r="P47">
+        <v>720</v>
+      </c>
+      <c r="T47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>47</v>
       </c>
@@ -51824,13 +51899,29 @@
       <c r="I48" s="7">
         <v>0</v>
       </c>
-      <c r="K48" s="7"/>
+      <c r="K48" s="7">
+        <v>55</v>
+      </c>
+      <c r="L48" s="4">
+        <v>82</v>
+      </c>
+      <c r="M48" s="4">
+        <v>82</v>
+      </c>
       <c r="N48">
-        <f t="shared" si="2"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O48">
+        <v>1930</v>
+      </c>
+      <c r="P48">
+        <v>720</v>
+      </c>
+      <c r="T48" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="49" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>48</v>
       </c>
@@ -51857,12 +51948,29 @@
       <c r="I49" s="7">
         <v>27</v>
       </c>
+      <c r="K49" s="7">
+        <v>43</v>
+      </c>
+      <c r="L49" s="4">
+        <v>35</v>
+      </c>
+      <c r="M49" s="4">
+        <v>36</v>
+      </c>
       <c r="N49">
-        <f t="shared" si="2"/>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+      <c r="O49">
+        <v>1930</v>
+      </c>
+      <c r="P49">
+        <v>720</v>
+      </c>
+      <c r="T49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>49</v>
       </c>
@@ -51889,12 +51997,26 @@
       <c r="I50" s="7">
         <v>28</v>
       </c>
+      <c r="K50" s="7">
+        <v>47</v>
+      </c>
+      <c r="L50" s="4">
+        <v>55</v>
+      </c>
+      <c r="M50" s="4">
+        <v>55</v>
+      </c>
       <c r="N50">
-        <f t="shared" si="2"/>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+      <c r="O50">
+        <v>1935</v>
+      </c>
+      <c r="P50">
+        <v>733</v>
+      </c>
+    </row>
+    <row r="51" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>50</v>
       </c>
@@ -51921,12 +52043,29 @@
       <c r="I51" s="7">
         <v>26</v>
       </c>
+      <c r="K51" s="7">
+        <v>45</v>
+      </c>
+      <c r="L51" s="4">
+        <v>41</v>
+      </c>
+      <c r="M51" s="4">
+        <v>40</v>
+      </c>
       <c r="N51">
-        <f t="shared" si="2"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O51">
+        <v>1935</v>
+      </c>
+      <c r="P51">
+        <v>733</v>
+      </c>
+      <c r="T51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>51</v>
       </c>
@@ -51953,12 +52092,26 @@
       <c r="I52" s="7">
         <v>14</v>
       </c>
+      <c r="K52" s="7">
+        <v>45</v>
+      </c>
+      <c r="L52" s="4">
+        <v>40</v>
+      </c>
+      <c r="M52" s="4">
+        <v>40</v>
+      </c>
       <c r="N52">
-        <f>C52-239</f>
         <v>7</v>
       </c>
-    </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O52">
+        <v>1935</v>
+      </c>
+      <c r="P52">
+        <v>733</v>
+      </c>
+    </row>
+    <row r="53" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>52</v>
       </c>
@@ -51985,12 +52138,29 @@
       <c r="I53" s="7">
         <v>17</v>
       </c>
+      <c r="K53" s="7">
+        <v>52</v>
+      </c>
+      <c r="L53" s="4">
+        <v>62</v>
+      </c>
+      <c r="M53" s="4">
+        <v>61</v>
+      </c>
       <c r="N53">
-        <f t="shared" ref="N53:N77" si="3">C53-239</f>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+      <c r="O53">
+        <v>1935</v>
+      </c>
+      <c r="P53">
+        <v>733</v>
+      </c>
+      <c r="T53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>53</v>
       </c>
@@ -52017,12 +52187,26 @@
       <c r="I54" s="7">
         <v>23</v>
       </c>
+      <c r="K54" s="7">
+        <v>50</v>
+      </c>
+      <c r="L54" s="4">
+        <v>57</v>
+      </c>
+      <c r="M54" s="4">
+        <v>57</v>
+      </c>
       <c r="N54">
-        <f t="shared" si="3"/>
         <v>7</v>
       </c>
-    </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O54">
+        <v>1935</v>
+      </c>
+      <c r="P54">
+        <v>733</v>
+      </c>
+    </row>
+    <row r="55" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>54</v>
       </c>
@@ -52049,12 +52233,26 @@
       <c r="I55" s="7">
         <v>0</v>
       </c>
+      <c r="K55" s="7">
+        <v>46</v>
+      </c>
+      <c r="L55" s="4">
+        <v>51</v>
+      </c>
+      <c r="M55" s="4">
+        <v>51</v>
+      </c>
       <c r="N55">
-        <f t="shared" si="3"/>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+      <c r="O55">
+        <v>1935</v>
+      </c>
+      <c r="P55">
+        <v>733</v>
+      </c>
+    </row>
+    <row r="56" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>55</v>
       </c>
@@ -52081,12 +52279,26 @@
       <c r="I56" s="7">
         <v>0</v>
       </c>
+      <c r="K56" s="7">
+        <v>45</v>
+      </c>
+      <c r="L56" s="4">
+        <v>41</v>
+      </c>
+      <c r="M56" s="4">
+        <v>42</v>
+      </c>
       <c r="N56">
-        <f t="shared" si="3"/>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+      <c r="O56">
+        <v>1935</v>
+      </c>
+      <c r="P56">
+        <v>733</v>
+      </c>
+    </row>
+    <row r="57" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>56</v>
       </c>
@@ -52113,12 +52325,26 @@
       <c r="I57" s="7">
         <v>10</v>
       </c>
+      <c r="K57" s="7">
+        <v>60</v>
+      </c>
+      <c r="L57" s="4">
+        <v>102</v>
+      </c>
+      <c r="M57" s="4">
+        <v>102</v>
+      </c>
       <c r="N57">
-        <f t="shared" si="3"/>
         <v>7</v>
       </c>
-    </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O57">
+        <v>1935</v>
+      </c>
+      <c r="P57">
+        <v>733</v>
+      </c>
+    </row>
+    <row r="58" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>57</v>
       </c>
@@ -52135,11 +52361,11 @@
         <v>61</v>
       </c>
       <c r="G58" t="str">
-        <f t="shared" ref="G58:G71" si="4">IF(I58&lt;=0, "Control", IF(I58&lt;=10, "Red", IF(I58&gt;=21, "Pink", "Orange")))</f>
+        <f t="shared" ref="G58:G71" si="3">IF(I58&lt;=0, "Control", IF(I58&lt;=10, "Red", IF(I58&gt;=21, "Pink", "Orange")))</f>
         <v>Red</v>
       </c>
       <c r="H58">
-        <f t="shared" ref="H58:H71" si="5">IF(G58="Control", 1, IF(G58="Red", 2, IF(G58="Orange", 3, 4)))</f>
+        <f t="shared" ref="H58:H71" si="4">IF(G58="Control", 1, IF(G58="Red", 2, IF(G58="Orange", 3, 4)))</f>
         <v>2</v>
       </c>
       <c r="I58" s="7">
@@ -52147,11 +52373,11 @@
       </c>
       <c r="K58" s="5"/>
       <c r="N58">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="N53:N77" si="5">C58-239</f>
         <v>8</v>
       </c>
     </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>58</v>
       </c>
@@ -52168,11 +52394,11 @@
         <v>60</v>
       </c>
       <c r="G59" t="str">
+        <f t="shared" si="3"/>
+        <v>Control</v>
+      </c>
+      <c r="H59">
         <f t="shared" si="4"/>
-        <v>Control</v>
-      </c>
-      <c r="H59">
-        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="I59" s="7">
@@ -52180,11 +52406,11 @@
       </c>
       <c r="K59" s="5"/>
       <c r="N59">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>8</v>
       </c>
     </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>59</v>
       </c>
@@ -52201,11 +52427,11 @@
         <v>61</v>
       </c>
       <c r="G60" t="str">
+        <f t="shared" si="3"/>
+        <v>Pink</v>
+      </c>
+      <c r="H60">
         <f t="shared" si="4"/>
-        <v>Pink</v>
-      </c>
-      <c r="H60">
-        <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="I60" s="5">
@@ -52213,11 +52439,11 @@
       </c>
       <c r="K60" s="5"/>
       <c r="N60">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>8</v>
       </c>
     </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>60</v>
       </c>
@@ -52234,11 +52460,11 @@
         <v>60</v>
       </c>
       <c r="G61" t="str">
+        <f t="shared" si="3"/>
+        <v>Red</v>
+      </c>
+      <c r="H61">
         <f t="shared" si="4"/>
-        <v>Red</v>
-      </c>
-      <c r="H61">
-        <f t="shared" si="5"/>
         <v>2</v>
       </c>
       <c r="I61" s="5">
@@ -52246,11 +52472,11 @@
       </c>
       <c r="K61" s="5"/>
       <c r="N61">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>8</v>
       </c>
     </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>61</v>
       </c>
@@ -52267,11 +52493,11 @@
         <v>60</v>
       </c>
       <c r="G62" t="str">
+        <f t="shared" si="3"/>
+        <v>Orange</v>
+      </c>
+      <c r="H62">
         <f t="shared" si="4"/>
-        <v>Orange</v>
-      </c>
-      <c r="H62">
-        <f t="shared" si="5"/>
         <v>3</v>
       </c>
       <c r="I62" s="5">
@@ -52279,11 +52505,11 @@
       </c>
       <c r="K62" s="5"/>
       <c r="N62">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>8</v>
       </c>
     </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>62</v>
       </c>
@@ -52300,11 +52526,11 @@
         <v>61</v>
       </c>
       <c r="G63" t="str">
+        <f t="shared" si="3"/>
+        <v>Orange</v>
+      </c>
+      <c r="H63">
         <f t="shared" si="4"/>
-        <v>Orange</v>
-      </c>
-      <c r="H63">
-        <f t="shared" si="5"/>
         <v>3</v>
       </c>
       <c r="I63" s="5">
@@ -52312,11 +52538,11 @@
       </c>
       <c r="K63" s="5"/>
       <c r="N63">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>8</v>
       </c>
     </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>63</v>
       </c>
@@ -52333,11 +52559,11 @@
         <v>60</v>
       </c>
       <c r="G64" t="str">
+        <f t="shared" si="3"/>
+        <v>Control</v>
+      </c>
+      <c r="H64">
         <f t="shared" si="4"/>
-        <v>Control</v>
-      </c>
-      <c r="H64">
-        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="I64" s="5">
@@ -52345,7 +52571,7 @@
       </c>
       <c r="K64" s="5"/>
       <c r="N64">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>8</v>
       </c>
     </row>
@@ -52366,11 +52592,11 @@
         <v>60</v>
       </c>
       <c r="G65" t="str">
+        <f t="shared" si="3"/>
+        <v>Red</v>
+      </c>
+      <c r="H65">
         <f t="shared" si="4"/>
-        <v>Red</v>
-      </c>
-      <c r="H65">
-        <f t="shared" si="5"/>
         <v>2</v>
       </c>
       <c r="I65" s="5">
@@ -52378,7 +52604,7 @@
       </c>
       <c r="K65" s="5"/>
       <c r="N65">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>8</v>
       </c>
     </row>
@@ -52399,11 +52625,11 @@
         <v>60</v>
       </c>
       <c r="G66" t="str">
+        <f t="shared" si="3"/>
+        <v>Control</v>
+      </c>
+      <c r="H66">
         <f t="shared" si="4"/>
-        <v>Control</v>
-      </c>
-      <c r="H66">
-        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="I66" s="7">
@@ -52411,7 +52637,7 @@
       </c>
       <c r="K66" s="7"/>
       <c r="N66">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>9</v>
       </c>
     </row>
@@ -52432,11 +52658,11 @@
         <v>60</v>
       </c>
       <c r="G67" t="str">
+        <f t="shared" si="3"/>
+        <v>Orange</v>
+      </c>
+      <c r="H67">
         <f t="shared" si="4"/>
-        <v>Orange</v>
-      </c>
-      <c r="H67">
-        <f t="shared" si="5"/>
         <v>3</v>
       </c>
       <c r="I67" s="7">
@@ -52444,7 +52670,7 @@
       </c>
       <c r="K67" s="5"/>
       <c r="N67">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>9</v>
       </c>
     </row>
@@ -52465,11 +52691,11 @@
         <v>60</v>
       </c>
       <c r="G68" t="str">
+        <f t="shared" si="3"/>
+        <v>Pink</v>
+      </c>
+      <c r="H68">
         <f t="shared" si="4"/>
-        <v>Pink</v>
-      </c>
-      <c r="H68">
-        <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="I68" s="7">
@@ -52477,7 +52703,7 @@
       </c>
       <c r="K68" s="5"/>
       <c r="N68">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>9</v>
       </c>
     </row>
@@ -52498,11 +52724,11 @@
         <v>61</v>
       </c>
       <c r="G69" t="str">
+        <f t="shared" si="3"/>
+        <v>Pink</v>
+      </c>
+      <c r="H69">
         <f t="shared" si="4"/>
-        <v>Pink</v>
-      </c>
-      <c r="H69">
-        <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="I69" s="7">
@@ -52510,7 +52736,7 @@
       </c>
       <c r="K69" s="5"/>
       <c r="N69">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>9</v>
       </c>
     </row>
@@ -52531,11 +52757,11 @@
         <v>61</v>
       </c>
       <c r="G70" t="str">
+        <f t="shared" si="3"/>
+        <v>Pink</v>
+      </c>
+      <c r="H70">
         <f t="shared" si="4"/>
-        <v>Pink</v>
-      </c>
-      <c r="H70">
-        <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="I70" s="7">
@@ -52543,7 +52769,7 @@
       </c>
       <c r="K70" s="5"/>
       <c r="N70">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>9</v>
       </c>
     </row>
@@ -52564,11 +52790,11 @@
         <v>60</v>
       </c>
       <c r="G71" t="str">
+        <f t="shared" si="3"/>
+        <v>Red</v>
+      </c>
+      <c r="H71">
         <f t="shared" si="4"/>
-        <v>Red</v>
-      </c>
-      <c r="H71">
-        <f t="shared" si="5"/>
         <v>2</v>
       </c>
       <c r="I71" s="7">
@@ -52576,7 +52802,7 @@
       </c>
       <c r="K71" s="5"/>
       <c r="N71">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>9</v>
       </c>
     </row>
@@ -52609,7 +52835,7 @@
       </c>
       <c r="K72" s="5"/>
       <c r="N72">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
     </row>
@@ -52642,7 +52868,7 @@
       </c>
       <c r="K73" s="5"/>
       <c r="N73">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
     </row>
@@ -52675,7 +52901,7 @@
       </c>
       <c r="K74" s="5"/>
       <c r="N74">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
     </row>
@@ -52708,7 +52934,7 @@
       </c>
       <c r="K75" s="5"/>
       <c r="N75">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
     </row>
@@ -52741,7 +52967,7 @@
       </c>
       <c r="K76" s="5"/>
       <c r="N76">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
     </row>
@@ -52774,7 +53000,7 @@
       </c>
       <c r="K77" s="5"/>
       <c r="N77">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
     </row>
@@ -52791,8 +53017,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55F6BF2F-CBB2-4331-929A-D3F4AD694052}">
   <dimension ref="A1:X45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E2" workbookViewId="0">
-      <selection activeCell="Q14" sqref="Q14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O30" sqref="O30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -53676,7 +53902,7 @@
         <v>720</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>32</v>
       </c>
@@ -53725,7 +53951,7 @@
         <v>720</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>33</v>
       </c>
@@ -53774,7 +54000,7 @@
         <v>720</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>34</v>
       </c>
@@ -53823,7 +54049,7 @@
         <v>720</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>43</v>
       </c>
@@ -53853,26 +54079,26 @@
       </c>
       <c r="I20">
         <f>'Kelp consumption'!K44</f>
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="J20">
         <f>'Kelp consumption'!L44</f>
-        <v>0</v>
+        <v>93</v>
       </c>
       <c r="K20">
         <f>'Kelp consumption'!N44</f>
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="L20">
         <f>'Kelp consumption'!O44</f>
-        <v>0</v>
+        <v>1930</v>
       </c>
       <c r="M20">
         <f>'Kelp consumption'!P44</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="21" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>44</v>
       </c>
@@ -53902,11 +54128,11 @@
       </c>
       <c r="I21">
         <f>'Kelp consumption'!K45</f>
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="J21">
         <f>'Kelp consumption'!L45</f>
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="K21">
         <f>'Kelp consumption'!N45</f>
@@ -53914,14 +54140,14 @@
       </c>
       <c r="L21">
         <f>'Kelp consumption'!O45</f>
-        <v>0</v>
+        <v>1930</v>
       </c>
       <c r="M21">
         <f>'Kelp consumption'!P45</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="22" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>45</v>
       </c>
@@ -53951,26 +54177,26 @@
       </c>
       <c r="I22">
         <f>'Kelp consumption'!K46</f>
-        <v>0</v>
+        <v>43</v>
       </c>
       <c r="J22">
         <f>'Kelp consumption'!L46</f>
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="K22">
         <f>'Kelp consumption'!N46</f>
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="L22">
         <f>'Kelp consumption'!O46</f>
-        <v>0</v>
+        <v>1930</v>
       </c>
       <c r="M22">
         <f>'Kelp consumption'!P46</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="23" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>46</v>
       </c>
@@ -54000,26 +54226,29 @@
       </c>
       <c r="I23">
         <f>'Kelp consumption'!K47</f>
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="J23">
         <f>'Kelp consumption'!L47</f>
-        <v>0</v>
+        <v>92</v>
       </c>
       <c r="K23">
         <f>'Kelp consumption'!N47</f>
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="L23">
         <f>'Kelp consumption'!O47</f>
-        <v>0</v>
+        <v>1930</v>
       </c>
       <c r="M23">
         <f>'Kelp consumption'!P47</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+        <v>720</v>
+      </c>
+      <c r="X23" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="24" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>47</v>
       </c>
@@ -54049,11 +54278,11 @@
       </c>
       <c r="I24">
         <f>'Kelp consumption'!K48</f>
-        <v>0</v>
+        <v>55</v>
       </c>
       <c r="J24">
         <f>'Kelp consumption'!L48</f>
-        <v>0</v>
+        <v>82</v>
       </c>
       <c r="K24">
         <f>'Kelp consumption'!N48</f>
@@ -54061,14 +54290,14 @@
       </c>
       <c r="L24">
         <f>'Kelp consumption'!O48</f>
-        <v>0</v>
+        <v>1930</v>
       </c>
       <c r="M24">
         <f>'Kelp consumption'!P48</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="25" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>48</v>
       </c>
@@ -54098,26 +54327,26 @@
       </c>
       <c r="I25">
         <f>'Kelp consumption'!K49</f>
-        <v>0</v>
+        <v>43</v>
       </c>
       <c r="J25">
         <f>'Kelp consumption'!L49</f>
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="K25">
         <f>'Kelp consumption'!N49</f>
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="L25">
         <f>'Kelp consumption'!O49</f>
-        <v>0</v>
+        <v>1930</v>
       </c>
       <c r="M25">
         <f>'Kelp consumption'!P49</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="26" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>65</v>
       </c>
@@ -54166,7 +54395,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>66</v>
       </c>
@@ -54215,7 +54444,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>67</v>
       </c>
@@ -54264,7 +54493,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>68</v>
       </c>
@@ -54313,7 +54542,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>69</v>
       </c>
@@ -54362,7 +54591,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>70</v>
       </c>
@@ -54411,7 +54640,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>71</v>
       </c>

</xml_diff>

<commit_message>
Sept 4 afternoon update, kelp photo update
</commit_message>
<xml_diff>
--- a/data/raw.xlsx
+++ b/data/raw.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/EcosystemRecoveryLab/Github/Ritger-Corynactis-urchin-deterrence/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{608B5E12-7104-8F42-A8BF-FAE3D0669640}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE8E8FAF-2251-7143-A30A-6CB66A9931C9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3840" yWindow="7500" windowWidth="33780" windowHeight="17400" activeTab="1" xr2:uid="{58E670A5-634C-427F-960F-9DA76C64E810}"/>
+    <workbookView xWindow="2600" yWindow="7260" windowWidth="33780" windowHeight="17400" activeTab="2" xr2:uid="{58E670A5-634C-427F-960F-9DA76C64E810}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="3" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="87">
   <si>
     <t>Day</t>
   </si>
@@ -258,6 +258,36 @@
   </si>
   <si>
     <t>0?</t>
+  </si>
+  <si>
+    <t>Double check GoPro - only 4 hours copied to computer</t>
+  </si>
+  <si>
+    <t>really fun urchin behavior</t>
+  </si>
+  <si>
+    <t>Times in contact with Cory</t>
+  </si>
+  <si>
+    <t>Times deterred from Cory</t>
+  </si>
+  <si>
+    <t>Time in Kelp zone (min)</t>
+  </si>
+  <si>
+    <t>Time in Cory zone (min)</t>
+  </si>
+  <si>
+    <t>Time spent with Kelp</t>
+  </si>
+  <si>
+    <t>Time to cross Cory (first)</t>
+  </si>
+  <si>
+    <t>Time to cross Cory (average)</t>
+  </si>
+  <si>
+    <t>N/A</t>
   </si>
 </sst>
 </file>
@@ -49546,9 +49576,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD5E687B-43EE-4B00-8604-7EB9984510DD}">
   <dimension ref="A1:V77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="T52" sqref="T52"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Q60" sqref="Q60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -49729,7 +49759,7 @@
         <v>35</v>
       </c>
       <c r="N3">
-        <f t="shared" ref="N3:N51" si="2">C3-236</f>
+        <f t="shared" ref="N3:N43" si="2">C3-236</f>
         <v>7</v>
       </c>
       <c r="O3">
@@ -52373,7 +52403,7 @@
       </c>
       <c r="K58" s="5"/>
       <c r="N58">
-        <f t="shared" ref="N53:N77" si="5">C58-239</f>
+        <f t="shared" ref="N58:N77" si="5">C58-239</f>
         <v>8</v>
       </c>
     </row>
@@ -53015,10 +53045,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55F6BF2F-CBB2-4331-929A-D3F4AD694052}">
-  <dimension ref="A1:X45"/>
+  <dimension ref="A1:AC45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O30" sqref="O30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S22" sqref="S22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -53038,17 +53068,21 @@
     <col min="13" max="13" width="9.5" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="16.1640625" bestFit="1" customWidth="1"/>
     <col min="15" max="16" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="17.83203125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="21.1640625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="18.83203125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="19.33203125" customWidth="1"/>
+    <col min="18" max="18" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="18.33203125" customWidth="1"/>
+    <col min="21" max="21" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="21" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="21.1640625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="10.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:29" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -53092,37 +53126,52 @@
         <v>15</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>49</v>
+        <v>82</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>16</v>
+        <v>81</v>
       </c>
       <c r="Q1" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="R1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="S1" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="W1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="X1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="Y1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="Z1" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="AA1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="AB1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="AC1" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -53170,11 +53219,11 @@
         <f>'Kelp consumption'!P2</f>
         <v>730</v>
       </c>
-      <c r="Q2">
+      <c r="R2">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -53222,11 +53271,11 @@
         <f>'Kelp consumption'!P3</f>
         <v>730</v>
       </c>
-      <c r="Q3">
+      <c r="R3">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -53274,14 +53323,14 @@
         <f>'Kelp consumption'!P4</f>
         <v>730</v>
       </c>
-      <c r="Q4">
+      <c r="R4">
         <v>1</v>
       </c>
-      <c r="X4" t="s">
+      <c r="AC4" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -53329,11 +53378,11 @@
         <f>'Kelp consumption'!P5</f>
         <v>730</v>
       </c>
-      <c r="Q5">
+      <c r="R5">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -53381,11 +53430,11 @@
         <f>'Kelp consumption'!P6</f>
         <v>730</v>
       </c>
-      <c r="Q6">
+      <c r="R6">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -53433,11 +53482,11 @@
         <f>'Kelp consumption'!P7</f>
         <v>730</v>
       </c>
-      <c r="Q7">
+      <c r="R7">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>15</v>
       </c>
@@ -53485,11 +53534,11 @@
         <f>'Kelp consumption'!P16</f>
         <v>710</v>
       </c>
-      <c r="Q8">
+      <c r="R8">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>16</v>
       </c>
@@ -53537,11 +53586,11 @@
         <f>'Kelp consumption'!P17</f>
         <v>710</v>
       </c>
-      <c r="Q9">
+      <c r="R9">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>17</v>
       </c>
@@ -53589,11 +53638,11 @@
         <f>'Kelp consumption'!P18</f>
         <v>710</v>
       </c>
-      <c r="Q10">
+      <c r="R10">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>18</v>
       </c>
@@ -53641,14 +53690,14 @@
         <f>'Kelp consumption'!P19</f>
         <v>710</v>
       </c>
-      <c r="Q11">
+      <c r="R11">
         <v>0</v>
       </c>
-      <c r="X11" t="s">
+      <c r="AC11" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>19</v>
       </c>
@@ -53696,11 +53745,11 @@
         <f>'Kelp consumption'!P20</f>
         <v>710</v>
       </c>
-      <c r="Q12">
+      <c r="R12">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>20</v>
       </c>
@@ -53748,11 +53797,11 @@
         <f>'Kelp consumption'!P21</f>
         <v>710</v>
       </c>
-      <c r="Q13">
+      <c r="R13">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>29</v>
       </c>
@@ -53800,11 +53849,14 @@
         <f>'Kelp consumption'!P30</f>
         <v>720</v>
       </c>
-      <c r="X14" t="s">
+      <c r="R14">
+        <v>1</v>
+      </c>
+      <c r="AC14" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>30</v>
       </c>
@@ -53852,8 +53904,11 @@
         <f>'Kelp consumption'!P31</f>
         <v>720</v>
       </c>
-    </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="R15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>31</v>
       </c>
@@ -53901,8 +53956,14 @@
         <f>'Kelp consumption'!P32</f>
         <v>720</v>
       </c>
-    </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="R16">
+        <v>1</v>
+      </c>
+      <c r="AC16" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="17" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>32</v>
       </c>
@@ -53950,8 +54011,11 @@
         <f>'Kelp consumption'!P33</f>
         <v>720</v>
       </c>
-    </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="R17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>33</v>
       </c>
@@ -53999,8 +54063,11 @@
         <f>'Kelp consumption'!P34</f>
         <v>720</v>
       </c>
-    </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="R18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>34</v>
       </c>
@@ -54048,8 +54115,11 @@
         <f>'Kelp consumption'!P35</f>
         <v>720</v>
       </c>
-    </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="R19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>43</v>
       </c>
@@ -54097,8 +54167,11 @@
         <f>'Kelp consumption'!P44</f>
         <v>720</v>
       </c>
-    </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="R20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>44</v>
       </c>
@@ -54146,8 +54219,11 @@
         <f>'Kelp consumption'!P45</f>
         <v>720</v>
       </c>
-    </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="R21">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>45</v>
       </c>
@@ -54195,8 +54271,11 @@
         <f>'Kelp consumption'!P46</f>
         <v>720</v>
       </c>
-    </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="R22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>46</v>
       </c>
@@ -54244,11 +54323,14 @@
         <f>'Kelp consumption'!P47</f>
         <v>720</v>
       </c>
-      <c r="X23" t="s">
+      <c r="R23" t="s">
+        <v>86</v>
+      </c>
+      <c r="AC23" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>47</v>
       </c>
@@ -54296,8 +54378,14 @@
         <f>'Kelp consumption'!P48</f>
         <v>720</v>
       </c>
-    </row>
-    <row r="25" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="R24">
+        <v>1</v>
+      </c>
+      <c r="AC24" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="25" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>48</v>
       </c>
@@ -54345,8 +54433,11 @@
         <f>'Kelp consumption'!P49</f>
         <v>720</v>
       </c>
-    </row>
-    <row r="26" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="R25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>65</v>
       </c>
@@ -54395,7 +54486,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>66</v>
       </c>
@@ -54444,7 +54535,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>67</v>
       </c>
@@ -54493,7 +54584,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>68</v>
       </c>
@@ -54542,7 +54633,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>69</v>
       </c>
@@ -54591,7 +54682,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>70</v>
       </c>
@@ -54640,7 +54731,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>71</v>
       </c>
@@ -54689,7 +54780,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>72</v>
       </c>
@@ -54738,7 +54829,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>73</v>
       </c>
@@ -54787,7 +54878,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>74</v>
       </c>
@@ -54836,7 +54927,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>75</v>
       </c>
@@ -54885,7 +54976,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>76</v>
       </c>
@@ -54934,75 +55025,75 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:27" x14ac:dyDescent="0.2">
       <c r="O43">
         <v>9</v>
       </c>
       <c r="P43">
         <v>81</v>
       </c>
-      <c r="Q43" t="s">
+      <c r="R43" t="s">
         <v>60</v>
       </c>
-      <c r="R43" t="s">
+      <c r="W43" t="s">
         <v>59</v>
       </c>
-      <c r="S43">
-        <f>IF(R43="Control", 1, IF(R43="Red", 2, IF(R43="Orange", 3, 4)))</f>
+      <c r="X43">
+        <f>IF(W43="Control", 1, IF(W43="Red", 2, IF(W43="Orange", 3, 4)))</f>
         <v>3</v>
       </c>
-      <c r="U43" t="s">
+      <c r="Z43" t="s">
         <v>62</v>
       </c>
-      <c r="V43" t="s">
+      <c r="AA43" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="44" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:27" x14ac:dyDescent="0.2">
       <c r="O44">
         <v>10</v>
       </c>
       <c r="P44">
         <v>82</v>
       </c>
-      <c r="Q44" t="s">
+      <c r="R44" t="s">
         <v>60</v>
       </c>
-      <c r="R44" t="s">
+      <c r="W44" t="s">
         <v>57</v>
       </c>
-      <c r="S44">
-        <f>IF(R44="Control", 1, IF(R44="Red", 2, IF(R44="Orange", 3, 4)))</f>
+      <c r="X44">
+        <f>IF(W44="Control", 1, IF(W44="Red", 2, IF(W44="Orange", 3, 4)))</f>
         <v>1</v>
       </c>
-      <c r="U44">
+      <c r="Z44">
         <v>26</v>
       </c>
-      <c r="V44">
+      <c r="AA44">
         <v>21</v>
       </c>
     </row>
-    <row r="45" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:27" x14ac:dyDescent="0.2">
       <c r="O45">
         <v>11</v>
       </c>
       <c r="P45">
         <v>83</v>
       </c>
-      <c r="Q45" t="s">
+      <c r="R45" t="s">
         <v>60</v>
       </c>
-      <c r="R45" t="s">
+      <c r="W45" t="s">
         <v>58</v>
       </c>
-      <c r="S45">
-        <f>IF(R45="Control", 1, IF(R45="Red", 2, IF(R45="Orange", 3, 4)))</f>
+      <c r="X45">
+        <f>IF(W45="Control", 1, IF(W45="Red", 2, IF(W45="Orange", 3, 4)))</f>
         <v>2</v>
       </c>
-      <c r="U45">
+      <c r="Z45">
         <v>6</v>
       </c>
-      <c r="V45">
+      <c r="AA45">
         <v>20</v>
       </c>
     </row>

</xml_diff>

<commit_message>
first kelp images analyzed
</commit_message>
<xml_diff>
--- a/data/raw.xlsx
+++ b/data/raw.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/EcosystemRecoveryLab/Github/Ritger-Corynactis-urchin-deterrence/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/EcosystemRecoveryLab/github/Ritger-Corynactis-urchin-deterrence/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE8E8FAF-2251-7143-A30A-6CB66A9931C9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2ADA8B6-570E-3C45-A0B4-A15B38E5F405}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2600" yWindow="7260" windowWidth="33780" windowHeight="17400" activeTab="2" xr2:uid="{58E670A5-634C-427F-960F-9DA76C64E810}"/>
+    <workbookView xWindow="24840" yWindow="6220" windowWidth="25320" windowHeight="17400" activeTab="1" xr2:uid="{58E670A5-634C-427F-960F-9DA76C64E810}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="3" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="89">
   <si>
     <t>Day</t>
   </si>
@@ -288,6 +288,12 @@
   </si>
   <si>
     <t>N/A</t>
+  </si>
+  <si>
+    <t>missed a little bit</t>
+  </si>
+  <si>
+    <t>or 108.065</t>
   </si>
 </sst>
 </file>
@@ -49576,9 +49582,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD5E687B-43EE-4B00-8604-7EB9984510DD}">
   <dimension ref="A1:V77"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q60" sqref="Q60"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="R17" sqref="R17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -50400,6 +50406,12 @@
       <c r="P16">
         <v>710</v>
       </c>
+      <c r="Q16">
+        <v>107.758</v>
+      </c>
+      <c r="R16" t="s">
+        <v>88</v>
+      </c>
       <c r="T16">
         <v>0</v>
       </c>
@@ -50450,6 +50462,9 @@
       <c r="P17">
         <v>710</v>
       </c>
+      <c r="Q17">
+        <v>101.61</v>
+      </c>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A18">
@@ -50497,6 +50512,9 @@
       <c r="P18">
         <v>710</v>
       </c>
+      <c r="Q18">
+        <v>90.218999999999994</v>
+      </c>
       <c r="T18">
         <v>0</v>
       </c>
@@ -50547,6 +50565,9 @@
       <c r="P19">
         <v>710</v>
       </c>
+      <c r="Q19">
+        <v>90.47</v>
+      </c>
       <c r="T19">
         <v>0</v>
       </c>
@@ -50597,6 +50618,9 @@
       <c r="P20">
         <v>710</v>
       </c>
+      <c r="Q20">
+        <v>131.33099999999999</v>
+      </c>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A21">
@@ -50644,6 +50668,9 @@
       <c r="P21">
         <v>710</v>
       </c>
+      <c r="Q21">
+        <v>94.843000000000004</v>
+      </c>
       <c r="T21">
         <v>0</v>
       </c>
@@ -50694,6 +50721,12 @@
       <c r="P22">
         <v>705</v>
       </c>
+      <c r="Q22">
+        <v>120.03700000000001</v>
+      </c>
+      <c r="R22" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A23">
@@ -50741,6 +50774,9 @@
       <c r="P23">
         <v>705</v>
       </c>
+      <c r="Q23">
+        <v>122.246</v>
+      </c>
       <c r="T23">
         <v>0</v>
       </c>
@@ -50791,6 +50827,9 @@
       <c r="P24">
         <v>705</v>
       </c>
+      <c r="Q24">
+        <v>100.352</v>
+      </c>
       <c r="T24">
         <v>0</v>
       </c>
@@ -50841,6 +50880,9 @@
       <c r="P25">
         <v>705</v>
       </c>
+      <c r="Q25">
+        <v>95.665999999999997</v>
+      </c>
       <c r="T25">
         <v>0</v>
       </c>
@@ -50891,6 +50933,9 @@
       <c r="P26">
         <v>705</v>
       </c>
+      <c r="Q26">
+        <v>103.68300000000001</v>
+      </c>
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A27">
@@ -50938,6 +50983,9 @@
       <c r="P27">
         <v>705</v>
       </c>
+      <c r="Q27">
+        <v>102.07</v>
+      </c>
       <c r="T27">
         <v>0</v>
       </c>
@@ -50988,6 +51036,9 @@
       <c r="P28">
         <v>705</v>
       </c>
+      <c r="Q28">
+        <v>105.818</v>
+      </c>
       <c r="T28">
         <v>0</v>
       </c>
@@ -51037,6 +51088,9 @@
       </c>
       <c r="P29">
         <v>705</v>
+      </c>
+      <c r="Q29">
+        <v>109.04</v>
       </c>
       <c r="T29">
         <v>0</v>
@@ -53047,7 +53101,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55F6BF2F-CBB2-4331-929A-D3F4AD694052}">
   <dimension ref="A1:AC45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="S22" sqref="S22"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
some kelp image analysis
</commit_message>
<xml_diff>
--- a/data/raw.xlsx
+++ b/data/raw.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/EcosystemRecoveryLab/github/Ritger-Corynactis-urchin-deterrence/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2ADA8B6-570E-3C45-A0B4-A15B38E5F405}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DE1DE6D-A1C9-8544-84C0-EF3F67210132}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24840" yWindow="6220" windowWidth="25320" windowHeight="17400" activeTab="1" xr2:uid="{58E670A5-634C-427F-960F-9DA76C64E810}"/>
+    <workbookView xWindow="13100" yWindow="5240" windowWidth="23780" windowHeight="13760" activeTab="2" xr2:uid="{58E670A5-634C-427F-960F-9DA76C64E810}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="3" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="93">
   <si>
     <t>Day</t>
   </si>
@@ -200,28 +200,13 @@
     <t>Comments on trial</t>
   </si>
   <si>
-    <t>Control</t>
-  </si>
-  <si>
-    <t>Red</t>
-  </si>
-  <si>
-    <t>Orange</t>
-  </si>
-  <si>
     <t>N</t>
   </si>
   <si>
     <t>S</t>
   </si>
   <si>
-    <t>tiles needing a home</t>
-  </si>
-  <si>
     <t>1-6 (boatyard), 5-14 (balcony)</t>
-  </si>
-  <si>
-    <t>tiles needing a video</t>
   </si>
   <si>
     <t>North (N/E) or South (S/W) in tank</t>
@@ -257,9 +242,6 @@
     <t>No video</t>
   </si>
   <si>
-    <t>0?</t>
-  </si>
-  <si>
     <t>Double check GoPro - only 4 hours copied to computer</t>
   </si>
   <si>
@@ -290,10 +272,40 @@
     <t>N/A</t>
   </si>
   <si>
-    <t>missed a little bit</t>
+    <t>too much measured on "after"</t>
   </si>
   <si>
-    <t>or 108.065</t>
+    <t>not enough measured on "before"</t>
+  </si>
+  <si>
+    <t>"after" included hole</t>
+  </si>
+  <si>
+    <t xml:space="preserve">too much measured on "after" </t>
+  </si>
+  <si>
+    <t>shade =&gt; guesstimate</t>
+  </si>
+  <si>
+    <t>"after" included some shadow</t>
+  </si>
+  <si>
+    <t>"before" and "after" included some shadow</t>
+  </si>
+  <si>
+    <t>Kelp consumed?</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>maybe no</t>
+  </si>
+  <si>
+    <t>NO</t>
   </si>
 </sst>
 </file>
@@ -706,7 +718,7 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -714,7 +726,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -722,7 +734,7 @@
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -730,7 +742,7 @@
         <v>27</v>
       </c>
       <c r="B8" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -738,7 +750,7 @@
         <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
@@ -746,7 +758,7 @@
         <v>5</v>
       </c>
       <c r="B10" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
@@ -49580,11 +49592,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD5E687B-43EE-4B00-8604-7EB9984510DD}">
-  <dimension ref="A1:V77"/>
+  <dimension ref="A1:W77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+    <sheetView topLeftCell="H1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="R17" sqref="R17"/>
+      <selection pane="bottomLeft" activeCell="R11" sqref="R11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -49608,12 +49620,12 @@
     <col min="17" max="17" width="17.6640625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="16.1640625" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="21.1640625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="24.1640625" customWidth="1"/>
-    <col min="21" max="21" width="7.1640625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="21" width="24.1640625" customWidth="1"/>
+    <col min="22" max="22" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="10.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -49648,10 +49660,10 @@
         <v>6</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="N1" s="2" t="s">
         <v>9</v>
@@ -49675,13 +49687,16 @@
         <v>14</v>
       </c>
       <c r="U1" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="V1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="W1" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -49695,7 +49710,7 @@
         <v>1</v>
       </c>
       <c r="F2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="G2" t="str">
         <f>IF(I2&lt;=0, "Control", IF(I2&lt;=10, "Red", IF(I2&gt;=21, "Pink", "Orange")))</f>
@@ -49727,8 +49742,23 @@
       <c r="P2">
         <v>730</v>
       </c>
-    </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="S2">
+        <f t="shared" ref="S2:S15" si="0">Q2-R2</f>
+        <v>0</v>
+      </c>
+      <c r="T2" t="e">
+        <f>S2/Q2</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U2" t="s">
+        <v>89</v>
+      </c>
+      <c r="V2" t="str">
+        <f>IF(E2&gt;6,"no","yes")</f>
+        <v>yes</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -49742,14 +49772,14 @@
         <v>2</v>
       </c>
       <c r="F3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="G3" t="str">
-        <f t="shared" ref="G3:G57" si="0">IF(I3&lt;=0, "Control", IF(I3&lt;=10, "Red", IF(I3&gt;=21, "Pink", "Orange")))</f>
+        <f t="shared" ref="G3:G57" si="1">IF(I3&lt;=0, "Control", IF(I3&lt;=10, "Red", IF(I3&gt;=21, "Pink", "Orange")))</f>
         <v>Orange</v>
       </c>
       <c r="H3">
-        <f t="shared" ref="H3:H57" si="1">IF(G3="Control", 1, IF(G3="Red", 2, IF(G3="Orange", 3, 4)))</f>
+        <f t="shared" ref="H3:H57" si="2">IF(G3="Control", 1, IF(G3="Red", 2, IF(G3="Orange", 3, 4)))</f>
         <v>3</v>
       </c>
       <c r="I3" s="7">
@@ -49765,7 +49795,7 @@
         <v>35</v>
       </c>
       <c r="N3">
-        <f t="shared" ref="N3:N43" si="2">C3-236</f>
+        <f t="shared" ref="N3:N43" si="3">C3-236</f>
         <v>7</v>
       </c>
       <c r="O3">
@@ -49774,11 +49804,23 @@
       <c r="P3">
         <v>730</v>
       </c>
-      <c r="T3">
+      <c r="S3">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="T3" t="e">
+        <f t="shared" ref="T3:T66" si="4">S3/Q3</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U3" t="s">
+        <v>90</v>
+      </c>
+      <c r="V3" t="str">
+        <f t="shared" ref="V3:V66" si="5">IF(E3&gt;6,"no","yes")</f>
+        <v>yes</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -49792,14 +49834,14 @@
         <v>3</v>
       </c>
       <c r="F4" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="G4" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Control</v>
       </c>
       <c r="H4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I4" s="7">
@@ -49815,7 +49857,7 @@
         <v>43</v>
       </c>
       <c r="N4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>7</v>
       </c>
       <c r="O4">
@@ -49824,11 +49866,26 @@
       <c r="P4">
         <v>730</v>
       </c>
-      <c r="V4" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="S4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="T4" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U4" t="s">
+        <v>89</v>
+      </c>
+      <c r="V4" t="str">
+        <f t="shared" si="5"/>
+        <v>yes</v>
+      </c>
+      <c r="W4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -49842,14 +49899,14 @@
         <v>4</v>
       </c>
       <c r="F5" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="G5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Red</v>
       </c>
       <c r="H5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="I5" s="7">
@@ -49865,7 +49922,7 @@
         <v>52</v>
       </c>
       <c r="N5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>7</v>
       </c>
       <c r="O5">
@@ -49874,8 +49931,23 @@
       <c r="P5">
         <v>730</v>
       </c>
-    </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="S5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="T5" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U5" t="s">
+        <v>89</v>
+      </c>
+      <c r="V5" t="str">
+        <f t="shared" si="5"/>
+        <v>yes</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -49889,14 +49961,14 @@
         <v>5</v>
       </c>
       <c r="F6" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="G6" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Pink</v>
       </c>
       <c r="H6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="I6" s="7">
@@ -49912,7 +49984,7 @@
         <v>58</v>
       </c>
       <c r="N6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>7</v>
       </c>
       <c r="O6">
@@ -49921,8 +49993,23 @@
       <c r="P6">
         <v>730</v>
       </c>
-    </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="S6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="T6" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U6" t="s">
+        <v>89</v>
+      </c>
+      <c r="V6" t="str">
+        <f t="shared" si="5"/>
+        <v>yes</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -49936,14 +50023,14 @@
         <v>6</v>
       </c>
       <c r="F7" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="G7" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Orange</v>
       </c>
       <c r="H7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="I7" s="7">
@@ -49959,7 +50046,7 @@
         <v>41</v>
       </c>
       <c r="N7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>7</v>
       </c>
       <c r="O7">
@@ -49968,8 +50055,23 @@
       <c r="P7">
         <v>730</v>
       </c>
-    </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="S7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="T7" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U7" t="s">
+        <v>89</v>
+      </c>
+      <c r="V7" t="str">
+        <f t="shared" si="5"/>
+        <v>yes</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -49983,14 +50085,14 @@
         <v>7</v>
       </c>
       <c r="F8" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="G8" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Orange</v>
       </c>
       <c r="H8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="I8" s="5">
@@ -50006,7 +50108,7 @@
         <v>78</v>
       </c>
       <c r="N8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>7</v>
       </c>
       <c r="O8">
@@ -50015,11 +50117,23 @@
       <c r="P8">
         <v>740</v>
       </c>
-      <c r="T8">
+      <c r="S8">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="T8" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U8" t="s">
+        <v>90</v>
+      </c>
+      <c r="V8" t="str">
+        <f t="shared" si="5"/>
+        <v>no</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -50033,14 +50147,14 @@
         <v>8</v>
       </c>
       <c r="F9" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="G9" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Pink</v>
       </c>
       <c r="H9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="I9" s="7">
@@ -50056,7 +50170,7 @@
         <v>95</v>
       </c>
       <c r="N9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>7</v>
       </c>
       <c r="O9">
@@ -50065,11 +50179,23 @@
       <c r="P9">
         <v>740</v>
       </c>
-      <c r="T9">
+      <c r="S9">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="T9" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U9" t="s">
+        <v>90</v>
+      </c>
+      <c r="V9" t="str">
+        <f t="shared" si="5"/>
+        <v>no</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -50083,14 +50209,14 @@
         <v>9</v>
       </c>
       <c r="F10" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="G10" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Red</v>
       </c>
       <c r="H10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="I10" s="5">
@@ -50106,7 +50232,7 @@
         <v>50</v>
       </c>
       <c r="N10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>7</v>
       </c>
       <c r="O10">
@@ -50115,11 +50241,23 @@
       <c r="P10">
         <v>740</v>
       </c>
-      <c r="T10">
+      <c r="S10">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="T10" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U10" t="s">
+        <v>90</v>
+      </c>
+      <c r="V10" t="str">
+        <f t="shared" si="5"/>
+        <v>no</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -50133,14 +50271,14 @@
         <v>10</v>
       </c>
       <c r="F11" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="G11" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Red</v>
       </c>
       <c r="H11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="I11" s="5">
@@ -50156,7 +50294,7 @@
         <v>62</v>
       </c>
       <c r="N11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>7</v>
       </c>
       <c r="O11">
@@ -50165,11 +50303,23 @@
       <c r="P11">
         <v>740</v>
       </c>
-      <c r="T11">
+      <c r="S11">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="T11" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U11" t="s">
+        <v>90</v>
+      </c>
+      <c r="V11" t="str">
+        <f t="shared" si="5"/>
+        <v>no</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -50183,14 +50333,14 @@
         <v>11</v>
       </c>
       <c r="F12" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="G12" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Control</v>
       </c>
       <c r="H12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I12" s="5">
@@ -50206,7 +50356,7 @@
         <v>89</v>
       </c>
       <c r="N12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>7</v>
       </c>
       <c r="O12">
@@ -50215,8 +50365,23 @@
       <c r="P12">
         <v>740</v>
       </c>
-    </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="S12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="T12" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U12" t="s">
+        <v>89</v>
+      </c>
+      <c r="V12" t="str">
+        <f t="shared" si="5"/>
+        <v>no</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -50230,14 +50395,14 @@
         <v>12</v>
       </c>
       <c r="F13" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="G13" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Orange</v>
       </c>
       <c r="H13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="I13" s="5">
@@ -50253,7 +50418,7 @@
         <v>43</v>
       </c>
       <c r="N13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>7</v>
       </c>
       <c r="O13">
@@ -50262,8 +50427,23 @@
       <c r="P13">
         <v>740</v>
       </c>
-    </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="S13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="T13" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U13" t="s">
+        <v>89</v>
+      </c>
+      <c r="V13" t="str">
+        <f t="shared" si="5"/>
+        <v>no</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -50277,14 +50457,14 @@
         <v>13</v>
       </c>
       <c r="F14" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="G14" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Control</v>
       </c>
       <c r="H14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I14" s="5">
@@ -50300,7 +50480,7 @@
         <v>53</v>
       </c>
       <c r="N14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>7</v>
       </c>
       <c r="O14">
@@ -50309,8 +50489,23 @@
       <c r="P14">
         <v>740</v>
       </c>
-    </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="S14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="T14" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U14" t="s">
+        <v>89</v>
+      </c>
+      <c r="V14" t="str">
+        <f t="shared" si="5"/>
+        <v>no</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -50324,14 +50519,14 @@
         <v>14</v>
       </c>
       <c r="F15" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="G15" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Pink</v>
       </c>
       <c r="H15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="I15" s="5">
@@ -50347,7 +50542,7 @@
         <v>60</v>
       </c>
       <c r="N15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>7</v>
       </c>
       <c r="O15">
@@ -50356,11 +50551,23 @@
       <c r="P15">
         <v>740</v>
       </c>
-      <c r="T15">
+      <c r="S15">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="T15" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U15" t="s">
+        <v>90</v>
+      </c>
+      <c r="V15" t="str">
+        <f t="shared" si="5"/>
+        <v>no</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -50374,14 +50581,14 @@
         <v>1</v>
       </c>
       <c r="F16" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="G16" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Red</v>
       </c>
       <c r="H16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="I16" s="7">
@@ -50397,7 +50604,7 @@
         <v>45</v>
       </c>
       <c r="N16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="O16">
@@ -50407,16 +50614,28 @@
         <v>710</v>
       </c>
       <c r="Q16">
-        <v>107.758</v>
-      </c>
-      <c r="R16" t="s">
-        <v>88</v>
+        <v>108.065</v>
+      </c>
+      <c r="R16">
+        <v>106.86199999999999</v>
+      </c>
+      <c r="S16">
+        <f>Q16-R16</f>
+        <v>1.203000000000003</v>
       </c>
       <c r="T16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.2">
+        <f t="shared" si="4"/>
+        <v>1.1132188960347966E-2</v>
+      </c>
+      <c r="U16" t="s">
+        <v>90</v>
+      </c>
+      <c r="V16" t="str">
+        <f t="shared" si="5"/>
+        <v>yes</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -50430,14 +50649,14 @@
         <v>2</v>
       </c>
       <c r="F17" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="G17" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Orange</v>
       </c>
       <c r="H17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="I17" s="7">
@@ -50453,7 +50672,7 @@
         <v>41</v>
       </c>
       <c r="N17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="O17">
@@ -50465,8 +50684,30 @@
       <c r="Q17">
         <v>101.61</v>
       </c>
-    </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="R17">
+        <f>55.005+11.278</f>
+        <v>66.283000000000001</v>
+      </c>
+      <c r="S17">
+        <f t="shared" ref="S17:S77" si="6">Q17-R17</f>
+        <v>35.326999999999998</v>
+      </c>
+      <c r="T17">
+        <f t="shared" si="4"/>
+        <v>0.34767247318177341</v>
+      </c>
+      <c r="U17" t="s">
+        <v>89</v>
+      </c>
+      <c r="V17" t="str">
+        <f t="shared" si="5"/>
+        <v>yes</v>
+      </c>
+      <c r="W17" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="18" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
@@ -50480,14 +50721,14 @@
         <v>3</v>
       </c>
       <c r="F18" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="G18" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Orange</v>
       </c>
       <c r="H18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="I18" s="7">
@@ -50503,7 +50744,7 @@
         <v>85</v>
       </c>
       <c r="N18">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="O18">
@@ -50515,11 +50756,29 @@
       <c r="Q18">
         <v>90.218999999999994</v>
       </c>
+      <c r="R18">
+        <v>88.927000000000007</v>
+      </c>
+      <c r="S18">
+        <f t="shared" si="6"/>
+        <v>1.2919999999999874</v>
+      </c>
       <c r="T18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.2">
+        <f t="shared" si="4"/>
+        <v>1.4320708498209772E-2</v>
+      </c>
+      <c r="U18" t="s">
+        <v>90</v>
+      </c>
+      <c r="V18" t="str">
+        <f t="shared" si="5"/>
+        <v>yes</v>
+      </c>
+      <c r="W18" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
@@ -50533,14 +50792,14 @@
         <v>4</v>
       </c>
       <c r="F19" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="G19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Control</v>
       </c>
       <c r="H19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I19" s="7">
@@ -50556,7 +50815,7 @@
         <v>51</v>
       </c>
       <c r="N19">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="O19">
@@ -50568,11 +50827,26 @@
       <c r="Q19">
         <v>90.47</v>
       </c>
+      <c r="R19">
+        <v>88.608999999999995</v>
+      </c>
+      <c r="S19">
+        <f t="shared" si="6"/>
+        <v>1.8610000000000042</v>
+      </c>
       <c r="T19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.2">
+        <f t="shared" si="4"/>
+        <v>2.0570354813750462E-2</v>
+      </c>
+      <c r="U19" t="s">
+        <v>90</v>
+      </c>
+      <c r="V19" t="str">
+        <f t="shared" si="5"/>
+        <v>yes</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
@@ -50586,14 +50860,14 @@
         <v>5</v>
       </c>
       <c r="F20" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="G20" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Pink</v>
       </c>
       <c r="H20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="I20" s="7">
@@ -50609,7 +50883,7 @@
         <v>61</v>
       </c>
       <c r="N20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="O20">
@@ -50621,8 +50895,26 @@
       <c r="Q20">
         <v>131.33099999999999</v>
       </c>
-    </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="R20">
+        <v>105.565</v>
+      </c>
+      <c r="S20">
+        <f t="shared" si="6"/>
+        <v>25.765999999999991</v>
+      </c>
+      <c r="T20">
+        <f t="shared" si="4"/>
+        <v>0.19619130289116807</v>
+      </c>
+      <c r="U20" t="s">
+        <v>89</v>
+      </c>
+      <c r="V20" t="str">
+        <f t="shared" si="5"/>
+        <v>yes</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
@@ -50636,14 +50928,14 @@
         <v>6</v>
       </c>
       <c r="F21" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="G21" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Red</v>
       </c>
       <c r="H21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="I21" s="7">
@@ -50659,7 +50951,7 @@
         <v>45</v>
       </c>
       <c r="N21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="O21">
@@ -50671,11 +50963,26 @@
       <c r="Q21">
         <v>94.843000000000004</v>
       </c>
+      <c r="R21">
+        <v>94.238</v>
+      </c>
+      <c r="S21">
+        <f t="shared" si="6"/>
+        <v>0.60500000000000398</v>
+      </c>
       <c r="T21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.2">
+        <f t="shared" si="4"/>
+        <v>6.3789631285387843E-3</v>
+      </c>
+      <c r="U21" t="s">
+        <v>90</v>
+      </c>
+      <c r="V21" t="str">
+        <f t="shared" si="5"/>
+        <v>yes</v>
+      </c>
+    </row>
+    <row r="22" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
@@ -50689,14 +50996,14 @@
         <v>7</v>
       </c>
       <c r="F22" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="G22" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Pink</v>
       </c>
       <c r="H22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="I22" s="7">
@@ -50712,7 +51019,7 @@
         <v>53</v>
       </c>
       <c r="N22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="O22">
@@ -50724,11 +51031,29 @@
       <c r="Q22">
         <v>120.03700000000001</v>
       </c>
-      <c r="R22" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="R22">
+        <v>118.857</v>
+      </c>
+      <c r="S22">
+        <f t="shared" si="6"/>
+        <v>1.1800000000000068</v>
+      </c>
+      <c r="T22">
+        <f t="shared" si="4"/>
+        <v>9.8303023234503264E-3</v>
+      </c>
+      <c r="U22" t="s">
+        <v>89</v>
+      </c>
+      <c r="V22" t="str">
+        <f t="shared" si="5"/>
+        <v>no</v>
+      </c>
+      <c r="W22" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="23" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
@@ -50742,14 +51067,14 @@
         <v>8</v>
       </c>
       <c r="F23" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="G23" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Red</v>
       </c>
       <c r="H23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="I23" s="7">
@@ -50765,7 +51090,7 @@
         <v>79</v>
       </c>
       <c r="N23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="O23">
@@ -50777,11 +51102,29 @@
       <c r="Q23">
         <v>122.246</v>
       </c>
+      <c r="R23">
+        <v>123.928</v>
+      </c>
+      <c r="S23">
+        <f t="shared" si="6"/>
+        <v>-1.6820000000000022</v>
+      </c>
       <c r="T23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.2">
+        <f t="shared" si="4"/>
+        <v>-1.3759141403399721E-2</v>
+      </c>
+      <c r="U23" t="s">
+        <v>90</v>
+      </c>
+      <c r="V23" t="str">
+        <f t="shared" si="5"/>
+        <v>no</v>
+      </c>
+      <c r="W23" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="24" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
@@ -50795,14 +51138,14 @@
         <v>9</v>
       </c>
       <c r="F24" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="G24" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Red</v>
       </c>
       <c r="H24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="I24" s="7">
@@ -50818,7 +51161,7 @@
         <v>51</v>
       </c>
       <c r="N24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="O24">
@@ -50830,11 +51173,26 @@
       <c r="Q24">
         <v>100.352</v>
       </c>
+      <c r="R24">
+        <v>99.629000000000005</v>
+      </c>
+      <c r="S24">
+        <f t="shared" si="6"/>
+        <v>0.72299999999999898</v>
+      </c>
       <c r="T24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.2">
+        <f t="shared" si="4"/>
+        <v>7.2046396683673368E-3</v>
+      </c>
+      <c r="U24" t="s">
+        <v>90</v>
+      </c>
+      <c r="V24" t="str">
+        <f t="shared" si="5"/>
+        <v>no</v>
+      </c>
+    </row>
+    <row r="25" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
@@ -50848,14 +51206,14 @@
         <v>10</v>
       </c>
       <c r="F25" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="G25" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Red</v>
       </c>
       <c r="H25">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="I25" s="7">
@@ -50871,7 +51229,7 @@
         <v>56</v>
       </c>
       <c r="N25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="O25">
@@ -50883,11 +51241,26 @@
       <c r="Q25">
         <v>95.665999999999997</v>
       </c>
+      <c r="R25">
+        <v>94.129000000000005</v>
+      </c>
+      <c r="S25">
+        <f t="shared" si="6"/>
+        <v>1.5369999999999919</v>
+      </c>
       <c r="T25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.2">
+        <f t="shared" si="4"/>
+        <v>1.6066314050968911E-2</v>
+      </c>
+      <c r="U25" t="s">
+        <v>90</v>
+      </c>
+      <c r="V25" t="str">
+        <f t="shared" si="5"/>
+        <v>no</v>
+      </c>
+    </row>
+    <row r="26" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
@@ -50901,14 +51274,14 @@
         <v>11</v>
       </c>
       <c r="F26" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="G26" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Control</v>
       </c>
       <c r="H26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I26" s="7">
@@ -50924,7 +51297,7 @@
         <v>94</v>
       </c>
       <c r="N26">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="O26">
@@ -50936,8 +51309,29 @@
       <c r="Q26">
         <v>103.68300000000001</v>
       </c>
-    </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="R26">
+        <v>92.808999999999997</v>
+      </c>
+      <c r="S26">
+        <f t="shared" si="6"/>
+        <v>10.874000000000009</v>
+      </c>
+      <c r="T26">
+        <f t="shared" si="4"/>
+        <v>0.104877366588544</v>
+      </c>
+      <c r="U26" t="s">
+        <v>89</v>
+      </c>
+      <c r="V26" t="str">
+        <f t="shared" si="5"/>
+        <v>no</v>
+      </c>
+      <c r="W26" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="27" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>26</v>
       </c>
@@ -50951,14 +51345,14 @@
         <v>12</v>
       </c>
       <c r="F27" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="G27" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Pink</v>
       </c>
       <c r="H27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="I27" s="7">
@@ -50974,7 +51368,7 @@
         <v>35</v>
       </c>
       <c r="N27">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="O27">
@@ -50986,11 +51380,26 @@
       <c r="Q27">
         <v>102.07</v>
       </c>
+      <c r="R27">
+        <v>101.742</v>
+      </c>
+      <c r="S27">
+        <f t="shared" si="6"/>
+        <v>0.32799999999998875</v>
+      </c>
       <c r="T27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.2">
+        <f t="shared" si="4"/>
+        <v>3.2134809444497774E-3</v>
+      </c>
+      <c r="U27" t="s">
+        <v>90</v>
+      </c>
+      <c r="V27" t="str">
+        <f t="shared" si="5"/>
+        <v>no</v>
+      </c>
+    </row>
+    <row r="28" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>27</v>
       </c>
@@ -51004,14 +51413,14 @@
         <v>13</v>
       </c>
       <c r="F28" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="G28" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Orange</v>
       </c>
       <c r="H28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="I28" s="7">
@@ -51027,7 +51436,7 @@
         <v>45</v>
       </c>
       <c r="N28">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="O28">
@@ -51039,11 +51448,26 @@
       <c r="Q28">
         <v>105.818</v>
       </c>
+      <c r="R28">
+        <v>104.006</v>
+      </c>
+      <c r="S28">
+        <f t="shared" si="6"/>
+        <v>1.8119999999999976</v>
+      </c>
       <c r="T28">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.2">
+        <f t="shared" si="4"/>
+        <v>1.712374076244115E-2</v>
+      </c>
+      <c r="U28" t="s">
+        <v>90</v>
+      </c>
+      <c r="V28" t="str">
+        <f t="shared" si="5"/>
+        <v>no</v>
+      </c>
+    </row>
+    <row r="29" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>28</v>
       </c>
@@ -51057,14 +51481,14 @@
         <v>14</v>
       </c>
       <c r="F29" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="G29" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Control</v>
       </c>
       <c r="H29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I29" s="7">
@@ -51080,7 +51504,7 @@
         <v>41</v>
       </c>
       <c r="N29">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="O29">
@@ -51092,11 +51516,26 @@
       <c r="Q29">
         <v>109.04</v>
       </c>
+      <c r="R29">
+        <v>104.875</v>
+      </c>
+      <c r="S29">
+        <f t="shared" si="6"/>
+        <v>4.1650000000000063</v>
+      </c>
       <c r="T29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.2">
+        <f t="shared" si="4"/>
+        <v>3.8196991929567187E-2</v>
+      </c>
+      <c r="U29" t="s">
+        <v>90</v>
+      </c>
+      <c r="V29" t="str">
+        <f t="shared" si="5"/>
+        <v>no</v>
+      </c>
+    </row>
+    <row r="30" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>29</v>
       </c>
@@ -51110,14 +51549,14 @@
         <v>1</v>
       </c>
       <c r="F30" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="G30" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Control</v>
       </c>
       <c r="H30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I30" s="7">
@@ -51133,7 +51572,7 @@
         <v>98</v>
       </c>
       <c r="N30">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>9</v>
       </c>
       <c r="O30">
@@ -51142,8 +51581,30 @@
       <c r="P30">
         <v>720</v>
       </c>
-    </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="Q30">
+        <v>90.497</v>
+      </c>
+      <c r="R30">
+        <f>37.586+17.242</f>
+        <v>54.828000000000003</v>
+      </c>
+      <c r="S30">
+        <f t="shared" si="6"/>
+        <v>35.668999999999997</v>
+      </c>
+      <c r="T30">
+        <f t="shared" si="4"/>
+        <v>0.39414566228714759</v>
+      </c>
+      <c r="U30" t="s">
+        <v>89</v>
+      </c>
+      <c r="V30" t="str">
+        <f t="shared" si="5"/>
+        <v>yes</v>
+      </c>
+    </row>
+    <row r="31" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>30</v>
       </c>
@@ -51157,14 +51618,14 @@
         <v>2</v>
       </c>
       <c r="F31" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="G31" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Pink</v>
       </c>
       <c r="H31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="I31" s="7">
@@ -51180,7 +51641,7 @@
         <v>42</v>
       </c>
       <c r="N31">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>9</v>
       </c>
       <c r="O31">
@@ -51189,8 +51650,29 @@
       <c r="P31">
         <v>720</v>
       </c>
-    </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="Q31">
+        <v>103.925</v>
+      </c>
+      <c r="R31">
+        <v>74.176000000000002</v>
+      </c>
+      <c r="S31">
+        <f t="shared" si="6"/>
+        <v>29.748999999999995</v>
+      </c>
+      <c r="T31">
+        <f t="shared" si="4"/>
+        <v>0.28625451046427708</v>
+      </c>
+      <c r="U31" t="s">
+        <v>89</v>
+      </c>
+      <c r="V31" t="str">
+        <f t="shared" si="5"/>
+        <v>yes</v>
+      </c>
+    </row>
+    <row r="32" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>31</v>
       </c>
@@ -51204,14 +51686,14 @@
         <v>3</v>
       </c>
       <c r="F32" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="G32" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Red</v>
       </c>
       <c r="H32">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="I32" s="7">
@@ -51227,7 +51709,7 @@
         <v>63</v>
       </c>
       <c r="N32">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>9</v>
       </c>
       <c r="O32">
@@ -51236,8 +51718,29 @@
       <c r="P32">
         <v>720</v>
       </c>
-    </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="Q32">
+        <v>74.209000000000003</v>
+      </c>
+      <c r="R32">
+        <v>61.512</v>
+      </c>
+      <c r="S32">
+        <f t="shared" si="6"/>
+        <v>12.697000000000003</v>
+      </c>
+      <c r="T32">
+        <f t="shared" si="4"/>
+        <v>0.17109784527483193</v>
+      </c>
+      <c r="U32" t="s">
+        <v>89</v>
+      </c>
+      <c r="V32" t="str">
+        <f t="shared" si="5"/>
+        <v>yes</v>
+      </c>
+    </row>
+    <row r="33" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>32</v>
       </c>
@@ -51251,14 +51754,14 @@
         <v>4</v>
       </c>
       <c r="F33" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="G33" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Orange</v>
       </c>
       <c r="H33">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="I33" s="7">
@@ -51274,7 +51777,7 @@
         <v>47</v>
       </c>
       <c r="N33">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>9</v>
       </c>
       <c r="O33">
@@ -51283,11 +51786,29 @@
       <c r="P33">
         <v>720</v>
       </c>
+      <c r="Q33">
+        <v>93.227999999999994</v>
+      </c>
+      <c r="R33">
+        <v>94.572000000000003</v>
+      </c>
+      <c r="S33">
+        <f t="shared" si="6"/>
+        <v>-1.3440000000000083</v>
+      </c>
       <c r="T33">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.2">
+        <f t="shared" si="4"/>
+        <v>-1.4416269790191878E-2</v>
+      </c>
+      <c r="U33" t="s">
+        <v>90</v>
+      </c>
+      <c r="V33" t="str">
+        <f t="shared" si="5"/>
+        <v>yes</v>
+      </c>
+    </row>
+    <row r="34" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>33</v>
       </c>
@@ -51301,14 +51822,14 @@
         <v>5</v>
       </c>
       <c r="F34" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="G34" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Orange</v>
       </c>
       <c r="H34">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="I34" s="7">
@@ -51324,7 +51845,7 @@
         <v>75</v>
       </c>
       <c r="N34">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>9</v>
       </c>
       <c r="O34">
@@ -51333,8 +51854,33 @@
       <c r="P34">
         <v>720</v>
       </c>
-    </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="Q34">
+        <v>84.347999999999999</v>
+      </c>
+      <c r="R34">
+        <f>41.388+15.325</f>
+        <v>56.712999999999994</v>
+      </c>
+      <c r="S34">
+        <f t="shared" si="6"/>
+        <v>27.635000000000005</v>
+      </c>
+      <c r="T34">
+        <f t="shared" si="4"/>
+        <v>0.32763076777161293</v>
+      </c>
+      <c r="U34" t="s">
+        <v>89</v>
+      </c>
+      <c r="V34" t="str">
+        <f t="shared" si="5"/>
+        <v>yes</v>
+      </c>
+      <c r="W34" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="35" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>34</v>
       </c>
@@ -51348,14 +51894,14 @@
         <v>6</v>
       </c>
       <c r="F35" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="G35" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Red</v>
       </c>
       <c r="H35">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="I35" s="7">
@@ -51371,7 +51917,7 @@
         <v>47</v>
       </c>
       <c r="N35">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>9</v>
       </c>
       <c r="O35">
@@ -51380,11 +51926,32 @@
       <c r="P35">
         <v>720</v>
       </c>
+      <c r="Q35">
+        <v>96.76</v>
+      </c>
+      <c r="R35">
+        <v>95.731999999999999</v>
+      </c>
+      <c r="S35">
+        <f t="shared" si="6"/>
+        <v>1.0280000000000058</v>
+      </c>
       <c r="T35">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.2">
+        <f t="shared" si="4"/>
+        <v>1.0624224886316719E-2</v>
+      </c>
+      <c r="U35" t="s">
+        <v>90</v>
+      </c>
+      <c r="V35" t="str">
+        <f t="shared" si="5"/>
+        <v>yes</v>
+      </c>
+      <c r="W35" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="36" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>35</v>
       </c>
@@ -51398,14 +51965,14 @@
         <v>7</v>
       </c>
       <c r="F36" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="G36" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Control</v>
       </c>
       <c r="H36">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I36" s="7">
@@ -51421,7 +51988,7 @@
         <v>63</v>
       </c>
       <c r="N36">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>9</v>
       </c>
       <c r="O36">
@@ -51430,8 +51997,29 @@
       <c r="P36">
         <v>720</v>
       </c>
-    </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="Q36">
+        <v>93.5</v>
+      </c>
+      <c r="R36">
+        <v>62.167000000000002</v>
+      </c>
+      <c r="S36">
+        <f t="shared" si="6"/>
+        <v>31.332999999999998</v>
+      </c>
+      <c r="T36">
+        <f t="shared" si="4"/>
+        <v>0.33511229946524063</v>
+      </c>
+      <c r="U36" t="s">
+        <v>89</v>
+      </c>
+      <c r="V36" t="str">
+        <f t="shared" si="5"/>
+        <v>no</v>
+      </c>
+    </row>
+    <row r="37" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>36</v>
       </c>
@@ -51445,14 +52033,14 @@
         <v>8</v>
       </c>
       <c r="F37" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="G37" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Control</v>
       </c>
       <c r="H37">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I37" s="7">
@@ -51468,7 +52056,7 @@
         <v>50</v>
       </c>
       <c r="N37">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>9</v>
       </c>
       <c r="O37">
@@ -51477,11 +52065,29 @@
       <c r="P37">
         <v>720</v>
       </c>
+      <c r="Q37">
+        <v>93.727999999999994</v>
+      </c>
+      <c r="R37">
+        <v>92.887</v>
+      </c>
+      <c r="S37">
+        <f t="shared" si="6"/>
+        <v>0.84099999999999397</v>
+      </c>
       <c r="T37">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.2">
+        <f t="shared" si="4"/>
+        <v>8.9727722772276596E-3</v>
+      </c>
+      <c r="U37" t="s">
+        <v>90</v>
+      </c>
+      <c r="V37" t="str">
+        <f t="shared" si="5"/>
+        <v>no</v>
+      </c>
+    </row>
+    <row r="38" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>37</v>
       </c>
@@ -51495,14 +52101,14 @@
         <v>9</v>
       </c>
       <c r="F38" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="G38" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Orange</v>
       </c>
       <c r="H38">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="I38" s="7">
@@ -51518,7 +52124,7 @@
         <v>47</v>
       </c>
       <c r="N38">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>9</v>
       </c>
       <c r="O38">
@@ -51527,8 +52133,32 @@
       <c r="P38">
         <v>720</v>
       </c>
-    </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="Q38">
+        <v>101.639</v>
+      </c>
+      <c r="R38">
+        <v>73.361999999999995</v>
+      </c>
+      <c r="S38">
+        <f t="shared" si="6"/>
+        <v>28.277000000000001</v>
+      </c>
+      <c r="T38">
+        <f t="shared" si="4"/>
+        <v>0.27821013587304089</v>
+      </c>
+      <c r="U38" t="s">
+        <v>89</v>
+      </c>
+      <c r="V38" t="str">
+        <f t="shared" si="5"/>
+        <v>no</v>
+      </c>
+      <c r="W38" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="39" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>38</v>
       </c>
@@ -51542,14 +52172,14 @@
         <v>10</v>
       </c>
       <c r="F39" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="G39" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Orange</v>
       </c>
       <c r="H39">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="I39" s="7">
@@ -51565,7 +52195,7 @@
         <v>73</v>
       </c>
       <c r="N39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>9</v>
       </c>
       <c r="O39">
@@ -51574,8 +52204,29 @@
       <c r="P39">
         <v>720</v>
       </c>
-    </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="Q39">
+        <v>80.153999999999996</v>
+      </c>
+      <c r="R39">
+        <v>39.979999999999997</v>
+      </c>
+      <c r="S39">
+        <f t="shared" si="6"/>
+        <v>40.173999999999999</v>
+      </c>
+      <c r="T39">
+        <f t="shared" si="4"/>
+        <v>0.50121017042193783</v>
+      </c>
+      <c r="U39" t="s">
+        <v>89</v>
+      </c>
+      <c r="V39" t="str">
+        <f t="shared" si="5"/>
+        <v>no</v>
+      </c>
+    </row>
+    <row r="40" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>39</v>
       </c>
@@ -51589,14 +52240,14 @@
         <v>11</v>
       </c>
       <c r="F40" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="G40" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Pink</v>
       </c>
       <c r="H40">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="I40" s="7">
@@ -51612,7 +52263,7 @@
         <v>70</v>
       </c>
       <c r="N40">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>9</v>
       </c>
       <c r="O40">
@@ -51621,8 +52272,29 @@
       <c r="P40">
         <v>720</v>
       </c>
-    </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="Q40">
+        <v>93.593000000000004</v>
+      </c>
+      <c r="R40">
+        <v>53.595999999999997</v>
+      </c>
+      <c r="S40">
+        <f t="shared" si="6"/>
+        <v>39.997000000000007</v>
+      </c>
+      <c r="T40">
+        <f t="shared" si="4"/>
+        <v>0.42735033602940398</v>
+      </c>
+      <c r="U40" t="s">
+        <v>89</v>
+      </c>
+      <c r="V40" t="str">
+        <f t="shared" si="5"/>
+        <v>no</v>
+      </c>
+    </row>
+    <row r="41" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>40</v>
       </c>
@@ -51636,14 +52308,14 @@
         <v>12</v>
       </c>
       <c r="F41" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="G41" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Red</v>
       </c>
       <c r="H41">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="I41" s="7">
@@ -51659,7 +52331,7 @@
         <v>89</v>
       </c>
       <c r="N41">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>9</v>
       </c>
       <c r="O41">
@@ -51668,8 +52340,30 @@
       <c r="P41">
         <v>720</v>
       </c>
-    </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="Q41">
+        <v>58.831000000000003</v>
+      </c>
+      <c r="R41">
+        <f>3.778+0.998+0.429</f>
+        <v>5.2050000000000001</v>
+      </c>
+      <c r="S41">
+        <f t="shared" si="6"/>
+        <v>53.626000000000005</v>
+      </c>
+      <c r="T41">
+        <f t="shared" si="4"/>
+        <v>0.91152623616800665</v>
+      </c>
+      <c r="U41" t="s">
+        <v>89</v>
+      </c>
+      <c r="V41" t="str">
+        <f t="shared" si="5"/>
+        <v>no</v>
+      </c>
+    </row>
+    <row r="42" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>41</v>
       </c>
@@ -51683,14 +52377,14 @@
         <v>13</v>
       </c>
       <c r="F42" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="G42" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Pink</v>
       </c>
       <c r="H42">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="I42" s="7">
@@ -51706,7 +52400,7 @@
         <v>83</v>
       </c>
       <c r="N42">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>9</v>
       </c>
       <c r="O42">
@@ -51715,8 +52409,29 @@
       <c r="P42">
         <v>720</v>
       </c>
-    </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="Q42">
+        <v>75.53</v>
+      </c>
+      <c r="R42">
+        <v>74.962000000000003</v>
+      </c>
+      <c r="S42">
+        <f t="shared" si="6"/>
+        <v>0.56799999999999784</v>
+      </c>
+      <c r="T42">
+        <f t="shared" si="4"/>
+        <v>7.5201906527207442E-3</v>
+      </c>
+      <c r="U42" t="s">
+        <v>89</v>
+      </c>
+      <c r="V42" t="str">
+        <f t="shared" si="5"/>
+        <v>no</v>
+      </c>
+    </row>
+    <row r="43" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>42</v>
       </c>
@@ -51730,14 +52445,14 @@
         <v>14</v>
       </c>
       <c r="F43" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="G43" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Orange</v>
       </c>
       <c r="H43">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="I43" s="7">
@@ -51753,7 +52468,7 @@
         <v>57</v>
       </c>
       <c r="N43">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>9</v>
       </c>
       <c r="O43">
@@ -51762,11 +52477,32 @@
       <c r="P43">
         <v>720</v>
       </c>
+      <c r="Q43">
+        <v>77.009</v>
+      </c>
+      <c r="R43">
+        <v>75.542000000000002</v>
+      </c>
+      <c r="S43">
+        <f t="shared" si="6"/>
+        <v>1.4669999999999987</v>
+      </c>
       <c r="T43">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.2">
+        <f t="shared" si="4"/>
+        <v>1.9049721461127905E-2</v>
+      </c>
+      <c r="U43" t="s">
+        <v>90</v>
+      </c>
+      <c r="V43" t="str">
+        <f t="shared" si="5"/>
+        <v>no</v>
+      </c>
+      <c r="W43" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="44" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>43</v>
       </c>
@@ -51780,14 +52516,14 @@
         <v>1</v>
       </c>
       <c r="F44" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="G44" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Red</v>
       </c>
       <c r="H44">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="I44" s="7">
@@ -51811,8 +52547,23 @@
       <c r="P44">
         <v>720</v>
       </c>
-    </row>
-    <row r="45" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="S44">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="T44" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U44" t="s">
+        <v>89</v>
+      </c>
+      <c r="V44" t="str">
+        <f t="shared" si="5"/>
+        <v>yes</v>
+      </c>
+    </row>
+    <row r="45" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>44</v>
       </c>
@@ -51826,14 +52577,14 @@
         <v>2</v>
       </c>
       <c r="F45" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="G45" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Pink</v>
       </c>
       <c r="H45">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="I45" s="7">
@@ -51857,8 +52608,23 @@
       <c r="P45">
         <v>720</v>
       </c>
-    </row>
-    <row r="46" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="S45">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="T45" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U45" t="s">
+        <v>89</v>
+      </c>
+      <c r="V45" t="str">
+        <f t="shared" si="5"/>
+        <v>yes</v>
+      </c>
+    </row>
+    <row r="46" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>45</v>
       </c>
@@ -51872,14 +52638,14 @@
         <v>3</v>
       </c>
       <c r="F46" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="G46" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Red</v>
       </c>
       <c r="H46">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="I46" s="7">
@@ -51903,11 +52669,23 @@
       <c r="P46">
         <v>720</v>
       </c>
-      <c r="T46">
+      <c r="S46">
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="47" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T46" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U46" t="s">
+        <v>90</v>
+      </c>
+      <c r="V46" t="str">
+        <f t="shared" si="5"/>
+        <v>yes</v>
+      </c>
+    </row>
+    <row r="47" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>46</v>
       </c>
@@ -51921,14 +52699,14 @@
         <v>4</v>
       </c>
       <c r="F47" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="G47" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Orange</v>
       </c>
       <c r="H47">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="I47" s="7">
@@ -51952,11 +52730,22 @@
       <c r="P47">
         <v>720</v>
       </c>
-      <c r="T47">
+      <c r="S47">
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="48" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T47" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U47" t="s">
+        <v>90</v>
+      </c>
+      <c r="V47" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="48" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>47</v>
       </c>
@@ -51970,14 +52759,14 @@
         <v>5</v>
       </c>
       <c r="F48" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="G48" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Control</v>
       </c>
       <c r="H48">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I48" s="7">
@@ -52001,11 +52790,23 @@
       <c r="P48">
         <v>720</v>
       </c>
-      <c r="T48" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="49" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="S48">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="T48" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U48" t="s">
+        <v>91</v>
+      </c>
+      <c r="V48" t="str">
+        <f t="shared" si="5"/>
+        <v>yes</v>
+      </c>
+    </row>
+    <row r="49" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>48</v>
       </c>
@@ -52019,14 +52820,14 @@
         <v>6</v>
       </c>
       <c r="F49" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="G49" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Pink</v>
       </c>
       <c r="H49">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="I49" s="7">
@@ -52050,11 +52851,23 @@
       <c r="P49">
         <v>720</v>
       </c>
-      <c r="T49">
+      <c r="S49">
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T49" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U49" t="s">
+        <v>90</v>
+      </c>
+      <c r="V49" t="str">
+        <f t="shared" si="5"/>
+        <v>yes</v>
+      </c>
+    </row>
+    <row r="50" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>49</v>
       </c>
@@ -52068,14 +52881,14 @@
         <v>7</v>
       </c>
       <c r="F50" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="G50" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Pink</v>
       </c>
       <c r="H50">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="I50" s="7">
@@ -52099,8 +52912,23 @@
       <c r="P50">
         <v>733</v>
       </c>
-    </row>
-    <row r="51" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="S50">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="T50" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U50" t="s">
+        <v>89</v>
+      </c>
+      <c r="V50" t="str">
+        <f t="shared" si="5"/>
+        <v>no</v>
+      </c>
+    </row>
+    <row r="51" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>50</v>
       </c>
@@ -52114,14 +52942,14 @@
         <v>8</v>
       </c>
       <c r="F51" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="G51" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Pink</v>
       </c>
       <c r="H51">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="I51" s="7">
@@ -52145,11 +52973,23 @@
       <c r="P51">
         <v>733</v>
       </c>
-      <c r="T51">
+      <c r="S51">
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="52" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T51" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U51" t="s">
+        <v>90</v>
+      </c>
+      <c r="V51" t="str">
+        <f t="shared" si="5"/>
+        <v>no</v>
+      </c>
+    </row>
+    <row r="52" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>51</v>
       </c>
@@ -52163,14 +53003,14 @@
         <v>9</v>
       </c>
       <c r="F52" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="G52" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Orange</v>
       </c>
       <c r="H52">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="I52" s="7">
@@ -52194,8 +53034,23 @@
       <c r="P52">
         <v>733</v>
       </c>
-    </row>
-    <row r="53" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="S52">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="T52" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U52" t="s">
+        <v>89</v>
+      </c>
+      <c r="V52" t="str">
+        <f t="shared" si="5"/>
+        <v>no</v>
+      </c>
+    </row>
+    <row r="53" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>52</v>
       </c>
@@ -52209,14 +53064,14 @@
         <v>10</v>
       </c>
       <c r="F53" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="G53" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Orange</v>
       </c>
       <c r="H53">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="I53" s="7">
@@ -52240,11 +53095,23 @@
       <c r="P53">
         <v>733</v>
       </c>
-      <c r="T53">
+      <c r="S53">
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="54" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T53" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U53" t="s">
+        <v>90</v>
+      </c>
+      <c r="V53" t="str">
+        <f t="shared" si="5"/>
+        <v>no</v>
+      </c>
+    </row>
+    <row r="54" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>53</v>
       </c>
@@ -52258,14 +53125,14 @@
         <v>11</v>
       </c>
       <c r="F54" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="G54" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Pink</v>
       </c>
       <c r="H54">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="I54" s="7">
@@ -52289,8 +53156,23 @@
       <c r="P54">
         <v>733</v>
       </c>
-    </row>
-    <row r="55" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="S54">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="T54" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U54" t="s">
+        <v>89</v>
+      </c>
+      <c r="V54" t="str">
+        <f t="shared" si="5"/>
+        <v>no</v>
+      </c>
+    </row>
+    <row r="55" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>54</v>
       </c>
@@ -52304,14 +53186,14 @@
         <v>12</v>
       </c>
       <c r="F55" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="G55" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Control</v>
       </c>
       <c r="H55">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I55" s="7">
@@ -52335,8 +53217,23 @@
       <c r="P55">
         <v>733</v>
       </c>
-    </row>
-    <row r="56" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="S55">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="T55" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U55" t="s">
+        <v>89</v>
+      </c>
+      <c r="V55" t="str">
+        <f t="shared" si="5"/>
+        <v>no</v>
+      </c>
+    </row>
+    <row r="56" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>55</v>
       </c>
@@ -52350,14 +53247,14 @@
         <v>13</v>
       </c>
       <c r="F56" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="G56" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Control</v>
       </c>
       <c r="H56">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I56" s="7">
@@ -52381,8 +53278,23 @@
       <c r="P56">
         <v>733</v>
       </c>
-    </row>
-    <row r="57" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="S56">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="T56" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U56" t="s">
+        <v>89</v>
+      </c>
+      <c r="V56" t="str">
+        <f t="shared" si="5"/>
+        <v>no</v>
+      </c>
+    </row>
+    <row r="57" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>56</v>
       </c>
@@ -52396,14 +53308,14 @@
         <v>14</v>
       </c>
       <c r="F57" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="G57" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Red</v>
       </c>
       <c r="H57">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="I57" s="7">
@@ -52427,8 +53339,23 @@
       <c r="P57">
         <v>733</v>
       </c>
-    </row>
-    <row r="58" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="S57">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="T57" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U57" t="s">
+        <v>90</v>
+      </c>
+      <c r="V57" t="str">
+        <f t="shared" si="5"/>
+        <v>no</v>
+      </c>
+    </row>
+    <row r="58" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>57</v>
       </c>
@@ -52442,14 +53369,14 @@
         <v>7</v>
       </c>
       <c r="F58" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="G58" t="str">
-        <f t="shared" ref="G58:G71" si="3">IF(I58&lt;=0, "Control", IF(I58&lt;=10, "Red", IF(I58&gt;=21, "Pink", "Orange")))</f>
+        <f t="shared" ref="G58:G71" si="7">IF(I58&lt;=0, "Control", IF(I58&lt;=10, "Red", IF(I58&gt;=21, "Pink", "Orange")))</f>
         <v>Red</v>
       </c>
       <c r="H58">
-        <f t="shared" ref="H58:H71" si="4">IF(G58="Control", 1, IF(G58="Red", 2, IF(G58="Orange", 3, 4)))</f>
+        <f t="shared" ref="H58:H71" si="8">IF(G58="Control", 1, IF(G58="Red", 2, IF(G58="Orange", 3, 4)))</f>
         <v>2</v>
       </c>
       <c r="I58" s="7">
@@ -52457,11 +53384,23 @@
       </c>
       <c r="K58" s="5"/>
       <c r="N58">
-        <f t="shared" ref="N58:N77" si="5">C58-239</f>
+        <f t="shared" ref="N58:N77" si="9">C58-239</f>
         <v>8</v>
       </c>
-    </row>
-    <row r="59" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="S58">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="T58" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V58" t="str">
+        <f t="shared" si="5"/>
+        <v>no</v>
+      </c>
+    </row>
+    <row r="59" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>58</v>
       </c>
@@ -52475,14 +53414,14 @@
         <v>8</v>
       </c>
       <c r="F59" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="G59" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>Control</v>
       </c>
       <c r="H59">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="I59" s="7">
@@ -52490,11 +53429,23 @@
       </c>
       <c r="K59" s="5"/>
       <c r="N59">
+        <f t="shared" si="9"/>
+        <v>8</v>
+      </c>
+      <c r="S59">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="T59" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V59" t="str">
         <f t="shared" si="5"/>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="60" spans="1:20" x14ac:dyDescent="0.2">
+        <v>no</v>
+      </c>
+    </row>
+    <row r="60" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>59</v>
       </c>
@@ -52508,14 +53459,14 @@
         <v>9</v>
       </c>
       <c r="F60" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="G60" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>Pink</v>
       </c>
       <c r="H60">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>4</v>
       </c>
       <c r="I60" s="5">
@@ -52523,11 +53474,23 @@
       </c>
       <c r="K60" s="5"/>
       <c r="N60">
+        <f t="shared" si="9"/>
+        <v>8</v>
+      </c>
+      <c r="S60">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="T60" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V60" t="str">
         <f t="shared" si="5"/>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="61" spans="1:20" x14ac:dyDescent="0.2">
+        <v>no</v>
+      </c>
+    </row>
+    <row r="61" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>60</v>
       </c>
@@ -52541,14 +53504,14 @@
         <v>10</v>
       </c>
       <c r="F61" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="G61" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>Red</v>
       </c>
       <c r="H61">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
       <c r="I61" s="5">
@@ -52556,11 +53519,23 @@
       </c>
       <c r="K61" s="5"/>
       <c r="N61">
+        <f t="shared" si="9"/>
+        <v>8</v>
+      </c>
+      <c r="S61">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="T61" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V61" t="str">
         <f t="shared" si="5"/>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="62" spans="1:20" x14ac:dyDescent="0.2">
+        <v>no</v>
+      </c>
+    </row>
+    <row r="62" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>61</v>
       </c>
@@ -52574,14 +53549,14 @@
         <v>11</v>
       </c>
       <c r="F62" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="G62" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>Orange</v>
       </c>
       <c r="H62">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>3</v>
       </c>
       <c r="I62" s="5">
@@ -52589,11 +53564,23 @@
       </c>
       <c r="K62" s="5"/>
       <c r="N62">
+        <f t="shared" si="9"/>
+        <v>8</v>
+      </c>
+      <c r="S62">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="T62" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V62" t="str">
         <f t="shared" si="5"/>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="63" spans="1:20" x14ac:dyDescent="0.2">
+        <v>no</v>
+      </c>
+    </row>
+    <row r="63" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>62</v>
       </c>
@@ -52607,14 +53594,14 @@
         <v>12</v>
       </c>
       <c r="F63" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="G63" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>Orange</v>
       </c>
       <c r="H63">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>3</v>
       </c>
       <c r="I63" s="5">
@@ -52622,11 +53609,23 @@
       </c>
       <c r="K63" s="5"/>
       <c r="N63">
+        <f t="shared" si="9"/>
+        <v>8</v>
+      </c>
+      <c r="S63">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="T63" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V63" t="str">
         <f t="shared" si="5"/>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="64" spans="1:20" x14ac:dyDescent="0.2">
+        <v>no</v>
+      </c>
+    </row>
+    <row r="64" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>63</v>
       </c>
@@ -52640,14 +53639,14 @@
         <v>13</v>
       </c>
       <c r="F64" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="G64" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>Control</v>
       </c>
       <c r="H64">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="I64" s="5">
@@ -52655,11 +53654,23 @@
       </c>
       <c r="K64" s="5"/>
       <c r="N64">
+        <f t="shared" si="9"/>
+        <v>8</v>
+      </c>
+      <c r="S64">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="T64" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V64" t="str">
         <f t="shared" si="5"/>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.2">
+        <v>no</v>
+      </c>
+    </row>
+    <row r="65" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>64</v>
       </c>
@@ -52673,14 +53684,14 @@
         <v>14</v>
       </c>
       <c r="F65" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="G65" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>Red</v>
       </c>
       <c r="H65">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
       <c r="I65" s="5">
@@ -52688,11 +53699,23 @@
       </c>
       <c r="K65" s="5"/>
       <c r="N65">
+        <f t="shared" si="9"/>
+        <v>8</v>
+      </c>
+      <c r="S65">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="T65" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V65" t="str">
         <f t="shared" si="5"/>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.2">
+        <v>no</v>
+      </c>
+    </row>
+    <row r="66" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>65</v>
       </c>
@@ -52706,14 +53729,14 @@
         <v>1</v>
       </c>
       <c r="F66" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="G66" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>Control</v>
       </c>
       <c r="H66">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="I66" s="7">
@@ -52721,11 +53744,23 @@
       </c>
       <c r="K66" s="7"/>
       <c r="N66">
+        <f t="shared" si="9"/>
+        <v>9</v>
+      </c>
+      <c r="S66">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="T66" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V66" t="str">
         <f t="shared" si="5"/>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.2">
+        <v>yes</v>
+      </c>
+    </row>
+    <row r="67" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>66</v>
       </c>
@@ -52739,14 +53774,14 @@
         <v>2</v>
       </c>
       <c r="F67" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="G67" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>Orange</v>
       </c>
       <c r="H67">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>3</v>
       </c>
       <c r="I67" s="7">
@@ -52754,11 +53789,23 @@
       </c>
       <c r="K67" s="5"/>
       <c r="N67">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="S67">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="T67" t="e">
+        <f t="shared" ref="T67:T77" si="10">S67/Q67</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V67" t="str">
+        <f t="shared" ref="V67:V77" si="11">IF(E67&gt;6,"no","yes")</f>
+        <v>yes</v>
+      </c>
+    </row>
+    <row r="68" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>67</v>
       </c>
@@ -52772,14 +53819,14 @@
         <v>3</v>
       </c>
       <c r="F68" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="G68" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>Pink</v>
       </c>
       <c r="H68">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>4</v>
       </c>
       <c r="I68" s="7">
@@ -52787,11 +53834,23 @@
       </c>
       <c r="K68" s="5"/>
       <c r="N68">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="S68">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="T68" t="e">
+        <f t="shared" si="10"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V68" t="str">
+        <f t="shared" si="11"/>
+        <v>yes</v>
+      </c>
+    </row>
+    <row r="69" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>68</v>
       </c>
@@ -52805,14 +53864,14 @@
         <v>4</v>
       </c>
       <c r="F69" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="G69" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>Pink</v>
       </c>
       <c r="H69">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>4</v>
       </c>
       <c r="I69" s="7">
@@ -52820,11 +53879,23 @@
       </c>
       <c r="K69" s="5"/>
       <c r="N69">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="S69">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="T69" t="e">
+        <f t="shared" si="10"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V69" t="str">
+        <f t="shared" si="11"/>
+        <v>yes</v>
+      </c>
+    </row>
+    <row r="70" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>69</v>
       </c>
@@ -52838,14 +53909,14 @@
         <v>5</v>
       </c>
       <c r="F70" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="G70" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>Pink</v>
       </c>
       <c r="H70">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>4</v>
       </c>
       <c r="I70" s="7">
@@ -52853,11 +53924,23 @@
       </c>
       <c r="K70" s="5"/>
       <c r="N70">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="S70">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="T70" t="e">
+        <f t="shared" si="10"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V70" t="str">
+        <f t="shared" si="11"/>
+        <v>yes</v>
+      </c>
+    </row>
+    <row r="71" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>70</v>
       </c>
@@ -52871,14 +53954,14 @@
         <v>6</v>
       </c>
       <c r="F71" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="G71" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>Red</v>
       </c>
       <c r="H71">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
       <c r="I71" s="7">
@@ -52886,11 +53969,23 @@
       </c>
       <c r="K71" s="5"/>
       <c r="N71">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="S71">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="T71" t="e">
+        <f t="shared" si="10"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V71" t="str">
+        <f t="shared" si="11"/>
+        <v>yes</v>
+      </c>
+    </row>
+    <row r="72" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>71</v>
       </c>
@@ -52904,14 +53999,14 @@
         <v>1</v>
       </c>
       <c r="F72" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="G72" t="str">
-        <f t="shared" ref="G72:G77" si="6">IF(I72&lt;=0, "Control", IF(I72&lt;=10, "Red", IF(I72&gt;=21, "Pink", "Orange")))</f>
+        <f t="shared" ref="G72:G77" si="12">IF(I72&lt;=0, "Control", IF(I72&lt;=10, "Red", IF(I72&gt;=21, "Pink", "Orange")))</f>
         <v>Control</v>
       </c>
       <c r="H72">
-        <f t="shared" ref="H72:H77" si="7">IF(G72="Control", 1, IF(G72="Red", 2, IF(G72="Orange", 3, 4)))</f>
+        <f t="shared" ref="H72:H77" si="13">IF(G72="Control", 1, IF(G72="Red", 2, IF(G72="Orange", 3, 4)))</f>
         <v>1</v>
       </c>
       <c r="I72" s="7">
@@ -52919,11 +54014,23 @@
       </c>
       <c r="K72" s="5"/>
       <c r="N72">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="S72">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="T72" t="e">
+        <f t="shared" si="10"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V72" t="str">
+        <f t="shared" si="11"/>
+        <v>yes</v>
+      </c>
+    </row>
+    <row r="73" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>72</v>
       </c>
@@ -52937,14 +54044,14 @@
         <v>2</v>
       </c>
       <c r="F73" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="G73" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>Pink</v>
       </c>
       <c r="H73">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>4</v>
       </c>
       <c r="I73" s="7">
@@ -52952,11 +54059,23 @@
       </c>
       <c r="K73" s="5"/>
       <c r="N73">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="S73">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="T73" t="e">
+        <f t="shared" si="10"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V73" t="str">
+        <f t="shared" si="11"/>
+        <v>yes</v>
+      </c>
+    </row>
+    <row r="74" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>73</v>
       </c>
@@ -52970,14 +54089,14 @@
         <v>3</v>
       </c>
       <c r="F74" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="G74" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>Orange</v>
       </c>
       <c r="H74">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>3</v>
       </c>
       <c r="I74" s="7">
@@ -52985,11 +54104,23 @@
       </c>
       <c r="K74" s="5"/>
       <c r="N74">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="S74">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="T74" t="e">
+        <f t="shared" si="10"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V74" t="str">
+        <f t="shared" si="11"/>
+        <v>yes</v>
+      </c>
+    </row>
+    <row r="75" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>74</v>
       </c>
@@ -53003,14 +54134,14 @@
         <v>4</v>
       </c>
       <c r="F75" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="G75" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>Red</v>
       </c>
       <c r="H75">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>2</v>
       </c>
       <c r="I75" s="7">
@@ -53018,11 +54149,23 @@
       </c>
       <c r="K75" s="5"/>
       <c r="N75">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="76" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="S75">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="T75" t="e">
+        <f t="shared" si="10"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V75" t="str">
+        <f t="shared" si="11"/>
+        <v>yes</v>
+      </c>
+    </row>
+    <row r="76" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>75</v>
       </c>
@@ -53036,14 +54179,14 @@
         <v>5</v>
       </c>
       <c r="F76" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="G76" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>Pink</v>
       </c>
       <c r="H76">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>4</v>
       </c>
       <c r="I76" s="7">
@@ -53051,11 +54194,23 @@
       </c>
       <c r="K76" s="5"/>
       <c r="N76">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="77" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="S76">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="T76" t="e">
+        <f t="shared" si="10"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V76" t="str">
+        <f t="shared" si="11"/>
+        <v>yes</v>
+      </c>
+    </row>
+    <row r="77" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>76</v>
       </c>
@@ -53069,14 +54224,14 @@
         <v>6</v>
       </c>
       <c r="F77" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="G77" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>Red</v>
       </c>
       <c r="H77">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>2</v>
       </c>
       <c r="I77" s="7">
@@ -53084,8 +54239,20 @@
       </c>
       <c r="K77" s="5"/>
       <c r="N77">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>10</v>
+      </c>
+      <c r="S77">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="T77" t="e">
+        <f t="shared" si="10"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V77" t="str">
+        <f t="shared" si="11"/>
+        <v>yes</v>
       </c>
     </row>
   </sheetData>
@@ -53099,10 +54266,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55F6BF2F-CBB2-4331-929A-D3F4AD694052}">
-  <dimension ref="A1:AC45"/>
+  <dimension ref="A1:AC37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="S22" sqref="S22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -53180,28 +54347,28 @@
         <v>15</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="R1" s="2" t="s">
         <v>17</v>
       </c>
       <c r="S1" s="2" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="T1" s="2" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="U1" s="2" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="V1" s="2" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="W1" s="2" t="s">
         <v>18</v>
@@ -53236,7 +54403,7 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E2" t="str">
         <f>IF(G2&lt;=0, "Control", IF(G2&lt;=10, "Red", IF(G2&gt;=21, "Pink", "Orange")))</f>
@@ -53288,7 +54455,7 @@
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E3" t="str">
         <f t="shared" ref="E3:E26" si="0">IF(G3&lt;=0, "Control", IF(G3&lt;=10, "Red", IF(G3&gt;=21, "Pink", "Orange")))</f>
@@ -53340,7 +54507,7 @@
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E4" t="str">
         <f t="shared" si="0"/>
@@ -53381,7 +54548,7 @@
         <v>1</v>
       </c>
       <c r="AC4" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:29" x14ac:dyDescent="0.2">
@@ -53395,7 +54562,7 @@
         <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E5" t="str">
         <f t="shared" si="0"/>
@@ -53447,7 +54614,7 @@
         <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E6" t="str">
         <f t="shared" si="0"/>
@@ -53499,7 +54666,7 @@
         <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E7" t="str">
         <f t="shared" si="0"/>
@@ -53551,7 +54718,7 @@
         <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E8" t="str">
         <f t="shared" si="0"/>
@@ -53603,7 +54770,7 @@
         <v>2</v>
       </c>
       <c r="D9" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E9" t="str">
         <f t="shared" si="0"/>
@@ -53655,7 +54822,7 @@
         <v>3</v>
       </c>
       <c r="D10" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E10" t="str">
         <f t="shared" si="0"/>
@@ -53707,7 +54874,7 @@
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E11" t="str">
         <f t="shared" si="0"/>
@@ -53748,7 +54915,7 @@
         <v>0</v>
       </c>
       <c r="AC11" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="12" spans="1:29" x14ac:dyDescent="0.2">
@@ -53762,7 +54929,7 @@
         <v>5</v>
       </c>
       <c r="D12" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E12" t="str">
         <f t="shared" si="0"/>
@@ -53814,7 +54981,7 @@
         <v>6</v>
       </c>
       <c r="D13" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E13" t="str">
         <f t="shared" si="0"/>
@@ -53866,7 +55033,7 @@
         <v>1</v>
       </c>
       <c r="D14" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E14" t="str">
         <f t="shared" si="0"/>
@@ -53907,7 +55074,7 @@
         <v>1</v>
       </c>
       <c r="AC14" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
     </row>
     <row r="15" spans="1:29" x14ac:dyDescent="0.2">
@@ -53921,7 +55088,7 @@
         <v>2</v>
       </c>
       <c r="D15" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E15" t="str">
         <f t="shared" si="0"/>
@@ -53973,7 +55140,7 @@
         <v>3</v>
       </c>
       <c r="D16" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E16" t="str">
         <f t="shared" si="0"/>
@@ -54014,7 +55181,7 @@
         <v>1</v>
       </c>
       <c r="AC16" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
     </row>
     <row r="17" spans="1:29" x14ac:dyDescent="0.2">
@@ -54028,7 +55195,7 @@
         <v>4</v>
       </c>
       <c r="D17" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E17" t="str">
         <f t="shared" si="0"/>
@@ -54080,7 +55247,7 @@
         <v>5</v>
       </c>
       <c r="D18" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E18" t="str">
         <f t="shared" si="0"/>
@@ -54132,7 +55299,7 @@
         <v>6</v>
       </c>
       <c r="D19" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E19" t="str">
         <f t="shared" si="0"/>
@@ -54184,7 +55351,7 @@
         <v>1</v>
       </c>
       <c r="D20" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E20" t="str">
         <f t="shared" si="0"/>
@@ -54236,7 +55403,7 @@
         <v>2</v>
       </c>
       <c r="D21" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E21" t="str">
         <f t="shared" si="0"/>
@@ -54288,7 +55455,7 @@
         <v>3</v>
       </c>
       <c r="D22" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E22" t="str">
         <f t="shared" si="0"/>
@@ -54340,7 +55507,7 @@
         <v>4</v>
       </c>
       <c r="D23" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E23" t="str">
         <f t="shared" si="0"/>
@@ -54377,11 +55544,53 @@
         <f>'Kelp consumption'!P47</f>
         <v>720</v>
       </c>
+      <c r="N23" t="s">
+        <v>80</v>
+      </c>
+      <c r="O23" t="s">
+        <v>80</v>
+      </c>
+      <c r="P23" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>80</v>
+      </c>
       <c r="R23" t="s">
-        <v>86</v>
+        <v>80</v>
+      </c>
+      <c r="S23" t="s">
+        <v>80</v>
+      </c>
+      <c r="T23" t="s">
+        <v>80</v>
+      </c>
+      <c r="U23" t="s">
+        <v>80</v>
+      </c>
+      <c r="V23" t="s">
+        <v>80</v>
+      </c>
+      <c r="W23" t="s">
+        <v>80</v>
+      </c>
+      <c r="X23" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y23" t="s">
+        <v>80</v>
+      </c>
+      <c r="Z23" t="s">
+        <v>80</v>
+      </c>
+      <c r="AA23" t="s">
+        <v>80</v>
+      </c>
+      <c r="AB23" t="s">
+        <v>80</v>
       </c>
       <c r="AC23" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
     <row r="24" spans="1:29" x14ac:dyDescent="0.2">
@@ -54395,7 +55604,7 @@
         <v>5</v>
       </c>
       <c r="D24" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E24" t="str">
         <f t="shared" si="0"/>
@@ -54436,7 +55645,7 @@
         <v>1</v>
       </c>
       <c r="AC24" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
     </row>
     <row r="25" spans="1:29" x14ac:dyDescent="0.2">
@@ -54450,7 +55659,7 @@
         <v>6</v>
       </c>
       <c r="D25" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E25" t="str">
         <f t="shared" si="0"/>
@@ -54502,7 +55711,7 @@
         <v>1</v>
       </c>
       <c r="D26" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E26" t="str">
         <f t="shared" si="0"/>
@@ -54551,7 +55760,7 @@
         <v>2</v>
       </c>
       <c r="D27" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E27" t="str">
         <f t="shared" ref="E27:E37" si="2">IF(G27&lt;=0, "Control", IF(G27&lt;=10, "Red", IF(G27&gt;=21, "Pink", "Orange")))</f>
@@ -54600,7 +55809,7 @@
         <v>3</v>
       </c>
       <c r="D28" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E28" t="str">
         <f t="shared" si="2"/>
@@ -54649,7 +55858,7 @@
         <v>4</v>
       </c>
       <c r="D29" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E29" t="str">
         <f t="shared" si="2"/>
@@ -54698,7 +55907,7 @@
         <v>5</v>
       </c>
       <c r="D30" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E30" t="str">
         <f t="shared" si="2"/>
@@ -54747,7 +55956,7 @@
         <v>6</v>
       </c>
       <c r="D31" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E31" t="str">
         <f t="shared" si="2"/>
@@ -54796,7 +56005,7 @@
         <v>1</v>
       </c>
       <c r="D32" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E32" t="str">
         <f t="shared" si="2"/>
@@ -54834,7 +56043,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>72</v>
       </c>
@@ -54845,7 +56054,7 @@
         <v>2</v>
       </c>
       <c r="D33" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E33" t="str">
         <f t="shared" si="2"/>
@@ -54883,7 +56092,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>73</v>
       </c>
@@ -54894,7 +56103,7 @@
         <v>3</v>
       </c>
       <c r="D34" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E34" t="str">
         <f t="shared" si="2"/>
@@ -54932,7 +56141,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>74</v>
       </c>
@@ -54943,7 +56152,7 @@
         <v>4</v>
       </c>
       <c r="D35" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E35" t="str">
         <f t="shared" si="2"/>
@@ -54981,7 +56190,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>75</v>
       </c>
@@ -54992,7 +56201,7 @@
         <v>5</v>
       </c>
       <c r="D36" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E36" t="str">
         <f t="shared" si="2"/>
@@ -55030,7 +56239,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>76</v>
       </c>
@@ -55041,7 +56250,7 @@
         <v>6</v>
       </c>
       <c r="D37" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E37" t="str">
         <f t="shared" si="2"/>
@@ -55077,78 +56286,6 @@
       <c r="M37">
         <f>'Kelp consumption'!P77</f>
         <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="O43">
-        <v>9</v>
-      </c>
-      <c r="P43">
-        <v>81</v>
-      </c>
-      <c r="R43" t="s">
-        <v>60</v>
-      </c>
-      <c r="W43" t="s">
-        <v>59</v>
-      </c>
-      <c r="X43">
-        <f>IF(W43="Control", 1, IF(W43="Red", 2, IF(W43="Orange", 3, 4)))</f>
-        <v>3</v>
-      </c>
-      <c r="Z43" t="s">
-        <v>62</v>
-      </c>
-      <c r="AA43" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="44" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="O44">
-        <v>10</v>
-      </c>
-      <c r="P44">
-        <v>82</v>
-      </c>
-      <c r="R44" t="s">
-        <v>60</v>
-      </c>
-      <c r="W44" t="s">
-        <v>57</v>
-      </c>
-      <c r="X44">
-        <f>IF(W44="Control", 1, IF(W44="Red", 2, IF(W44="Orange", 3, 4)))</f>
-        <v>1</v>
-      </c>
-      <c r="Z44">
-        <v>26</v>
-      </c>
-      <c r="AA44">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="45" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="O45">
-        <v>11</v>
-      </c>
-      <c r="P45">
-        <v>83</v>
-      </c>
-      <c r="R45" t="s">
-        <v>60</v>
-      </c>
-      <c r="W45" t="s">
-        <v>58</v>
-      </c>
-      <c r="X45">
-        <f>IF(W45="Control", 1, IF(W45="Red", 2, IF(W45="Orange", 3, 4)))</f>
-        <v>2</v>
-      </c>
-      <c r="Z45">
-        <v>6</v>
-      </c>
-      <c r="AA45">
-        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
more kelp image analysis
</commit_message>
<xml_diff>
--- a/data/raw.xlsx
+++ b/data/raw.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/EcosystemRecoveryLab/github/Ritger-Corynactis-urchin-deterrence/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBE5344B-79AF-5B44-85B0-C7219F71C4D0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42C50CB4-FB7B-DA4D-A627-5EBD340BE2AD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13100" yWindow="5240" windowWidth="23780" windowHeight="13760" activeTab="2" xr2:uid="{58E670A5-634C-427F-960F-9DA76C64E810}"/>
+    <workbookView xWindow="14820" yWindow="5920" windowWidth="23780" windowHeight="13760" activeTab="1" xr2:uid="{58E670A5-634C-427F-960F-9DA76C64E810}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="3" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="96">
   <si>
     <t>Day</t>
   </si>
@@ -306,6 +306,15 @@
   </si>
   <si>
     <t>NO</t>
+  </si>
+  <si>
+    <t>hole included in "after"</t>
+  </si>
+  <si>
+    <t>"before" included some shadow</t>
+  </si>
+  <si>
+    <t>hole included in "before"</t>
   </si>
 </sst>
 </file>
@@ -49594,9 +49603,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD5E687B-43EE-4B00-8604-7EB9984510DD}">
   <dimension ref="A1:W77"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="R11" sqref="R11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Q49" sqref="Q49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -52547,13 +52556,19 @@
       <c r="P44">
         <v>720</v>
       </c>
+      <c r="Q44">
+        <v>68.570999999999998</v>
+      </c>
+      <c r="R44">
+        <v>12.182</v>
+      </c>
       <c r="S44">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="T44" t="e">
+        <v>56.388999999999996</v>
+      </c>
+      <c r="T44">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
+        <v>0.82234472298785199</v>
       </c>
       <c r="U44" t="s">
         <v>89</v>
@@ -52608,13 +52623,20 @@
       <c r="P45">
         <v>720</v>
       </c>
+      <c r="Q45">
+        <v>107.02800000000001</v>
+      </c>
+      <c r="R45">
+        <f>92.07+2.895</f>
+        <v>94.964999999999989</v>
+      </c>
       <c r="S45">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="T45" t="e">
+        <v>12.063000000000017</v>
+      </c>
+      <c r="T45">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
+        <v>0.11270882385917719</v>
       </c>
       <c r="U45" t="s">
         <v>89</v>
@@ -52669,13 +52691,19 @@
       <c r="P46">
         <v>720</v>
       </c>
+      <c r="Q46">
+        <v>59.332000000000001</v>
+      </c>
+      <c r="R46">
+        <v>57.972000000000001</v>
+      </c>
       <c r="S46">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="T46" t="e">
+        <v>1.3599999999999994</v>
+      </c>
+      <c r="T46">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
+        <v>2.2921863412660948E-2</v>
       </c>
       <c r="U46" t="s">
         <v>90</v>
@@ -52730,13 +52758,19 @@
       <c r="P47">
         <v>720</v>
       </c>
+      <c r="Q47">
+        <v>63.07</v>
+      </c>
+      <c r="R47">
+        <v>62.152999999999999</v>
+      </c>
       <c r="S47">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="T47" t="e">
+        <v>0.91700000000000159</v>
+      </c>
+      <c r="T47">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
+        <v>1.4539400665926773E-2</v>
       </c>
       <c r="U47" t="s">
         <v>90</v>
@@ -52790,13 +52824,19 @@
       <c r="P48">
         <v>720</v>
       </c>
+      <c r="Q48">
+        <v>93.19</v>
+      </c>
+      <c r="R48">
+        <v>92.295000000000002</v>
+      </c>
       <c r="S48">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="T48" t="e">
+        <v>0.89499999999999602</v>
+      </c>
+      <c r="T48">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
+        <v>9.6040347676788936E-3</v>
       </c>
       <c r="U48" t="s">
         <v>91</v>
@@ -52805,8 +52845,11 @@
         <f t="shared" si="5"/>
         <v>yes</v>
       </c>
-    </row>
-    <row r="49" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W48" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="49" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>48</v>
       </c>
@@ -52851,13 +52894,19 @@
       <c r="P49">
         <v>720</v>
       </c>
+      <c r="Q49">
+        <v>60.268000000000001</v>
+      </c>
+      <c r="R49">
+        <v>58.454999999999998</v>
+      </c>
       <c r="S49">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="T49" t="e">
+        <v>1.8130000000000024</v>
+      </c>
+      <c r="T49">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
+        <v>3.0082299064180036E-2</v>
       </c>
       <c r="U49" t="s">
         <v>90</v>
@@ -52867,7 +52916,7 @@
         <v>yes</v>
       </c>
     </row>
-    <row r="50" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>49</v>
       </c>
@@ -52912,13 +52961,20 @@
       <c r="P50">
         <v>733</v>
       </c>
+      <c r="Q50">
+        <v>70.875</v>
+      </c>
+      <c r="R50">
+        <f>21.906+33.948</f>
+        <v>55.853999999999999</v>
+      </c>
       <c r="S50">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="T50" t="e">
+        <v>15.021000000000001</v>
+      </c>
+      <c r="T50">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
+        <v>0.21193650793650795</v>
       </c>
       <c r="U50" t="s">
         <v>89</v>
@@ -52927,8 +52983,11 @@
         <f t="shared" si="5"/>
         <v>no</v>
       </c>
-    </row>
-    <row r="51" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W50" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="51" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>50</v>
       </c>
@@ -52973,13 +53032,19 @@
       <c r="P51">
         <v>733</v>
       </c>
+      <c r="Q51">
+        <v>96.043999999999997</v>
+      </c>
+      <c r="R51">
+        <v>92.927000000000007</v>
+      </c>
       <c r="S51">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="T51" t="e">
+        <v>3.1169999999999902</v>
+      </c>
+      <c r="T51">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
+        <v>3.2453875307150791E-2</v>
       </c>
       <c r="U51" t="s">
         <v>90</v>
@@ -52989,7 +53054,7 @@
         <v>no</v>
       </c>
     </row>
-    <row r="52" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>51</v>
       </c>
@@ -53034,13 +53099,20 @@
       <c r="P52">
         <v>733</v>
       </c>
+      <c r="Q52">
+        <v>65.846000000000004</v>
+      </c>
+      <c r="R52">
+        <f>37.272+11.262</f>
+        <v>48.533999999999999</v>
+      </c>
       <c r="S52">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="T52" t="e">
+        <v>17.312000000000005</v>
+      </c>
+      <c r="T52">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
+        <v>0.2629165021413602</v>
       </c>
       <c r="U52" t="s">
         <v>89</v>
@@ -53050,7 +53122,7 @@
         <v>no</v>
       </c>
     </row>
-    <row r="53" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>52</v>
       </c>
@@ -53095,13 +53167,19 @@
       <c r="P53">
         <v>733</v>
       </c>
+      <c r="Q53">
+        <v>85.570999999999998</v>
+      </c>
+      <c r="R53">
+        <v>85.394000000000005</v>
+      </c>
       <c r="S53">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="T53" t="e">
+        <v>0.1769999999999925</v>
+      </c>
+      <c r="T53">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
+        <v>2.0684577719086196E-3</v>
       </c>
       <c r="U53" t="s">
         <v>90</v>
@@ -53110,8 +53188,11 @@
         <f t="shared" si="5"/>
         <v>no</v>
       </c>
-    </row>
-    <row r="54" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W53" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="54" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>53</v>
       </c>
@@ -53156,13 +53237,19 @@
       <c r="P54">
         <v>733</v>
       </c>
+      <c r="Q54">
+        <v>66.453000000000003</v>
+      </c>
+      <c r="R54">
+        <v>27.852</v>
+      </c>
       <c r="S54">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="T54" t="e">
+        <v>38.600999999999999</v>
+      </c>
+      <c r="T54">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
+        <v>0.58087670985508555</v>
       </c>
       <c r="U54" t="s">
         <v>89</v>
@@ -53171,8 +53258,11 @@
         <f t="shared" si="5"/>
         <v>no</v>
       </c>
-    </row>
-    <row r="55" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W54" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="55" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>54</v>
       </c>
@@ -53217,13 +53307,19 @@
       <c r="P55">
         <v>733</v>
       </c>
+      <c r="Q55">
+        <v>70.8</v>
+      </c>
+      <c r="R55">
+        <v>63.54</v>
+      </c>
       <c r="S55">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="T55" t="e">
+        <v>7.259999999999998</v>
+      </c>
+      <c r="T55">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
+        <v>0.10254237288135591</v>
       </c>
       <c r="U55" t="s">
         <v>89</v>
@@ -53233,7 +53329,7 @@
         <v>no</v>
       </c>
     </row>
-    <row r="56" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>55</v>
       </c>
@@ -53278,13 +53374,19 @@
       <c r="P56">
         <v>733</v>
       </c>
+      <c r="Q56">
+        <v>85.197000000000003</v>
+      </c>
+      <c r="R56">
+        <v>67.561999999999998</v>
+      </c>
       <c r="S56">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="T56" t="e">
+        <v>17.635000000000005</v>
+      </c>
+      <c r="T56">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
+        <v>0.20699085648555707</v>
       </c>
       <c r="U56" t="s">
         <v>89</v>
@@ -53293,8 +53395,11 @@
         <f t="shared" si="5"/>
         <v>no</v>
       </c>
-    </row>
-    <row r="57" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W56" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="57" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>56</v>
       </c>
@@ -53339,13 +53444,20 @@
       <c r="P57">
         <v>733</v>
       </c>
+      <c r="Q57">
+        <v>84.320999999999998</v>
+      </c>
+      <c r="R57">
+        <f>18.53+0.956+36.459</f>
+        <v>55.945000000000007</v>
+      </c>
       <c r="S57">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="T57" t="e">
+        <v>28.375999999999991</v>
+      </c>
+      <c r="T57">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
+        <v>0.33652352320299794</v>
       </c>
       <c r="U57" t="s">
         <v>90</v>
@@ -53355,7 +53467,7 @@
         <v>no</v>
       </c>
     </row>
-    <row r="58" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>57</v>
       </c>
@@ -53400,7 +53512,7 @@
         <v>no</v>
       </c>
     </row>
-    <row r="59" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>58</v>
       </c>
@@ -53445,7 +53557,7 @@
         <v>no</v>
       </c>
     </row>
-    <row r="60" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>59</v>
       </c>
@@ -53490,7 +53602,7 @@
         <v>no</v>
       </c>
     </row>
-    <row r="61" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>60</v>
       </c>
@@ -53535,7 +53647,7 @@
         <v>no</v>
       </c>
     </row>
-    <row r="62" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>61</v>
       </c>
@@ -53580,7 +53692,7 @@
         <v>no</v>
       </c>
     </row>
-    <row r="63" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>62</v>
       </c>
@@ -53625,7 +53737,7 @@
         <v>no</v>
       </c>
     </row>
-    <row r="64" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>63</v>
       </c>
@@ -54268,7 +54380,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55F6BF2F-CBB2-4331-929A-D3F4AD694052}">
   <dimension ref="A1:AC37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="D13" workbookViewId="0">
       <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Sept 5 morning - data added, kelp blade analysis
</commit_message>
<xml_diff>
--- a/data/raw.xlsx
+++ b/data/raw.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/EcosystemRecoveryLab/github/Ritger-Corynactis-urchin-deterrence/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42C50CB4-FB7B-DA4D-A627-5EBD340BE2AD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83886F9A-7E4B-4E47-82BD-A6FADDE2330F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14820" yWindow="5920" windowWidth="23780" windowHeight="13760" activeTab="1" xr2:uid="{58E670A5-634C-427F-960F-9DA76C64E810}"/>
+    <workbookView xWindow="22660" yWindow="13000" windowWidth="23780" windowHeight="13760" activeTab="1" xr2:uid="{58E670A5-634C-427F-960F-9DA76C64E810}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="3" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="97">
   <si>
     <t>Day</t>
   </si>
@@ -293,9 +293,6 @@
     <t>"before" and "after" included some shadow</t>
   </si>
   <si>
-    <t>Kelp consumed?</t>
-  </si>
-  <si>
     <t>yes</t>
   </si>
   <si>
@@ -315,6 +312,12 @@
   </si>
   <si>
     <t>hole included in "before"</t>
+  </si>
+  <si>
+    <t>Kelp visibly consumed?</t>
+  </si>
+  <si>
+    <t>shadow and rip ==&gt; guesstimate</t>
   </si>
 </sst>
 </file>
@@ -49604,8 +49607,8 @@
   <dimension ref="A1:W77"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q49" sqref="Q49"/>
+      <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="W66" sqref="W66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -49696,7 +49699,7 @@
         <v>14</v>
       </c>
       <c r="U1" s="2" t="s">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="V1" s="2" t="s">
         <v>25</v>
@@ -49760,7 +49763,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="V2" t="str">
         <f>IF(E2&gt;6,"no","yes")</f>
@@ -49822,7 +49825,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="V3" t="str">
         <f t="shared" ref="V3:V66" si="5">IF(E3&gt;6,"no","yes")</f>
@@ -49884,15 +49887,12 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="V4" t="str">
         <f t="shared" si="5"/>
         <v>yes</v>
       </c>
-      <c r="W4" t="s">
-        <v>67</v>
-      </c>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A5">
@@ -49949,7 +49949,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="V5" t="str">
         <f t="shared" si="5"/>
@@ -50011,7 +50011,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="V6" t="str">
         <f t="shared" si="5"/>
@@ -50073,7 +50073,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="V7" t="str">
         <f t="shared" si="5"/>
@@ -50135,7 +50135,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="V8" t="str">
         <f t="shared" si="5"/>
@@ -50197,7 +50197,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="V9" t="str">
         <f t="shared" si="5"/>
@@ -50259,7 +50259,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U10" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="V10" t="str">
         <f t="shared" si="5"/>
@@ -50321,7 +50321,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U11" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="V11" t="str">
         <f t="shared" si="5"/>
@@ -50383,7 +50383,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="V12" t="str">
         <f t="shared" si="5"/>
@@ -50445,7 +50445,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U13" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="V13" t="str">
         <f t="shared" si="5"/>
@@ -50507,7 +50507,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U14" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="V14" t="str">
         <f t="shared" si="5"/>
@@ -50569,7 +50569,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="V15" t="str">
         <f t="shared" si="5"/>
@@ -50637,7 +50637,7 @@
         <v>1.1132188960347966E-2</v>
       </c>
       <c r="U16" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="V16" t="str">
         <f t="shared" si="5"/>
@@ -50706,7 +50706,7 @@
         <v>0.34767247318177341</v>
       </c>
       <c r="U17" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="V17" t="str">
         <f t="shared" si="5"/>
@@ -50777,7 +50777,7 @@
         <v>1.4320708498209772E-2</v>
       </c>
       <c r="U18" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="V18" t="str">
         <f t="shared" si="5"/>
@@ -50848,7 +50848,7 @@
         <v>2.0570354813750462E-2</v>
       </c>
       <c r="U19" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="V19" t="str">
         <f t="shared" si="5"/>
@@ -50916,7 +50916,7 @@
         <v>0.19619130289116807</v>
       </c>
       <c r="U20" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="V20" t="str">
         <f t="shared" si="5"/>
@@ -50984,7 +50984,7 @@
         <v>6.3789631285387843E-3</v>
       </c>
       <c r="U21" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="V21" t="str">
         <f t="shared" si="5"/>
@@ -51052,7 +51052,7 @@
         <v>9.8303023234503264E-3</v>
       </c>
       <c r="U22" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="V22" t="str">
         <f t="shared" si="5"/>
@@ -51123,7 +51123,7 @@
         <v>-1.3759141403399721E-2</v>
       </c>
       <c r="U23" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="V23" t="str">
         <f t="shared" si="5"/>
@@ -51194,7 +51194,7 @@
         <v>7.2046396683673368E-3</v>
       </c>
       <c r="U24" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="V24" t="str">
         <f t="shared" si="5"/>
@@ -51262,7 +51262,7 @@
         <v>1.6066314050968911E-2</v>
       </c>
       <c r="U25" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="V25" t="str">
         <f t="shared" si="5"/>
@@ -51330,7 +51330,7 @@
         <v>0.104877366588544</v>
       </c>
       <c r="U26" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="V26" t="str">
         <f t="shared" si="5"/>
@@ -51401,7 +51401,7 @@
         <v>3.2134809444497774E-3</v>
       </c>
       <c r="U27" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="V27" t="str">
         <f t="shared" si="5"/>
@@ -51469,7 +51469,7 @@
         <v>1.712374076244115E-2</v>
       </c>
       <c r="U28" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="V28" t="str">
         <f t="shared" si="5"/>
@@ -51537,7 +51537,7 @@
         <v>3.8196991929567187E-2</v>
       </c>
       <c r="U29" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="V29" t="str">
         <f t="shared" si="5"/>
@@ -51606,7 +51606,7 @@
         <v>0.39414566228714759</v>
       </c>
       <c r="U30" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="V30" t="str">
         <f t="shared" si="5"/>
@@ -51674,7 +51674,7 @@
         <v>0.28625451046427708</v>
       </c>
       <c r="U31" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="V31" t="str">
         <f t="shared" si="5"/>
@@ -51742,7 +51742,7 @@
         <v>0.17109784527483193</v>
       </c>
       <c r="U32" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="V32" t="str">
         <f t="shared" si="5"/>
@@ -51810,7 +51810,7 @@
         <v>-1.4416269790191878E-2</v>
       </c>
       <c r="U33" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="V33" t="str">
         <f t="shared" si="5"/>
@@ -51879,7 +51879,7 @@
         <v>0.32763076777161293</v>
       </c>
       <c r="U34" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="V34" t="str">
         <f t="shared" si="5"/>
@@ -51950,7 +51950,7 @@
         <v>1.0624224886316719E-2</v>
       </c>
       <c r="U35" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="V35" t="str">
         <f t="shared" si="5"/>
@@ -52021,7 +52021,7 @@
         <v>0.33511229946524063</v>
       </c>
       <c r="U36" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="V36" t="str">
         <f t="shared" si="5"/>
@@ -52089,7 +52089,7 @@
         <v>8.9727722772276596E-3</v>
       </c>
       <c r="U37" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="V37" t="str">
         <f t="shared" si="5"/>
@@ -52157,7 +52157,7 @@
         <v>0.27821013587304089</v>
       </c>
       <c r="U38" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="V38" t="str">
         <f t="shared" si="5"/>
@@ -52228,7 +52228,7 @@
         <v>0.50121017042193783</v>
       </c>
       <c r="U39" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="V39" t="str">
         <f t="shared" si="5"/>
@@ -52296,7 +52296,7 @@
         <v>0.42735033602940398</v>
       </c>
       <c r="U40" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="V40" t="str">
         <f t="shared" si="5"/>
@@ -52365,7 +52365,7 @@
         <v>0.91152623616800665</v>
       </c>
       <c r="U41" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="V41" t="str">
         <f t="shared" si="5"/>
@@ -52433,7 +52433,7 @@
         <v>7.5201906527207442E-3</v>
       </c>
       <c r="U42" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="V42" t="str">
         <f t="shared" si="5"/>
@@ -52501,7 +52501,7 @@
         <v>1.9049721461127905E-2</v>
       </c>
       <c r="U43" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="V43" t="str">
         <f t="shared" si="5"/>
@@ -52571,7 +52571,7 @@
         <v>0.82234472298785199</v>
       </c>
       <c r="U44" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="V44" t="str">
         <f t="shared" si="5"/>
@@ -52639,7 +52639,7 @@
         <v>0.11270882385917719</v>
       </c>
       <c r="U45" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="V45" t="str">
         <f t="shared" si="5"/>
@@ -52706,7 +52706,7 @@
         <v>2.2921863412660948E-2</v>
       </c>
       <c r="U46" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="V46" t="str">
         <f t="shared" si="5"/>
@@ -52773,10 +52773,10 @@
         <v>1.4539400665926773E-2</v>
       </c>
       <c r="U47" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="V47" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="48" spans="1:23" x14ac:dyDescent="0.2">
@@ -52839,7 +52839,7 @@
         <v>9.6040347676788936E-3</v>
       </c>
       <c r="U48" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="V48" t="str">
         <f t="shared" si="5"/>
@@ -52909,7 +52909,7 @@
         <v>3.0082299064180036E-2</v>
       </c>
       <c r="U49" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="V49" t="str">
         <f t="shared" si="5"/>
@@ -52977,14 +52977,14 @@
         <v>0.21193650793650795</v>
       </c>
       <c r="U50" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="V50" t="str">
         <f t="shared" si="5"/>
         <v>no</v>
       </c>
       <c r="W50" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="51" spans="1:23" x14ac:dyDescent="0.2">
@@ -53047,7 +53047,7 @@
         <v>3.2453875307150791E-2</v>
       </c>
       <c r="U51" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="V51" t="str">
         <f t="shared" si="5"/>
@@ -53115,7 +53115,7 @@
         <v>0.2629165021413602</v>
       </c>
       <c r="U52" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="V52" t="str">
         <f t="shared" si="5"/>
@@ -53182,14 +53182,14 @@
         <v>2.0684577719086196E-3</v>
       </c>
       <c r="U53" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="V53" t="str">
         <f t="shared" si="5"/>
         <v>no</v>
       </c>
       <c r="W53" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="54" spans="1:23" x14ac:dyDescent="0.2">
@@ -53252,14 +53252,14 @@
         <v>0.58087670985508555</v>
       </c>
       <c r="U54" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="V54" t="str">
         <f t="shared" si="5"/>
         <v>no</v>
       </c>
       <c r="W54" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="55" spans="1:23" x14ac:dyDescent="0.2">
@@ -53322,7 +53322,7 @@
         <v>0.10254237288135591</v>
       </c>
       <c r="U55" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="V55" t="str">
         <f t="shared" si="5"/>
@@ -53389,14 +53389,14 @@
         <v>0.20699085648555707</v>
       </c>
       <c r="U56" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="V56" t="str">
         <f t="shared" si="5"/>
         <v>no</v>
       </c>
       <c r="W56" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="57" spans="1:23" x14ac:dyDescent="0.2">
@@ -53460,7 +53460,7 @@
         <v>0.33652352320299794</v>
       </c>
       <c r="U57" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="V57" t="str">
         <f t="shared" si="5"/>
@@ -53494,18 +53494,41 @@
       <c r="I58" s="7">
         <v>2</v>
       </c>
-      <c r="K58" s="5"/>
+      <c r="K58" s="7">
+        <v>58</v>
+      </c>
+      <c r="L58" s="4">
+        <v>96</v>
+      </c>
+      <c r="M58" s="4">
+        <v>99</v>
+      </c>
       <c r="N58">
         <f t="shared" ref="N58:N77" si="9">C58-239</f>
         <v>8</v>
       </c>
+      <c r="O58">
+        <v>1920</v>
+      </c>
+      <c r="P58">
+        <v>720</v>
+      </c>
+      <c r="Q58">
+        <v>83.355999999999995</v>
+      </c>
+      <c r="R58">
+        <v>83.33</v>
+      </c>
       <c r="S58">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="T58" t="e">
+        <v>2.5999999999996248E-2</v>
+      </c>
+      <c r="T58">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
+        <v>3.1191515907668613E-4</v>
+      </c>
+      <c r="U58" t="s">
+        <v>89</v>
       </c>
       <c r="V58" t="str">
         <f t="shared" si="5"/>
@@ -53539,18 +53562,42 @@
       <c r="I59" s="7">
         <v>0</v>
       </c>
-      <c r="K59" s="5"/>
+      <c r="K59" s="7">
+        <v>61</v>
+      </c>
+      <c r="L59" s="4">
+        <v>100</v>
+      </c>
+      <c r="M59" s="4">
+        <v>102</v>
+      </c>
       <c r="N59">
         <f t="shared" si="9"/>
         <v>8</v>
       </c>
+      <c r="O59">
+        <v>1920</v>
+      </c>
+      <c r="P59">
+        <v>720</v>
+      </c>
+      <c r="Q59">
+        <v>73.596999999999994</v>
+      </c>
+      <c r="R59">
+        <f>42.76+2.734</f>
+        <v>45.494</v>
+      </c>
       <c r="S59">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="T59" t="e">
+        <v>28.102999999999994</v>
+      </c>
+      <c r="T59">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
+        <v>0.38184980366047527</v>
+      </c>
+      <c r="U59" t="s">
+        <v>88</v>
       </c>
       <c r="V59" t="str">
         <f t="shared" si="5"/>
@@ -53584,18 +53631,41 @@
       <c r="I60" s="5">
         <v>29</v>
       </c>
-      <c r="K60" s="5"/>
+      <c r="K60">
+        <v>46</v>
+      </c>
+      <c r="L60" s="4">
+        <v>38</v>
+      </c>
+      <c r="M60" s="4">
+        <v>37</v>
+      </c>
       <c r="N60">
         <f t="shared" si="9"/>
         <v>8</v>
       </c>
+      <c r="O60">
+        <v>1920</v>
+      </c>
+      <c r="P60">
+        <v>720</v>
+      </c>
+      <c r="Q60">
+        <v>62.996000000000002</v>
+      </c>
+      <c r="R60">
+        <v>63.26</v>
+      </c>
       <c r="S60">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="T60" t="e">
+        <v>-0.26399999999999579</v>
+      </c>
+      <c r="T60">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
+        <v>-4.1907422693503683E-3</v>
+      </c>
+      <c r="U60" t="s">
+        <v>89</v>
       </c>
       <c r="V60" t="str">
         <f t="shared" si="5"/>
@@ -53629,18 +53699,41 @@
       <c r="I61" s="5">
         <v>9</v>
       </c>
-      <c r="K61" s="5"/>
+      <c r="K61">
+        <v>55</v>
+      </c>
+      <c r="L61" s="4">
+        <v>73</v>
+      </c>
+      <c r="M61" s="4">
+        <v>74</v>
+      </c>
       <c r="N61">
         <f t="shared" si="9"/>
         <v>8</v>
       </c>
+      <c r="O61">
+        <v>1920</v>
+      </c>
+      <c r="P61">
+        <v>720</v>
+      </c>
+      <c r="Q61">
+        <v>70.064999999999998</v>
+      </c>
+      <c r="R61">
+        <v>69.334000000000003</v>
+      </c>
       <c r="S61">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="T61" t="e">
+        <v>0.73099999999999454</v>
+      </c>
+      <c r="T61">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
+        <v>1.0433169200028467E-2</v>
+      </c>
+      <c r="U61" t="s">
+        <v>89</v>
       </c>
       <c r="V61" t="str">
         <f t="shared" si="5"/>
@@ -53674,18 +53767,42 @@
       <c r="I62" s="5">
         <v>18</v>
       </c>
-      <c r="K62" s="5"/>
+      <c r="K62">
+        <v>47</v>
+      </c>
+      <c r="L62" s="4">
+        <v>47</v>
+      </c>
+      <c r="M62" s="4">
+        <v>49</v>
+      </c>
       <c r="N62">
         <f t="shared" si="9"/>
         <v>8</v>
       </c>
+      <c r="O62">
+        <v>1920</v>
+      </c>
+      <c r="P62">
+        <v>720</v>
+      </c>
+      <c r="Q62">
+        <v>72.325999999999993</v>
+      </c>
+      <c r="R62">
+        <f>31.253+6.077+1.701</f>
+        <v>39.030999999999999</v>
+      </c>
       <c r="S62">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="T62" t="e">
+        <v>33.294999999999995</v>
+      </c>
+      <c r="T62">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
+        <v>0.46034621021486044</v>
+      </c>
+      <c r="U62" t="s">
+        <v>88</v>
       </c>
       <c r="V62" t="str">
         <f t="shared" si="5"/>
@@ -53719,23 +53836,49 @@
       <c r="I63" s="5">
         <v>12</v>
       </c>
-      <c r="K63" s="5"/>
+      <c r="K63">
+        <v>42</v>
+      </c>
+      <c r="L63" s="4">
+        <v>32</v>
+      </c>
+      <c r="M63" s="4">
+        <v>34</v>
+      </c>
       <c r="N63">
         <f t="shared" si="9"/>
         <v>8</v>
       </c>
+      <c r="O63">
+        <v>1920</v>
+      </c>
+      <c r="P63">
+        <v>720</v>
+      </c>
+      <c r="Q63">
+        <v>69.322999999999993</v>
+      </c>
+      <c r="R63">
+        <v>57.683</v>
+      </c>
       <c r="S63">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="T63" t="e">
+        <v>11.639999999999993</v>
+      </c>
+      <c r="T63">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
+        <v>0.16790964037909489</v>
+      </c>
+      <c r="U63" t="s">
+        <v>88</v>
       </c>
       <c r="V63" t="str">
         <f t="shared" si="5"/>
         <v>no</v>
       </c>
+      <c r="W63" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="64" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A64">
@@ -53764,25 +53907,51 @@
       <c r="I64" s="5">
         <v>0</v>
       </c>
-      <c r="K64" s="5"/>
+      <c r="K64">
+        <v>46</v>
+      </c>
+      <c r="L64" s="4">
+        <v>44</v>
+      </c>
+      <c r="M64" s="4">
+        <v>44</v>
+      </c>
       <c r="N64">
         <f t="shared" si="9"/>
         <v>8</v>
       </c>
+      <c r="O64">
+        <v>1920</v>
+      </c>
+      <c r="P64">
+        <v>720</v>
+      </c>
+      <c r="Q64">
+        <v>63.42</v>
+      </c>
+      <c r="R64">
+        <v>45.901000000000003</v>
+      </c>
       <c r="S64">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="T64" t="e">
+        <v>17.518999999999998</v>
+      </c>
+      <c r="T64">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
+        <v>0.27623777988016396</v>
+      </c>
+      <c r="U64" t="s">
+        <v>88</v>
       </c>
       <c r="V64" t="str">
         <f t="shared" si="5"/>
         <v>no</v>
       </c>
-    </row>
-    <row r="65" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W64" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="65" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>64</v>
       </c>
@@ -53809,25 +53978,51 @@
       <c r="I65" s="5">
         <v>1</v>
       </c>
-      <c r="K65" s="5"/>
+      <c r="K65">
+        <v>62</v>
+      </c>
+      <c r="L65" s="4">
+        <v>102</v>
+      </c>
+      <c r="M65" s="4">
+        <v>101</v>
+      </c>
       <c r="N65">
         <f t="shared" si="9"/>
         <v>8</v>
       </c>
+      <c r="O65">
+        <v>1920</v>
+      </c>
+      <c r="P65">
+        <v>720</v>
+      </c>
+      <c r="Q65">
+        <v>72.263000000000005</v>
+      </c>
+      <c r="R65">
+        <v>71.108999999999995</v>
+      </c>
       <c r="S65">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="T65" t="e">
+        <v>1.1540000000000106</v>
+      </c>
+      <c r="T65">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
+        <v>1.5969444944162442E-2</v>
+      </c>
+      <c r="U65" t="s">
+        <v>89</v>
       </c>
       <c r="V65" t="str">
         <f t="shared" si="5"/>
         <v>no</v>
       </c>
-    </row>
-    <row r="66" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W65" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="66" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>65</v>
       </c>
@@ -53872,7 +54067,7 @@
         <v>yes</v>
       </c>
     </row>
-    <row r="67" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>66</v>
       </c>
@@ -53917,7 +54112,7 @@
         <v>yes</v>
       </c>
     </row>
-    <row r="68" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>67</v>
       </c>
@@ -53962,7 +54157,7 @@
         <v>yes</v>
       </c>
     </row>
-    <row r="69" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>68</v>
       </c>
@@ -54007,7 +54202,7 @@
         <v>yes</v>
       </c>
     </row>
-    <row r="70" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>69</v>
       </c>
@@ -54052,7 +54247,7 @@
         <v>yes</v>
       </c>
     </row>
-    <row r="71" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>70</v>
       </c>
@@ -54097,7 +54292,7 @@
         <v>yes</v>
       </c>
     </row>
-    <row r="72" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>71</v>
       </c>
@@ -54142,7 +54337,7 @@
         <v>yes</v>
       </c>
     </row>
-    <row r="73" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>72</v>
       </c>
@@ -54187,7 +54382,7 @@
         <v>yes</v>
       </c>
     </row>
-    <row r="74" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>73</v>
       </c>
@@ -54232,7 +54427,7 @@
         <v>yes</v>
       </c>
     </row>
-    <row r="75" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>74</v>
       </c>
@@ -54277,7 +54472,7 @@
         <v>yes</v>
       </c>
     </row>
-    <row r="76" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>75</v>
       </c>
@@ -54322,7 +54517,7 @@
         <v>yes</v>
       </c>
     </row>
-    <row r="77" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>76</v>
       </c>
@@ -54380,8 +54575,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55F6BF2F-CBB2-4331-929A-D3F4AD694052}">
   <dimension ref="A1:AC37"/>
   <sheetViews>
-    <sheetView topLeftCell="D13" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="AC26" sqref="AC26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -54660,7 +54855,7 @@
         <v>1</v>
       </c>
       <c r="AC4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:29" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Morning Sept 5 rest of kelp blade analysis from 8.31
</commit_message>
<xml_diff>
--- a/data/raw.xlsx
+++ b/data/raw.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/EcosystemRecoveryLab/github/Ritger-Corynactis-urchin-deterrence/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83886F9A-7E4B-4E47-82BD-A6FADDE2330F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0C7E187-B889-3743-AE86-EE45BBFA6EEB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22660" yWindow="13000" windowWidth="23780" windowHeight="13760" activeTab="1" xr2:uid="{58E670A5-634C-427F-960F-9DA76C64E810}"/>
+    <workbookView xWindow="20520" yWindow="12000" windowWidth="23780" windowHeight="13760" activeTab="1" xr2:uid="{58E670A5-634C-427F-960F-9DA76C64E810}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="3" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="101">
   <si>
     <t>Day</t>
   </si>
@@ -318,6 +318,18 @@
   </si>
   <si>
     <t>shadow and rip ==&gt; guesstimate</t>
+  </si>
+  <si>
+    <t>"before" out of focus</t>
+  </si>
+  <si>
+    <t>"after" includes shadows</t>
+  </si>
+  <si>
+    <t>"before" out of focus, "after" includes shadows</t>
+  </si>
+  <si>
+    <t>"before" included some holes, "after" includes holes</t>
   </si>
 </sst>
 </file>
@@ -49606,9 +49618,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD5E687B-43EE-4B00-8604-7EB9984510DD}">
   <dimension ref="A1:W77"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="W66" sqref="W66"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="W8" sqref="W8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -49754,13 +49766,19 @@
       <c r="P2">
         <v>730</v>
       </c>
+      <c r="Q2">
+        <v>129.304</v>
+      </c>
+      <c r="R2">
+        <v>115.282</v>
+      </c>
       <c r="S2">
         <f t="shared" ref="S2:S15" si="0">Q2-R2</f>
-        <v>0</v>
-      </c>
-      <c r="T2" t="e">
+        <v>14.022000000000006</v>
+      </c>
+      <c r="T2">
         <f>S2/Q2</f>
-        <v>#DIV/0!</v>
+        <v>0.10844212089339854</v>
       </c>
       <c r="U2" t="s">
         <v>88</v>
@@ -49816,13 +49834,19 @@
       <c r="P3">
         <v>730</v>
       </c>
+      <c r="Q3">
+        <v>125.295</v>
+      </c>
+      <c r="R3">
+        <v>123.61</v>
+      </c>
       <c r="S3">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="T3" t="e">
+        <v>1.6850000000000023</v>
+      </c>
+      <c r="T3">
         <f t="shared" ref="T3:T66" si="4">S3/Q3</f>
-        <v>#DIV/0!</v>
+        <v>1.3448262101440619E-2</v>
       </c>
       <c r="U3" t="s">
         <v>89</v>
@@ -49831,6 +49855,9 @@
         <f t="shared" ref="V3:V66" si="5">IF(E3&gt;6,"no","yes")</f>
         <v>yes</v>
       </c>
+      <c r="W3" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A4">
@@ -49878,13 +49905,19 @@
       <c r="P4">
         <v>730</v>
       </c>
+      <c r="Q4">
+        <v>97.843000000000004</v>
+      </c>
+      <c r="R4">
+        <v>70.075000000000003</v>
+      </c>
       <c r="S4">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="T4" t="e">
+        <v>27.768000000000001</v>
+      </c>
+      <c r="T4">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
+        <v>0.28380160052328729</v>
       </c>
       <c r="U4" t="s">
         <v>88</v>
@@ -49940,13 +49973,19 @@
       <c r="P5">
         <v>730</v>
       </c>
+      <c r="Q5">
+        <v>123.244</v>
+      </c>
+      <c r="R5">
+        <v>106.542</v>
+      </c>
       <c r="S5">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="T5" t="e">
+        <v>16.701999999999998</v>
+      </c>
+      <c r="T5">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
+        <v>0.13551978189607605</v>
       </c>
       <c r="U5" t="s">
         <v>88</v>
@@ -49955,6 +49994,9 @@
         <f t="shared" si="5"/>
         <v>yes</v>
       </c>
+      <c r="W5" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A6">
@@ -50002,13 +50044,19 @@
       <c r="P6">
         <v>730</v>
       </c>
+      <c r="Q6">
+        <v>113.479</v>
+      </c>
+      <c r="R6">
+        <v>84.423000000000002</v>
+      </c>
       <c r="S6">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="T6" t="e">
+        <v>29.055999999999997</v>
+      </c>
+      <c r="T6">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
+        <v>0.25604737440407477</v>
       </c>
       <c r="U6" t="s">
         <v>88</v>
@@ -50017,6 +50065,9 @@
         <f t="shared" si="5"/>
         <v>yes</v>
       </c>
+      <c r="W6" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A7">
@@ -50064,13 +50115,19 @@
       <c r="P7">
         <v>730</v>
       </c>
+      <c r="Q7">
+        <v>119.378</v>
+      </c>
+      <c r="R7">
+        <v>105.98</v>
+      </c>
       <c r="S7">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="T7" t="e">
+        <v>13.397999999999996</v>
+      </c>
+      <c r="T7">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
+        <v>0.11223173449044209</v>
       </c>
       <c r="U7" t="s">
         <v>88</v>
@@ -50079,6 +50136,9 @@
         <f t="shared" si="5"/>
         <v>yes</v>
       </c>
+      <c r="W7" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A8">
@@ -50126,13 +50186,19 @@
       <c r="P8">
         <v>740</v>
       </c>
+      <c r="Q8">
+        <v>90.466999999999999</v>
+      </c>
+      <c r="R8">
+        <v>90.677999999999997</v>
+      </c>
       <c r="S8">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="T8" t="e">
+        <v>-0.21099999999999852</v>
+      </c>
+      <c r="T8">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
+        <v>-2.3323421800214282E-3</v>
       </c>
       <c r="U8" t="s">
         <v>89</v>
@@ -50188,13 +50254,19 @@
       <c r="P9">
         <v>740</v>
       </c>
+      <c r="Q9">
+        <v>114.098</v>
+      </c>
+      <c r="R9">
+        <v>114.75</v>
+      </c>
       <c r="S9">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="T9" t="e">
+        <v>-0.65200000000000102</v>
+      </c>
+      <c r="T9">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
+        <v>-5.7143858788059479E-3</v>
       </c>
       <c r="U9" t="s">
         <v>89</v>
@@ -50250,13 +50322,19 @@
       <c r="P10">
         <v>740</v>
       </c>
+      <c r="Q10">
+        <v>108.271</v>
+      </c>
+      <c r="R10">
+        <v>108.896</v>
+      </c>
       <c r="S10">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="T10" t="e">
+        <v>-0.625</v>
+      </c>
+      <c r="T10">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
+        <v>-5.7725522069621595E-3</v>
       </c>
       <c r="U10" t="s">
         <v>89</v>
@@ -50265,6 +50343,9 @@
         <f t="shared" si="5"/>
         <v>no</v>
       </c>
+      <c r="W10" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A11">
@@ -50312,13 +50393,19 @@
       <c r="P11">
         <v>740</v>
       </c>
+      <c r="Q11">
+        <v>104.895</v>
+      </c>
+      <c r="R11">
+        <v>102.779</v>
+      </c>
       <c r="S11">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="T11" t="e">
+        <v>2.1159999999999997</v>
+      </c>
+      <c r="T11">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
+        <v>2.0172553505886835E-2</v>
       </c>
       <c r="U11" t="s">
         <v>89</v>
@@ -50327,6 +50414,9 @@
         <f t="shared" si="5"/>
         <v>no</v>
       </c>
+      <c r="W11" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A12">
@@ -50374,13 +50464,19 @@
       <c r="P12">
         <v>740</v>
       </c>
+      <c r="Q12">
+        <v>118.879</v>
+      </c>
+      <c r="R12">
+        <v>90.667000000000002</v>
+      </c>
       <c r="S12">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="T12" t="e">
+        <v>28.212000000000003</v>
+      </c>
+      <c r="T12">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
+        <v>0.23731693570773646</v>
       </c>
       <c r="U12" t="s">
         <v>88</v>
@@ -50389,6 +50485,9 @@
         <f t="shared" si="5"/>
         <v>no</v>
       </c>
+      <c r="W12" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A13">
@@ -50436,13 +50535,19 @@
       <c r="P13">
         <v>740</v>
       </c>
+      <c r="Q13">
+        <v>128.02099999999999</v>
+      </c>
+      <c r="R13">
+        <v>100.726</v>
+      </c>
       <c r="S13">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="T13" t="e">
+        <v>27.294999999999987</v>
+      </c>
+      <c r="T13">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
+        <v>0.21320720819240585</v>
       </c>
       <c r="U13" t="s">
         <v>88</v>
@@ -50451,6 +50556,9 @@
         <f t="shared" si="5"/>
         <v>no</v>
       </c>
+      <c r="W13" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A14">
@@ -50498,13 +50606,19 @@
       <c r="P14">
         <v>740</v>
       </c>
+      <c r="Q14">
+        <v>117.839</v>
+      </c>
+      <c r="R14">
+        <v>105.361</v>
+      </c>
       <c r="S14">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="T14" t="e">
+        <v>12.477999999999994</v>
+      </c>
+      <c r="T14">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
+        <v>0.10589024007332033</v>
       </c>
       <c r="U14" t="s">
         <v>88</v>
@@ -50513,6 +50627,9 @@
         <f t="shared" si="5"/>
         <v>no</v>
       </c>
+      <c r="W14" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A15">
@@ -50560,13 +50677,19 @@
       <c r="P15">
         <v>740</v>
       </c>
+      <c r="Q15">
+        <v>88.838999999999999</v>
+      </c>
+      <c r="R15">
+        <v>87.475999999999999</v>
+      </c>
       <c r="S15">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="T15" t="e">
+        <v>1.3629999999999995</v>
+      </c>
+      <c r="T15">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
+        <v>1.5342360900055151E-2</v>
       </c>
       <c r="U15" t="s">
         <v>89</v>
@@ -50574,6 +50697,9 @@
       <c r="V15" t="str">
         <f t="shared" si="5"/>
         <v>no</v>
+      </c>
+      <c r="W15" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Afternoon sept 5 update
</commit_message>
<xml_diff>
--- a/data/raw.xlsx
+++ b/data/raw.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/EcosystemRecoveryLab/github/Ritger-Corynactis-urchin-deterrence/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0C7E187-B889-3743-AE86-EE45BBFA6EEB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE8E0985-FD73-FF45-8752-4E7C51C4347B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20520" yWindow="12000" windowWidth="23780" windowHeight="13760" activeTab="1" xr2:uid="{58E670A5-634C-427F-960F-9DA76C64E810}"/>
+    <workbookView xWindow="24900" yWindow="740" windowWidth="23780" windowHeight="25300" activeTab="1" xr2:uid="{58E670A5-634C-427F-960F-9DA76C64E810}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="3" r:id="rId1"/>
@@ -242,9 +242,6 @@
     <t>No video</t>
   </si>
   <si>
-    <t>Double check GoPro - only 4 hours copied to computer</t>
-  </si>
-  <si>
     <t>really fun urchin behavior</t>
   </si>
   <si>
@@ -330,6 +327,9 @@
   </si>
   <si>
     <t>"before" included some holes, "after" includes holes</t>
+  </si>
+  <si>
+    <t>4 hours video</t>
   </si>
 </sst>
 </file>
@@ -49618,9 +49618,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD5E687B-43EE-4B00-8604-7EB9984510DD}">
   <dimension ref="A1:W77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="W8" sqref="W8"/>
+      <selection pane="bottomLeft" activeCell="U48" sqref="U48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -49711,7 +49711,7 @@
         <v>14</v>
       </c>
       <c r="U1" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="V1" s="2" t="s">
         <v>25</v>
@@ -49781,7 +49781,7 @@
         <v>0.10844212089339854</v>
       </c>
       <c r="U2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="V2" t="str">
         <f>IF(E2&gt;6,"no","yes")</f>
@@ -49849,14 +49849,14 @@
         <v>1.3448262101440619E-2</v>
       </c>
       <c r="U3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="V3" t="str">
         <f t="shared" ref="V3:V66" si="5">IF(E3&gt;6,"no","yes")</f>
         <v>yes</v>
       </c>
       <c r="W3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.2">
@@ -49920,7 +49920,7 @@
         <v>0.28380160052328729</v>
       </c>
       <c r="U4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="V4" t="str">
         <f t="shared" si="5"/>
@@ -49988,14 +49988,14 @@
         <v>0.13551978189607605</v>
       </c>
       <c r="U5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="V5" t="str">
         <f t="shared" si="5"/>
         <v>yes</v>
       </c>
       <c r="W5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.2">
@@ -50059,14 +50059,14 @@
         <v>0.25604737440407477</v>
       </c>
       <c r="U6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="V6" t="str">
         <f t="shared" si="5"/>
         <v>yes</v>
       </c>
       <c r="W6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.2">
@@ -50130,14 +50130,14 @@
         <v>0.11223173449044209</v>
       </c>
       <c r="U7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="V7" t="str">
         <f t="shared" si="5"/>
         <v>yes</v>
       </c>
       <c r="W7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.2">
@@ -50201,7 +50201,7 @@
         <v>-2.3323421800214282E-3</v>
       </c>
       <c r="U8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="V8" t="str">
         <f t="shared" si="5"/>
@@ -50269,7 +50269,7 @@
         <v>-5.7143858788059479E-3</v>
       </c>
       <c r="U9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="V9" t="str">
         <f t="shared" si="5"/>
@@ -50337,14 +50337,14 @@
         <v>-5.7725522069621595E-3</v>
       </c>
       <c r="U10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="V10" t="str">
         <f t="shared" si="5"/>
         <v>no</v>
       </c>
       <c r="W10" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.2">
@@ -50408,14 +50408,14 @@
         <v>2.0172553505886835E-2</v>
       </c>
       <c r="U11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="V11" t="str">
         <f t="shared" si="5"/>
         <v>no</v>
       </c>
       <c r="W11" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.2">
@@ -50479,14 +50479,14 @@
         <v>0.23731693570773646</v>
       </c>
       <c r="U12" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="V12" t="str">
         <f t="shared" si="5"/>
         <v>no</v>
       </c>
       <c r="W12" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.2">
@@ -50550,14 +50550,14 @@
         <v>0.21320720819240585</v>
       </c>
       <c r="U13" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="V13" t="str">
         <f t="shared" si="5"/>
         <v>no</v>
       </c>
       <c r="W13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.2">
@@ -50621,14 +50621,14 @@
         <v>0.10589024007332033</v>
       </c>
       <c r="U14" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="V14" t="str">
         <f t="shared" si="5"/>
         <v>no</v>
       </c>
       <c r="W14" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.2">
@@ -50692,14 +50692,14 @@
         <v>1.5342360900055151E-2</v>
       </c>
       <c r="U15" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="V15" t="str">
         <f t="shared" si="5"/>
         <v>no</v>
       </c>
       <c r="W15" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.2">
@@ -50763,7 +50763,7 @@
         <v>1.1132188960347966E-2</v>
       </c>
       <c r="U16" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="V16" t="str">
         <f t="shared" si="5"/>
@@ -50832,14 +50832,14 @@
         <v>0.34767247318177341</v>
       </c>
       <c r="U17" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="V17" t="str">
         <f t="shared" si="5"/>
         <v>yes</v>
       </c>
       <c r="W17" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="18" spans="1:23" x14ac:dyDescent="0.2">
@@ -50903,14 +50903,14 @@
         <v>1.4320708498209772E-2</v>
       </c>
       <c r="U18" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="V18" t="str">
         <f t="shared" si="5"/>
         <v>yes</v>
       </c>
       <c r="W18" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="19" spans="1:23" x14ac:dyDescent="0.2">
@@ -50974,7 +50974,7 @@
         <v>2.0570354813750462E-2</v>
       </c>
       <c r="U19" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="V19" t="str">
         <f t="shared" si="5"/>
@@ -51042,7 +51042,7 @@
         <v>0.19619130289116807</v>
       </c>
       <c r="U20" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="V20" t="str">
         <f t="shared" si="5"/>
@@ -51110,7 +51110,7 @@
         <v>6.3789631285387843E-3</v>
       </c>
       <c r="U21" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="V21" t="str">
         <f t="shared" si="5"/>
@@ -51178,14 +51178,14 @@
         <v>9.8303023234503264E-3</v>
       </c>
       <c r="U22" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="V22" t="str">
         <f t="shared" si="5"/>
         <v>no</v>
       </c>
       <c r="W22" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="23" spans="1:23" x14ac:dyDescent="0.2">
@@ -51249,14 +51249,14 @@
         <v>-1.3759141403399721E-2</v>
       </c>
       <c r="U23" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="V23" t="str">
         <f t="shared" si="5"/>
         <v>no</v>
       </c>
       <c r="W23" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="24" spans="1:23" x14ac:dyDescent="0.2">
@@ -51320,7 +51320,7 @@
         <v>7.2046396683673368E-3</v>
       </c>
       <c r="U24" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="V24" t="str">
         <f t="shared" si="5"/>
@@ -51388,7 +51388,7 @@
         <v>1.6066314050968911E-2</v>
       </c>
       <c r="U25" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="V25" t="str">
         <f t="shared" si="5"/>
@@ -51456,14 +51456,14 @@
         <v>0.104877366588544</v>
       </c>
       <c r="U26" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="V26" t="str">
         <f t="shared" si="5"/>
         <v>no</v>
       </c>
       <c r="W26" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="27" spans="1:23" x14ac:dyDescent="0.2">
@@ -51527,7 +51527,7 @@
         <v>3.2134809444497774E-3</v>
       </c>
       <c r="U27" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="V27" t="str">
         <f t="shared" si="5"/>
@@ -51595,7 +51595,7 @@
         <v>1.712374076244115E-2</v>
       </c>
       <c r="U28" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="V28" t="str">
         <f t="shared" si="5"/>
@@ -51663,7 +51663,7 @@
         <v>3.8196991929567187E-2</v>
       </c>
       <c r="U29" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="V29" t="str">
         <f t="shared" si="5"/>
@@ -51732,7 +51732,7 @@
         <v>0.39414566228714759</v>
       </c>
       <c r="U30" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="V30" t="str">
         <f t="shared" si="5"/>
@@ -51800,7 +51800,7 @@
         <v>0.28625451046427708</v>
       </c>
       <c r="U31" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="V31" t="str">
         <f t="shared" si="5"/>
@@ -51868,7 +51868,7 @@
         <v>0.17109784527483193</v>
       </c>
       <c r="U32" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="V32" t="str">
         <f t="shared" si="5"/>
@@ -51936,7 +51936,7 @@
         <v>-1.4416269790191878E-2</v>
       </c>
       <c r="U33" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="V33" t="str">
         <f t="shared" si="5"/>
@@ -52005,14 +52005,14 @@
         <v>0.32763076777161293</v>
       </c>
       <c r="U34" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="V34" t="str">
         <f t="shared" si="5"/>
         <v>yes</v>
       </c>
       <c r="W34" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="35" spans="1:23" x14ac:dyDescent="0.2">
@@ -52076,14 +52076,14 @@
         <v>1.0624224886316719E-2</v>
       </c>
       <c r="U35" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="V35" t="str">
         <f t="shared" si="5"/>
         <v>yes</v>
       </c>
       <c r="W35" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="36" spans="1:23" x14ac:dyDescent="0.2">
@@ -52147,7 +52147,7 @@
         <v>0.33511229946524063</v>
       </c>
       <c r="U36" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="V36" t="str">
         <f t="shared" si="5"/>
@@ -52215,7 +52215,7 @@
         <v>8.9727722772276596E-3</v>
       </c>
       <c r="U37" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="V37" t="str">
         <f t="shared" si="5"/>
@@ -52283,14 +52283,14 @@
         <v>0.27821013587304089</v>
       </c>
       <c r="U38" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="V38" t="str">
         <f t="shared" si="5"/>
         <v>no</v>
       </c>
       <c r="W38" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="39" spans="1:23" x14ac:dyDescent="0.2">
@@ -52354,7 +52354,7 @@
         <v>0.50121017042193783</v>
       </c>
       <c r="U39" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="V39" t="str">
         <f t="shared" si="5"/>
@@ -52422,7 +52422,7 @@
         <v>0.42735033602940398</v>
       </c>
       <c r="U40" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="V40" t="str">
         <f t="shared" si="5"/>
@@ -52491,7 +52491,7 @@
         <v>0.91152623616800665</v>
       </c>
       <c r="U41" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="V41" t="str">
         <f t="shared" si="5"/>
@@ -52559,7 +52559,7 @@
         <v>7.5201906527207442E-3</v>
       </c>
       <c r="U42" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="V42" t="str">
         <f t="shared" si="5"/>
@@ -52627,14 +52627,14 @@
         <v>1.9049721461127905E-2</v>
       </c>
       <c r="U43" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="V43" t="str">
         <f t="shared" si="5"/>
         <v>no</v>
       </c>
       <c r="W43" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="44" spans="1:23" x14ac:dyDescent="0.2">
@@ -52697,7 +52697,7 @@
         <v>0.82234472298785199</v>
       </c>
       <c r="U44" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="V44" t="str">
         <f t="shared" si="5"/>
@@ -52765,7 +52765,7 @@
         <v>0.11270882385917719</v>
       </c>
       <c r="U45" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="V45" t="str">
         <f t="shared" si="5"/>
@@ -52832,7 +52832,7 @@
         <v>2.2921863412660948E-2</v>
       </c>
       <c r="U46" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="V46" t="str">
         <f t="shared" si="5"/>
@@ -52899,10 +52899,10 @@
         <v>1.4539400665926773E-2</v>
       </c>
       <c r="U47" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="V47" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="48" spans="1:23" x14ac:dyDescent="0.2">
@@ -52965,14 +52965,14 @@
         <v>9.6040347676788936E-3</v>
       </c>
       <c r="U48" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="V48" t="str">
         <f t="shared" si="5"/>
         <v>yes</v>
       </c>
       <c r="W48" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="49" spans="1:23" x14ac:dyDescent="0.2">
@@ -53035,7 +53035,7 @@
         <v>3.0082299064180036E-2</v>
       </c>
       <c r="U49" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="V49" t="str">
         <f t="shared" si="5"/>
@@ -53103,14 +53103,14 @@
         <v>0.21193650793650795</v>
       </c>
       <c r="U50" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="V50" t="str">
         <f t="shared" si="5"/>
         <v>no</v>
       </c>
       <c r="W50" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="51" spans="1:23" x14ac:dyDescent="0.2">
@@ -53173,7 +53173,7 @@
         <v>3.2453875307150791E-2</v>
       </c>
       <c r="U51" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="V51" t="str">
         <f t="shared" si="5"/>
@@ -53241,7 +53241,7 @@
         <v>0.2629165021413602</v>
       </c>
       <c r="U52" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="V52" t="str">
         <f t="shared" si="5"/>
@@ -53308,14 +53308,14 @@
         <v>2.0684577719086196E-3</v>
       </c>
       <c r="U53" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="V53" t="str">
         <f t="shared" si="5"/>
         <v>no</v>
       </c>
       <c r="W53" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="54" spans="1:23" x14ac:dyDescent="0.2">
@@ -53378,14 +53378,14 @@
         <v>0.58087670985508555</v>
       </c>
       <c r="U54" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="V54" t="str">
         <f t="shared" si="5"/>
         <v>no</v>
       </c>
       <c r="W54" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="55" spans="1:23" x14ac:dyDescent="0.2">
@@ -53448,7 +53448,7 @@
         <v>0.10254237288135591</v>
       </c>
       <c r="U55" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="V55" t="str">
         <f t="shared" si="5"/>
@@ -53515,14 +53515,14 @@
         <v>0.20699085648555707</v>
       </c>
       <c r="U56" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="V56" t="str">
         <f t="shared" si="5"/>
         <v>no</v>
       </c>
       <c r="W56" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="57" spans="1:23" x14ac:dyDescent="0.2">
@@ -53586,7 +53586,7 @@
         <v>0.33652352320299794</v>
       </c>
       <c r="U57" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="V57" t="str">
         <f t="shared" si="5"/>
@@ -53654,7 +53654,7 @@
         <v>3.1191515907668613E-4</v>
       </c>
       <c r="U58" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="V58" t="str">
         <f t="shared" si="5"/>
@@ -53723,7 +53723,7 @@
         <v>0.38184980366047527</v>
       </c>
       <c r="U59" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="V59" t="str">
         <f t="shared" si="5"/>
@@ -53791,7 +53791,7 @@
         <v>-4.1907422693503683E-3</v>
       </c>
       <c r="U60" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="V60" t="str">
         <f t="shared" si="5"/>
@@ -53859,7 +53859,7 @@
         <v>1.0433169200028467E-2</v>
       </c>
       <c r="U61" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="V61" t="str">
         <f t="shared" si="5"/>
@@ -53928,7 +53928,7 @@
         <v>0.46034621021486044</v>
       </c>
       <c r="U62" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="V62" t="str">
         <f t="shared" si="5"/>
@@ -53996,14 +53996,14 @@
         <v>0.16790964037909489</v>
       </c>
       <c r="U63" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="V63" t="str">
         <f t="shared" si="5"/>
         <v>no</v>
       </c>
       <c r="W63" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="64" spans="1:23" x14ac:dyDescent="0.2">
@@ -54067,14 +54067,14 @@
         <v>0.27623777988016396</v>
       </c>
       <c r="U64" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="V64" t="str">
         <f t="shared" si="5"/>
         <v>no</v>
       </c>
       <c r="W64" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="65" spans="1:23" x14ac:dyDescent="0.2">
@@ -54138,14 +54138,14 @@
         <v>1.5969444944162442E-2</v>
       </c>
       <c r="U65" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="V65" t="str">
         <f t="shared" si="5"/>
         <v>no</v>
       </c>
       <c r="W65" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="66" spans="1:23" x14ac:dyDescent="0.2">
@@ -54701,8 +54701,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55F6BF2F-CBB2-4331-929A-D3F4AD694052}">
   <dimension ref="A1:AC37"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="AC26" sqref="AC26"/>
+    <sheetView topLeftCell="A17" zoomScale="107" workbookViewId="0">
+      <selection activeCell="R24" sqref="R24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -54780,28 +54780,28 @@
         <v>15</v>
       </c>
       <c r="O1" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q1" s="2" t="s">
         <v>76</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>77</v>
       </c>
       <c r="R1" s="2" t="s">
         <v>17</v>
       </c>
       <c r="S1" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="T1" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="T1" s="2" t="s">
-        <v>79</v>
-      </c>
       <c r="U1" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="V1" s="2" t="s">
         <v>73</v>
-      </c>
-      <c r="V1" s="2" t="s">
-        <v>74</v>
       </c>
       <c r="W1" s="2" t="s">
         <v>18</v>
@@ -55614,7 +55614,7 @@
         <v>1</v>
       </c>
       <c r="AC16" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="17" spans="1:29" x14ac:dyDescent="0.2">
@@ -55978,49 +55978,49 @@
         <v>720</v>
       </c>
       <c r="N23" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="O23" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="P23" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="Q23" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="R23" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="S23" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="T23" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="U23" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="V23" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="W23" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="X23" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="Y23" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="Z23" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="AA23" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="AB23" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="AC23" t="s">
         <v>70</v>
@@ -56078,7 +56078,7 @@
         <v>1</v>
       </c>
       <c r="AC24" t="s">
-        <v>71</v>
+        <v>100</v>
       </c>
     </row>
     <row r="25" spans="1:29" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
balcony temp hobo logger data added
</commit_message>
<xml_diff>
--- a/data/raw.xlsx
+++ b/data/raw.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/EcosystemRecoveryLab/github/Ritger-Corynactis-urchin-deterrence/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE8E0985-FD73-FF45-8752-4E7C51C4347B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BF6C789-1BBE-3D4F-891C-C12AB4D07C35}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24900" yWindow="740" windowWidth="23780" windowHeight="25300" activeTab="1" xr2:uid="{58E670A5-634C-427F-960F-9DA76C64E810}"/>
+    <workbookView xWindow="17680" yWindow="2080" windowWidth="33520" windowHeight="25300" activeTab="2" xr2:uid="{58E670A5-634C-427F-960F-9DA76C64E810}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="3" r:id="rId1"/>
     <sheet name="Kelp consumption" sheetId="1" r:id="rId2"/>
-    <sheet name="Videos" sheetId="2" r:id="rId3"/>
+    <sheet name="Balcony temp" sheetId="4" r:id="rId3"/>
+    <sheet name="Videos" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="102">
   <si>
     <t>Day</t>
   </si>
@@ -296,9 +297,6 @@
     <t>no</t>
   </si>
   <si>
-    <t>maybe no</t>
-  </si>
-  <si>
     <t>NO</t>
   </si>
   <si>
@@ -331,12 +329,21 @@
   <si>
     <t>4 hours video</t>
   </si>
+  <si>
+    <t>Temp, °C</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="h:mm;@"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -351,6 +358,18 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -379,7 +398,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -389,9 +408,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -724,10 +748,10 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="B3" s="9"/>
+      <c r="B3" s="12"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
@@ -893,10 +917,10 @@
       <c r="A24" s="2"/>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25" s="9" t="s">
+      <c r="A25" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="B25" s="9"/>
+      <c r="B25" s="12"/>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
@@ -49618,9 +49642,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD5E687B-43EE-4B00-8604-7EB9984510DD}">
   <dimension ref="A1:W77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="U48" sqref="U48"/>
+      <selection pane="bottomLeft" activeCell="O29" sqref="O29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -49711,7 +49735,7 @@
         <v>14</v>
       </c>
       <c r="U1" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="V1" s="2" t="s">
         <v>25</v>
@@ -49856,7 +49880,7 @@
         <v>yes</v>
       </c>
       <c r="W3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.2">
@@ -49995,7 +50019,7 @@
         <v>yes</v>
       </c>
       <c r="W5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.2">
@@ -50066,7 +50090,7 @@
         <v>yes</v>
       </c>
       <c r="W6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.2">
@@ -50344,7 +50368,7 @@
         <v>no</v>
       </c>
       <c r="W10" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.2">
@@ -50415,7 +50439,7 @@
         <v>no</v>
       </c>
       <c r="W11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.2">
@@ -50486,7 +50510,7 @@
         <v>no</v>
       </c>
       <c r="W12" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.2">
@@ -50557,7 +50581,7 @@
         <v>no</v>
       </c>
       <c r="W13" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.2">
@@ -50628,7 +50652,7 @@
         <v>no</v>
       </c>
       <c r="W14" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.2">
@@ -50699,7 +50723,7 @@
         <v>no</v>
       </c>
       <c r="W15" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.2">
@@ -52902,7 +52926,7 @@
         <v>88</v>
       </c>
       <c r="V47" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="48" spans="1:23" x14ac:dyDescent="0.2">
@@ -52965,7 +52989,7 @@
         <v>9.6040347676788936E-3</v>
       </c>
       <c r="U48" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="V48" t="str">
         <f t="shared" si="5"/>
@@ -53110,7 +53134,7 @@
         <v>no</v>
       </c>
       <c r="W50" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="51" spans="1:23" x14ac:dyDescent="0.2">
@@ -53315,7 +53339,7 @@
         <v>no</v>
       </c>
       <c r="W53" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="54" spans="1:23" x14ac:dyDescent="0.2">
@@ -53385,7 +53409,7 @@
         <v>no</v>
       </c>
       <c r="W54" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="55" spans="1:23" x14ac:dyDescent="0.2">
@@ -53522,7 +53546,7 @@
         <v>no</v>
       </c>
       <c r="W56" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="57" spans="1:23" x14ac:dyDescent="0.2">
@@ -53586,7 +53610,7 @@
         <v>0.33652352320299794</v>
       </c>
       <c r="U57" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="V57" t="str">
         <f t="shared" si="5"/>
@@ -54003,7 +54027,7 @@
         <v>no</v>
       </c>
       <c r="W63" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="64" spans="1:23" x14ac:dyDescent="0.2">
@@ -54074,7 +54098,7 @@
         <v>no</v>
       </c>
       <c r="W64" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="65" spans="1:23" x14ac:dyDescent="0.2">
@@ -54145,7 +54169,7 @@
         <v>no</v>
       </c>
       <c r="W65" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="66" spans="1:23" x14ac:dyDescent="0.2">
@@ -54698,6 +54722,4323 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD361DC7-8609-2B43-BAD7-7A02AAE3248D}">
+  <dimension ref="A1:C391"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="7.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.6640625" style="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="C1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="11">
+        <v>43708</v>
+      </c>
+      <c r="B2" s="13">
+        <v>0.80309027777777775</v>
+      </c>
+      <c r="C2" s="10">
+        <v>17.690000000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="11">
+        <v>43708</v>
+      </c>
+      <c r="B3" s="13">
+        <v>0.81003472222222228</v>
+      </c>
+      <c r="C3" s="10">
+        <v>16.59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="11">
+        <v>43708</v>
+      </c>
+      <c r="B4" s="13">
+        <v>0.8169791666666667</v>
+      </c>
+      <c r="C4" s="10">
+        <v>16.260000000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="11">
+        <v>43708</v>
+      </c>
+      <c r="B5" s="13">
+        <v>0.82392361111111112</v>
+      </c>
+      <c r="C5" s="10">
+        <v>16.12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="11">
+        <v>43708</v>
+      </c>
+      <c r="B6" s="13">
+        <v>0.83086805555555554</v>
+      </c>
+      <c r="C6" s="10">
+        <v>16.079999999999998</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="11">
+        <v>43708</v>
+      </c>
+      <c r="B7" s="13">
+        <v>0.83781250000000007</v>
+      </c>
+      <c r="C7" s="10">
+        <v>16.04</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="11">
+        <v>43708</v>
+      </c>
+      <c r="B8" s="13">
+        <v>0.84475694444444438</v>
+      </c>
+      <c r="C8" s="10">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="11">
+        <v>43708</v>
+      </c>
+      <c r="B9" s="13">
+        <v>0.85170138888888891</v>
+      </c>
+      <c r="C9" s="10">
+        <v>15.95</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="11">
+        <v>43708</v>
+      </c>
+      <c r="B10" s="13">
+        <v>0.85864583333333344</v>
+      </c>
+      <c r="C10" s="10">
+        <v>15.9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="11">
+        <v>43708</v>
+      </c>
+      <c r="B11" s="13">
+        <v>0.86559027777777775</v>
+      </c>
+      <c r="C11" s="10">
+        <v>15.92</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="11">
+        <v>43708</v>
+      </c>
+      <c r="B12" s="13">
+        <v>0.87253472222222228</v>
+      </c>
+      <c r="C12" s="10">
+        <v>15.95</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="11">
+        <v>43708</v>
+      </c>
+      <c r="B13" s="13">
+        <v>0.8794791666666667</v>
+      </c>
+      <c r="C13" s="10">
+        <v>15.9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="11">
+        <v>43708</v>
+      </c>
+      <c r="B14" s="13">
+        <v>0.88642361111111112</v>
+      </c>
+      <c r="C14" s="10">
+        <v>15.95</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" s="11">
+        <v>43708</v>
+      </c>
+      <c r="B15" s="13">
+        <v>0.89336805555555554</v>
+      </c>
+      <c r="C15" s="10">
+        <v>15.93</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" s="11">
+        <v>43708</v>
+      </c>
+      <c r="B16" s="13">
+        <v>0.90031250000000007</v>
+      </c>
+      <c r="C16" s="10">
+        <v>15.95</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="11">
+        <v>43708</v>
+      </c>
+      <c r="B17" s="13">
+        <v>0.90725694444444438</v>
+      </c>
+      <c r="C17" s="10">
+        <v>16.03</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="11">
+        <v>43708</v>
+      </c>
+      <c r="B18" s="13">
+        <v>0.91420138888888891</v>
+      </c>
+      <c r="C18" s="10">
+        <v>15.98</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" s="11">
+        <v>43708</v>
+      </c>
+      <c r="B19" s="13">
+        <v>0.92114583333333344</v>
+      </c>
+      <c r="C19" s="10">
+        <v>16.059999999999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="11">
+        <v>43708</v>
+      </c>
+      <c r="B20" s="13">
+        <v>0.92809027777777775</v>
+      </c>
+      <c r="C20" s="10">
+        <v>15.99</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" s="11">
+        <v>43708</v>
+      </c>
+      <c r="B21" s="13">
+        <v>0.93503472222222228</v>
+      </c>
+      <c r="C21" s="10">
+        <v>16.07</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" s="11">
+        <v>43708</v>
+      </c>
+      <c r="B22" s="13">
+        <v>0.9419791666666667</v>
+      </c>
+      <c r="C22" s="10">
+        <v>15.99</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" s="11">
+        <v>43708</v>
+      </c>
+      <c r="B23" s="13">
+        <v>0.94892361111111112</v>
+      </c>
+      <c r="C23" s="10">
+        <v>15.97</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" s="11">
+        <v>43708</v>
+      </c>
+      <c r="B24" s="13">
+        <v>0.95586805555555554</v>
+      </c>
+      <c r="C24" s="10">
+        <v>15.91</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" s="11">
+        <v>43708</v>
+      </c>
+      <c r="B25" s="13">
+        <v>0.96281250000000007</v>
+      </c>
+      <c r="C25" s="10">
+        <v>15.93</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" s="11">
+        <v>43708</v>
+      </c>
+      <c r="B26" s="13">
+        <v>0.96975694444444438</v>
+      </c>
+      <c r="C26" s="10">
+        <v>15.96</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" s="11">
+        <v>43708</v>
+      </c>
+      <c r="B27" s="13">
+        <v>0.97670138888888891</v>
+      </c>
+      <c r="C27" s="10">
+        <v>15.96</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" s="11">
+        <v>43708</v>
+      </c>
+      <c r="B28" s="13">
+        <v>0.98364583333333344</v>
+      </c>
+      <c r="C28" s="10">
+        <v>15.95</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" s="11">
+        <v>43708</v>
+      </c>
+      <c r="B29" s="13">
+        <v>0.99059027777777775</v>
+      </c>
+      <c r="C29" s="10">
+        <v>15.89</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" s="11">
+        <v>43708</v>
+      </c>
+      <c r="B30" s="13">
+        <v>0.99753472222222228</v>
+      </c>
+      <c r="C30" s="10">
+        <v>15.9</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" s="11">
+        <v>43709</v>
+      </c>
+      <c r="B31" s="13">
+        <v>4.4791666666666669E-3</v>
+      </c>
+      <c r="C31" s="10">
+        <v>15.86</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" s="11">
+        <v>43709</v>
+      </c>
+      <c r="B32" s="13">
+        <v>1.1423611111111112E-2</v>
+      </c>
+      <c r="C32" s="10">
+        <v>15.82</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" s="11">
+        <v>43709</v>
+      </c>
+      <c r="B33" s="13">
+        <v>1.8368055555555554E-2</v>
+      </c>
+      <c r="C33" s="10">
+        <v>15.86</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" s="11">
+        <v>43709</v>
+      </c>
+      <c r="B34" s="13">
+        <v>2.5312500000000002E-2</v>
+      </c>
+      <c r="C34" s="10">
+        <v>15.9</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" s="11">
+        <v>43709</v>
+      </c>
+      <c r="B35" s="13">
+        <v>3.2256944444444442E-2</v>
+      </c>
+      <c r="C35" s="10">
+        <v>15.95</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" s="11">
+        <v>43709</v>
+      </c>
+      <c r="B36" s="13">
+        <v>3.920138888888889E-2</v>
+      </c>
+      <c r="C36" s="10">
+        <v>15.9</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37" s="11">
+        <v>43709</v>
+      </c>
+      <c r="B37" s="13">
+        <v>4.614583333333333E-2</v>
+      </c>
+      <c r="C37" s="10">
+        <v>15.91</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38" s="11">
+        <v>43709</v>
+      </c>
+      <c r="B38" s="13">
+        <v>5.3090277777777778E-2</v>
+      </c>
+      <c r="C38" s="10">
+        <v>15.86</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39" s="11">
+        <v>43709</v>
+      </c>
+      <c r="B39" s="13">
+        <v>6.0034722222222225E-2</v>
+      </c>
+      <c r="C39" s="10">
+        <v>15.85</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40" s="11">
+        <v>43709</v>
+      </c>
+      <c r="B40" s="13">
+        <v>6.6979166666666659E-2</v>
+      </c>
+      <c r="C40" s="10">
+        <v>15.76</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41" s="11">
+        <v>43709</v>
+      </c>
+      <c r="B41" s="13">
+        <v>7.3923611111111107E-2</v>
+      </c>
+      <c r="C41" s="10">
+        <v>15.76</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42" s="11">
+        <v>43709</v>
+      </c>
+      <c r="B42" s="13">
+        <v>8.0868055555555554E-2</v>
+      </c>
+      <c r="C42" s="10">
+        <v>15.72</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43" s="11">
+        <v>43709</v>
+      </c>
+      <c r="B43" s="13">
+        <v>8.7812500000000002E-2</v>
+      </c>
+      <c r="C43" s="10">
+        <v>15.69</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44" s="11">
+        <v>43709</v>
+      </c>
+      <c r="B44" s="13">
+        <v>9.4756944444444449E-2</v>
+      </c>
+      <c r="C44" s="10">
+        <v>15.67</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A45" s="11">
+        <v>43709</v>
+      </c>
+      <c r="B45" s="13">
+        <v>0.1017013888888889</v>
+      </c>
+      <c r="C45" s="10">
+        <v>15.59</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46" s="11">
+        <v>43709</v>
+      </c>
+      <c r="B46" s="13">
+        <v>0.10864583333333333</v>
+      </c>
+      <c r="C46" s="10">
+        <v>15.57</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A47" s="11">
+        <v>43709</v>
+      </c>
+      <c r="B47" s="13">
+        <v>0.11559027777777779</v>
+      </c>
+      <c r="C47" s="10">
+        <v>15.55</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A48" s="11">
+        <v>43709</v>
+      </c>
+      <c r="B48" s="13">
+        <v>0.12253472222222223</v>
+      </c>
+      <c r="C48" s="10">
+        <v>15.55</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A49" s="11">
+        <v>43709</v>
+      </c>
+      <c r="B49" s="13">
+        <v>0.12947916666666667</v>
+      </c>
+      <c r="C49" s="10">
+        <v>15.53</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A50" s="11">
+        <v>43709</v>
+      </c>
+      <c r="B50" s="13">
+        <v>0.13642361111111112</v>
+      </c>
+      <c r="C50" s="10">
+        <v>15.58</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A51" s="11">
+        <v>43709</v>
+      </c>
+      <c r="B51" s="13">
+        <v>0.14336805555555557</v>
+      </c>
+      <c r="C51" s="10">
+        <v>15.57</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A52" s="11">
+        <v>43709</v>
+      </c>
+      <c r="B52" s="13">
+        <v>0.15031249999999999</v>
+      </c>
+      <c r="C52" s="10">
+        <v>15.56</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A53" s="11">
+        <v>43709</v>
+      </c>
+      <c r="B53" s="13">
+        <v>0.15725694444444446</v>
+      </c>
+      <c r="C53" s="10">
+        <v>15.54</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A54" s="11">
+        <v>43709</v>
+      </c>
+      <c r="B54" s="13">
+        <v>0.16420138888888888</v>
+      </c>
+      <c r="C54" s="10">
+        <v>15.51</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A55" s="11">
+        <v>43709</v>
+      </c>
+      <c r="B55" s="13">
+        <v>0.17114583333333333</v>
+      </c>
+      <c r="C55" s="10">
+        <v>15.49</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A56" s="11">
+        <v>43709</v>
+      </c>
+      <c r="B56" s="13">
+        <v>0.17809027777777778</v>
+      </c>
+      <c r="C56" s="10">
+        <v>15.52</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A57" s="11">
+        <v>43709</v>
+      </c>
+      <c r="B57" s="13">
+        <v>0.1850347222222222</v>
+      </c>
+      <c r="C57" s="10">
+        <v>15.53</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A58" s="11">
+        <v>43709</v>
+      </c>
+      <c r="B58" s="13">
+        <v>0.19197916666666667</v>
+      </c>
+      <c r="C58" s="10">
+        <v>15.58</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A59" s="11">
+        <v>43709</v>
+      </c>
+      <c r="B59" s="13">
+        <v>0.19892361111111112</v>
+      </c>
+      <c r="C59" s="10">
+        <v>15.57</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A60" s="11">
+        <v>43709</v>
+      </c>
+      <c r="B60" s="13">
+        <v>0.20586805555555557</v>
+      </c>
+      <c r="C60" s="10">
+        <v>15.49</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A61" s="11">
+        <v>43709</v>
+      </c>
+      <c r="B61" s="13">
+        <v>0.21281249999999999</v>
+      </c>
+      <c r="C61" s="10">
+        <v>15.45</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A62" s="11">
+        <v>43709</v>
+      </c>
+      <c r="B62" s="13">
+        <v>0.21975694444444446</v>
+      </c>
+      <c r="C62" s="10">
+        <v>15.4</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A63" s="11">
+        <v>43709</v>
+      </c>
+      <c r="B63" s="13">
+        <v>0.22670138888888888</v>
+      </c>
+      <c r="C63" s="10">
+        <v>15.33</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A64" s="11">
+        <v>43709</v>
+      </c>
+      <c r="B64" s="13">
+        <v>0.23364583333333333</v>
+      </c>
+      <c r="C64" s="10">
+        <v>15.32</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A65" s="11">
+        <v>43709</v>
+      </c>
+      <c r="B65" s="13">
+        <v>0.24059027777777778</v>
+      </c>
+      <c r="C65" s="10">
+        <v>15.36</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A66" s="11">
+        <v>43709</v>
+      </c>
+      <c r="B66" s="13">
+        <v>0.24753472222222225</v>
+      </c>
+      <c r="C66" s="10">
+        <v>15.32</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A67" s="11">
+        <v>43709</v>
+      </c>
+      <c r="B67" s="13">
+        <v>0.25447916666666665</v>
+      </c>
+      <c r="C67" s="10">
+        <v>15.31</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A68" s="11">
+        <v>43709</v>
+      </c>
+      <c r="B68" s="13">
+        <v>0.26142361111111112</v>
+      </c>
+      <c r="C68" s="10">
+        <v>15.36</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A69" s="11">
+        <v>43709</v>
+      </c>
+      <c r="B69" s="13">
+        <v>0.26836805555555554</v>
+      </c>
+      <c r="C69" s="10">
+        <v>15.32</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A70" s="11">
+        <v>43709</v>
+      </c>
+      <c r="B70" s="13">
+        <v>0.27531250000000002</v>
+      </c>
+      <c r="C70" s="10">
+        <v>15.25</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A71" s="11">
+        <v>43709</v>
+      </c>
+      <c r="B71" s="13">
+        <v>0.28225694444444444</v>
+      </c>
+      <c r="C71" s="10">
+        <v>15.23</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A72" s="11">
+        <v>43709</v>
+      </c>
+      <c r="B72" s="13">
+        <v>0.28920138888888891</v>
+      </c>
+      <c r="C72" s="10">
+        <v>15.22</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A73" s="11">
+        <v>43709</v>
+      </c>
+      <c r="B73" s="13">
+        <v>0.29614583333333333</v>
+      </c>
+      <c r="C73" s="10">
+        <v>15.19</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A74" s="11">
+        <v>43709</v>
+      </c>
+      <c r="B74" s="13">
+        <v>0.30309027777777781</v>
+      </c>
+      <c r="C74" s="10">
+        <v>15.31</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A75" s="11">
+        <v>43709</v>
+      </c>
+      <c r="B75" s="13">
+        <v>0.31003472222222223</v>
+      </c>
+      <c r="C75" s="10">
+        <v>15.44</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A76" s="11">
+        <v>43709</v>
+      </c>
+      <c r="B76" s="13">
+        <v>0.31697916666666665</v>
+      </c>
+      <c r="C76" s="10">
+        <v>15.47</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A77" s="11">
+        <v>43709</v>
+      </c>
+      <c r="B77" s="13">
+        <v>0.32392361111111112</v>
+      </c>
+      <c r="C77" s="10">
+        <v>15.54</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A78" s="11">
+        <v>43709</v>
+      </c>
+      <c r="B78" s="13">
+        <v>0.3308680555555556</v>
+      </c>
+      <c r="C78" s="10">
+        <v>15.63</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A79" s="11">
+        <v>43709</v>
+      </c>
+      <c r="B79" s="13">
+        <v>0.79614583333333344</v>
+      </c>
+      <c r="C79" s="10">
+        <v>15.84</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A80" s="11">
+        <v>43709</v>
+      </c>
+      <c r="B80" s="13">
+        <v>0.80309027777777775</v>
+      </c>
+      <c r="C80" s="10">
+        <v>15.74</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A81" s="11">
+        <v>43709</v>
+      </c>
+      <c r="B81" s="13">
+        <v>0.81003472222222228</v>
+      </c>
+      <c r="C81" s="10">
+        <v>15.66</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A82" s="11">
+        <v>43709</v>
+      </c>
+      <c r="B82" s="13">
+        <v>0.8169791666666667</v>
+      </c>
+      <c r="C82" s="10">
+        <v>15.58</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A83" s="11">
+        <v>43709</v>
+      </c>
+      <c r="B83" s="13">
+        <v>0.82392361111111112</v>
+      </c>
+      <c r="C83" s="10">
+        <v>15.53</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A84" s="11">
+        <v>43709</v>
+      </c>
+      <c r="B84" s="13">
+        <v>0.83086805555555554</v>
+      </c>
+      <c r="C84" s="10">
+        <v>15.45</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A85" s="11">
+        <v>43709</v>
+      </c>
+      <c r="B85" s="13">
+        <v>0.83781250000000007</v>
+      </c>
+      <c r="C85" s="10">
+        <v>15.44</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A86" s="11">
+        <v>43709</v>
+      </c>
+      <c r="B86" s="13">
+        <v>0.84475694444444438</v>
+      </c>
+      <c r="C86" s="10">
+        <v>15.39</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A87" s="11">
+        <v>43709</v>
+      </c>
+      <c r="B87" s="13">
+        <v>0.85170138888888891</v>
+      </c>
+      <c r="C87" s="10">
+        <v>15.32</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A88" s="11">
+        <v>43709</v>
+      </c>
+      <c r="B88" s="13">
+        <v>0.85864583333333344</v>
+      </c>
+      <c r="C88" s="10">
+        <v>15.28</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A89" s="11">
+        <v>43709</v>
+      </c>
+      <c r="B89" s="13">
+        <v>0.86559027777777775</v>
+      </c>
+      <c r="C89" s="10">
+        <v>15.25</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A90" s="11">
+        <v>43709</v>
+      </c>
+      <c r="B90" s="13">
+        <v>0.87253472222222228</v>
+      </c>
+      <c r="C90" s="10">
+        <v>15.19</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A91" s="11">
+        <v>43709</v>
+      </c>
+      <c r="B91" s="13">
+        <v>0.8794791666666667</v>
+      </c>
+      <c r="C91" s="10">
+        <v>15.17</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A92" s="11">
+        <v>43709</v>
+      </c>
+      <c r="B92" s="13">
+        <v>0.88642361111111112</v>
+      </c>
+      <c r="C92" s="10">
+        <v>15.15</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A93" s="11">
+        <v>43709</v>
+      </c>
+      <c r="B93" s="13">
+        <v>0.89336805555555554</v>
+      </c>
+      <c r="C93" s="10">
+        <v>15.18</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A94" s="11">
+        <v>43709</v>
+      </c>
+      <c r="B94" s="13">
+        <v>0.90031250000000007</v>
+      </c>
+      <c r="C94" s="10">
+        <v>15.18</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A95" s="11">
+        <v>43709</v>
+      </c>
+      <c r="B95" s="13">
+        <v>0.90725694444444438</v>
+      </c>
+      <c r="C95" s="10">
+        <v>15.19</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A96" s="11">
+        <v>43709</v>
+      </c>
+      <c r="B96" s="13">
+        <v>0.91420138888888891</v>
+      </c>
+      <c r="C96" s="10">
+        <v>15.19</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A97" s="11">
+        <v>43709</v>
+      </c>
+      <c r="B97" s="13">
+        <v>0.92114583333333344</v>
+      </c>
+      <c r="C97" s="10">
+        <v>15.19</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A98" s="11">
+        <v>43709</v>
+      </c>
+      <c r="B98" s="13">
+        <v>0.92809027777777775</v>
+      </c>
+      <c r="C98" s="10">
+        <v>15.18</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A99" s="11">
+        <v>43709</v>
+      </c>
+      <c r="B99" s="13">
+        <v>0.93503472222222228</v>
+      </c>
+      <c r="C99" s="10">
+        <v>15.19</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A100" s="11">
+        <v>43709</v>
+      </c>
+      <c r="B100" s="13">
+        <v>0.9419791666666667</v>
+      </c>
+      <c r="C100" s="10">
+        <v>15.19</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A101" s="11">
+        <v>43709</v>
+      </c>
+      <c r="B101" s="13">
+        <v>0.94892361111111112</v>
+      </c>
+      <c r="C101" s="10">
+        <v>15.21</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A102" s="11">
+        <v>43709</v>
+      </c>
+      <c r="B102" s="13">
+        <v>0.95586805555555554</v>
+      </c>
+      <c r="C102" s="10">
+        <v>15.22</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A103" s="11">
+        <v>43709</v>
+      </c>
+      <c r="B103" s="13">
+        <v>0.96281250000000007</v>
+      </c>
+      <c r="C103" s="10">
+        <v>15.21</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A104" s="11">
+        <v>43709</v>
+      </c>
+      <c r="B104" s="13">
+        <v>0.96975694444444438</v>
+      </c>
+      <c r="C104" s="10">
+        <v>15.21</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A105" s="11">
+        <v>43709</v>
+      </c>
+      <c r="B105" s="13">
+        <v>0.97670138888888891</v>
+      </c>
+      <c r="C105" s="10">
+        <v>15.19</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A106" s="11">
+        <v>43709</v>
+      </c>
+      <c r="B106" s="13">
+        <v>0.98364583333333344</v>
+      </c>
+      <c r="C106" s="10">
+        <v>15.26</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A107" s="11">
+        <v>43709</v>
+      </c>
+      <c r="B107" s="13">
+        <v>0.99059027777777775</v>
+      </c>
+      <c r="C107" s="10">
+        <v>15.31</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A108" s="11">
+        <v>43709</v>
+      </c>
+      <c r="B108" s="13">
+        <v>0.99753472222222228</v>
+      </c>
+      <c r="C108" s="10">
+        <v>15.32</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A109" s="11">
+        <v>43710</v>
+      </c>
+      <c r="B109" s="13">
+        <v>4.4791666666666669E-3</v>
+      </c>
+      <c r="C109" s="10">
+        <v>15.38</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A110" s="11">
+        <v>43710</v>
+      </c>
+      <c r="B110" s="13">
+        <v>1.1423611111111112E-2</v>
+      </c>
+      <c r="C110" s="10">
+        <v>15.42</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A111" s="11">
+        <v>43710</v>
+      </c>
+      <c r="B111" s="13">
+        <v>1.8368055555555554E-2</v>
+      </c>
+      <c r="C111" s="10">
+        <v>15.44</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A112" s="11">
+        <v>43710</v>
+      </c>
+      <c r="B112" s="13">
+        <v>2.5312500000000002E-2</v>
+      </c>
+      <c r="C112" s="10">
+        <v>15.47</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A113" s="11">
+        <v>43710</v>
+      </c>
+      <c r="B113" s="13">
+        <v>3.2256944444444442E-2</v>
+      </c>
+      <c r="C113" s="10">
+        <v>15.48</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A114" s="11">
+        <v>43710</v>
+      </c>
+      <c r="B114" s="13">
+        <v>3.920138888888889E-2</v>
+      </c>
+      <c r="C114" s="10">
+        <v>15.51</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A115" s="11">
+        <v>43710</v>
+      </c>
+      <c r="B115" s="13">
+        <v>4.614583333333333E-2</v>
+      </c>
+      <c r="C115" s="10">
+        <v>15.56</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A116" s="11">
+        <v>43710</v>
+      </c>
+      <c r="B116" s="13">
+        <v>5.3090277777777778E-2</v>
+      </c>
+      <c r="C116" s="10">
+        <v>15.56</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A117" s="11">
+        <v>43710</v>
+      </c>
+      <c r="B117" s="13">
+        <v>6.0034722222222225E-2</v>
+      </c>
+      <c r="C117" s="10">
+        <v>15.52</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A118" s="11">
+        <v>43710</v>
+      </c>
+      <c r="B118" s="13">
+        <v>6.6979166666666659E-2</v>
+      </c>
+      <c r="C118" s="10">
+        <v>15.48</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A119" s="11">
+        <v>43710</v>
+      </c>
+      <c r="B119" s="13">
+        <v>7.3923611111111107E-2</v>
+      </c>
+      <c r="C119" s="10">
+        <v>15.43</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A120" s="11">
+        <v>43710</v>
+      </c>
+      <c r="B120" s="13">
+        <v>8.0868055555555554E-2</v>
+      </c>
+      <c r="C120" s="10">
+        <v>15.43</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A121" s="11">
+        <v>43710</v>
+      </c>
+      <c r="B121" s="13">
+        <v>8.7812500000000002E-2</v>
+      </c>
+      <c r="C121" s="10">
+        <v>15.43</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A122" s="11">
+        <v>43710</v>
+      </c>
+      <c r="B122" s="13">
+        <v>9.4756944444444449E-2</v>
+      </c>
+      <c r="C122" s="10">
+        <v>15.43</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A123" s="11">
+        <v>43710</v>
+      </c>
+      <c r="B123" s="13">
+        <v>0.1017013888888889</v>
+      </c>
+      <c r="C123" s="10">
+        <v>15.43</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A124" s="11">
+        <v>43710</v>
+      </c>
+      <c r="B124" s="13">
+        <v>0.10864583333333333</v>
+      </c>
+      <c r="C124" s="10">
+        <v>15.42</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A125" s="11">
+        <v>43710</v>
+      </c>
+      <c r="B125" s="13">
+        <v>0.11559027777777779</v>
+      </c>
+      <c r="C125" s="10">
+        <v>15.47</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A126" s="11">
+        <v>43710</v>
+      </c>
+      <c r="B126" s="13">
+        <v>0.12253472222222223</v>
+      </c>
+      <c r="C126" s="10">
+        <v>15.49</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A127" s="11">
+        <v>43710</v>
+      </c>
+      <c r="B127" s="13">
+        <v>0.12947916666666667</v>
+      </c>
+      <c r="C127" s="10">
+        <v>15.49</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A128" s="11">
+        <v>43710</v>
+      </c>
+      <c r="B128" s="13">
+        <v>0.13642361111111112</v>
+      </c>
+      <c r="C128" s="10">
+        <v>15.47</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A129" s="11">
+        <v>43710</v>
+      </c>
+      <c r="B129" s="13">
+        <v>0.14336805555555557</v>
+      </c>
+      <c r="C129" s="10">
+        <v>15.46</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A130" s="11">
+        <v>43710</v>
+      </c>
+      <c r="B130" s="13">
+        <v>0.15031249999999999</v>
+      </c>
+      <c r="C130" s="10">
+        <v>15.48</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A131" s="11">
+        <v>43710</v>
+      </c>
+      <c r="B131" s="13">
+        <v>0.15725694444444446</v>
+      </c>
+      <c r="C131" s="10">
+        <v>15.46</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A132" s="11">
+        <v>43710</v>
+      </c>
+      <c r="B132" s="13">
+        <v>0.16420138888888888</v>
+      </c>
+      <c r="C132" s="10">
+        <v>15.44</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A133" s="11">
+        <v>43710</v>
+      </c>
+      <c r="B133" s="13">
+        <v>0.17114583333333333</v>
+      </c>
+      <c r="C133" s="10">
+        <v>15.45</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A134" s="11">
+        <v>43710</v>
+      </c>
+      <c r="B134" s="13">
+        <v>0.17809027777777778</v>
+      </c>
+      <c r="C134" s="10">
+        <v>15.44</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A135" s="11">
+        <v>43710</v>
+      </c>
+      <c r="B135" s="13">
+        <v>0.1850347222222222</v>
+      </c>
+      <c r="C135" s="10">
+        <v>15.45</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A136" s="11">
+        <v>43710</v>
+      </c>
+      <c r="B136" s="13">
+        <v>0.19197916666666667</v>
+      </c>
+      <c r="C136" s="10">
+        <v>15.45</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A137" s="11">
+        <v>43710</v>
+      </c>
+      <c r="B137" s="13">
+        <v>0.19892361111111112</v>
+      </c>
+      <c r="C137" s="10">
+        <v>15.48</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A138" s="11">
+        <v>43710</v>
+      </c>
+      <c r="B138" s="13">
+        <v>0.20586805555555557</v>
+      </c>
+      <c r="C138" s="10">
+        <v>15.61</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A139" s="11">
+        <v>43710</v>
+      </c>
+      <c r="B139" s="13">
+        <v>0.21281249999999999</v>
+      </c>
+      <c r="C139" s="10">
+        <v>15.67</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A140" s="11">
+        <v>43710</v>
+      </c>
+      <c r="B140" s="13">
+        <v>0.21975694444444446</v>
+      </c>
+      <c r="C140" s="10">
+        <v>15.68</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A141" s="11">
+        <v>43710</v>
+      </c>
+      <c r="B141" s="13">
+        <v>0.22670138888888888</v>
+      </c>
+      <c r="C141" s="10">
+        <v>15.66</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A142" s="11">
+        <v>43710</v>
+      </c>
+      <c r="B142" s="13">
+        <v>0.23364583333333333</v>
+      </c>
+      <c r="C142" s="10">
+        <v>15.66</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A143" s="11">
+        <v>43710</v>
+      </c>
+      <c r="B143" s="13">
+        <v>0.24059027777777778</v>
+      </c>
+      <c r="C143" s="10">
+        <v>15.63</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A144" s="11">
+        <v>43710</v>
+      </c>
+      <c r="B144" s="13">
+        <v>0.24753472222222225</v>
+      </c>
+      <c r="C144" s="10">
+        <v>15.59</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A145" s="11">
+        <v>43710</v>
+      </c>
+      <c r="B145" s="13">
+        <v>0.25447916666666665</v>
+      </c>
+      <c r="C145" s="10">
+        <v>15.57</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A146" s="11">
+        <v>43710</v>
+      </c>
+      <c r="B146" s="13">
+        <v>0.26142361111111112</v>
+      </c>
+      <c r="C146" s="10">
+        <v>15.6</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A147" s="11">
+        <v>43710</v>
+      </c>
+      <c r="B147" s="13">
+        <v>0.26836805555555554</v>
+      </c>
+      <c r="C147" s="10">
+        <v>15.58</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A148" s="11">
+        <v>43710</v>
+      </c>
+      <c r="B148" s="13">
+        <v>0.27531250000000002</v>
+      </c>
+      <c r="C148" s="10">
+        <v>15.54</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A149" s="11">
+        <v>43710</v>
+      </c>
+      <c r="B149" s="13">
+        <v>0.28225694444444444</v>
+      </c>
+      <c r="C149" s="10">
+        <v>15.54</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A150" s="11">
+        <v>43710</v>
+      </c>
+      <c r="B150" s="13">
+        <v>0.28920138888888891</v>
+      </c>
+      <c r="C150" s="10">
+        <v>15.52</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A151" s="11">
+        <v>43710</v>
+      </c>
+      <c r="B151" s="13">
+        <v>0.29614583333333333</v>
+      </c>
+      <c r="C151" s="10">
+        <v>15.52</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A152" s="11">
+        <v>43710</v>
+      </c>
+      <c r="B152" s="13">
+        <v>0.30309027777777781</v>
+      </c>
+      <c r="C152" s="10">
+        <v>15.56</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A153" s="11">
+        <v>43710</v>
+      </c>
+      <c r="B153" s="13">
+        <v>0.31003472222222223</v>
+      </c>
+      <c r="C153" s="10">
+        <v>15.59</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A154" s="11">
+        <v>43710</v>
+      </c>
+      <c r="B154" s="13">
+        <v>0.31697916666666665</v>
+      </c>
+      <c r="C154" s="10">
+        <v>15.32</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A155" s="11">
+        <v>43710</v>
+      </c>
+      <c r="B155" s="13">
+        <v>0.32392361111111112</v>
+      </c>
+      <c r="C155" s="10">
+        <v>15.31</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A156" s="11">
+        <v>43710</v>
+      </c>
+      <c r="B156" s="13">
+        <v>0.3308680555555556</v>
+      </c>
+      <c r="C156" s="10">
+        <v>15.32</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A157" s="11">
+        <v>43710</v>
+      </c>
+      <c r="B157" s="13">
+        <v>0.79614583333333344</v>
+      </c>
+      <c r="C157" s="10">
+        <v>16.010000000000002</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A158" s="11">
+        <v>43710</v>
+      </c>
+      <c r="B158" s="13">
+        <v>0.80309027777777775</v>
+      </c>
+      <c r="C158" s="10">
+        <v>15.97</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A159" s="11">
+        <v>43710</v>
+      </c>
+      <c r="B159" s="13">
+        <v>0.81003472222222228</v>
+      </c>
+      <c r="C159" s="10">
+        <v>15.92</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A160" s="11">
+        <v>43710</v>
+      </c>
+      <c r="B160" s="13">
+        <v>0.8169791666666667</v>
+      </c>
+      <c r="C160" s="10">
+        <v>15.89</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A161" s="11">
+        <v>43710</v>
+      </c>
+      <c r="B161" s="13">
+        <v>0.82392361111111112</v>
+      </c>
+      <c r="C161" s="10">
+        <v>15.89</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A162" s="11">
+        <v>43710</v>
+      </c>
+      <c r="B162" s="13">
+        <v>0.83086805555555554</v>
+      </c>
+      <c r="C162" s="10">
+        <v>15.8</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A163" s="11">
+        <v>43710</v>
+      </c>
+      <c r="B163" s="13">
+        <v>0.83781250000000007</v>
+      </c>
+      <c r="C163" s="10">
+        <v>15.71</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A164" s="11">
+        <v>43710</v>
+      </c>
+      <c r="B164" s="13">
+        <v>0.84475694444444438</v>
+      </c>
+      <c r="C164" s="10">
+        <v>15.72</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A165" s="11">
+        <v>43710</v>
+      </c>
+      <c r="B165" s="13">
+        <v>0.85170138888888891</v>
+      </c>
+      <c r="C165" s="10">
+        <v>15.7</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A166" s="11">
+        <v>43710</v>
+      </c>
+      <c r="B166" s="13">
+        <v>0.85864583333333344</v>
+      </c>
+      <c r="C166" s="10">
+        <v>15.69</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A167" s="11">
+        <v>43710</v>
+      </c>
+      <c r="B167" s="13">
+        <v>0.86559027777777775</v>
+      </c>
+      <c r="C167" s="10">
+        <v>15.68</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A168" s="11">
+        <v>43710</v>
+      </c>
+      <c r="B168" s="13">
+        <v>0.87253472222222228</v>
+      </c>
+      <c r="C168" s="10">
+        <v>15.67</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A169" s="11">
+        <v>43710</v>
+      </c>
+      <c r="B169" s="13">
+        <v>0.8794791666666667</v>
+      </c>
+      <c r="C169" s="10">
+        <v>15.65</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A170" s="11">
+        <v>43710</v>
+      </c>
+      <c r="B170" s="13">
+        <v>0.88642361111111112</v>
+      </c>
+      <c r="C170" s="10">
+        <v>15.65</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A171" s="11">
+        <v>43710</v>
+      </c>
+      <c r="B171" s="13">
+        <v>0.89336805555555554</v>
+      </c>
+      <c r="C171" s="10">
+        <v>15.62</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A172" s="11">
+        <v>43710</v>
+      </c>
+      <c r="B172" s="13">
+        <v>0.90031250000000007</v>
+      </c>
+      <c r="C172" s="10">
+        <v>15.62</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A173" s="11">
+        <v>43710</v>
+      </c>
+      <c r="B173" s="13">
+        <v>0.90725694444444438</v>
+      </c>
+      <c r="C173" s="10">
+        <v>15.59</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A174" s="11">
+        <v>43710</v>
+      </c>
+      <c r="B174" s="13">
+        <v>0.91420138888888891</v>
+      </c>
+      <c r="C174" s="10">
+        <v>15.57</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A175" s="11">
+        <v>43710</v>
+      </c>
+      <c r="B175" s="13">
+        <v>0.92114583333333344</v>
+      </c>
+      <c r="C175" s="10">
+        <v>15.56</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A176" s="11">
+        <v>43710</v>
+      </c>
+      <c r="B176" s="13">
+        <v>0.92809027777777775</v>
+      </c>
+      <c r="C176" s="10">
+        <v>15.53</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A177" s="11">
+        <v>43710</v>
+      </c>
+      <c r="B177" s="13">
+        <v>0.93503472222222228</v>
+      </c>
+      <c r="C177" s="10">
+        <v>15.51</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A178" s="11">
+        <v>43710</v>
+      </c>
+      <c r="B178" s="13">
+        <v>0.9419791666666667</v>
+      </c>
+      <c r="C178" s="10">
+        <v>15.53</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A179" s="11">
+        <v>43710</v>
+      </c>
+      <c r="B179" s="13">
+        <v>0.94892361111111112</v>
+      </c>
+      <c r="C179" s="10">
+        <v>15.49</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A180" s="11">
+        <v>43710</v>
+      </c>
+      <c r="B180" s="13">
+        <v>0.95586805555555554</v>
+      </c>
+      <c r="C180" s="10">
+        <v>15.48</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A181" s="11">
+        <v>43710</v>
+      </c>
+      <c r="B181" s="13">
+        <v>0.96281250000000007</v>
+      </c>
+      <c r="C181" s="10">
+        <v>15.48</v>
+      </c>
+    </row>
+    <row r="182" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A182" s="11">
+        <v>43710</v>
+      </c>
+      <c r="B182" s="13">
+        <v>0.96975694444444438</v>
+      </c>
+      <c r="C182" s="10">
+        <v>15.48</v>
+      </c>
+    </row>
+    <row r="183" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A183" s="11">
+        <v>43710</v>
+      </c>
+      <c r="B183" s="13">
+        <v>0.97670138888888891</v>
+      </c>
+      <c r="C183" s="10">
+        <v>15.46</v>
+      </c>
+    </row>
+    <row r="184" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A184" s="11">
+        <v>43710</v>
+      </c>
+      <c r="B184" s="13">
+        <v>0.98364583333333344</v>
+      </c>
+      <c r="C184" s="10">
+        <v>15.48</v>
+      </c>
+    </row>
+    <row r="185" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A185" s="11">
+        <v>43710</v>
+      </c>
+      <c r="B185" s="13">
+        <v>0.99059027777777775</v>
+      </c>
+      <c r="C185" s="10">
+        <v>15.49</v>
+      </c>
+    </row>
+    <row r="186" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A186" s="11">
+        <v>43710</v>
+      </c>
+      <c r="B186" s="13">
+        <v>0.99753472222222228</v>
+      </c>
+      <c r="C186" s="10">
+        <v>15.48</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A187" s="11">
+        <v>43711</v>
+      </c>
+      <c r="B187" s="13">
+        <v>4.4791666666666669E-3</v>
+      </c>
+      <c r="C187" s="10">
+        <v>15.55</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A188" s="11">
+        <v>43711</v>
+      </c>
+      <c r="B188" s="13">
+        <v>1.1423611111111112E-2</v>
+      </c>
+      <c r="C188" s="10">
+        <v>15.55</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A189" s="11">
+        <v>43711</v>
+      </c>
+      <c r="B189" s="13">
+        <v>1.8368055555555554E-2</v>
+      </c>
+      <c r="C189" s="10">
+        <v>15.56</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A190" s="11">
+        <v>43711</v>
+      </c>
+      <c r="B190" s="13">
+        <v>2.5312500000000002E-2</v>
+      </c>
+      <c r="C190" s="10">
+        <v>15.54</v>
+      </c>
+    </row>
+    <row r="191" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A191" s="11">
+        <v>43711</v>
+      </c>
+      <c r="B191" s="13">
+        <v>3.2256944444444442E-2</v>
+      </c>
+      <c r="C191" s="10">
+        <v>15.56</v>
+      </c>
+    </row>
+    <row r="192" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A192" s="11">
+        <v>43711</v>
+      </c>
+      <c r="B192" s="13">
+        <v>3.920138888888889E-2</v>
+      </c>
+      <c r="C192" s="10">
+        <v>15.58</v>
+      </c>
+    </row>
+    <row r="193" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A193" s="11">
+        <v>43711</v>
+      </c>
+      <c r="B193" s="13">
+        <v>4.614583333333333E-2</v>
+      </c>
+      <c r="C193" s="10">
+        <v>15.63</v>
+      </c>
+    </row>
+    <row r="194" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A194" s="11">
+        <v>43711</v>
+      </c>
+      <c r="B194" s="13">
+        <v>5.3090277777777778E-2</v>
+      </c>
+      <c r="C194" s="10">
+        <v>15.67</v>
+      </c>
+    </row>
+    <row r="195" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A195" s="11">
+        <v>43711</v>
+      </c>
+      <c r="B195" s="13">
+        <v>6.0034722222222225E-2</v>
+      </c>
+      <c r="C195" s="10">
+        <v>15.67</v>
+      </c>
+    </row>
+    <row r="196" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A196" s="11">
+        <v>43711</v>
+      </c>
+      <c r="B196" s="13">
+        <v>6.6979166666666659E-2</v>
+      </c>
+      <c r="C196" s="10">
+        <v>15.68</v>
+      </c>
+    </row>
+    <row r="197" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A197" s="11">
+        <v>43711</v>
+      </c>
+      <c r="B197" s="13">
+        <v>7.3923611111111107E-2</v>
+      </c>
+      <c r="C197" s="10">
+        <v>15.7</v>
+      </c>
+    </row>
+    <row r="198" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A198" s="11">
+        <v>43711</v>
+      </c>
+      <c r="B198" s="13">
+        <v>8.0868055555555554E-2</v>
+      </c>
+      <c r="C198" s="10">
+        <v>15.69</v>
+      </c>
+    </row>
+    <row r="199" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A199" s="11">
+        <v>43711</v>
+      </c>
+      <c r="B199" s="13">
+        <v>8.7812500000000002E-2</v>
+      </c>
+      <c r="C199" s="10">
+        <v>15.71</v>
+      </c>
+    </row>
+    <row r="200" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A200" s="11">
+        <v>43711</v>
+      </c>
+      <c r="B200" s="13">
+        <v>9.4756944444444449E-2</v>
+      </c>
+      <c r="C200" s="10">
+        <v>15.72</v>
+      </c>
+    </row>
+    <row r="201" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A201" s="11">
+        <v>43711</v>
+      </c>
+      <c r="B201" s="13">
+        <v>0.1017013888888889</v>
+      </c>
+      <c r="C201" s="10">
+        <v>15.73</v>
+      </c>
+    </row>
+    <row r="202" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A202" s="11">
+        <v>43711</v>
+      </c>
+      <c r="B202" s="13">
+        <v>0.10864583333333333</v>
+      </c>
+      <c r="C202" s="10">
+        <v>15.69</v>
+      </c>
+    </row>
+    <row r="203" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A203" s="11">
+        <v>43711</v>
+      </c>
+      <c r="B203" s="13">
+        <v>0.11559027777777779</v>
+      </c>
+      <c r="C203" s="10">
+        <v>15.69</v>
+      </c>
+    </row>
+    <row r="204" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A204" s="11">
+        <v>43711</v>
+      </c>
+      <c r="B204" s="13">
+        <v>0.12253472222222223</v>
+      </c>
+      <c r="C204" s="10">
+        <v>15.67</v>
+      </c>
+    </row>
+    <row r="205" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A205" s="11">
+        <v>43711</v>
+      </c>
+      <c r="B205" s="13">
+        <v>0.12947916666666667</v>
+      </c>
+      <c r="C205" s="10">
+        <v>15.67</v>
+      </c>
+    </row>
+    <row r="206" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A206" s="11">
+        <v>43711</v>
+      </c>
+      <c r="B206" s="13">
+        <v>0.13642361111111112</v>
+      </c>
+      <c r="C206" s="10">
+        <v>15.65</v>
+      </c>
+    </row>
+    <row r="207" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A207" s="11">
+        <v>43711</v>
+      </c>
+      <c r="B207" s="13">
+        <v>0.14336805555555557</v>
+      </c>
+      <c r="C207" s="10">
+        <v>15.67</v>
+      </c>
+    </row>
+    <row r="208" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A208" s="11">
+        <v>43711</v>
+      </c>
+      <c r="B208" s="13">
+        <v>0.15031249999999999</v>
+      </c>
+      <c r="C208" s="10">
+        <v>15.71</v>
+      </c>
+    </row>
+    <row r="209" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A209" s="11">
+        <v>43711</v>
+      </c>
+      <c r="B209" s="13">
+        <v>0.15725694444444446</v>
+      </c>
+      <c r="C209" s="10">
+        <v>15.65</v>
+      </c>
+    </row>
+    <row r="210" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A210" s="11">
+        <v>43711</v>
+      </c>
+      <c r="B210" s="13">
+        <v>0.16420138888888888</v>
+      </c>
+      <c r="C210" s="10">
+        <v>15.68</v>
+      </c>
+    </row>
+    <row r="211" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A211" s="11">
+        <v>43711</v>
+      </c>
+      <c r="B211" s="13">
+        <v>0.17114583333333333</v>
+      </c>
+      <c r="C211" s="10">
+        <v>15.67</v>
+      </c>
+    </row>
+    <row r="212" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A212" s="11">
+        <v>43711</v>
+      </c>
+      <c r="B212" s="13">
+        <v>0.17809027777777778</v>
+      </c>
+      <c r="C212" s="10">
+        <v>15.69</v>
+      </c>
+    </row>
+    <row r="213" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A213" s="11">
+        <v>43711</v>
+      </c>
+      <c r="B213" s="13">
+        <v>0.1850347222222222</v>
+      </c>
+      <c r="C213" s="10">
+        <v>15.69</v>
+      </c>
+    </row>
+    <row r="214" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A214" s="11">
+        <v>43711</v>
+      </c>
+      <c r="B214" s="13">
+        <v>0.19197916666666667</v>
+      </c>
+      <c r="C214" s="10">
+        <v>15.63</v>
+      </c>
+    </row>
+    <row r="215" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A215" s="11">
+        <v>43711</v>
+      </c>
+      <c r="B215" s="13">
+        <v>0.19892361111111112</v>
+      </c>
+      <c r="C215" s="10">
+        <v>15.63</v>
+      </c>
+    </row>
+    <row r="216" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A216" s="11">
+        <v>43711</v>
+      </c>
+      <c r="B216" s="13">
+        <v>0.20586805555555557</v>
+      </c>
+      <c r="C216" s="10">
+        <v>15.56</v>
+      </c>
+    </row>
+    <row r="217" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A217" s="11">
+        <v>43711</v>
+      </c>
+      <c r="B217" s="13">
+        <v>0.21281249999999999</v>
+      </c>
+      <c r="C217" s="10">
+        <v>15.53</v>
+      </c>
+    </row>
+    <row r="218" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A218" s="11">
+        <v>43711</v>
+      </c>
+      <c r="B218" s="13">
+        <v>0.21975694444444446</v>
+      </c>
+      <c r="C218" s="10">
+        <v>15.55</v>
+      </c>
+    </row>
+    <row r="219" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A219" s="11">
+        <v>43711</v>
+      </c>
+      <c r="B219" s="13">
+        <v>0.22670138888888888</v>
+      </c>
+      <c r="C219" s="10">
+        <v>15.56</v>
+      </c>
+    </row>
+    <row r="220" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A220" s="11">
+        <v>43711</v>
+      </c>
+      <c r="B220" s="13">
+        <v>0.23364583333333333</v>
+      </c>
+      <c r="C220" s="10">
+        <v>15.55</v>
+      </c>
+    </row>
+    <row r="221" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A221" s="11">
+        <v>43711</v>
+      </c>
+      <c r="B221" s="13">
+        <v>0.24059027777777778</v>
+      </c>
+      <c r="C221" s="10">
+        <v>15.55</v>
+      </c>
+    </row>
+    <row r="222" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A222" s="11">
+        <v>43711</v>
+      </c>
+      <c r="B222" s="13">
+        <v>0.24753472222222225</v>
+      </c>
+      <c r="C222" s="10">
+        <v>15.53</v>
+      </c>
+    </row>
+    <row r="223" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A223" s="11">
+        <v>43711</v>
+      </c>
+      <c r="B223" s="13">
+        <v>0.25447916666666665</v>
+      </c>
+      <c r="C223" s="10">
+        <v>15.51</v>
+      </c>
+    </row>
+    <row r="224" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A224" s="11">
+        <v>43711</v>
+      </c>
+      <c r="B224" s="13">
+        <v>0.26142361111111112</v>
+      </c>
+      <c r="C224" s="10">
+        <v>15.53</v>
+      </c>
+    </row>
+    <row r="225" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A225" s="11">
+        <v>43711</v>
+      </c>
+      <c r="B225" s="13">
+        <v>0.26836805555555554</v>
+      </c>
+      <c r="C225" s="10">
+        <v>15.57</v>
+      </c>
+    </row>
+    <row r="226" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A226" s="11">
+        <v>43711</v>
+      </c>
+      <c r="B226" s="13">
+        <v>0.27531250000000002</v>
+      </c>
+      <c r="C226" s="10">
+        <v>15.6</v>
+      </c>
+    </row>
+    <row r="227" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A227" s="11">
+        <v>43711</v>
+      </c>
+      <c r="B227" s="13">
+        <v>0.28225694444444444</v>
+      </c>
+      <c r="C227" s="10">
+        <v>15.62</v>
+      </c>
+    </row>
+    <row r="228" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A228" s="11">
+        <v>43711</v>
+      </c>
+      <c r="B228" s="13">
+        <v>0.28920138888888891</v>
+      </c>
+      <c r="C228" s="10">
+        <v>15.62</v>
+      </c>
+    </row>
+    <row r="229" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A229" s="11">
+        <v>43711</v>
+      </c>
+      <c r="B229" s="13">
+        <v>0.29614583333333333</v>
+      </c>
+      <c r="C229" s="10">
+        <v>15.63</v>
+      </c>
+    </row>
+    <row r="230" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A230" s="11">
+        <v>43711</v>
+      </c>
+      <c r="B230" s="13">
+        <v>0.30309027777777781</v>
+      </c>
+      <c r="C230" s="10">
+        <v>15.65</v>
+      </c>
+    </row>
+    <row r="231" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A231" s="11">
+        <v>43711</v>
+      </c>
+      <c r="B231" s="13">
+        <v>0.31003472222222223</v>
+      </c>
+      <c r="C231" s="10">
+        <v>15.69</v>
+      </c>
+    </row>
+    <row r="232" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A232" s="11">
+        <v>43711</v>
+      </c>
+      <c r="B232" s="13">
+        <v>0.31697916666666665</v>
+      </c>
+      <c r="C232" s="10">
+        <v>15.7</v>
+      </c>
+    </row>
+    <row r="233" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A233" s="11">
+        <v>43711</v>
+      </c>
+      <c r="B233" s="13">
+        <v>0.32392361111111112</v>
+      </c>
+      <c r="C233" s="10">
+        <v>15.7</v>
+      </c>
+    </row>
+    <row r="234" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A234" s="11">
+        <v>43711</v>
+      </c>
+      <c r="B234" s="13">
+        <v>0.3308680555555556</v>
+      </c>
+      <c r="C234" s="10">
+        <v>15.72</v>
+      </c>
+    </row>
+    <row r="235" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A235" s="11">
+        <v>43711</v>
+      </c>
+      <c r="B235" s="13">
+        <v>0.79614583333333344</v>
+      </c>
+      <c r="C235" s="10">
+        <v>16.010000000000002</v>
+      </c>
+    </row>
+    <row r="236" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A236" s="11">
+        <v>43711</v>
+      </c>
+      <c r="B236" s="13">
+        <v>0.80309027777777775</v>
+      </c>
+      <c r="C236" s="10">
+        <v>15.91</v>
+      </c>
+    </row>
+    <row r="237" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A237" s="11">
+        <v>43711</v>
+      </c>
+      <c r="B237" s="13">
+        <v>0.81003472222222228</v>
+      </c>
+      <c r="C237" s="10">
+        <v>15.9</v>
+      </c>
+    </row>
+    <row r="238" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A238" s="11">
+        <v>43711</v>
+      </c>
+      <c r="B238" s="13">
+        <v>0.8169791666666667</v>
+      </c>
+      <c r="C238" s="10">
+        <v>15.84</v>
+      </c>
+    </row>
+    <row r="239" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A239" s="11">
+        <v>43711</v>
+      </c>
+      <c r="B239" s="13">
+        <v>0.82392361111111112</v>
+      </c>
+      <c r="C239" s="10">
+        <v>15.82</v>
+      </c>
+    </row>
+    <row r="240" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A240" s="11">
+        <v>43711</v>
+      </c>
+      <c r="B240" s="13">
+        <v>0.83086805555555554</v>
+      </c>
+      <c r="C240" s="10">
+        <v>15.8</v>
+      </c>
+    </row>
+    <row r="241" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A241" s="11">
+        <v>43711</v>
+      </c>
+      <c r="B241" s="13">
+        <v>0.83781250000000007</v>
+      </c>
+      <c r="C241" s="10">
+        <v>15.76</v>
+      </c>
+    </row>
+    <row r="242" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A242" s="11">
+        <v>43711</v>
+      </c>
+      <c r="B242" s="13">
+        <v>0.84475694444444438</v>
+      </c>
+      <c r="C242" s="10">
+        <v>15.76</v>
+      </c>
+    </row>
+    <row r="243" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A243" s="11">
+        <v>43711</v>
+      </c>
+      <c r="B243" s="13">
+        <v>0.85170138888888891</v>
+      </c>
+      <c r="C243" s="10">
+        <v>15.76</v>
+      </c>
+    </row>
+    <row r="244" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A244" s="11">
+        <v>43711</v>
+      </c>
+      <c r="B244" s="13">
+        <v>0.85864583333333344</v>
+      </c>
+      <c r="C244" s="10">
+        <v>15.75</v>
+      </c>
+    </row>
+    <row r="245" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A245" s="11">
+        <v>43711</v>
+      </c>
+      <c r="B245" s="13">
+        <v>0.86559027777777775</v>
+      </c>
+      <c r="C245" s="10">
+        <v>15.73</v>
+      </c>
+    </row>
+    <row r="246" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A246" s="11">
+        <v>43711</v>
+      </c>
+      <c r="B246" s="13">
+        <v>0.87253472222222228</v>
+      </c>
+      <c r="C246" s="10">
+        <v>15.74</v>
+      </c>
+    </row>
+    <row r="247" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A247" s="11">
+        <v>43711</v>
+      </c>
+      <c r="B247" s="13">
+        <v>0.8794791666666667</v>
+      </c>
+      <c r="C247" s="10">
+        <v>15.74</v>
+      </c>
+    </row>
+    <row r="248" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A248" s="11">
+        <v>43711</v>
+      </c>
+      <c r="B248" s="13">
+        <v>0.88642361111111112</v>
+      </c>
+      <c r="C248" s="10">
+        <v>15.73</v>
+      </c>
+    </row>
+    <row r="249" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A249" s="11">
+        <v>43711</v>
+      </c>
+      <c r="B249" s="13">
+        <v>0.89336805555555554</v>
+      </c>
+      <c r="C249" s="10">
+        <v>15.72</v>
+      </c>
+    </row>
+    <row r="250" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A250" s="11">
+        <v>43711</v>
+      </c>
+      <c r="B250" s="13">
+        <v>0.90031250000000007</v>
+      </c>
+      <c r="C250" s="10">
+        <v>15.7</v>
+      </c>
+    </row>
+    <row r="251" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A251" s="11">
+        <v>43711</v>
+      </c>
+      <c r="B251" s="13">
+        <v>0.90725694444444438</v>
+      </c>
+      <c r="C251" s="10">
+        <v>15.68</v>
+      </c>
+    </row>
+    <row r="252" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A252" s="11">
+        <v>43711</v>
+      </c>
+      <c r="B252" s="13">
+        <v>0.91420138888888891</v>
+      </c>
+      <c r="C252" s="10">
+        <v>15.65</v>
+      </c>
+    </row>
+    <row r="253" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A253" s="11">
+        <v>43711</v>
+      </c>
+      <c r="B253" s="13">
+        <v>0.92114583333333344</v>
+      </c>
+      <c r="C253" s="10">
+        <v>15.61</v>
+      </c>
+    </row>
+    <row r="254" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A254" s="11">
+        <v>43711</v>
+      </c>
+      <c r="B254" s="13">
+        <v>0.92809027777777775</v>
+      </c>
+      <c r="C254" s="10">
+        <v>15.61</v>
+      </c>
+    </row>
+    <row r="255" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A255" s="11">
+        <v>43711</v>
+      </c>
+      <c r="B255" s="13">
+        <v>0.93503472222222228</v>
+      </c>
+      <c r="C255" s="10">
+        <v>15.61</v>
+      </c>
+    </row>
+    <row r="256" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A256" s="11">
+        <v>43711</v>
+      </c>
+      <c r="B256" s="13">
+        <v>0.9419791666666667</v>
+      </c>
+      <c r="C256" s="10">
+        <v>15.62</v>
+      </c>
+    </row>
+    <row r="257" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A257" s="11">
+        <v>43711</v>
+      </c>
+      <c r="B257" s="13">
+        <v>0.94892361111111112</v>
+      </c>
+      <c r="C257" s="10">
+        <v>15.62</v>
+      </c>
+    </row>
+    <row r="258" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A258" s="11">
+        <v>43711</v>
+      </c>
+      <c r="B258" s="13">
+        <v>0.95586805555555554</v>
+      </c>
+      <c r="C258" s="10">
+        <v>15.58</v>
+      </c>
+    </row>
+    <row r="259" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A259" s="11">
+        <v>43711</v>
+      </c>
+      <c r="B259" s="13">
+        <v>0.96281250000000007</v>
+      </c>
+      <c r="C259" s="10">
+        <v>15.61</v>
+      </c>
+    </row>
+    <row r="260" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A260" s="11">
+        <v>43711</v>
+      </c>
+      <c r="B260" s="13">
+        <v>0.96975694444444438</v>
+      </c>
+      <c r="C260" s="10">
+        <v>15.59</v>
+      </c>
+    </row>
+    <row r="261" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A261" s="11">
+        <v>43711</v>
+      </c>
+      <c r="B261" s="13">
+        <v>0.97670138888888891</v>
+      </c>
+      <c r="C261" s="10">
+        <v>15.57</v>
+      </c>
+    </row>
+    <row r="262" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A262" s="11">
+        <v>43711</v>
+      </c>
+      <c r="B262" s="13">
+        <v>0.98364583333333344</v>
+      </c>
+      <c r="C262" s="10">
+        <v>15.58</v>
+      </c>
+    </row>
+    <row r="263" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A263" s="11">
+        <v>43711</v>
+      </c>
+      <c r="B263" s="13">
+        <v>0.99059027777777775</v>
+      </c>
+      <c r="C263" s="10">
+        <v>15.57</v>
+      </c>
+    </row>
+    <row r="264" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A264" s="11">
+        <v>43711</v>
+      </c>
+      <c r="B264" s="13">
+        <v>0.99753472222222228</v>
+      </c>
+      <c r="C264" s="10">
+        <v>15.61</v>
+      </c>
+    </row>
+    <row r="265" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A265" s="11">
+        <v>43712</v>
+      </c>
+      <c r="B265" s="13">
+        <v>4.4791666666666669E-3</v>
+      </c>
+      <c r="C265" s="10">
+        <v>15.65</v>
+      </c>
+    </row>
+    <row r="266" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A266" s="11">
+        <v>43712</v>
+      </c>
+      <c r="B266" s="13">
+        <v>1.1423611111111112E-2</v>
+      </c>
+      <c r="C266" s="10">
+        <v>15.65</v>
+      </c>
+    </row>
+    <row r="267" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A267" s="11">
+        <v>43712</v>
+      </c>
+      <c r="B267" s="13">
+        <v>1.8368055555555554E-2</v>
+      </c>
+      <c r="C267" s="10">
+        <v>15.61</v>
+      </c>
+    </row>
+    <row r="268" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A268" s="11">
+        <v>43712</v>
+      </c>
+      <c r="B268" s="13">
+        <v>2.5312500000000002E-2</v>
+      </c>
+      <c r="C268" s="10">
+        <v>15.6</v>
+      </c>
+    </row>
+    <row r="269" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A269" s="11">
+        <v>43712</v>
+      </c>
+      <c r="B269" s="13">
+        <v>3.2256944444444442E-2</v>
+      </c>
+      <c r="C269" s="10">
+        <v>15.65</v>
+      </c>
+    </row>
+    <row r="270" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A270" s="11">
+        <v>43712</v>
+      </c>
+      <c r="B270" s="13">
+        <v>3.920138888888889E-2</v>
+      </c>
+      <c r="C270" s="10">
+        <v>15.62</v>
+      </c>
+    </row>
+    <row r="271" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A271" s="11">
+        <v>43712</v>
+      </c>
+      <c r="B271" s="13">
+        <v>4.614583333333333E-2</v>
+      </c>
+      <c r="C271" s="10">
+        <v>15.65</v>
+      </c>
+    </row>
+    <row r="272" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A272" s="11">
+        <v>43712</v>
+      </c>
+      <c r="B272" s="13">
+        <v>5.3090277777777778E-2</v>
+      </c>
+      <c r="C272" s="10">
+        <v>15.63</v>
+      </c>
+    </row>
+    <row r="273" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A273" s="11">
+        <v>43712</v>
+      </c>
+      <c r="B273" s="13">
+        <v>6.0034722222222225E-2</v>
+      </c>
+      <c r="C273" s="10">
+        <v>15.62</v>
+      </c>
+    </row>
+    <row r="274" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A274" s="11">
+        <v>43712</v>
+      </c>
+      <c r="B274" s="13">
+        <v>6.6979166666666659E-2</v>
+      </c>
+      <c r="C274" s="10">
+        <v>15.63</v>
+      </c>
+    </row>
+    <row r="275" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A275" s="11">
+        <v>43712</v>
+      </c>
+      <c r="B275" s="13">
+        <v>7.3923611111111107E-2</v>
+      </c>
+      <c r="C275" s="10">
+        <v>15.63</v>
+      </c>
+    </row>
+    <row r="276" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A276" s="11">
+        <v>43712</v>
+      </c>
+      <c r="B276" s="13">
+        <v>8.0868055555555554E-2</v>
+      </c>
+      <c r="C276" s="10">
+        <v>15.63</v>
+      </c>
+    </row>
+    <row r="277" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A277" s="11">
+        <v>43712</v>
+      </c>
+      <c r="B277" s="13">
+        <v>8.7812500000000002E-2</v>
+      </c>
+      <c r="C277" s="10">
+        <v>15.62</v>
+      </c>
+    </row>
+    <row r="278" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A278" s="11">
+        <v>43712</v>
+      </c>
+      <c r="B278" s="13">
+        <v>9.4756944444444449E-2</v>
+      </c>
+      <c r="C278" s="10">
+        <v>15.63</v>
+      </c>
+    </row>
+    <row r="279" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A279" s="11">
+        <v>43712</v>
+      </c>
+      <c r="B279" s="13">
+        <v>0.1017013888888889</v>
+      </c>
+      <c r="C279" s="10">
+        <v>15.63</v>
+      </c>
+    </row>
+    <row r="280" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A280" s="11">
+        <v>43712</v>
+      </c>
+      <c r="B280" s="13">
+        <v>0.10864583333333333</v>
+      </c>
+      <c r="C280" s="10">
+        <v>15.66</v>
+      </c>
+    </row>
+    <row r="281" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A281" s="11">
+        <v>43712</v>
+      </c>
+      <c r="B281" s="13">
+        <v>0.11559027777777779</v>
+      </c>
+      <c r="C281" s="10">
+        <v>15.67</v>
+      </c>
+    </row>
+    <row r="282" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A282" s="11">
+        <v>43712</v>
+      </c>
+      <c r="B282" s="13">
+        <v>0.12253472222222223</v>
+      </c>
+      <c r="C282" s="10">
+        <v>15.72</v>
+      </c>
+    </row>
+    <row r="283" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A283" s="11">
+        <v>43712</v>
+      </c>
+      <c r="B283" s="13">
+        <v>0.12947916666666667</v>
+      </c>
+      <c r="C283" s="10">
+        <v>15.76</v>
+      </c>
+    </row>
+    <row r="284" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A284" s="11">
+        <v>43712</v>
+      </c>
+      <c r="B284" s="13">
+        <v>0.13642361111111112</v>
+      </c>
+      <c r="C284" s="10">
+        <v>15.71</v>
+      </c>
+    </row>
+    <row r="285" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A285" s="11">
+        <v>43712</v>
+      </c>
+      <c r="B285" s="13">
+        <v>0.14336805555555557</v>
+      </c>
+      <c r="C285" s="10">
+        <v>15.73</v>
+      </c>
+    </row>
+    <row r="286" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A286" s="11">
+        <v>43712</v>
+      </c>
+      <c r="B286" s="13">
+        <v>0.15031249999999999</v>
+      </c>
+      <c r="C286" s="10">
+        <v>15.74</v>
+      </c>
+    </row>
+    <row r="287" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A287" s="11">
+        <v>43712</v>
+      </c>
+      <c r="B287" s="13">
+        <v>0.15725694444444446</v>
+      </c>
+      <c r="C287" s="10">
+        <v>15.73</v>
+      </c>
+    </row>
+    <row r="288" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A288" s="11">
+        <v>43712</v>
+      </c>
+      <c r="B288" s="13">
+        <v>0.16420138888888888</v>
+      </c>
+      <c r="C288" s="10">
+        <v>15.74</v>
+      </c>
+    </row>
+    <row r="289" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A289" s="11">
+        <v>43712</v>
+      </c>
+      <c r="B289" s="13">
+        <v>0.17114583333333333</v>
+      </c>
+      <c r="C289" s="10">
+        <v>15.74</v>
+      </c>
+    </row>
+    <row r="290" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A290" s="11">
+        <v>43712</v>
+      </c>
+      <c r="B290" s="13">
+        <v>0.17809027777777778</v>
+      </c>
+      <c r="C290" s="10">
+        <v>15.74</v>
+      </c>
+    </row>
+    <row r="291" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A291" s="11">
+        <v>43712</v>
+      </c>
+      <c r="B291" s="13">
+        <v>0.1850347222222222</v>
+      </c>
+      <c r="C291" s="10">
+        <v>15.76</v>
+      </c>
+    </row>
+    <row r="292" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A292" s="11">
+        <v>43712</v>
+      </c>
+      <c r="B292" s="13">
+        <v>0.19197916666666667</v>
+      </c>
+      <c r="C292" s="10">
+        <v>15.73</v>
+      </c>
+    </row>
+    <row r="293" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A293" s="11">
+        <v>43712</v>
+      </c>
+      <c r="B293" s="13">
+        <v>0.19892361111111112</v>
+      </c>
+      <c r="C293" s="10">
+        <v>15.73</v>
+      </c>
+    </row>
+    <row r="294" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A294" s="11">
+        <v>43712</v>
+      </c>
+      <c r="B294" s="13">
+        <v>0.20586805555555557</v>
+      </c>
+      <c r="C294" s="10">
+        <v>15.78</v>
+      </c>
+    </row>
+    <row r="295" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A295" s="11">
+        <v>43712</v>
+      </c>
+      <c r="B295" s="13">
+        <v>0.21281249999999999</v>
+      </c>
+      <c r="C295" s="10">
+        <v>15.76</v>
+      </c>
+    </row>
+    <row r="296" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A296" s="11">
+        <v>43712</v>
+      </c>
+      <c r="B296" s="13">
+        <v>0.21975694444444446</v>
+      </c>
+      <c r="C296" s="10">
+        <v>15.74</v>
+      </c>
+    </row>
+    <row r="297" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A297" s="11">
+        <v>43712</v>
+      </c>
+      <c r="B297" s="13">
+        <v>0.22670138888888888</v>
+      </c>
+      <c r="C297" s="10">
+        <v>15.73</v>
+      </c>
+    </row>
+    <row r="298" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A298" s="11">
+        <v>43712</v>
+      </c>
+      <c r="B298" s="13">
+        <v>0.23364583333333333</v>
+      </c>
+      <c r="C298" s="10">
+        <v>15.71</v>
+      </c>
+    </row>
+    <row r="299" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A299" s="11">
+        <v>43712</v>
+      </c>
+      <c r="B299" s="13">
+        <v>0.24059027777777778</v>
+      </c>
+      <c r="C299" s="10">
+        <v>15.72</v>
+      </c>
+    </row>
+    <row r="300" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A300" s="11">
+        <v>43712</v>
+      </c>
+      <c r="B300" s="13">
+        <v>0.24753472222222225</v>
+      </c>
+      <c r="C300" s="10">
+        <v>15.73</v>
+      </c>
+    </row>
+    <row r="301" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A301" s="11">
+        <v>43712</v>
+      </c>
+      <c r="B301" s="13">
+        <v>0.25447916666666665</v>
+      </c>
+      <c r="C301" s="10">
+        <v>15.74</v>
+      </c>
+    </row>
+    <row r="302" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A302" s="11">
+        <v>43712</v>
+      </c>
+      <c r="B302" s="13">
+        <v>0.26142361111111112</v>
+      </c>
+      <c r="C302" s="10">
+        <v>15.74</v>
+      </c>
+    </row>
+    <row r="303" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A303" s="11">
+        <v>43712</v>
+      </c>
+      <c r="B303" s="13">
+        <v>0.26836805555555554</v>
+      </c>
+      <c r="C303" s="10">
+        <v>15.73</v>
+      </c>
+    </row>
+    <row r="304" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A304" s="11">
+        <v>43712</v>
+      </c>
+      <c r="B304" s="13">
+        <v>0.27531250000000002</v>
+      </c>
+      <c r="C304" s="10">
+        <v>15.77</v>
+      </c>
+    </row>
+    <row r="305" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A305" s="11">
+        <v>43712</v>
+      </c>
+      <c r="B305" s="13">
+        <v>0.28225694444444444</v>
+      </c>
+      <c r="C305" s="10">
+        <v>15.82</v>
+      </c>
+    </row>
+    <row r="306" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A306" s="11">
+        <v>43712</v>
+      </c>
+      <c r="B306" s="13">
+        <v>0.28920138888888891</v>
+      </c>
+      <c r="C306" s="10">
+        <v>15.77</v>
+      </c>
+    </row>
+    <row r="307" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A307" s="11">
+        <v>43712</v>
+      </c>
+      <c r="B307" s="13">
+        <v>0.29614583333333333</v>
+      </c>
+      <c r="C307" s="10">
+        <v>15.76</v>
+      </c>
+    </row>
+    <row r="308" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A308" s="11">
+        <v>43712</v>
+      </c>
+      <c r="B308" s="13">
+        <v>0.30309027777777781</v>
+      </c>
+      <c r="C308" s="10">
+        <v>15.78</v>
+      </c>
+    </row>
+    <row r="309" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A309" s="11">
+        <v>43712</v>
+      </c>
+      <c r="B309" s="13">
+        <v>0.31003472222222223</v>
+      </c>
+      <c r="C309" s="10">
+        <v>15.76</v>
+      </c>
+    </row>
+    <row r="310" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A310" s="11">
+        <v>43712</v>
+      </c>
+      <c r="B310" s="13">
+        <v>0.31697916666666665</v>
+      </c>
+      <c r="C310" s="10">
+        <v>15.81</v>
+      </c>
+    </row>
+    <row r="311" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A311" s="11">
+        <v>43712</v>
+      </c>
+      <c r="B311" s="13">
+        <v>0.32392361111111112</v>
+      </c>
+      <c r="C311" s="10">
+        <v>15.83</v>
+      </c>
+    </row>
+    <row r="312" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A312" s="11">
+        <v>43712</v>
+      </c>
+      <c r="B312" s="13">
+        <v>0.3308680555555556</v>
+      </c>
+      <c r="C312" s="10">
+        <v>15.9</v>
+      </c>
+    </row>
+    <row r="313" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A313" s="11">
+        <v>43712</v>
+      </c>
+      <c r="B313" s="13">
+        <v>0.79614583333333344</v>
+      </c>
+      <c r="C313" s="10">
+        <v>15.85</v>
+      </c>
+    </row>
+    <row r="314" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A314" s="11">
+        <v>43712</v>
+      </c>
+      <c r="B314" s="13">
+        <v>0.80309027777777775</v>
+      </c>
+      <c r="C314" s="10">
+        <v>15.8</v>
+      </c>
+    </row>
+    <row r="315" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A315" s="11">
+        <v>43712</v>
+      </c>
+      <c r="B315" s="13">
+        <v>0.81003472222222228</v>
+      </c>
+      <c r="C315" s="10">
+        <v>15.67</v>
+      </c>
+    </row>
+    <row r="316" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A316" s="11">
+        <v>43712</v>
+      </c>
+      <c r="B316" s="13">
+        <v>0.8169791666666667</v>
+      </c>
+      <c r="C316" s="10">
+        <v>15.7</v>
+      </c>
+    </row>
+    <row r="317" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A317" s="11">
+        <v>43712</v>
+      </c>
+      <c r="B317" s="13">
+        <v>0.82392361111111112</v>
+      </c>
+      <c r="C317" s="10">
+        <v>15.65</v>
+      </c>
+    </row>
+    <row r="318" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A318" s="11">
+        <v>43712</v>
+      </c>
+      <c r="B318" s="13">
+        <v>0.83086805555555554</v>
+      </c>
+      <c r="C318" s="10">
+        <v>15.62</v>
+      </c>
+    </row>
+    <row r="319" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A319" s="11">
+        <v>43712</v>
+      </c>
+      <c r="B319" s="13">
+        <v>0.83781250000000007</v>
+      </c>
+      <c r="C319" s="10">
+        <v>15.55</v>
+      </c>
+    </row>
+    <row r="320" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A320" s="11">
+        <v>43712</v>
+      </c>
+      <c r="B320" s="13">
+        <v>0.84475694444444438</v>
+      </c>
+      <c r="C320" s="10">
+        <v>15.55</v>
+      </c>
+    </row>
+    <row r="321" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A321" s="11">
+        <v>43712</v>
+      </c>
+      <c r="B321" s="13">
+        <v>0.85170138888888891</v>
+      </c>
+      <c r="C321" s="10">
+        <v>15.53</v>
+      </c>
+    </row>
+    <row r="322" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A322" s="11">
+        <v>43712</v>
+      </c>
+      <c r="B322" s="13">
+        <v>0.85864583333333344</v>
+      </c>
+      <c r="C322" s="10">
+        <v>15.49</v>
+      </c>
+    </row>
+    <row r="323" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A323" s="11">
+        <v>43712</v>
+      </c>
+      <c r="B323" s="13">
+        <v>0.86559027777777775</v>
+      </c>
+      <c r="C323" s="10">
+        <v>15.54</v>
+      </c>
+    </row>
+    <row r="324" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A324" s="11">
+        <v>43712</v>
+      </c>
+      <c r="B324" s="13">
+        <v>0.87253472222222228</v>
+      </c>
+      <c r="C324" s="10">
+        <v>15.47</v>
+      </c>
+    </row>
+    <row r="325" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A325" s="11">
+        <v>43712</v>
+      </c>
+      <c r="B325" s="13">
+        <v>0.8794791666666667</v>
+      </c>
+      <c r="C325" s="10">
+        <v>15.48</v>
+      </c>
+    </row>
+    <row r="326" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A326" s="11">
+        <v>43712</v>
+      </c>
+      <c r="B326" s="13">
+        <v>0.88642361111111112</v>
+      </c>
+      <c r="C326" s="10">
+        <v>15.47</v>
+      </c>
+    </row>
+    <row r="327" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A327" s="11">
+        <v>43712</v>
+      </c>
+      <c r="B327" s="13">
+        <v>0.89336805555555554</v>
+      </c>
+      <c r="C327" s="10">
+        <v>15.45</v>
+      </c>
+    </row>
+    <row r="328" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A328" s="11">
+        <v>43712</v>
+      </c>
+      <c r="B328" s="13">
+        <v>0.90031250000000007</v>
+      </c>
+      <c r="C328" s="10">
+        <v>15.47</v>
+      </c>
+    </row>
+    <row r="329" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A329" s="11">
+        <v>43712</v>
+      </c>
+      <c r="B329" s="13">
+        <v>0.90725694444444438</v>
+      </c>
+      <c r="C329" s="10">
+        <v>15.48</v>
+      </c>
+    </row>
+    <row r="330" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A330" s="11">
+        <v>43712</v>
+      </c>
+      <c r="B330" s="13">
+        <v>0.91420138888888891</v>
+      </c>
+      <c r="C330" s="10">
+        <v>15.44</v>
+      </c>
+    </row>
+    <row r="331" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A331" s="11">
+        <v>43712</v>
+      </c>
+      <c r="B331" s="13">
+        <v>0.92114583333333344</v>
+      </c>
+      <c r="C331" s="10">
+        <v>15.42</v>
+      </c>
+    </row>
+    <row r="332" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A332" s="11">
+        <v>43712</v>
+      </c>
+      <c r="B332" s="13">
+        <v>0.92809027777777775</v>
+      </c>
+      <c r="C332" s="10">
+        <v>15.4</v>
+      </c>
+    </row>
+    <row r="333" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A333" s="11">
+        <v>43712</v>
+      </c>
+      <c r="B333" s="13">
+        <v>0.93503472222222228</v>
+      </c>
+      <c r="C333" s="10">
+        <v>15.42</v>
+      </c>
+    </row>
+    <row r="334" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A334" s="11">
+        <v>43712</v>
+      </c>
+      <c r="B334" s="13">
+        <v>0.9419791666666667</v>
+      </c>
+      <c r="C334" s="10">
+        <v>15.4</v>
+      </c>
+    </row>
+    <row r="335" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A335" s="11">
+        <v>43712</v>
+      </c>
+      <c r="B335" s="13">
+        <v>0.94892361111111112</v>
+      </c>
+      <c r="C335" s="10">
+        <v>15.41</v>
+      </c>
+    </row>
+    <row r="336" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A336" s="11">
+        <v>43712</v>
+      </c>
+      <c r="B336" s="13">
+        <v>0.95586805555555554</v>
+      </c>
+      <c r="C336" s="10">
+        <v>15.38</v>
+      </c>
+    </row>
+    <row r="337" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A337" s="11">
+        <v>43712</v>
+      </c>
+      <c r="B337" s="13">
+        <v>0.96281250000000007</v>
+      </c>
+      <c r="C337" s="10">
+        <v>15.4</v>
+      </c>
+    </row>
+    <row r="338" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A338" s="11">
+        <v>43712</v>
+      </c>
+      <c r="B338" s="13">
+        <v>0.96975694444444438</v>
+      </c>
+      <c r="C338" s="10">
+        <v>15.44</v>
+      </c>
+    </row>
+    <row r="339" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A339" s="11">
+        <v>43712</v>
+      </c>
+      <c r="B339" s="13">
+        <v>0.97670138888888891</v>
+      </c>
+      <c r="C339" s="10">
+        <v>15.45</v>
+      </c>
+    </row>
+    <row r="340" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A340" s="11">
+        <v>43712</v>
+      </c>
+      <c r="B340" s="13">
+        <v>0.98364583333333344</v>
+      </c>
+      <c r="C340" s="10">
+        <v>15.46</v>
+      </c>
+    </row>
+    <row r="341" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A341" s="11">
+        <v>43712</v>
+      </c>
+      <c r="B341" s="13">
+        <v>0.99059027777777775</v>
+      </c>
+      <c r="C341" s="10">
+        <v>15.45</v>
+      </c>
+    </row>
+    <row r="342" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A342" s="11">
+        <v>43712</v>
+      </c>
+      <c r="B342" s="13">
+        <v>0.99753472222222228</v>
+      </c>
+      <c r="C342" s="10">
+        <v>15.49</v>
+      </c>
+    </row>
+    <row r="343" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A343" s="11">
+        <v>43713</v>
+      </c>
+      <c r="B343" s="13">
+        <v>4.4791666666666669E-3</v>
+      </c>
+      <c r="C343" s="10">
+        <v>15.51</v>
+      </c>
+    </row>
+    <row r="344" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A344" s="11">
+        <v>43713</v>
+      </c>
+      <c r="B344" s="13">
+        <v>1.1423611111111112E-2</v>
+      </c>
+      <c r="C344" s="10">
+        <v>15.51</v>
+      </c>
+    </row>
+    <row r="345" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A345" s="11">
+        <v>43713</v>
+      </c>
+      <c r="B345" s="13">
+        <v>1.8368055555555554E-2</v>
+      </c>
+      <c r="C345" s="10">
+        <v>15.54</v>
+      </c>
+    </row>
+    <row r="346" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A346" s="11">
+        <v>43713</v>
+      </c>
+      <c r="B346" s="13">
+        <v>2.5312500000000002E-2</v>
+      </c>
+      <c r="C346" s="10">
+        <v>15.56</v>
+      </c>
+    </row>
+    <row r="347" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A347" s="11">
+        <v>43713</v>
+      </c>
+      <c r="B347" s="13">
+        <v>3.2256944444444442E-2</v>
+      </c>
+      <c r="C347" s="10">
+        <v>15.56</v>
+      </c>
+    </row>
+    <row r="348" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A348" s="11">
+        <v>43713</v>
+      </c>
+      <c r="B348" s="13">
+        <v>3.920138888888889E-2</v>
+      </c>
+      <c r="C348" s="10">
+        <v>15.55</v>
+      </c>
+    </row>
+    <row r="349" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A349" s="11">
+        <v>43713</v>
+      </c>
+      <c r="B349" s="13">
+        <v>4.614583333333333E-2</v>
+      </c>
+      <c r="C349" s="10">
+        <v>15.51</v>
+      </c>
+    </row>
+    <row r="350" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A350" s="11">
+        <v>43713</v>
+      </c>
+      <c r="B350" s="13">
+        <v>5.3090277777777778E-2</v>
+      </c>
+      <c r="C350" s="10">
+        <v>15.56</v>
+      </c>
+    </row>
+    <row r="351" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A351" s="11">
+        <v>43713</v>
+      </c>
+      <c r="B351" s="13">
+        <v>6.0034722222222225E-2</v>
+      </c>
+      <c r="C351" s="10">
+        <v>15.62</v>
+      </c>
+    </row>
+    <row r="352" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A352" s="11">
+        <v>43713</v>
+      </c>
+      <c r="B352" s="13">
+        <v>6.6979166666666659E-2</v>
+      </c>
+      <c r="C352" s="10">
+        <v>15.6</v>
+      </c>
+    </row>
+    <row r="353" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A353" s="11">
+        <v>43713</v>
+      </c>
+      <c r="B353" s="13">
+        <v>7.3923611111111107E-2</v>
+      </c>
+      <c r="C353" s="10">
+        <v>15.6</v>
+      </c>
+    </row>
+    <row r="354" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A354" s="11">
+        <v>43713</v>
+      </c>
+      <c r="B354" s="13">
+        <v>8.0868055555555554E-2</v>
+      </c>
+      <c r="C354" s="10">
+        <v>15.59</v>
+      </c>
+    </row>
+    <row r="355" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A355" s="11">
+        <v>43713</v>
+      </c>
+      <c r="B355" s="13">
+        <v>8.7812500000000002E-2</v>
+      </c>
+      <c r="C355" s="10">
+        <v>15.58</v>
+      </c>
+    </row>
+    <row r="356" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A356" s="11">
+        <v>43713</v>
+      </c>
+      <c r="B356" s="13">
+        <v>9.4756944444444449E-2</v>
+      </c>
+      <c r="C356" s="10">
+        <v>15.59</v>
+      </c>
+    </row>
+    <row r="357" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A357" s="11">
+        <v>43713</v>
+      </c>
+      <c r="B357" s="13">
+        <v>0.1017013888888889</v>
+      </c>
+      <c r="C357" s="10">
+        <v>15.57</v>
+      </c>
+    </row>
+    <row r="358" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A358" s="11">
+        <v>43713</v>
+      </c>
+      <c r="B358" s="13">
+        <v>0.10864583333333333</v>
+      </c>
+      <c r="C358" s="10">
+        <v>15.53</v>
+      </c>
+    </row>
+    <row r="359" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A359" s="11">
+        <v>43713</v>
+      </c>
+      <c r="B359" s="13">
+        <v>0.11559027777777779</v>
+      </c>
+      <c r="C359" s="10">
+        <v>15.48</v>
+      </c>
+    </row>
+    <row r="360" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A360" s="11">
+        <v>43713</v>
+      </c>
+      <c r="B360" s="13">
+        <v>0.12253472222222223</v>
+      </c>
+      <c r="C360" s="10">
+        <v>15.52</v>
+      </c>
+    </row>
+    <row r="361" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A361" s="11">
+        <v>43713</v>
+      </c>
+      <c r="B361" s="13">
+        <v>0.12947916666666667</v>
+      </c>
+      <c r="C361" s="10">
+        <v>15.45</v>
+      </c>
+    </row>
+    <row r="362" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A362" s="11">
+        <v>43713</v>
+      </c>
+      <c r="B362" s="13">
+        <v>0.13642361111111112</v>
+      </c>
+      <c r="C362" s="10">
+        <v>15.39</v>
+      </c>
+    </row>
+    <row r="363" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A363" s="11">
+        <v>43713</v>
+      </c>
+      <c r="B363" s="13">
+        <v>0.14336805555555557</v>
+      </c>
+      <c r="C363" s="10">
+        <v>15.38</v>
+      </c>
+    </row>
+    <row r="364" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A364" s="11">
+        <v>43713</v>
+      </c>
+      <c r="B364" s="13">
+        <v>0.15031249999999999</v>
+      </c>
+      <c r="C364" s="10">
+        <v>15.39</v>
+      </c>
+    </row>
+    <row r="365" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A365" s="11">
+        <v>43713</v>
+      </c>
+      <c r="B365" s="13">
+        <v>0.15725694444444446</v>
+      </c>
+      <c r="C365" s="10">
+        <v>15.37</v>
+      </c>
+    </row>
+    <row r="366" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A366" s="11">
+        <v>43713</v>
+      </c>
+      <c r="B366" s="13">
+        <v>0.16420138888888888</v>
+      </c>
+      <c r="C366" s="10">
+        <v>15.32</v>
+      </c>
+    </row>
+    <row r="367" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A367" s="11">
+        <v>43713</v>
+      </c>
+      <c r="B367" s="13">
+        <v>0.17114583333333333</v>
+      </c>
+      <c r="C367" s="10">
+        <v>15.27</v>
+      </c>
+    </row>
+    <row r="368" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A368" s="11">
+        <v>43713</v>
+      </c>
+      <c r="B368" s="13">
+        <v>0.17809027777777778</v>
+      </c>
+      <c r="C368" s="10">
+        <v>15.23</v>
+      </c>
+    </row>
+    <row r="369" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A369" s="11">
+        <v>43713</v>
+      </c>
+      <c r="B369" s="13">
+        <v>0.1850347222222222</v>
+      </c>
+      <c r="C369" s="10">
+        <v>15.23</v>
+      </c>
+    </row>
+    <row r="370" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A370" s="11">
+        <v>43713</v>
+      </c>
+      <c r="B370" s="13">
+        <v>0.19197916666666667</v>
+      </c>
+      <c r="C370" s="10">
+        <v>15.23</v>
+      </c>
+    </row>
+    <row r="371" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A371" s="11">
+        <v>43713</v>
+      </c>
+      <c r="B371" s="13">
+        <v>0.19892361111111112</v>
+      </c>
+      <c r="C371" s="10">
+        <v>15.19</v>
+      </c>
+    </row>
+    <row r="372" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A372" s="11">
+        <v>43713</v>
+      </c>
+      <c r="B372" s="13">
+        <v>0.20586805555555557</v>
+      </c>
+      <c r="C372" s="10">
+        <v>15.17</v>
+      </c>
+    </row>
+    <row r="373" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A373" s="11">
+        <v>43713</v>
+      </c>
+      <c r="B373" s="13">
+        <v>0.21281249999999999</v>
+      </c>
+      <c r="C373" s="10">
+        <v>15.18</v>
+      </c>
+    </row>
+    <row r="374" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A374" s="11">
+        <v>43713</v>
+      </c>
+      <c r="B374" s="13">
+        <v>0.21975694444444446</v>
+      </c>
+      <c r="C374" s="10">
+        <v>15.12</v>
+      </c>
+    </row>
+    <row r="375" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A375" s="11">
+        <v>43713</v>
+      </c>
+      <c r="B375" s="13">
+        <v>0.22670138888888888</v>
+      </c>
+      <c r="C375" s="10">
+        <v>15.11</v>
+      </c>
+    </row>
+    <row r="376" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A376" s="11">
+        <v>43713</v>
+      </c>
+      <c r="B376" s="13">
+        <v>0.23364583333333333</v>
+      </c>
+      <c r="C376" s="10">
+        <v>15.09</v>
+      </c>
+    </row>
+    <row r="377" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A377" s="11">
+        <v>43713</v>
+      </c>
+      <c r="B377" s="13">
+        <v>0.24059027777777778</v>
+      </c>
+      <c r="C377" s="10">
+        <v>15.07</v>
+      </c>
+    </row>
+    <row r="378" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A378" s="11">
+        <v>43713</v>
+      </c>
+      <c r="B378" s="13">
+        <v>0.24753472222222225</v>
+      </c>
+      <c r="C378" s="10">
+        <v>15.08</v>
+      </c>
+    </row>
+    <row r="379" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A379" s="11">
+        <v>43713</v>
+      </c>
+      <c r="B379" s="13">
+        <v>0.25447916666666665</v>
+      </c>
+      <c r="C379" s="10">
+        <v>15.12</v>
+      </c>
+    </row>
+    <row r="380" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A380" s="11">
+        <v>43713</v>
+      </c>
+      <c r="B380" s="13">
+        <v>0.26142361111111112</v>
+      </c>
+      <c r="C380" s="10">
+        <v>15.06</v>
+      </c>
+    </row>
+    <row r="381" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A381" s="11">
+        <v>43713</v>
+      </c>
+      <c r="B381" s="13">
+        <v>0.26836805555555554</v>
+      </c>
+      <c r="C381" s="10">
+        <v>15.06</v>
+      </c>
+    </row>
+    <row r="382" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A382" s="11">
+        <v>43713</v>
+      </c>
+      <c r="B382" s="13">
+        <v>0.27531250000000002</v>
+      </c>
+      <c r="C382" s="10">
+        <v>15.08</v>
+      </c>
+    </row>
+    <row r="383" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A383" s="11">
+        <v>43713</v>
+      </c>
+      <c r="B383" s="13">
+        <v>0.28225694444444444</v>
+      </c>
+      <c r="C383" s="10">
+        <v>15.1</v>
+      </c>
+    </row>
+    <row r="384" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A384" s="11">
+        <v>43713</v>
+      </c>
+      <c r="B384" s="13">
+        <v>0.28920138888888891</v>
+      </c>
+      <c r="C384" s="10">
+        <v>15.18</v>
+      </c>
+    </row>
+    <row r="385" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A385" s="11">
+        <v>43713</v>
+      </c>
+      <c r="B385" s="13">
+        <v>0.29614583333333333</v>
+      </c>
+      <c r="C385" s="10">
+        <v>15.21</v>
+      </c>
+    </row>
+    <row r="386" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A386" s="11">
+        <v>43713</v>
+      </c>
+      <c r="B386" s="13">
+        <v>0.30309027777777781</v>
+      </c>
+      <c r="C386" s="10">
+        <v>15.22</v>
+      </c>
+    </row>
+    <row r="387" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A387" s="11">
+        <v>43713</v>
+      </c>
+      <c r="B387" s="13">
+        <v>0.31003472222222223</v>
+      </c>
+      <c r="C387" s="10">
+        <v>15.25</v>
+      </c>
+    </row>
+    <row r="388" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A388" s="11">
+        <v>43713</v>
+      </c>
+      <c r="B388" s="13">
+        <v>0.31697916666666665</v>
+      </c>
+      <c r="C388" s="10">
+        <v>15.23</v>
+      </c>
+    </row>
+    <row r="389" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A389" s="11">
+        <v>43713</v>
+      </c>
+      <c r="B389" s="13">
+        <v>0.32392361111111112</v>
+      </c>
+      <c r="C389" s="10">
+        <v>15.27</v>
+      </c>
+    </row>
+    <row r="390" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A390" s="11">
+        <v>43713</v>
+      </c>
+      <c r="B390" s="13">
+        <v>0.32826388888888891</v>
+      </c>
+      <c r="C390" s="9"/>
+    </row>
+    <row r="391" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A391" s="11">
+        <v>43713</v>
+      </c>
+      <c r="B391" s="13">
+        <v>0.32836805555555554</v>
+      </c>
+      <c r="C391" s="9"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55F6BF2F-CBB2-4331-929A-D3F4AD694052}">
   <dimension ref="A1:AC37"/>
   <sheetViews>
@@ -56078,7 +60419,7 @@
         <v>1</v>
       </c>
       <c r="AC24" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="25" spans="1:29" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Sept 6 morning kelp photos, data update
</commit_message>
<xml_diff>
--- a/data/raw.xlsx
+++ b/data/raw.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/EcosystemRecoveryLab/github/Ritger-Corynactis-urchin-deterrence/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5B170A2-78E2-4E4D-B883-45B17E322EDA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2357E454-3074-9940-ABBB-D3298DE8BA57}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14940" yWindow="2400" windowWidth="33520" windowHeight="25300" activeTab="1" xr2:uid="{58E670A5-634C-427F-960F-9DA76C64E810}"/>
+    <workbookView xWindow="21520" yWindow="14200" windowWidth="25720" windowHeight="12840" activeTab="1" xr2:uid="{58E670A5-634C-427F-960F-9DA76C64E810}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="3" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="108">
   <si>
     <t>Day</t>
   </si>
@@ -349,6 +349,9 @@
   </si>
   <si>
     <t>New</t>
+  </si>
+  <si>
+    <t>rip in "after", includes shadows, "before" is also a mess</t>
   </si>
 </sst>
 </file>
@@ -49650,9 +49653,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD5E687B-43EE-4B00-8604-7EB9984510DD}">
   <dimension ref="A1:Y77"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M69" sqref="M69"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A49" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="S72" sqref="S72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -54787,7 +54790,13 @@
         <v>0</v>
       </c>
       <c r="L66" s="7">
-        <v>0</v>
+        <v>56</v>
+      </c>
+      <c r="M66" s="4">
+        <v>82</v>
+      </c>
+      <c r="N66" s="4">
+        <v>88</v>
       </c>
       <c r="O66" s="4" t="s">
         <v>106</v>
@@ -54796,13 +54805,29 @@
         <f t="shared" si="10"/>
         <v>9</v>
       </c>
+      <c r="Q66">
+        <v>1920</v>
+      </c>
+      <c r="R66">
+        <v>720</v>
+      </c>
+      <c r="S66">
+        <v>69.959000000000003</v>
+      </c>
+      <c r="T66">
+        <f>52.246+3.913</f>
+        <v>56.158999999999999</v>
+      </c>
       <c r="U66">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="V66" t="e">
+        <v>13.800000000000004</v>
+      </c>
+      <c r="V66">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
+        <v>0.19725839420231855</v>
+      </c>
+      <c r="W66" t="s">
+        <v>87</v>
       </c>
       <c r="X66" t="str">
         <f t="shared" si="6"/>
@@ -54841,7 +54866,13 @@
         <v>17</v>
       </c>
       <c r="L67" s="7">
-        <v>0</v>
+        <v>43</v>
+      </c>
+      <c r="M67" s="4">
+        <v>36</v>
+      </c>
+      <c r="N67" s="4">
+        <v>38</v>
       </c>
       <c r="O67" s="4" t="s">
         <v>106</v>
@@ -54850,13 +54881,28 @@
         <f t="shared" si="10"/>
         <v>9</v>
       </c>
+      <c r="Q67">
+        <v>1920</v>
+      </c>
+      <c r="R67">
+        <v>720</v>
+      </c>
+      <c r="S67">
+        <v>79.831999999999994</v>
+      </c>
+      <c r="T67">
+        <v>58.262999999999998</v>
+      </c>
       <c r="U67">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="V67" t="e">
+        <v>21.568999999999996</v>
+      </c>
+      <c r="V67">
         <f t="shared" ref="V67:V77" si="12">U67/S67</f>
-        <v>#DIV/0!</v>
+        <v>0.2701798777432608</v>
+      </c>
+      <c r="W67" t="s">
+        <v>87</v>
       </c>
       <c r="X67" t="str">
         <f t="shared" ref="X67:X77" si="13">IF(E67&gt;6,"no","yes")</f>
@@ -54895,7 +54941,13 @@
         <v>24</v>
       </c>
       <c r="L68" s="7">
-        <v>0</v>
+        <v>56</v>
+      </c>
+      <c r="M68" s="4">
+        <v>88</v>
+      </c>
+      <c r="N68" s="4">
+        <v>86</v>
       </c>
       <c r="O68" s="4" t="s">
         <v>106</v>
@@ -54904,18 +54956,36 @@
         <f t="shared" si="10"/>
         <v>9</v>
       </c>
+      <c r="Q68">
+        <v>1920</v>
+      </c>
+      <c r="R68">
+        <v>720</v>
+      </c>
+      <c r="S68">
+        <v>79.995000000000005</v>
+      </c>
+      <c r="T68">
+        <v>82.188999999999993</v>
+      </c>
       <c r="U68">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="V68" t="e">
+        <v>-2.1939999999999884</v>
+      </c>
+      <c r="V68">
         <f t="shared" si="12"/>
-        <v>#DIV/0!</v>
+        <v>-2.7426714169635456E-2</v>
+      </c>
+      <c r="W68" t="s">
+        <v>88</v>
       </c>
       <c r="X68" t="str">
         <f t="shared" si="13"/>
         <v>yes</v>
       </c>
+      <c r="Y68" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="69" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A69">
@@ -54949,7 +55019,13 @@
         <v>22</v>
       </c>
       <c r="L69" s="7">
-        <v>0</v>
+        <v>58</v>
+      </c>
+      <c r="M69" s="4">
+        <v>84</v>
+      </c>
+      <c r="N69" s="4">
+        <v>86</v>
       </c>
       <c r="O69" s="4" t="s">
         <v>106</v>
@@ -54958,13 +55034,28 @@
         <f t="shared" si="10"/>
         <v>9</v>
       </c>
+      <c r="Q69">
+        <v>1920</v>
+      </c>
+      <c r="R69">
+        <v>720</v>
+      </c>
+      <c r="S69">
+        <v>74.331000000000003</v>
+      </c>
+      <c r="T69">
+        <v>44.713000000000001</v>
+      </c>
       <c r="U69">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="V69" t="e">
+        <v>29.618000000000002</v>
+      </c>
+      <c r="V69">
         <f t="shared" si="12"/>
-        <v>#DIV/0!</v>
+        <v>0.39846093823572937</v>
+      </c>
+      <c r="W69" t="s">
+        <v>87</v>
       </c>
       <c r="X69" t="str">
         <f t="shared" si="13"/>
@@ -55003,7 +55094,13 @@
         <v>28</v>
       </c>
       <c r="L70" s="7">
-        <v>0</v>
+        <v>60</v>
+      </c>
+      <c r="M70" s="4">
+        <v>101</v>
+      </c>
+      <c r="N70" s="4">
+        <v>102</v>
       </c>
       <c r="O70" s="4" t="s">
         <v>106</v>
@@ -55012,13 +55109,28 @@
         <f t="shared" si="10"/>
         <v>9</v>
       </c>
+      <c r="Q70">
+        <v>1920</v>
+      </c>
+      <c r="R70">
+        <v>720</v>
+      </c>
+      <c r="S70">
+        <v>55.595999999999997</v>
+      </c>
+      <c r="T70">
+        <v>56.017000000000003</v>
+      </c>
       <c r="U70">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="V70" t="e">
+        <v>-0.42100000000000648</v>
+      </c>
+      <c r="V70">
         <f t="shared" si="12"/>
-        <v>#DIV/0!</v>
+        <v>-7.572487229297189E-3</v>
+      </c>
+      <c r="W70" t="s">
+        <v>88</v>
       </c>
       <c r="X70" t="str">
         <f t="shared" si="13"/>
@@ -55057,7 +55169,13 @@
         <v>10</v>
       </c>
       <c r="L71" s="7">
-        <v>0</v>
+        <v>42</v>
+      </c>
+      <c r="M71" s="4">
+        <v>36</v>
+      </c>
+      <c r="N71" s="4">
+        <v>39</v>
       </c>
       <c r="O71" s="4" t="s">
         <v>106</v>
@@ -55066,13 +55184,28 @@
         <f t="shared" si="10"/>
         <v>9</v>
       </c>
+      <c r="Q71">
+        <v>1920</v>
+      </c>
+      <c r="R71">
+        <v>720</v>
+      </c>
+      <c r="S71">
+        <v>73.046999999999997</v>
+      </c>
+      <c r="T71">
+        <v>45.68</v>
+      </c>
       <c r="U71">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="V71" t="e">
+        <v>27.366999999999997</v>
+      </c>
+      <c r="V71">
         <f t="shared" si="12"/>
-        <v>#DIV/0!</v>
+        <v>0.37464919846126465</v>
+      </c>
+      <c r="W71" t="s">
+        <v>87</v>
       </c>
       <c r="X71" t="str">
         <f t="shared" si="13"/>
@@ -62344,11 +62477,11 @@
       </c>
       <c r="I26">
         <f>'Kelp consumption'!L66</f>
-        <v>0</v>
+        <v>56</v>
       </c>
       <c r="J26">
         <f>'Kelp consumption'!M66</f>
-        <v>0</v>
+        <v>82</v>
       </c>
       <c r="K26">
         <f>'Kelp consumption'!P66</f>
@@ -62356,11 +62489,11 @@
       </c>
       <c r="L26">
         <f>'Kelp consumption'!Q66</f>
-        <v>0</v>
+        <v>1920</v>
       </c>
       <c r="M26">
         <f>'Kelp consumption'!R66</f>
-        <v>0</v>
+        <v>720</v>
       </c>
     </row>
     <row r="27" spans="1:29" x14ac:dyDescent="0.2">
@@ -62393,11 +62526,11 @@
       </c>
       <c r="I27">
         <f>'Kelp consumption'!L67</f>
-        <v>0</v>
+        <v>43</v>
       </c>
       <c r="J27">
         <f>'Kelp consumption'!M67</f>
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="K27">
         <f>'Kelp consumption'!P67</f>
@@ -62405,11 +62538,11 @@
       </c>
       <c r="L27">
         <f>'Kelp consumption'!Q67</f>
-        <v>0</v>
+        <v>1920</v>
       </c>
       <c r="M27">
         <f>'Kelp consumption'!R67</f>
-        <v>0</v>
+        <v>720</v>
       </c>
     </row>
     <row r="28" spans="1:29" x14ac:dyDescent="0.2">
@@ -62442,11 +62575,11 @@
       </c>
       <c r="I28">
         <f>'Kelp consumption'!L68</f>
-        <v>0</v>
+        <v>56</v>
       </c>
       <c r="J28">
         <f>'Kelp consumption'!M68</f>
-        <v>0</v>
+        <v>88</v>
       </c>
       <c r="K28">
         <f>'Kelp consumption'!P68</f>
@@ -62454,11 +62587,11 @@
       </c>
       <c r="L28">
         <f>'Kelp consumption'!Q68</f>
-        <v>0</v>
+        <v>1920</v>
       </c>
       <c r="M28">
         <f>'Kelp consumption'!R68</f>
-        <v>0</v>
+        <v>720</v>
       </c>
     </row>
     <row r="29" spans="1:29" x14ac:dyDescent="0.2">
@@ -62491,11 +62624,11 @@
       </c>
       <c r="I29">
         <f>'Kelp consumption'!L69</f>
-        <v>0</v>
+        <v>58</v>
       </c>
       <c r="J29">
         <f>'Kelp consumption'!M69</f>
-        <v>0</v>
+        <v>84</v>
       </c>
       <c r="K29">
         <f>'Kelp consumption'!P69</f>
@@ -62503,11 +62636,11 @@
       </c>
       <c r="L29">
         <f>'Kelp consumption'!Q69</f>
-        <v>0</v>
+        <v>1920</v>
       </c>
       <c r="M29">
         <f>'Kelp consumption'!R69</f>
-        <v>0</v>
+        <v>720</v>
       </c>
     </row>
     <row r="30" spans="1:29" x14ac:dyDescent="0.2">
@@ -62540,11 +62673,11 @@
       </c>
       <c r="I30">
         <f>'Kelp consumption'!L70</f>
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="J30">
         <f>'Kelp consumption'!M70</f>
-        <v>0</v>
+        <v>101</v>
       </c>
       <c r="K30">
         <f>'Kelp consumption'!P70</f>
@@ -62552,11 +62685,11 @@
       </c>
       <c r="L30">
         <f>'Kelp consumption'!Q70</f>
-        <v>0</v>
+        <v>1920</v>
       </c>
       <c r="M30">
         <f>'Kelp consumption'!R70</f>
-        <v>0</v>
+        <v>720</v>
       </c>
     </row>
     <row r="31" spans="1:29" x14ac:dyDescent="0.2">
@@ -62589,11 +62722,11 @@
       </c>
       <c r="I31">
         <f>'Kelp consumption'!L71</f>
-        <v>0</v>
+        <v>42</v>
       </c>
       <c r="J31">
         <f>'Kelp consumption'!M71</f>
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="K31">
         <f>'Kelp consumption'!P71</f>
@@ -62601,11 +62734,11 @@
       </c>
       <c r="L31">
         <f>'Kelp consumption'!Q71</f>
-        <v>0</v>
+        <v>1920</v>
       </c>
       <c r="M31">
         <f>'Kelp consumption'!R71</f>
-        <v>0</v>
+        <v>720</v>
       </c>
     </row>
     <row r="32" spans="1:29" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
updated to remove "holes" from kelp photos
</commit_message>
<xml_diff>
--- a/data/raw.xlsx
+++ b/data/raw.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/EcosystemRecoveryLab/github/Ritger-Corynactis-urchin-deterrence/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2357E454-3074-9940-ABBB-D3298DE8BA57}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF01F890-3348-EA4E-862F-12AFA2D528F7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21520" yWindow="14200" windowWidth="25720" windowHeight="12840" activeTab="1" xr2:uid="{58E670A5-634C-427F-960F-9DA76C64E810}"/>
+    <workbookView xWindow="4820" yWindow="15900" windowWidth="44860" windowHeight="10140" activeTab="1" xr2:uid="{58E670A5-634C-427F-960F-9DA76C64E810}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="3" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="102">
   <si>
     <t>Day</t>
   </si>
@@ -270,22 +270,10 @@
     <t>N/A</t>
   </si>
   <si>
-    <t>too much measured on "after"</t>
-  </si>
-  <si>
-    <t>not enough measured on "before"</t>
-  </si>
-  <si>
-    <t>"after" included hole</t>
-  </si>
-  <si>
     <t xml:space="preserve">too much measured on "after" </t>
   </si>
   <si>
     <t>shade =&gt; guesstimate</t>
-  </si>
-  <si>
-    <t>"after" included some shadow</t>
   </si>
   <si>
     <t>"before" and "after" included some shadow</t>
@@ -300,13 +288,7 @@
     <t>NO</t>
   </si>
   <si>
-    <t>hole included in "after"</t>
-  </si>
-  <si>
     <t>"before" included some shadow</t>
-  </si>
-  <si>
-    <t>hole included in "before"</t>
   </si>
   <si>
     <t>Kelp visibly consumed?</t>
@@ -322,9 +304,6 @@
   </si>
   <si>
     <t>"before" out of focus, "after" includes shadows</t>
-  </si>
-  <si>
-    <t>"before" included some holes, "after" includes holes</t>
   </si>
   <si>
     <t>4 hours video</t>
@@ -352,6 +331,9 @@
   </si>
   <si>
     <t>rip in "after", includes shadows, "before" is also a mess</t>
+  </si>
+  <si>
+    <t>"after" has hole (-0.264), doesn't look like consumption</t>
   </si>
 </sst>
 </file>
@@ -49653,9 +49635,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD5E687B-43EE-4B00-8604-7EB9984510DD}">
   <dimension ref="A1:Y77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A49" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S72" sqref="S72"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="V2" sqref="V2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -49696,13 +49678,13 @@
         <v>53</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>3</v>
@@ -49729,7 +49711,7 @@
         <v>65</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="P1" s="2" t="s">
         <v>9</v>
@@ -49753,7 +49735,7 @@
         <v>14</v>
       </c>
       <c r="W1" s="2" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="X1" s="2" t="s">
         <v>25</v>
@@ -49803,7 +49785,7 @@
         <v>72</v>
       </c>
       <c r="O2" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="P2">
         <f>C2-236</f>
@@ -49830,7 +49812,7 @@
         <v>0.10844212089339854</v>
       </c>
       <c r="W2" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="X2" t="str">
         <f>IF(E2&gt;6,"no","yes")</f>
@@ -49878,7 +49860,7 @@
         <v>35</v>
       </c>
       <c r="O3" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="P3">
         <f t="shared" ref="P3:P43" si="4">C3-236</f>
@@ -49905,14 +49887,14 @@
         <v>1.3448262101440619E-2</v>
       </c>
       <c r="W3" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="X3" t="str">
         <f t="shared" ref="X3:X66" si="6">IF(E3&gt;6,"no","yes")</f>
         <v>yes</v>
       </c>
       <c r="Y3" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.2">
@@ -49956,7 +49938,7 @@
         <v>43</v>
       </c>
       <c r="O4" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="P4">
         <f t="shared" si="4"/>
@@ -49983,7 +49965,7 @@
         <v>0.28380160052328729</v>
       </c>
       <c r="W4" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="X4" t="str">
         <f t="shared" si="6"/>
@@ -50031,7 +50013,7 @@
         <v>52</v>
       </c>
       <c r="O5" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="P5">
         <f t="shared" si="4"/>
@@ -50044,29 +50026,27 @@
         <v>730</v>
       </c>
       <c r="S5">
-        <v>123.244</v>
+        <v>122.58199999999999</v>
       </c>
       <c r="T5">
-        <v>106.542</v>
+        <f>106.542-2.069</f>
+        <v>104.473</v>
       </c>
       <c r="U5">
         <f t="shared" si="0"/>
-        <v>16.701999999999998</v>
+        <v>18.108999999999995</v>
       </c>
       <c r="V5">
         <f t="shared" si="5"/>
-        <v>0.13551978189607605</v>
+        <v>0.1477296829877143</v>
       </c>
       <c r="W5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="X5" t="str">
         <f t="shared" si="6"/>
         <v>yes</v>
       </c>
-      <c r="Y5" t="s">
-        <v>98</v>
-      </c>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A6">
@@ -50109,7 +50089,7 @@
         <v>58</v>
       </c>
       <c r="O6" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="P6">
         <f t="shared" si="4"/>
@@ -50136,14 +50116,14 @@
         <v>0.25604737440407477</v>
       </c>
       <c r="W6" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="X6" t="str">
         <f t="shared" si="6"/>
         <v>yes</v>
       </c>
       <c r="Y6" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.2">
@@ -50187,7 +50167,7 @@
         <v>41</v>
       </c>
       <c r="O7" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="P7">
         <f t="shared" si="4"/>
@@ -50203,26 +50183,24 @@
         <v>119.378</v>
       </c>
       <c r="T7">
-        <v>105.98</v>
+        <f>105.98-0.246</f>
+        <v>105.73400000000001</v>
       </c>
       <c r="U7">
         <f t="shared" si="0"/>
-        <v>13.397999999999996</v>
+        <v>13.643999999999991</v>
       </c>
       <c r="V7">
         <f t="shared" si="5"/>
-        <v>0.11223173449044209</v>
+        <v>0.11429241568798264</v>
       </c>
       <c r="W7" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="X7" t="str">
         <f t="shared" si="6"/>
         <v>yes</v>
       </c>
-      <c r="Y7" t="s">
-        <v>82</v>
-      </c>
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A8">
@@ -50268,7 +50246,7 @@
         <v>78</v>
       </c>
       <c r="O8" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="P8">
         <f t="shared" si="4"/>
@@ -50295,7 +50273,7 @@
         <v>-2.3323421800214282E-3</v>
       </c>
       <c r="W8" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="X8" t="str">
         <f t="shared" si="6"/>
@@ -50346,7 +50324,7 @@
         <v>95</v>
       </c>
       <c r="O9" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="P9">
         <f t="shared" si="4"/>
@@ -50373,7 +50351,7 @@
         <v>-5.7143858788059479E-3</v>
       </c>
       <c r="W9" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="X9" t="str">
         <f t="shared" si="6"/>
@@ -50424,7 +50402,7 @@
         <v>50</v>
       </c>
       <c r="O10" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="P10">
         <f t="shared" si="4"/>
@@ -50451,14 +50429,14 @@
         <v>-5.7725522069621595E-3</v>
       </c>
       <c r="W10" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="X10" t="str">
         <f t="shared" si="6"/>
         <v>no</v>
       </c>
       <c r="Y10" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.2">
@@ -50505,7 +50483,7 @@
         <v>62</v>
       </c>
       <c r="O11" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="P11">
         <f t="shared" si="4"/>
@@ -50532,14 +50510,14 @@
         <v>2.0172553505886835E-2</v>
       </c>
       <c r="W11" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="X11" t="str">
         <f t="shared" si="6"/>
         <v>no</v>
       </c>
       <c r="Y11" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.2">
@@ -50586,7 +50564,7 @@
         <v>89</v>
       </c>
       <c r="O12" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="P12">
         <f t="shared" si="4"/>
@@ -50613,14 +50591,14 @@
         <v>0.23731693570773646</v>
       </c>
       <c r="W12" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="X12" t="str">
         <f t="shared" si="6"/>
         <v>no</v>
       </c>
       <c r="Y12" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.2">
@@ -50667,7 +50645,7 @@
         <v>43</v>
       </c>
       <c r="O13" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="P13">
         <f t="shared" si="4"/>
@@ -50694,14 +50672,14 @@
         <v>0.21320720819240585</v>
       </c>
       <c r="W13" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="X13" t="str">
         <f t="shared" si="6"/>
         <v>no</v>
       </c>
       <c r="Y13" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.2">
@@ -50748,7 +50726,7 @@
         <v>53</v>
       </c>
       <c r="O14" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="P14">
         <f t="shared" si="4"/>
@@ -50775,14 +50753,14 @@
         <v>0.10589024007332033</v>
       </c>
       <c r="W14" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="X14" t="str">
         <f t="shared" si="6"/>
         <v>no</v>
       </c>
       <c r="Y14" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.2">
@@ -50829,7 +50807,7 @@
         <v>60</v>
       </c>
       <c r="O15" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="P15">
         <f t="shared" si="4"/>
@@ -50856,14 +50834,14 @@
         <v>1.5342360900055151E-2</v>
       </c>
       <c r="W15" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="X15" t="str">
         <f t="shared" si="6"/>
         <v>no</v>
       </c>
       <c r="Y15" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.2">
@@ -50907,7 +50885,7 @@
         <v>45</v>
       </c>
       <c r="O16" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="P16">
         <f t="shared" si="4"/>
@@ -50934,7 +50912,7 @@
         <v>1.1132188960347966E-2</v>
       </c>
       <c r="W16" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="X16" t="str">
         <f t="shared" si="6"/>
@@ -50982,7 +50960,7 @@
         <v>41</v>
       </c>
       <c r="O17" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="P17">
         <f t="shared" si="4"/>
@@ -51010,14 +50988,14 @@
         <v>0.34767247318177341</v>
       </c>
       <c r="W17" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="X17" t="str">
         <f t="shared" si="6"/>
         <v>yes</v>
       </c>
       <c r="Y17" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="18" spans="1:25" x14ac:dyDescent="0.2">
@@ -51061,7 +51039,7 @@
         <v>85</v>
       </c>
       <c r="O18" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="P18">
         <f t="shared" si="4"/>
@@ -51088,14 +51066,14 @@
         <v>1.4320708498209772E-2</v>
       </c>
       <c r="W18" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="X18" t="str">
         <f t="shared" si="6"/>
         <v>yes</v>
       </c>
       <c r="Y18" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="19" spans="1:25" x14ac:dyDescent="0.2">
@@ -51139,7 +51117,7 @@
         <v>51</v>
       </c>
       <c r="O19" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="P19">
         <f t="shared" si="4"/>
@@ -51166,7 +51144,7 @@
         <v>2.0570354813750462E-2</v>
       </c>
       <c r="W19" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="X19" t="str">
         <f t="shared" si="6"/>
@@ -51214,7 +51192,7 @@
         <v>61</v>
       </c>
       <c r="O20" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="P20">
         <f t="shared" si="4"/>
@@ -51241,7 +51219,7 @@
         <v>0.19619130289116807</v>
       </c>
       <c r="W20" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="X20" t="str">
         <f t="shared" si="6"/>
@@ -51289,7 +51267,7 @@
         <v>45</v>
       </c>
       <c r="O21" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="P21">
         <f t="shared" si="4"/>
@@ -51316,7 +51294,7 @@
         <v>6.3789631285387843E-3</v>
       </c>
       <c r="W21" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="X21" t="str">
         <f t="shared" si="6"/>
@@ -51367,7 +51345,7 @@
         <v>53</v>
       </c>
       <c r="O22" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="P22">
         <f t="shared" si="4"/>
@@ -51394,15 +51372,12 @@
         <v>9.8303023234503264E-3</v>
       </c>
       <c r="W22" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="X22" t="str">
         <f t="shared" si="6"/>
         <v>no</v>
       </c>
-      <c r="Y22" t="s">
-        <v>81</v>
-      </c>
     </row>
     <row r="23" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A23">
@@ -51448,7 +51423,7 @@
         <v>79</v>
       </c>
       <c r="O23" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="P23">
         <f t="shared" si="4"/>
@@ -51464,26 +51439,23 @@
         <v>122.246</v>
       </c>
       <c r="T23">
-        <v>123.928</v>
+        <v>122.38800000000001</v>
       </c>
       <c r="U23">
         <f t="shared" si="7"/>
-        <v>-1.6820000000000022</v>
+        <v>-0.14200000000001012</v>
       </c>
       <c r="V23">
         <f t="shared" si="5"/>
-        <v>-1.3759141403399721E-2</v>
+        <v>-1.1615921993358483E-3</v>
       </c>
       <c r="W23" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="X23" t="str">
         <f t="shared" si="6"/>
         <v>no</v>
       </c>
-      <c r="Y23" t="s">
-        <v>80</v>
-      </c>
     </row>
     <row r="24" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A24">
@@ -51529,7 +51501,7 @@
         <v>51</v>
       </c>
       <c r="O24" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="P24">
         <f t="shared" si="4"/>
@@ -51556,7 +51528,7 @@
         <v>7.2046396683673368E-3</v>
       </c>
       <c r="W24" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="X24" t="str">
         <f t="shared" si="6"/>
@@ -51607,7 +51579,7 @@
         <v>56</v>
       </c>
       <c r="O25" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="P25">
         <f t="shared" si="4"/>
@@ -51634,7 +51606,7 @@
         <v>1.6066314050968911E-2</v>
       </c>
       <c r="W25" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="X25" t="str">
         <f t="shared" si="6"/>
@@ -51685,7 +51657,7 @@
         <v>94</v>
       </c>
       <c r="O26" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="P26">
         <f t="shared" si="4"/>
@@ -51701,26 +51673,24 @@
         <v>103.68300000000001</v>
       </c>
       <c r="T26">
-        <v>92.808999999999997</v>
+        <f>92.809-0.322</f>
+        <v>92.486999999999995</v>
       </c>
       <c r="U26">
         <f t="shared" si="7"/>
-        <v>10.874000000000009</v>
+        <v>11.196000000000012</v>
       </c>
       <c r="V26">
         <f t="shared" si="5"/>
-        <v>0.104877366588544</v>
+        <v>0.107982986603397</v>
       </c>
       <c r="W26" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="X26" t="str">
         <f t="shared" si="6"/>
         <v>no</v>
       </c>
-      <c r="Y26" t="s">
-        <v>82</v>
-      </c>
     </row>
     <row r="27" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A27">
@@ -51766,7 +51736,7 @@
         <v>35</v>
       </c>
       <c r="O27" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="P27">
         <f t="shared" si="4"/>
@@ -51793,7 +51763,7 @@
         <v>3.2134809444497774E-3</v>
       </c>
       <c r="W27" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="X27" t="str">
         <f t="shared" si="6"/>
@@ -51844,7 +51814,7 @@
         <v>45</v>
       </c>
       <c r="O28" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="P28">
         <f t="shared" si="4"/>
@@ -51871,7 +51841,7 @@
         <v>1.712374076244115E-2</v>
       </c>
       <c r="W28" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="X28" t="str">
         <f t="shared" si="6"/>
@@ -51922,7 +51892,7 @@
         <v>41</v>
       </c>
       <c r="O29" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="P29">
         <f t="shared" si="4"/>
@@ -51949,7 +51919,7 @@
         <v>3.8196991929567187E-2</v>
       </c>
       <c r="W29" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="X29" t="str">
         <f t="shared" si="6"/>
@@ -51997,7 +51967,7 @@
         <v>98</v>
       </c>
       <c r="O30" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="P30">
         <f t="shared" si="4"/>
@@ -52025,7 +51995,7 @@
         <v>0.39414566228714759</v>
       </c>
       <c r="W30" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="X30" t="str">
         <f t="shared" si="6"/>
@@ -52073,7 +52043,7 @@
         <v>42</v>
       </c>
       <c r="O31" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="P31">
         <f t="shared" si="4"/>
@@ -52100,7 +52070,7 @@
         <v>0.28625451046427708</v>
       </c>
       <c r="W31" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="X31" t="str">
         <f t="shared" si="6"/>
@@ -52148,7 +52118,7 @@
         <v>63</v>
       </c>
       <c r="O32" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="P32">
         <f t="shared" si="4"/>
@@ -52175,7 +52145,7 @@
         <v>0.17109784527483193</v>
       </c>
       <c r="W32" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="X32" t="str">
         <f t="shared" si="6"/>
@@ -52223,7 +52193,7 @@
         <v>47</v>
       </c>
       <c r="O33" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="P33">
         <f t="shared" si="4"/>
@@ -52250,7 +52220,7 @@
         <v>-1.4416269790191878E-2</v>
       </c>
       <c r="W33" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="X33" t="str">
         <f t="shared" si="6"/>
@@ -52298,7 +52268,7 @@
         <v>75</v>
       </c>
       <c r="O34" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="P34">
         <f t="shared" si="4"/>
@@ -52314,27 +52284,24 @@
         <v>84.347999999999999</v>
       </c>
       <c r="T34">
-        <f>41.388+15.325</f>
-        <v>56.712999999999994</v>
+        <f>41.388+15.325-0.131</f>
+        <v>56.581999999999994</v>
       </c>
       <c r="U34">
         <f t="shared" si="7"/>
-        <v>27.635000000000005</v>
+        <v>27.766000000000005</v>
       </c>
       <c r="V34">
         <f t="shared" si="5"/>
-        <v>0.32763076777161293</v>
+        <v>0.32918385735287148</v>
       </c>
       <c r="W34" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="X34" t="str">
         <f t="shared" si="6"/>
         <v>yes</v>
       </c>
-      <c r="Y34" t="s">
-        <v>82</v>
-      </c>
     </row>
     <row r="35" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A35">
@@ -52377,7 +52344,7 @@
         <v>47</v>
       </c>
       <c r="O35" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="P35">
         <f t="shared" si="4"/>
@@ -52404,15 +52371,12 @@
         <v>1.0624224886316719E-2</v>
       </c>
       <c r="W35" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="X35" t="str">
         <f t="shared" si="6"/>
         <v>yes</v>
       </c>
-      <c r="Y35" t="s">
-        <v>85</v>
-      </c>
     </row>
     <row r="36" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A36">
@@ -52458,7 +52422,7 @@
         <v>63</v>
       </c>
       <c r="O36" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="P36">
         <f t="shared" si="4"/>
@@ -52485,7 +52449,7 @@
         <v>0.33511229946524063</v>
       </c>
       <c r="W36" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="X36" t="str">
         <f t="shared" si="6"/>
@@ -52536,7 +52500,7 @@
         <v>50</v>
       </c>
       <c r="O37" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="P37">
         <f t="shared" si="4"/>
@@ -52563,7 +52527,7 @@
         <v>8.9727722772276596E-3</v>
       </c>
       <c r="W37" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="X37" t="str">
         <f t="shared" si="6"/>
@@ -52614,7 +52578,7 @@
         <v>47</v>
       </c>
       <c r="O38" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="P38">
         <f t="shared" si="4"/>
@@ -52630,26 +52594,24 @@
         <v>101.639</v>
       </c>
       <c r="T38">
-        <v>73.361999999999995</v>
+        <f>73.362-0.067</f>
+        <v>73.295000000000002</v>
       </c>
       <c r="U38">
         <f t="shared" si="7"/>
-        <v>28.277000000000001</v>
+        <v>28.343999999999994</v>
       </c>
       <c r="V38">
         <f t="shared" si="5"/>
-        <v>0.27821013587304089</v>
+        <v>0.27886933165418781</v>
       </c>
       <c r="W38" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="X38" t="str">
         <f t="shared" si="6"/>
         <v>no</v>
       </c>
-      <c r="Y38" t="s">
-        <v>82</v>
-      </c>
     </row>
     <row r="39" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A39">
@@ -52695,7 +52657,7 @@
         <v>73</v>
       </c>
       <c r="O39" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="P39">
         <f t="shared" si="4"/>
@@ -52722,7 +52684,7 @@
         <v>0.50121017042193783</v>
       </c>
       <c r="W39" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="X39" t="str">
         <f t="shared" si="6"/>
@@ -52773,7 +52735,7 @@
         <v>70</v>
       </c>
       <c r="O40" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="P40">
         <f t="shared" si="4"/>
@@ -52800,7 +52762,7 @@
         <v>0.42735033602940398</v>
       </c>
       <c r="W40" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="X40" t="str">
         <f t="shared" si="6"/>
@@ -52851,7 +52813,7 @@
         <v>89</v>
       </c>
       <c r="O41" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="P41">
         <f t="shared" si="4"/>
@@ -52879,7 +52841,7 @@
         <v>0.91152623616800665</v>
       </c>
       <c r="W41" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="X41" t="str">
         <f t="shared" si="6"/>
@@ -52930,7 +52892,7 @@
         <v>83</v>
       </c>
       <c r="O42" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="P42">
         <f t="shared" si="4"/>
@@ -52957,7 +52919,7 @@
         <v>7.5201906527207442E-3</v>
       </c>
       <c r="W42" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="X42" t="str">
         <f t="shared" si="6"/>
@@ -53008,7 +52970,7 @@
         <v>57</v>
       </c>
       <c r="O43" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="P43">
         <f t="shared" si="4"/>
@@ -53035,14 +52997,14 @@
         <v>1.9049721461127905E-2</v>
       </c>
       <c r="W43" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="X43" t="str">
         <f t="shared" si="6"/>
         <v>no</v>
       </c>
       <c r="Y43" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="44" spans="1:25" x14ac:dyDescent="0.2">
@@ -53086,7 +53048,7 @@
         <v>93</v>
       </c>
       <c r="O44" s="4" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="P44">
         <v>7</v>
@@ -53112,7 +53074,7 @@
         <v>0.82234472298785199</v>
       </c>
       <c r="W44" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="X44" t="str">
         <f t="shared" si="6"/>
@@ -53160,7 +53122,7 @@
         <v>69</v>
       </c>
       <c r="O45" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="P45">
         <v>10</v>
@@ -53187,7 +53149,7 @@
         <v>0.11270882385917719</v>
       </c>
       <c r="W45" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="X45" t="str">
         <f t="shared" si="6"/>
@@ -53235,7 +53197,7 @@
         <v>35</v>
       </c>
       <c r="O46" s="4" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="P46">
         <v>7</v>
@@ -53261,7 +53223,7 @@
         <v>2.2921863412660948E-2</v>
       </c>
       <c r="W46" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="X46" t="str">
         <f t="shared" si="6"/>
@@ -53309,7 +53271,7 @@
         <v>91</v>
       </c>
       <c r="O47" s="4" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="P47">
         <v>7</v>
@@ -53335,10 +53297,10 @@
         <v>1.4539400665926773E-2</v>
       </c>
       <c r="W47" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="X47" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="48" spans="1:25" x14ac:dyDescent="0.2">
@@ -53382,7 +53344,7 @@
         <v>82</v>
       </c>
       <c r="O48" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="P48">
         <v>10</v>
@@ -53397,6 +53359,7 @@
         <v>93.19</v>
       </c>
       <c r="T48">
+        <f>92.295</f>
         <v>92.295000000000002</v>
       </c>
       <c r="U48">
@@ -53408,14 +53371,14 @@
         <v>9.6040347676788936E-3</v>
       </c>
       <c r="W48" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="X48" t="str">
         <f t="shared" si="6"/>
         <v>yes</v>
       </c>
       <c r="Y48" t="s">
-        <v>82</v>
+        <v>101</v>
       </c>
     </row>
     <row r="49" spans="1:25" x14ac:dyDescent="0.2">
@@ -53459,7 +53422,7 @@
         <v>36</v>
       </c>
       <c r="O49" s="4" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="P49">
         <v>7</v>
@@ -53485,7 +53448,7 @@
         <v>3.0082299064180036E-2</v>
       </c>
       <c r="W49" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="X49" t="str">
         <f t="shared" si="6"/>
@@ -53536,7 +53499,7 @@
         <v>55</v>
       </c>
       <c r="O50" s="4" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="P50">
         <v>7</v>
@@ -53563,14 +53526,14 @@
         <v>0.21193650793650795</v>
       </c>
       <c r="W50" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="X50" t="str">
         <f t="shared" si="6"/>
         <v>no</v>
       </c>
       <c r="Y50" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="51" spans="1:25" x14ac:dyDescent="0.2">
@@ -53617,7 +53580,7 @@
         <v>40</v>
       </c>
       <c r="O51" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="P51">
         <v>10</v>
@@ -53643,7 +53606,7 @@
         <v>3.2453875307150791E-2</v>
       </c>
       <c r="W51" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="X51" t="str">
         <f t="shared" si="6"/>
@@ -53694,7 +53657,7 @@
         <v>40</v>
       </c>
       <c r="O52" s="4" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="P52">
         <v>7</v>
@@ -53721,7 +53684,7 @@
         <v>0.2629165021413602</v>
       </c>
       <c r="W52" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="X52" t="str">
         <f t="shared" si="6"/>
@@ -53772,7 +53735,7 @@
         <v>61</v>
       </c>
       <c r="O53" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="P53">
         <v>10</v>
@@ -53784,29 +53747,27 @@
         <v>733</v>
       </c>
       <c r="S53">
-        <v>85.570999999999998</v>
+        <f>85.571-0.08</f>
+        <v>85.491</v>
       </c>
       <c r="T53">
         <v>85.394000000000005</v>
       </c>
       <c r="U53">
         <f t="shared" si="7"/>
-        <v>0.1769999999999925</v>
+        <v>9.6999999999994202E-2</v>
       </c>
       <c r="V53">
         <f t="shared" si="5"/>
-        <v>2.0684577719086196E-3</v>
+        <v>1.1346223579089519E-3</v>
       </c>
       <c r="W53" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="X53" t="str">
         <f t="shared" si="6"/>
         <v>no</v>
       </c>
-      <c r="Y53" t="s">
-        <v>92</v>
-      </c>
     </row>
     <row r="54" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A54">
@@ -53852,7 +53813,7 @@
         <v>57</v>
       </c>
       <c r="O54" s="4" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="P54">
         <v>7</v>
@@ -53867,26 +53828,24 @@
         <v>66.453000000000003</v>
       </c>
       <c r="T54">
-        <v>27.852</v>
+        <f>27.852-0.084</f>
+        <v>27.768000000000001</v>
       </c>
       <c r="U54">
         <f t="shared" si="7"/>
-        <v>38.600999999999999</v>
+        <v>38.685000000000002</v>
       </c>
       <c r="V54">
         <f t="shared" si="5"/>
-        <v>0.58087670985508555</v>
+        <v>0.5821407611394519</v>
       </c>
       <c r="W54" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="X54" t="str">
         <f t="shared" si="6"/>
         <v>no</v>
       </c>
-      <c r="Y54" t="s">
-        <v>90</v>
-      </c>
     </row>
     <row r="55" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A55">
@@ -53932,7 +53891,7 @@
         <v>51</v>
       </c>
       <c r="O55" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="P55">
         <v>10</v>
@@ -53958,7 +53917,7 @@
         <v>0.10254237288135591</v>
       </c>
       <c r="W55" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="X55" t="str">
         <f t="shared" si="6"/>
@@ -54009,7 +53968,7 @@
         <v>42</v>
       </c>
       <c r="O56" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="P56">
         <v>10</v>
@@ -54024,26 +53983,24 @@
         <v>85.197000000000003</v>
       </c>
       <c r="T56">
-        <v>67.561999999999998</v>
+        <f>67.562-0.061-0.044</f>
+        <v>67.456999999999994</v>
       </c>
       <c r="U56">
         <f t="shared" si="7"/>
-        <v>17.635000000000005</v>
+        <v>17.740000000000009</v>
       </c>
       <c r="V56">
         <f t="shared" si="5"/>
-        <v>0.20699085648555707</v>
+        <v>0.20822329424745012</v>
       </c>
       <c r="W56" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="X56" t="str">
         <f t="shared" si="6"/>
         <v>no</v>
       </c>
-      <c r="Y56" t="s">
-        <v>90</v>
-      </c>
     </row>
     <row r="57" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A57">
@@ -54089,7 +54046,7 @@
         <v>102</v>
       </c>
       <c r="O57" s="4" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="P57">
         <v>7</v>
@@ -54116,7 +54073,7 @@
         <v>0.33652352320299794</v>
       </c>
       <c r="W57" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="X57" t="str">
         <f t="shared" si="6"/>
@@ -54167,7 +54124,7 @@
         <v>99</v>
       </c>
       <c r="O58" s="4" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="P58">
         <f t="shared" ref="P58:P77" si="10">C58-239</f>
@@ -54194,7 +54151,7 @@
         <v>3.1191515907668613E-4</v>
       </c>
       <c r="W58" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="X58" t="str">
         <f t="shared" si="6"/>
@@ -54245,7 +54202,7 @@
         <v>102</v>
       </c>
       <c r="O59" s="4" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="P59">
         <f t="shared" si="10"/>
@@ -54273,7 +54230,7 @@
         <v>0.38184980366047527</v>
       </c>
       <c r="W59" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="X59" t="str">
         <f t="shared" si="6"/>
@@ -54324,7 +54281,7 @@
         <v>37</v>
       </c>
       <c r="O60" s="4" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="P60">
         <f t="shared" si="10"/>
@@ -54351,7 +54308,7 @@
         <v>-4.1907422693503683E-3</v>
       </c>
       <c r="W60" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="X60" t="str">
         <f t="shared" si="6"/>
@@ -54402,7 +54359,7 @@
         <v>74</v>
       </c>
       <c r="O61" s="4" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="P61">
         <f t="shared" si="10"/>
@@ -54429,7 +54386,7 @@
         <v>1.0433169200028467E-2</v>
       </c>
       <c r="W61" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="X61" t="str">
         <f t="shared" si="6"/>
@@ -54480,7 +54437,7 @@
         <v>49</v>
       </c>
       <c r="O62" s="4" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="P62">
         <f t="shared" si="10"/>
@@ -54508,7 +54465,7 @@
         <v>0.46034621021486044</v>
       </c>
       <c r="W62" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="X62" t="str">
         <f t="shared" si="6"/>
@@ -54559,7 +54516,7 @@
         <v>34</v>
       </c>
       <c r="O63" s="4" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="P63">
         <f t="shared" si="10"/>
@@ -54575,26 +54532,24 @@
         <v>69.322999999999993</v>
       </c>
       <c r="T63">
-        <v>57.683</v>
+        <f>57.683-1.625</f>
+        <v>56.058</v>
       </c>
       <c r="U63">
         <f t="shared" si="7"/>
-        <v>11.639999999999993</v>
+        <v>13.264999999999993</v>
       </c>
       <c r="V63">
         <f t="shared" si="5"/>
-        <v>0.16790964037909489</v>
+        <v>0.1913506339887194</v>
       </c>
       <c r="W63" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="X63" t="str">
         <f t="shared" si="6"/>
         <v>no</v>
       </c>
-      <c r="Y63" t="s">
-        <v>90</v>
-      </c>
     </row>
     <row r="64" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A64">
@@ -54640,7 +54595,7 @@
         <v>44</v>
       </c>
       <c r="O64" s="4" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="P64">
         <f t="shared" si="10"/>
@@ -54656,26 +54611,24 @@
         <v>63.42</v>
       </c>
       <c r="T64">
-        <v>45.901000000000003</v>
+        <f>45.901-2.918</f>
+        <v>42.983000000000004</v>
       </c>
       <c r="U64">
         <f t="shared" si="7"/>
-        <v>17.518999999999998</v>
+        <v>20.436999999999998</v>
       </c>
       <c r="V64">
         <f t="shared" si="5"/>
-        <v>0.27623777988016396</v>
+        <v>0.32224850204982652</v>
       </c>
       <c r="W64" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="X64" t="str">
         <f t="shared" si="6"/>
         <v>no</v>
       </c>
-      <c r="Y64" t="s">
-        <v>90</v>
-      </c>
     </row>
     <row r="65" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A65">
@@ -54721,7 +54674,7 @@
         <v>101</v>
       </c>
       <c r="O65" s="4" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="P65">
         <f t="shared" si="10"/>
@@ -54748,14 +54701,14 @@
         <v>1.5969444944162442E-2</v>
       </c>
       <c r="W65" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="X65" t="str">
         <f t="shared" si="6"/>
         <v>no</v>
       </c>
       <c r="Y65" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
     </row>
     <row r="66" spans="1:25" x14ac:dyDescent="0.2">
@@ -54799,7 +54752,7 @@
         <v>88</v>
       </c>
       <c r="O66" s="4" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="P66">
         <f t="shared" si="10"/>
@@ -54827,7 +54780,7 @@
         <v>0.19725839420231855</v>
       </c>
       <c r="W66" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="X66" t="str">
         <f t="shared" si="6"/>
@@ -54875,7 +54828,7 @@
         <v>38</v>
       </c>
       <c r="O67" s="4" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="P67">
         <f t="shared" si="10"/>
@@ -54902,7 +54855,7 @@
         <v>0.2701798777432608</v>
       </c>
       <c r="W67" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="X67" t="str">
         <f t="shared" ref="X67:X77" si="13">IF(E67&gt;6,"no","yes")</f>
@@ -54950,7 +54903,7 @@
         <v>86</v>
       </c>
       <c r="O68" s="4" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="P68">
         <f t="shared" si="10"/>
@@ -54977,14 +54930,14 @@
         <v>-2.7426714169635456E-2</v>
       </c>
       <c r="W68" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="X68" t="str">
         <f t="shared" si="13"/>
         <v>yes</v>
       </c>
       <c r="Y68" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
     </row>
     <row r="69" spans="1:25" x14ac:dyDescent="0.2">
@@ -55028,7 +54981,7 @@
         <v>86</v>
       </c>
       <c r="O69" s="4" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="P69">
         <f t="shared" si="10"/>
@@ -55055,7 +55008,7 @@
         <v>0.39846093823572937</v>
       </c>
       <c r="W69" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="X69" t="str">
         <f t="shared" si="13"/>
@@ -55103,7 +55056,7 @@
         <v>102</v>
       </c>
       <c r="O70" s="4" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="P70">
         <f t="shared" si="10"/>
@@ -55130,7 +55083,7 @@
         <v>-7.572487229297189E-3</v>
       </c>
       <c r="W70" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="X70" t="str">
         <f t="shared" si="13"/>
@@ -55178,7 +55131,7 @@
         <v>39</v>
       </c>
       <c r="O71" s="4" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="P71">
         <f t="shared" si="10"/>
@@ -55205,7 +55158,7 @@
         <v>0.37464919846126465</v>
       </c>
       <c r="W71" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="X71" t="str">
         <f t="shared" si="13"/>
@@ -55247,7 +55200,7 @@
         <v>0</v>
       </c>
       <c r="O72" s="4" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="P72">
         <f t="shared" si="10"/>
@@ -55301,7 +55254,7 @@
         <v>0</v>
       </c>
       <c r="O73" s="4" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="P73">
         <f t="shared" si="10"/>
@@ -55355,7 +55308,7 @@
         <v>0</v>
       </c>
       <c r="O74" s="4" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="P74">
         <f t="shared" si="10"/>
@@ -55409,7 +55362,7 @@
         <v>0</v>
       </c>
       <c r="O75" s="4" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="P75">
         <f t="shared" si="10"/>
@@ -55463,7 +55416,7 @@
         <v>0</v>
       </c>
       <c r="O76" s="4" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="P76">
         <f t="shared" si="10"/>
@@ -55517,7 +55470,7 @@
         <v>0</v>
       </c>
       <c r="O77" s="4" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="P77">
         <f t="shared" si="10"/>
@@ -55565,10 +55518,10 @@
         <v>52</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="C1" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -62392,7 +62345,7 @@
         <v>1</v>
       </c>
       <c r="AC24" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
     </row>
     <row r="25" spans="1:29" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
urchin size updated, "first run" plot update
</commit_message>
<xml_diff>
--- a/data/raw.xlsx
+++ b/data/raw.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/EcosystemRecoveryLab/github/Ritger-Corynactis-urchin-deterrence/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF01F890-3348-EA4E-862F-12AFA2D528F7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C881B83-FCD3-B44A-9DEF-3D3DD838A4D9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4820" yWindow="15900" windowWidth="44860" windowHeight="10140" activeTab="1" xr2:uid="{58E670A5-634C-427F-960F-9DA76C64E810}"/>
+    <workbookView xWindow="5740" yWindow="12720" windowWidth="44860" windowHeight="10140" activeTab="1" xr2:uid="{58E670A5-634C-427F-960F-9DA76C64E810}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="3" r:id="rId1"/>
@@ -49635,9 +49635,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD5E687B-43EE-4B00-8604-7EB9984510DD}">
   <dimension ref="A1:Y77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="V2" sqref="V2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L42" sqref="L42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -52804,7 +52804,7 @@
         <v>6</v>
       </c>
       <c r="L41" s="7">
-        <v>5</v>
+        <v>58</v>
       </c>
       <c r="M41" s="4">
         <v>90</v>

</xml_diff>

<commit_message>
Turn negative and non significant percent consumption values to zero
</commit_message>
<xml_diff>
--- a/data/raw.xlsx
+++ b/data/raw.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/EcosystemRecoveryLab/github/Ritger-Corynactis-urchin-deterrence/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C881B83-FCD3-B44A-9DEF-3D3DD838A4D9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F511EFA7-3BA2-5D4A-86B2-DD9E2AA956D1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5740" yWindow="12720" windowWidth="44860" windowHeight="10140" activeTab="1" xr2:uid="{58E670A5-634C-427F-960F-9DA76C64E810}"/>
+    <workbookView xWindow="9660" yWindow="1320" windowWidth="31280" windowHeight="17040" activeTab="1" xr2:uid="{58E670A5-634C-427F-960F-9DA76C64E810}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="3" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="106">
   <si>
     <t>Day</t>
   </si>
@@ -334,6 +334,18 @@
   </si>
   <si>
     <t>"after" has hole (-0.264), doesn't look like consumption</t>
+  </si>
+  <si>
+    <t>polyps not out</t>
+  </si>
+  <si>
+    <t>really good deterrence video</t>
+  </si>
+  <si>
+    <t>urchin tried crossing</t>
+  </si>
+  <si>
+    <t>No zero</t>
   </si>
 </sst>
 </file>
@@ -49633,11 +49645,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD5E687B-43EE-4B00-8604-7EB9984510DD}">
-  <dimension ref="A1:Y77"/>
+  <dimension ref="A1:Z77"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L42" sqref="L42"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="X11" sqref="X11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -49662,12 +49674,12 @@
     <col min="19" max="19" width="17.6640625" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="16.1640625" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="21.1640625" bestFit="1" customWidth="1"/>
-    <col min="22" max="23" width="24.1640625" customWidth="1"/>
-    <col min="24" max="24" width="7.1640625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="24" width="24.1640625" customWidth="1"/>
+    <col min="25" max="25" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="10.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -49738,13 +49750,16 @@
         <v>87</v>
       </c>
       <c r="X1" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="Y1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="Y1" s="2" t="s">
+      <c r="Z1" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -49814,12 +49829,16 @@
       <c r="W2" t="s">
         <v>83</v>
       </c>
-      <c r="X2" t="str">
+      <c r="X2">
+        <f>IF(V2&lt;0.05, 0,V2)</f>
+        <v>0.10844212089339854</v>
+      </c>
+      <c r="Y2" t="str">
         <f>IF(E2&gt;6,"no","yes")</f>
         <v>yes</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -49889,15 +49908,19 @@
       <c r="W3" t="s">
         <v>84</v>
       </c>
-      <c r="X3" t="str">
-        <f t="shared" ref="X3:X66" si="6">IF(E3&gt;6,"no","yes")</f>
+      <c r="X3">
+        <f t="shared" ref="X3:X66" si="6">IF(V3&lt;0.05, 0,V3)</f>
+        <v>0</v>
+      </c>
+      <c r="Y3" t="str">
+        <f t="shared" ref="Y3:Y66" si="7">IF(E3&gt;6,"no","yes")</f>
         <v>yes</v>
       </c>
-      <c r="Y3" t="s">
+      <c r="Z3" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -49967,12 +49990,16 @@
       <c r="W4" t="s">
         <v>83</v>
       </c>
-      <c r="X4" t="str">
+      <c r="X4">
         <f t="shared" si="6"/>
+        <v>0.28380160052328729</v>
+      </c>
+      <c r="Y4" t="str">
+        <f t="shared" si="7"/>
         <v>yes</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -50043,12 +50070,16 @@
       <c r="W5" t="s">
         <v>83</v>
       </c>
-      <c r="X5" t="str">
+      <c r="X5">
         <f t="shared" si="6"/>
+        <v>0.1477296829877143</v>
+      </c>
+      <c r="Y5" t="str">
+        <f t="shared" si="7"/>
         <v>yes</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -50118,15 +50149,19 @@
       <c r="W6" t="s">
         <v>83</v>
       </c>
-      <c r="X6" t="str">
+      <c r="X6">
         <f t="shared" si="6"/>
+        <v>0.25604737440407477</v>
+      </c>
+      <c r="Y6" t="str">
+        <f t="shared" si="7"/>
         <v>yes</v>
       </c>
-      <c r="Y6" t="s">
+      <c r="Z6" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -50197,12 +50232,16 @@
       <c r="W7" t="s">
         <v>83</v>
       </c>
-      <c r="X7" t="str">
+      <c r="X7">
         <f t="shared" si="6"/>
+        <v>0.11429241568798264</v>
+      </c>
+      <c r="Y7" t="str">
+        <f t="shared" si="7"/>
         <v>yes</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -50275,12 +50314,16 @@
       <c r="W8" t="s">
         <v>84</v>
       </c>
-      <c r="X8" t="str">
+      <c r="X8">
         <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Y8" t="str">
+        <f t="shared" si="7"/>
         <v>no</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -50353,12 +50396,16 @@
       <c r="W9" t="s">
         <v>84</v>
       </c>
-      <c r="X9" t="str">
+      <c r="X9">
         <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Y9" t="str">
+        <f t="shared" si="7"/>
         <v>no</v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -50431,15 +50478,19 @@
       <c r="W10" t="s">
         <v>84</v>
       </c>
-      <c r="X10" t="str">
+      <c r="X10">
         <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Y10" t="str">
+        <f t="shared" si="7"/>
         <v>no</v>
       </c>
-      <c r="Y10" t="s">
+      <c r="Z10" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -50512,15 +50563,19 @@
       <c r="W11" t="s">
         <v>84</v>
       </c>
-      <c r="X11" t="str">
+      <c r="X11">
         <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Y11" t="str">
+        <f t="shared" si="7"/>
         <v>no</v>
       </c>
-      <c r="Y11" t="s">
+      <c r="Z11" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -50593,15 +50648,19 @@
       <c r="W12" t="s">
         <v>83</v>
       </c>
-      <c r="X12" t="str">
+      <c r="X12">
         <f t="shared" si="6"/>
+        <v>0.23731693570773646</v>
+      </c>
+      <c r="Y12" t="str">
+        <f t="shared" si="7"/>
         <v>no</v>
       </c>
-      <c r="Y12" t="s">
+      <c r="Z12" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -50674,15 +50733,19 @@
       <c r="W13" t="s">
         <v>83</v>
       </c>
-      <c r="X13" t="str">
+      <c r="X13">
         <f t="shared" si="6"/>
+        <v>0.21320720819240585</v>
+      </c>
+      <c r="Y13" t="str">
+        <f t="shared" si="7"/>
         <v>no</v>
       </c>
-      <c r="Y13" t="s">
+      <c r="Z13" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -50755,15 +50818,19 @@
       <c r="W14" t="s">
         <v>83</v>
       </c>
-      <c r="X14" t="str">
+      <c r="X14">
         <f t="shared" si="6"/>
+        <v>0.10589024007332033</v>
+      </c>
+      <c r="Y14" t="str">
+        <f t="shared" si="7"/>
         <v>no</v>
       </c>
-      <c r="Y14" t="s">
+      <c r="Z14" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -50836,15 +50903,19 @@
       <c r="W15" t="s">
         <v>84</v>
       </c>
-      <c r="X15" t="str">
+      <c r="X15">
         <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Y15" t="str">
+        <f t="shared" si="7"/>
         <v>no</v>
       </c>
-      <c r="Y15" t="s">
+      <c r="Z15" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -50914,12 +50985,16 @@
       <c r="W16" t="s">
         <v>84</v>
       </c>
-      <c r="X16" t="str">
+      <c r="X16">
         <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Y16" t="str">
+        <f t="shared" si="7"/>
         <v>yes</v>
       </c>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -50980,7 +51055,7 @@
         <v>66.283000000000001</v>
       </c>
       <c r="U17">
-        <f t="shared" ref="U17:U77" si="7">S17-T17</f>
+        <f t="shared" ref="U17:U77" si="8">S17-T17</f>
         <v>35.326999999999998</v>
       </c>
       <c r="V17">
@@ -50990,15 +51065,19 @@
       <c r="W17" t="s">
         <v>83</v>
       </c>
-      <c r="X17" t="str">
+      <c r="X17">
         <f t="shared" si="6"/>
+        <v>0.34767247318177341</v>
+      </c>
+      <c r="Y17" t="str">
+        <f t="shared" si="7"/>
         <v>yes</v>
       </c>
-      <c r="Y17" t="s">
+      <c r="Z17" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
@@ -51058,7 +51137,7 @@
         <v>88.927000000000007</v>
       </c>
       <c r="U18">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.2919999999999874</v>
       </c>
       <c r="V18">
@@ -51068,15 +51147,19 @@
       <c r="W18" t="s">
         <v>84</v>
       </c>
-      <c r="X18" t="str">
+      <c r="X18">
         <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Y18" t="str">
+        <f t="shared" si="7"/>
         <v>yes</v>
       </c>
-      <c r="Y18" t="s">
+      <c r="Z18" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
@@ -51136,7 +51219,7 @@
         <v>88.608999999999995</v>
       </c>
       <c r="U19">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.8610000000000042</v>
       </c>
       <c r="V19">
@@ -51146,12 +51229,16 @@
       <c r="W19" t="s">
         <v>84</v>
       </c>
-      <c r="X19" t="str">
+      <c r="X19">
         <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Y19" t="str">
+        <f t="shared" si="7"/>
         <v>yes</v>
       </c>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
@@ -51211,7 +51298,7 @@
         <v>105.565</v>
       </c>
       <c r="U20">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>25.765999999999991</v>
       </c>
       <c r="V20">
@@ -51221,12 +51308,16 @@
       <c r="W20" t="s">
         <v>83</v>
       </c>
-      <c r="X20" t="str">
+      <c r="X20">
         <f t="shared" si="6"/>
+        <v>0.19619130289116807</v>
+      </c>
+      <c r="Y20" t="str">
+        <f t="shared" si="7"/>
         <v>yes</v>
       </c>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
@@ -51286,7 +51377,7 @@
         <v>94.238</v>
       </c>
       <c r="U21">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.60500000000000398</v>
       </c>
       <c r="V21">
@@ -51296,12 +51387,16 @@
       <c r="W21" t="s">
         <v>84</v>
       </c>
-      <c r="X21" t="str">
+      <c r="X21">
         <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Y21" t="str">
+        <f t="shared" si="7"/>
         <v>yes</v>
       </c>
     </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
@@ -51364,7 +51459,7 @@
         <v>118.857</v>
       </c>
       <c r="U22">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.1800000000000068</v>
       </c>
       <c r="V22">
@@ -51374,12 +51469,16 @@
       <c r="W22" t="s">
         <v>84</v>
       </c>
-      <c r="X22" t="str">
+      <c r="X22">
         <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Y22" t="str">
+        <f t="shared" si="7"/>
         <v>no</v>
       </c>
     </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
@@ -51442,7 +51541,7 @@
         <v>122.38800000000001</v>
       </c>
       <c r="U23">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>-0.14200000000001012</v>
       </c>
       <c r="V23">
@@ -51452,12 +51551,16 @@
       <c r="W23" t="s">
         <v>84</v>
       </c>
-      <c r="X23" t="str">
+      <c r="X23">
         <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Y23" t="str">
+        <f t="shared" si="7"/>
         <v>no</v>
       </c>
     </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
@@ -51520,7 +51623,7 @@
         <v>99.629000000000005</v>
       </c>
       <c r="U24">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.72299999999999898</v>
       </c>
       <c r="V24">
@@ -51530,12 +51633,16 @@
       <c r="W24" t="s">
         <v>84</v>
       </c>
-      <c r="X24" t="str">
+      <c r="X24">
         <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Y24" t="str">
+        <f t="shared" si="7"/>
         <v>no</v>
       </c>
     </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
@@ -51598,7 +51705,7 @@
         <v>94.129000000000005</v>
       </c>
       <c r="U25">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.5369999999999919</v>
       </c>
       <c r="V25">
@@ -51608,12 +51715,16 @@
       <c r="W25" t="s">
         <v>84</v>
       </c>
-      <c r="X25" t="str">
+      <c r="X25">
         <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Y25" t="str">
+        <f t="shared" si="7"/>
         <v>no</v>
       </c>
     </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
@@ -51677,7 +51788,7 @@
         <v>92.486999999999995</v>
       </c>
       <c r="U26">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>11.196000000000012</v>
       </c>
       <c r="V26">
@@ -51687,12 +51798,16 @@
       <c r="W26" t="s">
         <v>83</v>
       </c>
-      <c r="X26" t="str">
+      <c r="X26">
         <f t="shared" si="6"/>
+        <v>0.107982986603397</v>
+      </c>
+      <c r="Y26" t="str">
+        <f t="shared" si="7"/>
         <v>no</v>
       </c>
     </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>26</v>
       </c>
@@ -51755,7 +51870,7 @@
         <v>101.742</v>
       </c>
       <c r="U27">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.32799999999998875</v>
       </c>
       <c r="V27">
@@ -51765,12 +51880,16 @@
       <c r="W27" t="s">
         <v>84</v>
       </c>
-      <c r="X27" t="str">
+      <c r="X27">
         <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Y27" t="str">
+        <f t="shared" si="7"/>
         <v>no</v>
       </c>
     </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>27</v>
       </c>
@@ -51833,7 +51952,7 @@
         <v>104.006</v>
       </c>
       <c r="U28">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.8119999999999976</v>
       </c>
       <c r="V28">
@@ -51843,12 +51962,16 @@
       <c r="W28" t="s">
         <v>84</v>
       </c>
-      <c r="X28" t="str">
+      <c r="X28">
         <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Y28" t="str">
+        <f t="shared" si="7"/>
         <v>no</v>
       </c>
     </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>28</v>
       </c>
@@ -51911,7 +52034,7 @@
         <v>104.875</v>
       </c>
       <c r="U29">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>4.1650000000000063</v>
       </c>
       <c r="V29">
@@ -51921,12 +52044,16 @@
       <c r="W29" t="s">
         <v>84</v>
       </c>
-      <c r="X29" t="str">
+      <c r="X29">
         <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Y29" t="str">
+        <f t="shared" si="7"/>
         <v>no</v>
       </c>
     </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>29</v>
       </c>
@@ -51987,7 +52114,7 @@
         <v>54.828000000000003</v>
       </c>
       <c r="U30">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>35.668999999999997</v>
       </c>
       <c r="V30">
@@ -51997,12 +52124,16 @@
       <c r="W30" t="s">
         <v>83</v>
       </c>
-      <c r="X30" t="str">
+      <c r="X30">
         <f t="shared" si="6"/>
+        <v>0.39414566228714759</v>
+      </c>
+      <c r="Y30" t="str">
+        <f t="shared" si="7"/>
         <v>yes</v>
       </c>
     </row>
-    <row r="31" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>30</v>
       </c>
@@ -52062,7 +52193,7 @@
         <v>74.176000000000002</v>
       </c>
       <c r="U31">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>29.748999999999995</v>
       </c>
       <c r="V31">
@@ -52072,12 +52203,16 @@
       <c r="W31" t="s">
         <v>83</v>
       </c>
-      <c r="X31" t="str">
+      <c r="X31">
         <f t="shared" si="6"/>
+        <v>0.28625451046427708</v>
+      </c>
+      <c r="Y31" t="str">
+        <f t="shared" si="7"/>
         <v>yes</v>
       </c>
     </row>
-    <row r="32" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>31</v>
       </c>
@@ -52137,7 +52272,7 @@
         <v>61.512</v>
       </c>
       <c r="U32">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>12.697000000000003</v>
       </c>
       <c r="V32">
@@ -52147,12 +52282,16 @@
       <c r="W32" t="s">
         <v>83</v>
       </c>
-      <c r="X32" t="str">
+      <c r="X32">
         <f t="shared" si="6"/>
+        <v>0.17109784527483193</v>
+      </c>
+      <c r="Y32" t="str">
+        <f t="shared" si="7"/>
         <v>yes</v>
       </c>
     </row>
-    <row r="33" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>32</v>
       </c>
@@ -52212,7 +52351,7 @@
         <v>94.572000000000003</v>
       </c>
       <c r="U33">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>-1.3440000000000083</v>
       </c>
       <c r="V33">
@@ -52222,12 +52361,16 @@
       <c r="W33" t="s">
         <v>84</v>
       </c>
-      <c r="X33" t="str">
+      <c r="X33">
         <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Y33" t="str">
+        <f t="shared" si="7"/>
         <v>yes</v>
       </c>
     </row>
-    <row r="34" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>33</v>
       </c>
@@ -52288,7 +52431,7 @@
         <v>56.581999999999994</v>
       </c>
       <c r="U34">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>27.766000000000005</v>
       </c>
       <c r="V34">
@@ -52298,12 +52441,16 @@
       <c r="W34" t="s">
         <v>83</v>
       </c>
-      <c r="X34" t="str">
+      <c r="X34">
         <f t="shared" si="6"/>
+        <v>0.32918385735287148</v>
+      </c>
+      <c r="Y34" t="str">
+        <f t="shared" si="7"/>
         <v>yes</v>
       </c>
     </row>
-    <row r="35" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>34</v>
       </c>
@@ -52363,7 +52510,7 @@
         <v>95.731999999999999</v>
       </c>
       <c r="U35">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.0280000000000058</v>
       </c>
       <c r="V35">
@@ -52373,12 +52520,16 @@
       <c r="W35" t="s">
         <v>84</v>
       </c>
-      <c r="X35" t="str">
+      <c r="X35">
         <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Y35" t="str">
+        <f t="shared" si="7"/>
         <v>yes</v>
       </c>
     </row>
-    <row r="36" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>35</v>
       </c>
@@ -52441,7 +52592,7 @@
         <v>62.167000000000002</v>
       </c>
       <c r="U36">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>31.332999999999998</v>
       </c>
       <c r="V36">
@@ -52451,12 +52602,16 @@
       <c r="W36" t="s">
         <v>83</v>
       </c>
-      <c r="X36" t="str">
+      <c r="X36">
         <f t="shared" si="6"/>
+        <v>0.33511229946524063</v>
+      </c>
+      <c r="Y36" t="str">
+        <f t="shared" si="7"/>
         <v>no</v>
       </c>
     </row>
-    <row r="37" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>36</v>
       </c>
@@ -52519,7 +52674,7 @@
         <v>92.887</v>
       </c>
       <c r="U37">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.84099999999999397</v>
       </c>
       <c r="V37">
@@ -52529,12 +52684,16 @@
       <c r="W37" t="s">
         <v>84</v>
       </c>
-      <c r="X37" t="str">
+      <c r="X37">
         <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Y37" t="str">
+        <f t="shared" si="7"/>
         <v>no</v>
       </c>
     </row>
-    <row r="38" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>37</v>
       </c>
@@ -52598,7 +52757,7 @@
         <v>73.295000000000002</v>
       </c>
       <c r="U38">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>28.343999999999994</v>
       </c>
       <c r="V38">
@@ -52608,12 +52767,16 @@
       <c r="W38" t="s">
         <v>83</v>
       </c>
-      <c r="X38" t="str">
+      <c r="X38">
         <f t="shared" si="6"/>
+        <v>0.27886933165418781</v>
+      </c>
+      <c r="Y38" t="str">
+        <f t="shared" si="7"/>
         <v>no</v>
       </c>
     </row>
-    <row r="39" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>38</v>
       </c>
@@ -52676,7 +52839,7 @@
         <v>39.979999999999997</v>
       </c>
       <c r="U39">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>40.173999999999999</v>
       </c>
       <c r="V39">
@@ -52686,12 +52849,16 @@
       <c r="W39" t="s">
         <v>83</v>
       </c>
-      <c r="X39" t="str">
+      <c r="X39">
         <f t="shared" si="6"/>
+        <v>0.50121017042193783</v>
+      </c>
+      <c r="Y39" t="str">
+        <f t="shared" si="7"/>
         <v>no</v>
       </c>
     </row>
-    <row r="40" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>39</v>
       </c>
@@ -52754,7 +52921,7 @@
         <v>53.595999999999997</v>
       </c>
       <c r="U40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>39.997000000000007</v>
       </c>
       <c r="V40">
@@ -52764,12 +52931,16 @@
       <c r="W40" t="s">
         <v>83</v>
       </c>
-      <c r="X40" t="str">
+      <c r="X40">
         <f t="shared" si="6"/>
+        <v>0.42735033602940398</v>
+      </c>
+      <c r="Y40" t="str">
+        <f t="shared" si="7"/>
         <v>no</v>
       </c>
     </row>
-    <row r="41" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>40</v>
       </c>
@@ -52833,7 +53004,7 @@
         <v>5.2050000000000001</v>
       </c>
       <c r="U41">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>53.626000000000005</v>
       </c>
       <c r="V41">
@@ -52843,12 +53014,16 @@
       <c r="W41" t="s">
         <v>83</v>
       </c>
-      <c r="X41" t="str">
+      <c r="X41">
         <f t="shared" si="6"/>
+        <v>0.91152623616800665</v>
+      </c>
+      <c r="Y41" t="str">
+        <f t="shared" si="7"/>
         <v>no</v>
       </c>
     </row>
-    <row r="42" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>41</v>
       </c>
@@ -52911,7 +53086,7 @@
         <v>74.962000000000003</v>
       </c>
       <c r="U42">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.56799999999999784</v>
       </c>
       <c r="V42">
@@ -52921,12 +53096,16 @@
       <c r="W42" t="s">
         <v>83</v>
       </c>
-      <c r="X42" t="str">
+      <c r="X42">
         <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Y42" t="str">
+        <f t="shared" si="7"/>
         <v>no</v>
       </c>
     </row>
-    <row r="43" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>42</v>
       </c>
@@ -52989,7 +53168,7 @@
         <v>75.542000000000002</v>
       </c>
       <c r="U43">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.4669999999999987</v>
       </c>
       <c r="V43">
@@ -52999,15 +53178,19 @@
       <c r="W43" t="s">
         <v>84</v>
       </c>
-      <c r="X43" t="str">
+      <c r="X43">
         <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Y43" t="str">
+        <f t="shared" si="7"/>
         <v>no</v>
       </c>
-      <c r="Y43" t="s">
+      <c r="Z43" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="44" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>43</v>
       </c>
@@ -53066,7 +53249,7 @@
         <v>12.182</v>
       </c>
       <c r="U44">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>56.388999999999996</v>
       </c>
       <c r="V44">
@@ -53076,12 +53259,16 @@
       <c r="W44" t="s">
         <v>83</v>
       </c>
-      <c r="X44" t="str">
+      <c r="X44">
         <f t="shared" si="6"/>
+        <v>0.82234472298785199</v>
+      </c>
+      <c r="Y44" t="str">
+        <f t="shared" si="7"/>
         <v>yes</v>
       </c>
     </row>
-    <row r="45" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>44</v>
       </c>
@@ -53141,7 +53328,7 @@
         <v>94.964999999999989</v>
       </c>
       <c r="U45">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>12.063000000000017</v>
       </c>
       <c r="V45">
@@ -53151,12 +53338,16 @@
       <c r="W45" t="s">
         <v>83</v>
       </c>
-      <c r="X45" t="str">
+      <c r="X45">
         <f t="shared" si="6"/>
+        <v>0.11270882385917719</v>
+      </c>
+      <c r="Y45" t="str">
+        <f t="shared" si="7"/>
         <v>yes</v>
       </c>
     </row>
-    <row r="46" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>45</v>
       </c>
@@ -53215,7 +53406,7 @@
         <v>57.972000000000001</v>
       </c>
       <c r="U46">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.3599999999999994</v>
       </c>
       <c r="V46">
@@ -53225,12 +53416,16 @@
       <c r="W46" t="s">
         <v>84</v>
       </c>
-      <c r="X46" t="str">
+      <c r="X46">
         <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Y46" t="str">
+        <f t="shared" si="7"/>
         <v>yes</v>
       </c>
     </row>
-    <row r="47" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>46</v>
       </c>
@@ -53289,7 +53484,7 @@
         <v>62.152999999999999</v>
       </c>
       <c r="U47">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.91700000000000159</v>
       </c>
       <c r="V47">
@@ -53299,11 +53494,15 @@
       <c r="W47" t="s">
         <v>84</v>
       </c>
-      <c r="X47" t="s">
+      <c r="X47">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Y47" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="48" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>47</v>
       </c>
@@ -53363,7 +53562,7 @@
         <v>92.295000000000002</v>
       </c>
       <c r="U48">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.89499999999999602</v>
       </c>
       <c r="V48">
@@ -53373,15 +53572,19 @@
       <c r="W48" t="s">
         <v>84</v>
       </c>
-      <c r="X48" t="str">
+      <c r="X48">
         <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Y48" t="str">
+        <f t="shared" si="7"/>
         <v>yes</v>
       </c>
-      <c r="Y48" t="s">
+      <c r="Z48" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="49" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>48</v>
       </c>
@@ -53440,7 +53643,7 @@
         <v>58.454999999999998</v>
       </c>
       <c r="U49">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.8130000000000024</v>
       </c>
       <c r="V49">
@@ -53450,12 +53653,16 @@
       <c r="W49" t="s">
         <v>84</v>
       </c>
-      <c r="X49" t="str">
+      <c r="X49">
         <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Y49" t="str">
+        <f t="shared" si="7"/>
         <v>yes</v>
       </c>
     </row>
-    <row r="50" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>49</v>
       </c>
@@ -53518,7 +53725,7 @@
         <v>55.853999999999999</v>
       </c>
       <c r="U50">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>15.021000000000001</v>
       </c>
       <c r="V50">
@@ -53528,15 +53735,19 @@
       <c r="W50" t="s">
         <v>83</v>
       </c>
-      <c r="X50" t="str">
+      <c r="X50">
         <f t="shared" si="6"/>
+        <v>0.21193650793650795</v>
+      </c>
+      <c r="Y50" t="str">
+        <f t="shared" si="7"/>
         <v>no</v>
       </c>
-      <c r="Y50" t="s">
+      <c r="Z50" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="51" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>50</v>
       </c>
@@ -53598,7 +53809,7 @@
         <v>92.927000000000007</v>
       </c>
       <c r="U51">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>3.1169999999999902</v>
       </c>
       <c r="V51">
@@ -53608,12 +53819,16 @@
       <c r="W51" t="s">
         <v>84</v>
       </c>
-      <c r="X51" t="str">
+      <c r="X51">
         <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Y51" t="str">
+        <f t="shared" si="7"/>
         <v>no</v>
       </c>
     </row>
-    <row r="52" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>51</v>
       </c>
@@ -53676,7 +53891,7 @@
         <v>48.533999999999999</v>
       </c>
       <c r="U52">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>17.312000000000005</v>
       </c>
       <c r="V52">
@@ -53686,12 +53901,16 @@
       <c r="W52" t="s">
         <v>83</v>
       </c>
-      <c r="X52" t="str">
+      <c r="X52">
         <f t="shared" si="6"/>
+        <v>0.2629165021413602</v>
+      </c>
+      <c r="Y52" t="str">
+        <f t="shared" si="7"/>
         <v>no</v>
       </c>
     </row>
-    <row r="53" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>52</v>
       </c>
@@ -53754,7 +53973,7 @@
         <v>85.394000000000005</v>
       </c>
       <c r="U53">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>9.6999999999994202E-2</v>
       </c>
       <c r="V53">
@@ -53764,12 +53983,16 @@
       <c r="W53" t="s">
         <v>84</v>
       </c>
-      <c r="X53" t="str">
+      <c r="X53">
         <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Y53" t="str">
+        <f t="shared" si="7"/>
         <v>no</v>
       </c>
     </row>
-    <row r="54" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>53</v>
       </c>
@@ -53832,7 +54055,7 @@
         <v>27.768000000000001</v>
       </c>
       <c r="U54">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>38.685000000000002</v>
       </c>
       <c r="V54">
@@ -53842,12 +54065,16 @@
       <c r="W54" t="s">
         <v>83</v>
       </c>
-      <c r="X54" t="str">
+      <c r="X54">
         <f t="shared" si="6"/>
+        <v>0.5821407611394519</v>
+      </c>
+      <c r="Y54" t="str">
+        <f t="shared" si="7"/>
         <v>no</v>
       </c>
     </row>
-    <row r="55" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>54</v>
       </c>
@@ -53909,7 +54136,7 @@
         <v>63.54</v>
       </c>
       <c r="U55">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>7.259999999999998</v>
       </c>
       <c r="V55">
@@ -53919,12 +54146,16 @@
       <c r="W55" t="s">
         <v>83</v>
       </c>
-      <c r="X55" t="str">
+      <c r="X55">
         <f t="shared" si="6"/>
+        <v>0.10254237288135591</v>
+      </c>
+      <c r="Y55" t="str">
+        <f t="shared" si="7"/>
         <v>no</v>
       </c>
     </row>
-    <row r="56" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>55</v>
       </c>
@@ -53987,7 +54218,7 @@
         <v>67.456999999999994</v>
       </c>
       <c r="U56">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>17.740000000000009</v>
       </c>
       <c r="V56">
@@ -53997,12 +54228,16 @@
       <c r="W56" t="s">
         <v>83</v>
       </c>
-      <c r="X56" t="str">
+      <c r="X56">
         <f t="shared" si="6"/>
+        <v>0.20822329424745012</v>
+      </c>
+      <c r="Y56" t="str">
+        <f t="shared" si="7"/>
         <v>no</v>
       </c>
     </row>
-    <row r="57" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>56</v>
       </c>
@@ -54065,7 +54300,7 @@
         <v>55.945000000000007</v>
       </c>
       <c r="U57">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>28.375999999999991</v>
       </c>
       <c r="V57">
@@ -54075,12 +54310,16 @@
       <c r="W57" t="s">
         <v>83</v>
       </c>
-      <c r="X57" t="str">
+      <c r="X57">
         <f t="shared" si="6"/>
+        <v>0.33652352320299794</v>
+      </c>
+      <c r="Y57" t="str">
+        <f t="shared" si="7"/>
         <v>no</v>
       </c>
     </row>
-    <row r="58" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>57</v>
       </c>
@@ -54104,11 +54343,11 @@
         <v>58</v>
       </c>
       <c r="H58" t="str">
-        <f t="shared" ref="H58:H71" si="8">IF(J58&lt;=0, "Control", IF(J58&lt;=10, "Red", IF(J58&gt;=21, "Pink", "Orange")))</f>
+        <f t="shared" ref="H58:H71" si="9">IF(J58&lt;=0, "Control", IF(J58&lt;=10, "Red", IF(J58&gt;=21, "Pink", "Orange")))</f>
         <v>Red</v>
       </c>
       <c r="I58">
-        <f t="shared" ref="I58:I71" si="9">IF(H58="Control", 1, IF(H58="Red", 2, IF(H58="Orange", 3, 4)))</f>
+        <f t="shared" ref="I58:I71" si="10">IF(H58="Control", 1, IF(H58="Red", 2, IF(H58="Orange", 3, 4)))</f>
         <v>2</v>
       </c>
       <c r="J58" s="7">
@@ -54127,7 +54366,7 @@
         <v>99</v>
       </c>
       <c r="P58">
-        <f t="shared" ref="P58:P77" si="10">C58-239</f>
+        <f t="shared" ref="P58:P77" si="11">C58-239</f>
         <v>8</v>
       </c>
       <c r="Q58">
@@ -54143,7 +54382,7 @@
         <v>83.33</v>
       </c>
       <c r="U58">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>2.5999999999996248E-2</v>
       </c>
       <c r="V58">
@@ -54153,12 +54392,16 @@
       <c r="W58" t="s">
         <v>84</v>
       </c>
-      <c r="X58" t="str">
+      <c r="X58">
         <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Y58" t="str">
+        <f t="shared" si="7"/>
         <v>no</v>
       </c>
     </row>
-    <row r="59" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>58</v>
       </c>
@@ -54182,11 +54425,11 @@
         <v>57</v>
       </c>
       <c r="H59" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>Control</v>
       </c>
       <c r="I59">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="J59" s="7">
@@ -54205,7 +54448,7 @@
         <v>99</v>
       </c>
       <c r="P59">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>8</v>
       </c>
       <c r="Q59">
@@ -54222,7 +54465,7 @@
         <v>45.494</v>
       </c>
       <c r="U59">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>28.102999999999994</v>
       </c>
       <c r="V59">
@@ -54232,12 +54475,16 @@
       <c r="W59" t="s">
         <v>83</v>
       </c>
-      <c r="X59" t="str">
+      <c r="X59">
         <f t="shared" si="6"/>
+        <v>0.38184980366047527</v>
+      </c>
+      <c r="Y59" t="str">
+        <f t="shared" si="7"/>
         <v>no</v>
       </c>
     </row>
-    <row r="60" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>59</v>
       </c>
@@ -54261,11 +54508,11 @@
         <v>58</v>
       </c>
       <c r="H60" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>Pink</v>
       </c>
       <c r="I60">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>4</v>
       </c>
       <c r="J60" s="5">
@@ -54284,7 +54531,7 @@
         <v>99</v>
       </c>
       <c r="P60">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>8</v>
       </c>
       <c r="Q60">
@@ -54300,7 +54547,7 @@
         <v>63.26</v>
       </c>
       <c r="U60">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>-0.26399999999999579</v>
       </c>
       <c r="V60">
@@ -54310,12 +54557,16 @@
       <c r="W60" t="s">
         <v>84</v>
       </c>
-      <c r="X60" t="str">
+      <c r="X60">
         <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Y60" t="str">
+        <f t="shared" si="7"/>
         <v>no</v>
       </c>
     </row>
-    <row r="61" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>60</v>
       </c>
@@ -54339,11 +54590,11 @@
         <v>57</v>
       </c>
       <c r="H61" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>Red</v>
       </c>
       <c r="I61">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>2</v>
       </c>
       <c r="J61" s="5">
@@ -54362,7 +54613,7 @@
         <v>99</v>
       </c>
       <c r="P61">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>8</v>
       </c>
       <c r="Q61">
@@ -54378,7 +54629,7 @@
         <v>69.334000000000003</v>
       </c>
       <c r="U61">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.73099999999999454</v>
       </c>
       <c r="V61">
@@ -54388,12 +54639,16 @@
       <c r="W61" t="s">
         <v>84</v>
       </c>
-      <c r="X61" t="str">
+      <c r="X61">
         <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Y61" t="str">
+        <f t="shared" si="7"/>
         <v>no</v>
       </c>
     </row>
-    <row r="62" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>61</v>
       </c>
@@ -54417,11 +54672,11 @@
         <v>57</v>
       </c>
       <c r="H62" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>Orange</v>
       </c>
       <c r="I62">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>3</v>
       </c>
       <c r="J62" s="5">
@@ -54440,7 +54695,7 @@
         <v>99</v>
       </c>
       <c r="P62">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>8</v>
       </c>
       <c r="Q62">
@@ -54457,7 +54712,7 @@
         <v>39.030999999999999</v>
       </c>
       <c r="U62">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>33.294999999999995</v>
       </c>
       <c r="V62">
@@ -54467,12 +54722,16 @@
       <c r="W62" t="s">
         <v>83</v>
       </c>
-      <c r="X62" t="str">
+      <c r="X62">
         <f t="shared" si="6"/>
+        <v>0.46034621021486044</v>
+      </c>
+      <c r="Y62" t="str">
+        <f t="shared" si="7"/>
         <v>no</v>
       </c>
     </row>
-    <row r="63" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>62</v>
       </c>
@@ -54496,11 +54755,11 @@
         <v>58</v>
       </c>
       <c r="H63" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>Orange</v>
       </c>
       <c r="I63">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>3</v>
       </c>
       <c r="J63" s="5">
@@ -54519,7 +54778,7 @@
         <v>99</v>
       </c>
       <c r="P63">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>8</v>
       </c>
       <c r="Q63">
@@ -54536,7 +54795,7 @@
         <v>56.058</v>
       </c>
       <c r="U63">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>13.264999999999993</v>
       </c>
       <c r="V63">
@@ -54546,12 +54805,16 @@
       <c r="W63" t="s">
         <v>83</v>
       </c>
-      <c r="X63" t="str">
+      <c r="X63">
         <f t="shared" si="6"/>
+        <v>0.1913506339887194</v>
+      </c>
+      <c r="Y63" t="str">
+        <f t="shared" si="7"/>
         <v>no</v>
       </c>
     </row>
-    <row r="64" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>63</v>
       </c>
@@ -54575,11 +54838,11 @@
         <v>57</v>
       </c>
       <c r="H64" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>Control</v>
       </c>
       <c r="I64">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="J64" s="5">
@@ -54598,7 +54861,7 @@
         <v>99</v>
       </c>
       <c r="P64">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>8</v>
       </c>
       <c r="Q64">
@@ -54615,7 +54878,7 @@
         <v>42.983000000000004</v>
       </c>
       <c r="U64">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>20.436999999999998</v>
       </c>
       <c r="V64">
@@ -54625,12 +54888,16 @@
       <c r="W64" t="s">
         <v>83</v>
       </c>
-      <c r="X64" t="str">
+      <c r="X64">
         <f t="shared" si="6"/>
+        <v>0.32224850204982652</v>
+      </c>
+      <c r="Y64" t="str">
+        <f t="shared" si="7"/>
         <v>no</v>
       </c>
     </row>
-    <row r="65" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>64</v>
       </c>
@@ -54654,11 +54921,11 @@
         <v>57</v>
       </c>
       <c r="H65" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>Red</v>
       </c>
       <c r="I65">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>2</v>
       </c>
       <c r="J65" s="5">
@@ -54677,7 +54944,7 @@
         <v>99</v>
       </c>
       <c r="P65">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>8</v>
       </c>
       <c r="Q65">
@@ -54693,7 +54960,7 @@
         <v>71.108999999999995</v>
       </c>
       <c r="U65">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.1540000000000106</v>
       </c>
       <c r="V65">
@@ -54703,15 +54970,19 @@
       <c r="W65" t="s">
         <v>84</v>
       </c>
-      <c r="X65" t="str">
+      <c r="X65">
         <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Y65" t="str">
+        <f t="shared" si="7"/>
         <v>no</v>
       </c>
-      <c r="Y65" t="s">
+      <c r="Z65" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="66" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>65</v>
       </c>
@@ -54732,11 +55003,11 @@
         <v>57</v>
       </c>
       <c r="H66" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>Control</v>
       </c>
       <c r="I66">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="J66" s="7">
@@ -54755,7 +55026,7 @@
         <v>99</v>
       </c>
       <c r="P66">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>9</v>
       </c>
       <c r="Q66">
@@ -54772,7 +55043,7 @@
         <v>56.158999999999999</v>
       </c>
       <c r="U66">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>13.800000000000004</v>
       </c>
       <c r="V66">
@@ -54782,12 +55053,16 @@
       <c r="W66" t="s">
         <v>83</v>
       </c>
-      <c r="X66" t="str">
+      <c r="X66">
         <f t="shared" si="6"/>
+        <v>0.19725839420231855</v>
+      </c>
+      <c r="Y66" t="str">
+        <f t="shared" si="7"/>
         <v>yes</v>
       </c>
     </row>
-    <row r="67" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>66</v>
       </c>
@@ -54801,18 +55076,18 @@
         <v>2</v>
       </c>
       <c r="F67" t="str">
-        <f t="shared" ref="F67:F77" si="11">IF(E67&lt;7, "Lab", "Balcony")</f>
+        <f t="shared" ref="F67:F77" si="12">IF(E67&lt;7, "Lab", "Balcony")</f>
         <v>Lab</v>
       </c>
       <c r="G67" t="s">
         <v>57</v>
       </c>
       <c r="H67" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>Orange</v>
       </c>
       <c r="I67">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>3</v>
       </c>
       <c r="J67" s="7">
@@ -54831,7 +55106,7 @@
         <v>99</v>
       </c>
       <c r="P67">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>9</v>
       </c>
       <c r="Q67">
@@ -54847,22 +55122,26 @@
         <v>58.262999999999998</v>
       </c>
       <c r="U67">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>21.568999999999996</v>
       </c>
       <c r="V67">
-        <f t="shared" ref="V67:V77" si="12">U67/S67</f>
+        <f t="shared" ref="V67:V77" si="13">U67/S67</f>
         <v>0.2701798777432608</v>
       </c>
       <c r="W67" t="s">
         <v>83</v>
       </c>
-      <c r="X67" t="str">
-        <f t="shared" ref="X67:X77" si="13">IF(E67&gt;6,"no","yes")</f>
+      <c r="X67">
+        <f t="shared" ref="X67:X77" si="14">IF(V67&lt;0.05, 0,V67)</f>
+        <v>0.2701798777432608</v>
+      </c>
+      <c r="Y67" t="str">
+        <f t="shared" ref="Y67:Y77" si="15">IF(E67&gt;6,"no","yes")</f>
         <v>yes</v>
       </c>
     </row>
-    <row r="68" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>67</v>
       </c>
@@ -54876,18 +55155,18 @@
         <v>3</v>
       </c>
       <c r="F68" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>Lab</v>
       </c>
       <c r="G68" t="s">
         <v>57</v>
       </c>
       <c r="H68" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>Pink</v>
       </c>
       <c r="I68">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>4</v>
       </c>
       <c r="J68" s="7">
@@ -54906,7 +55185,7 @@
         <v>99</v>
       </c>
       <c r="P68">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>9</v>
       </c>
       <c r="Q68">
@@ -54922,25 +55201,29 @@
         <v>82.188999999999993</v>
       </c>
       <c r="U68">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>-2.1939999999999884</v>
       </c>
       <c r="V68">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>-2.7426714169635456E-2</v>
       </c>
       <c r="W68" t="s">
         <v>84</v>
       </c>
-      <c r="X68" t="str">
-        <f t="shared" si="13"/>
+      <c r="X68">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="Y68" t="str">
+        <f t="shared" si="15"/>
         <v>yes</v>
       </c>
-      <c r="Y68" t="s">
+      <c r="Z68" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="69" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>68</v>
       </c>
@@ -54954,18 +55237,18 @@
         <v>4</v>
       </c>
       <c r="F69" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>Lab</v>
       </c>
       <c r="G69" t="s">
         <v>58</v>
       </c>
       <c r="H69" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>Pink</v>
       </c>
       <c r="I69">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>4</v>
       </c>
       <c r="J69" s="7">
@@ -54984,7 +55267,7 @@
         <v>99</v>
       </c>
       <c r="P69">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>9</v>
       </c>
       <c r="Q69">
@@ -55000,22 +55283,26 @@
         <v>44.713000000000001</v>
       </c>
       <c r="U69">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>29.618000000000002</v>
       </c>
       <c r="V69">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0.39846093823572937</v>
       </c>
       <c r="W69" t="s">
         <v>83</v>
       </c>
-      <c r="X69" t="str">
-        <f t="shared" si="13"/>
+      <c r="X69">
+        <f t="shared" si="14"/>
+        <v>0.39846093823572937</v>
+      </c>
+      <c r="Y69" t="str">
+        <f t="shared" si="15"/>
         <v>yes</v>
       </c>
     </row>
-    <row r="70" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>69</v>
       </c>
@@ -55029,18 +55316,18 @@
         <v>5</v>
       </c>
       <c r="F70" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>Lab</v>
       </c>
       <c r="G70" t="s">
         <v>58</v>
       </c>
       <c r="H70" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>Pink</v>
       </c>
       <c r="I70">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>4</v>
       </c>
       <c r="J70" s="7">
@@ -55059,7 +55346,7 @@
         <v>99</v>
       </c>
       <c r="P70">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>9</v>
       </c>
       <c r="Q70">
@@ -55075,22 +55362,26 @@
         <v>56.017000000000003</v>
       </c>
       <c r="U70">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>-0.42100000000000648</v>
       </c>
       <c r="V70">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>-7.572487229297189E-3</v>
       </c>
       <c r="W70" t="s">
         <v>84</v>
       </c>
-      <c r="X70" t="str">
-        <f t="shared" si="13"/>
+      <c r="X70">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="Y70" t="str">
+        <f t="shared" si="15"/>
         <v>yes</v>
       </c>
     </row>
-    <row r="71" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>70</v>
       </c>
@@ -55104,18 +55395,18 @@
         <v>6</v>
       </c>
       <c r="F71" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>Lab</v>
       </c>
       <c r="G71" t="s">
         <v>57</v>
       </c>
       <c r="H71" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>Red</v>
       </c>
       <c r="I71">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>2</v>
       </c>
       <c r="J71" s="7">
@@ -55134,7 +55425,7 @@
         <v>99</v>
       </c>
       <c r="P71">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>9</v>
       </c>
       <c r="Q71">
@@ -55150,22 +55441,26 @@
         <v>45.68</v>
       </c>
       <c r="U71">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>27.366999999999997</v>
       </c>
       <c r="V71">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0.37464919846126465</v>
       </c>
       <c r="W71" t="s">
         <v>83</v>
       </c>
-      <c r="X71" t="str">
-        <f t="shared" si="13"/>
+      <c r="X71">
+        <f t="shared" si="14"/>
+        <v>0.37464919846126465</v>
+      </c>
+      <c r="Y71" t="str">
+        <f t="shared" si="15"/>
         <v>yes</v>
       </c>
     </row>
-    <row r="72" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>71</v>
       </c>
@@ -55179,18 +55474,18 @@
         <v>1</v>
       </c>
       <c r="F72" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>Lab</v>
       </c>
       <c r="G72" t="s">
         <v>57</v>
       </c>
       <c r="H72" t="str">
-        <f t="shared" ref="H72:H77" si="14">IF(J72&lt;=0, "Control", IF(J72&lt;=10, "Red", IF(J72&gt;=21, "Pink", "Orange")))</f>
+        <f t="shared" ref="H72:H77" si="16">IF(J72&lt;=0, "Control", IF(J72&lt;=10, "Red", IF(J72&gt;=21, "Pink", "Orange")))</f>
         <v>Control</v>
       </c>
       <c r="I72">
-        <f t="shared" ref="I72:I77" si="15">IF(H72="Control", 1, IF(H72="Red", 2, IF(H72="Orange", 3, 4)))</f>
+        <f t="shared" ref="I72:I77" si="17">IF(H72="Control", 1, IF(H72="Red", 2, IF(H72="Orange", 3, 4)))</f>
         <v>1</v>
       </c>
       <c r="J72" s="7">
@@ -55203,23 +55498,27 @@
         <v>99</v>
       </c>
       <c r="P72">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>10</v>
       </c>
       <c r="U72">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="V72" t="e">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="X72" t="str">
-        <f t="shared" si="13"/>
+      <c r="X72" t="e">
+        <f t="shared" si="14"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Y72" t="str">
+        <f t="shared" si="15"/>
         <v>yes</v>
       </c>
     </row>
-    <row r="73" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>72</v>
       </c>
@@ -55233,18 +55532,18 @@
         <v>2</v>
       </c>
       <c r="F73" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>Lab</v>
       </c>
       <c r="G73" t="s">
         <v>58</v>
       </c>
       <c r="H73" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>Pink</v>
       </c>
       <c r="I73">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>4</v>
       </c>
       <c r="J73" s="7">
@@ -55257,23 +55556,27 @@
         <v>99</v>
       </c>
       <c r="P73">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>10</v>
       </c>
       <c r="U73">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="V73" t="e">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="X73" t="str">
-        <f t="shared" si="13"/>
+      <c r="X73" t="e">
+        <f t="shared" si="14"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Y73" t="str">
+        <f t="shared" si="15"/>
         <v>yes</v>
       </c>
     </row>
-    <row r="74" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>73</v>
       </c>
@@ -55287,18 +55590,18 @@
         <v>3</v>
       </c>
       <c r="F74" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>Lab</v>
       </c>
       <c r="G74" t="s">
         <v>58</v>
       </c>
       <c r="H74" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>Orange</v>
       </c>
       <c r="I74">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>3</v>
       </c>
       <c r="J74" s="7">
@@ -55311,23 +55614,27 @@
         <v>99</v>
       </c>
       <c r="P74">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>10</v>
       </c>
       <c r="U74">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="V74" t="e">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="X74" t="str">
-        <f t="shared" si="13"/>
+      <c r="X74" t="e">
+        <f t="shared" si="14"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Y74" t="str">
+        <f t="shared" si="15"/>
         <v>yes</v>
       </c>
     </row>
-    <row r="75" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>74</v>
       </c>
@@ -55341,18 +55648,18 @@
         <v>4</v>
       </c>
       <c r="F75" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>Lab</v>
       </c>
       <c r="G75" t="s">
         <v>58</v>
       </c>
       <c r="H75" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>Red</v>
       </c>
       <c r="I75">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>2</v>
       </c>
       <c r="J75" s="7">
@@ -55365,23 +55672,27 @@
         <v>99</v>
       </c>
       <c r="P75">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>10</v>
       </c>
       <c r="U75">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="V75" t="e">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="X75" t="str">
-        <f t="shared" si="13"/>
+      <c r="X75" t="e">
+        <f t="shared" si="14"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Y75" t="str">
+        <f t="shared" si="15"/>
         <v>yes</v>
       </c>
     </row>
-    <row r="76" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>75</v>
       </c>
@@ -55395,18 +55706,18 @@
         <v>5</v>
       </c>
       <c r="F76" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>Lab</v>
       </c>
       <c r="G76" t="s">
         <v>57</v>
       </c>
       <c r="H76" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>Pink</v>
       </c>
       <c r="I76">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>4</v>
       </c>
       <c r="J76" s="7">
@@ -55419,23 +55730,27 @@
         <v>99</v>
       </c>
       <c r="P76">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>10</v>
       </c>
       <c r="U76">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="V76" t="e">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="X76" t="str">
-        <f t="shared" si="13"/>
+      <c r="X76" t="e">
+        <f t="shared" si="14"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Y76" t="str">
+        <f t="shared" si="15"/>
         <v>yes</v>
       </c>
     </row>
-    <row r="77" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>76</v>
       </c>
@@ -55449,18 +55764,18 @@
         <v>6</v>
       </c>
       <c r="F77" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>Lab</v>
       </c>
       <c r="G77" t="s">
         <v>57</v>
       </c>
       <c r="H77" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>Red</v>
       </c>
       <c r="I77">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>2</v>
       </c>
       <c r="J77" s="7">
@@ -55473,19 +55788,23 @@
         <v>99</v>
       </c>
       <c r="P77">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>10</v>
       </c>
       <c r="U77">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="V77" t="e">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="X77" t="str">
-        <f t="shared" si="13"/>
+      <c r="X77" t="e">
+        <f t="shared" si="14"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Y77" t="str">
+        <f t="shared" si="15"/>
         <v>yes</v>
       </c>
     </row>
@@ -60968,8 +61287,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55F6BF2F-CBB2-4331-929A-D3F4AD694052}">
   <dimension ref="A1:AC37"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" zoomScale="107" workbookViewId="0">
-      <selection activeCell="R24" sqref="R24"/>
+    <sheetView topLeftCell="B1" zoomScale="107" workbookViewId="0">
+      <selection activeCell="O34" sqref="O34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -62448,6 +62767,12 @@
         <f>'Kelp consumption'!R66</f>
         <v>720</v>
       </c>
+      <c r="R26">
+        <v>0</v>
+      </c>
+      <c r="AC26" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="27" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A27">
@@ -62497,6 +62822,12 @@
         <f>'Kelp consumption'!R67</f>
         <v>720</v>
       </c>
+      <c r="R27">
+        <v>1</v>
+      </c>
+      <c r="AC27" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="28" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A28">
@@ -62546,6 +62877,12 @@
         <f>'Kelp consumption'!R68</f>
         <v>720</v>
       </c>
+      <c r="R28">
+        <v>0</v>
+      </c>
+      <c r="AC28" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="29" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A29">
@@ -62595,6 +62932,9 @@
         <f>'Kelp consumption'!R69</f>
         <v>720</v>
       </c>
+      <c r="R29">
+        <v>1</v>
+      </c>
     </row>
     <row r="30" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A30">
@@ -62644,6 +62984,9 @@
         <f>'Kelp consumption'!R70</f>
         <v>720</v>
       </c>
+      <c r="R30">
+        <v>0</v>
+      </c>
     </row>
     <row r="31" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A31">
@@ -62692,6 +63035,12 @@
       <c r="M31">
         <f>'Kelp consumption'!R71</f>
         <v>720</v>
+      </c>
+      <c r="R31">
+        <v>1</v>
+      </c>
+      <c r="AC31" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="32" spans="1:29" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
urhcin sizes double checked
</commit_message>
<xml_diff>
--- a/data/raw.xlsx
+++ b/data/raw.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/EcosystemRecoveryLab/github/Ritger-Corynactis-urchin-deterrence/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EAB887E-43A8-C346-973E-D7E17B484738}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E21AAAC3-5B8D-424C-952A-38E1CAE15AAA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2100" yWindow="1080" windowWidth="29380" windowHeight="22900" activeTab="2" xr2:uid="{58E670A5-634C-427F-960F-9DA76C64E810}"/>
+    <workbookView xWindow="3260" yWindow="1280" windowWidth="29380" windowHeight="22900" activeTab="1" xr2:uid="{58E670A5-634C-427F-960F-9DA76C64E810}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="3" r:id="rId1"/>
@@ -438,12 +438,12 @@
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="21" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="21" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -776,10 +776,10 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="13"/>
+      <c r="B3" s="16"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
@@ -961,10 +961,10 @@
       <c r="A26" s="2"/>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A27" s="13" t="s">
+      <c r="A27" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="B27" s="13"/>
+      <c r="B27" s="16"/>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
@@ -49726,9 +49726,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD5E687B-43EE-4B00-8604-7EB9984510DD}">
   <dimension ref="A1:V77"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:V1"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A70" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M77" sqref="M77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -50890,7 +50890,7 @@
         <v>43</v>
       </c>
       <c r="L17">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="M17">
         <v>41</v>
@@ -53587,7 +53587,7 @@
         <v>102</v>
       </c>
       <c r="M57" s="4">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="N57" s="4" t="s">
         <v>80</v>
@@ -54988,7 +54988,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55F6BF2F-CBB2-4331-929A-D3F4AD694052}">
   <dimension ref="A1:AD37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="107" workbookViewId="0">
+    <sheetView zoomScale="107" workbookViewId="0">
       <selection activeCell="P10" sqref="P10"/>
     </sheetView>
   </sheetViews>
@@ -55692,7 +55692,7 @@
       </c>
       <c r="K9">
         <f>'Kelp consumption'!L17</f>
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="L9">
         <f>'Kelp consumption'!O17</f>
@@ -57937,10 +57937,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="15" t="s">
         <v>76</v>
       </c>
       <c r="C1" s="2" t="s">
@@ -57954,7 +57954,7 @@
       <c r="A2" s="10">
         <v>43708</v>
       </c>
-      <c r="B2" s="15">
+      <c r="B2" s="14">
         <v>0.79820601851851858</v>
       </c>
       <c r="C2" s="9">
@@ -57968,7 +57968,7 @@
       <c r="A3" s="10">
         <v>43708</v>
       </c>
-      <c r="B3" s="15">
+      <c r="B3" s="14">
         <v>0.805150462962963</v>
       </c>
       <c r="C3" s="9">
@@ -57982,7 +57982,7 @@
       <c r="A4" s="10">
         <v>43708</v>
       </c>
-      <c r="B4" s="15">
+      <c r="B4" s="14">
         <v>0.81209490740740742</v>
       </c>
       <c r="C4" s="9">
@@ -57996,7 +57996,7 @@
       <c r="A5" s="10">
         <v>43708</v>
       </c>
-      <c r="B5" s="15">
+      <c r="B5" s="14">
         <v>0.81903935185185184</v>
       </c>
       <c r="C5" s="9">
@@ -58010,7 +58010,7 @@
       <c r="A6" s="10">
         <v>43708</v>
       </c>
-      <c r="B6" s="15">
+      <c r="B6" s="14">
         <v>0.82598379629629637</v>
       </c>
       <c r="C6" s="9">
@@ -58024,7 +58024,7 @@
       <c r="A7" s="10">
         <v>43708</v>
       </c>
-      <c r="B7" s="15">
+      <c r="B7" s="14">
         <v>0.83292824074074068</v>
       </c>
       <c r="C7" s="9">
@@ -58038,7 +58038,7 @@
       <c r="A8" s="10">
         <v>43708</v>
       </c>
-      <c r="B8" s="15">
+      <c r="B8" s="14">
         <v>0.83987268518518521</v>
       </c>
       <c r="C8" s="9">
@@ -58052,7 +58052,7 @@
       <c r="A9" s="10">
         <v>43708</v>
       </c>
-      <c r="B9" s="15">
+      <c r="B9" s="14">
         <v>0.84681712962962974</v>
       </c>
       <c r="C9" s="9">
@@ -58066,7 +58066,7 @@
       <c r="A10" s="10">
         <v>43708</v>
       </c>
-      <c r="B10" s="15">
+      <c r="B10" s="14">
         <v>0.85376157407407405</v>
       </c>
       <c r="C10" s="9">
@@ -58080,7 +58080,7 @@
       <c r="A11" s="10">
         <v>43708</v>
       </c>
-      <c r="B11" s="15">
+      <c r="B11" s="14">
         <v>0.86070601851851858</v>
       </c>
       <c r="C11" s="9">
@@ -58094,7 +58094,7 @@
       <c r="A12" s="10">
         <v>43708</v>
       </c>
-      <c r="B12" s="15">
+      <c r="B12" s="14">
         <v>0.867650462962963</v>
       </c>
       <c r="C12" s="9">
@@ -58108,7 +58108,7 @@
       <c r="A13" s="10">
         <v>43708</v>
       </c>
-      <c r="B13" s="15">
+      <c r="B13" s="14">
         <v>0.87459490740740742</v>
       </c>
       <c r="C13" s="9">
@@ -58122,7 +58122,7 @@
       <c r="A14" s="10">
         <v>43708</v>
       </c>
-      <c r="B14" s="15">
+      <c r="B14" s="14">
         <v>0.88153935185185184</v>
       </c>
       <c r="C14" s="9">
@@ -58136,7 +58136,7 @@
       <c r="A15" s="10">
         <v>43708</v>
       </c>
-      <c r="B15" s="15">
+      <c r="B15" s="14">
         <v>0.88848379629629637</v>
       </c>
       <c r="C15" s="9">
@@ -58150,7 +58150,7 @@
       <c r="A16" s="10">
         <v>43708</v>
       </c>
-      <c r="B16" s="15">
+      <c r="B16" s="14">
         <v>0.89542824074074068</v>
       </c>
       <c r="C16" s="9">
@@ -58164,7 +58164,7 @@
       <c r="A17" s="10">
         <v>43708</v>
       </c>
-      <c r="B17" s="15">
+      <c r="B17" s="14">
         <v>0.90237268518518521</v>
       </c>
       <c r="C17" s="9">
@@ -58178,7 +58178,7 @@
       <c r="A18" s="10">
         <v>43708</v>
       </c>
-      <c r="B18" s="15">
+      <c r="B18" s="14">
         <v>0.90931712962962974</v>
       </c>
       <c r="C18" s="9">
@@ -58192,7 +58192,7 @@
       <c r="A19" s="10">
         <v>43708</v>
       </c>
-      <c r="B19" s="15">
+      <c r="B19" s="14">
         <v>0.91626157407407405</v>
       </c>
       <c r="C19" s="9">
@@ -58206,7 +58206,7 @@
       <c r="A20" s="10">
         <v>43708</v>
       </c>
-      <c r="B20" s="15">
+      <c r="B20" s="14">
         <v>0.92320601851851858</v>
       </c>
       <c r="C20" s="9">
@@ -58220,7 +58220,7 @@
       <c r="A21" s="10">
         <v>43708</v>
       </c>
-      <c r="B21" s="15">
+      <c r="B21" s="14">
         <v>0.930150462962963</v>
       </c>
       <c r="C21" s="9">
@@ -58234,7 +58234,7 @@
       <c r="A22" s="10">
         <v>43708</v>
       </c>
-      <c r="B22" s="15">
+      <c r="B22" s="14">
         <v>0.93709490740740742</v>
       </c>
       <c r="C22" s="9">
@@ -58248,7 +58248,7 @@
       <c r="A23" s="10">
         <v>43708</v>
       </c>
-      <c r="B23" s="15">
+      <c r="B23" s="14">
         <v>0.94403935185185184</v>
       </c>
       <c r="C23" s="9">
@@ -58262,7 +58262,7 @@
       <c r="A24" s="10">
         <v>43708</v>
       </c>
-      <c r="B24" s="15">
+      <c r="B24" s="14">
         <v>0.95098379629629637</v>
       </c>
       <c r="C24" s="9">
@@ -58276,7 +58276,7 @@
       <c r="A25" s="10">
         <v>43708</v>
       </c>
-      <c r="B25" s="15">
+      <c r="B25" s="14">
         <v>0.95792824074074068</v>
       </c>
       <c r="C25" s="9">
@@ -58290,7 +58290,7 @@
       <c r="A26" s="10">
         <v>43708</v>
       </c>
-      <c r="B26" s="15">
+      <c r="B26" s="14">
         <v>0.96487268518518521</v>
       </c>
       <c r="C26" s="9">
@@ -58304,7 +58304,7 @@
       <c r="A27" s="10">
         <v>43708</v>
       </c>
-      <c r="B27" s="15">
+      <c r="B27" s="14">
         <v>0.97181712962962974</v>
       </c>
       <c r="C27" s="9">
@@ -58318,7 +58318,7 @@
       <c r="A28" s="10">
         <v>43708</v>
       </c>
-      <c r="B28" s="15">
+      <c r="B28" s="14">
         <v>0.97876157407407405</v>
       </c>
       <c r="C28" s="9">
@@ -58332,7 +58332,7 @@
       <c r="A29" s="10">
         <v>43708</v>
       </c>
-      <c r="B29" s="15">
+      <c r="B29" s="14">
         <v>0.98570601851851858</v>
       </c>
       <c r="C29" s="9">
@@ -58346,7 +58346,7 @@
       <c r="A30" s="10">
         <v>43708</v>
       </c>
-      <c r="B30" s="15">
+      <c r="B30" s="14">
         <v>0.992650462962963</v>
       </c>
       <c r="C30" s="9">
@@ -58360,7 +58360,7 @@
       <c r="A31" s="10">
         <v>43708</v>
       </c>
-      <c r="B31" s="15">
+      <c r="B31" s="14">
         <v>0.99959490740740742</v>
       </c>
       <c r="C31" s="9">
@@ -58374,7 +58374,7 @@
       <c r="A32" s="10">
         <v>43709</v>
       </c>
-      <c r="B32" s="15">
+      <c r="B32" s="14">
         <v>6.5393518518518517E-3</v>
       </c>
       <c r="C32" s="9">
@@ -58388,7 +58388,7 @@
       <c r="A33" s="10">
         <v>43709</v>
       </c>
-      <c r="B33" s="15">
+      <c r="B33" s="14">
         <v>1.3483796296296298E-2</v>
       </c>
       <c r="C33" s="9">
@@ -58402,7 +58402,7 @@
       <c r="A34" s="10">
         <v>43709</v>
       </c>
-      <c r="B34" s="15">
+      <c r="B34" s="14">
         <v>2.0428240740740743E-2</v>
       </c>
       <c r="C34" s="9">
@@ -58416,7 +58416,7 @@
       <c r="A35" s="10">
         <v>43709</v>
       </c>
-      <c r="B35" s="15">
+      <c r="B35" s="14">
         <v>2.7372685185185184E-2</v>
       </c>
       <c r="C35" s="9">
@@ -58430,7 +58430,7 @@
       <c r="A36" s="10">
         <v>43709</v>
       </c>
-      <c r="B36" s="15">
+      <c r="B36" s="14">
         <v>3.4317129629629628E-2</v>
       </c>
       <c r="C36" s="9">
@@ -58444,7 +58444,7 @@
       <c r="A37" s="10">
         <v>43709</v>
       </c>
-      <c r="B37" s="15">
+      <c r="B37" s="14">
         <v>4.1261574074074069E-2</v>
       </c>
       <c r="C37" s="9">
@@ -58458,7 +58458,7 @@
       <c r="A38" s="10">
         <v>43709</v>
       </c>
-      <c r="B38" s="15">
+      <c r="B38" s="14">
         <v>4.8206018518518523E-2</v>
       </c>
       <c r="C38" s="9">
@@ -58472,7 +58472,7 @@
       <c r="A39" s="10">
         <v>43709</v>
       </c>
-      <c r="B39" s="15">
+      <c r="B39" s="14">
         <v>5.5150462962962964E-2</v>
       </c>
       <c r="C39" s="9">
@@ -58486,7 +58486,7 @@
       <c r="A40" s="10">
         <v>43709</v>
       </c>
-      <c r="B40" s="15">
+      <c r="B40" s="14">
         <v>6.2094907407407411E-2</v>
       </c>
       <c r="C40" s="9">
@@ -58500,7 +58500,7 @@
       <c r="A41" s="10">
         <v>43709</v>
       </c>
-      <c r="B41" s="15">
+      <c r="B41" s="14">
         <v>6.9039351851851852E-2</v>
       </c>
       <c r="C41" s="9">
@@ -58514,7 +58514,7 @@
       <c r="A42" s="10">
         <v>43709</v>
       </c>
-      <c r="B42" s="15">
+      <c r="B42" s="14">
         <v>7.5983796296296299E-2</v>
       </c>
       <c r="C42" s="9">
@@ -58528,7 +58528,7 @@
       <c r="A43" s="10">
         <v>43709</v>
       </c>
-      <c r="B43" s="15">
+      <c r="B43" s="14">
         <v>8.2928240740740733E-2</v>
       </c>
       <c r="C43" s="9">
@@ -58542,7 +58542,7 @@
       <c r="A44" s="10">
         <v>43709</v>
       </c>
-      <c r="B44" s="15">
+      <c r="B44" s="14">
         <v>8.9872685185185194E-2</v>
       </c>
       <c r="C44" s="9">
@@ -58556,7 +58556,7 @@
       <c r="A45" s="10">
         <v>43709</v>
       </c>
-      <c r="B45" s="15">
+      <c r="B45" s="14">
         <v>9.6817129629629628E-2</v>
       </c>
       <c r="C45" s="9">
@@ -58570,7 +58570,7 @@
       <c r="A46" s="10">
         <v>43709</v>
       </c>
-      <c r="B46" s="15">
+      <c r="B46" s="14">
         <v>0.10376157407407409</v>
       </c>
       <c r="C46" s="9">
@@ -58584,7 +58584,7 @@
       <c r="A47" s="10">
         <v>43709</v>
       </c>
-      <c r="B47" s="15">
+      <c r="B47" s="14">
         <v>0.11070601851851852</v>
       </c>
       <c r="C47" s="9">
@@ -58598,7 +58598,7 @@
       <c r="A48" s="10">
         <v>43709</v>
       </c>
-      <c r="B48" s="15">
+      <c r="B48" s="14">
         <v>0.11765046296296296</v>
       </c>
       <c r="C48" s="9">
@@ -58612,7 +58612,7 @@
       <c r="A49" s="10">
         <v>43709</v>
       </c>
-      <c r="B49" s="15">
+      <c r="B49" s="14">
         <v>0.1245949074074074</v>
       </c>
       <c r="C49" s="9">
@@ -58626,7 +58626,7 @@
       <c r="A50" s="10">
         <v>43709</v>
       </c>
-      <c r="B50" s="15">
+      <c r="B50" s="14">
         <v>0.13153935185185187</v>
       </c>
       <c r="C50" s="9">
@@ -58640,7 +58640,7 @@
       <c r="A51" s="10">
         <v>43709</v>
       </c>
-      <c r="B51" s="15">
+      <c r="B51" s="14">
         <v>0.13848379629629629</v>
       </c>
       <c r="C51" s="9">
@@ -58654,7 +58654,7 @@
       <c r="A52" s="10">
         <v>43709</v>
       </c>
-      <c r="B52" s="15">
+      <c r="B52" s="14">
         <v>0.14542824074074076</v>
       </c>
       <c r="C52" s="9">
@@ -58668,7 +58668,7 @@
       <c r="A53" s="10">
         <v>43709</v>
       </c>
-      <c r="B53" s="15">
+      <c r="B53" s="14">
         <v>0.15237268518518518</v>
       </c>
       <c r="C53" s="9">
@@ -58682,7 +58682,7 @@
       <c r="A54" s="10">
         <v>43709</v>
       </c>
-      <c r="B54" s="15">
+      <c r="B54" s="14">
         <v>0.15931712962962963</v>
       </c>
       <c r="C54" s="9">
@@ -58696,7 +58696,7 @@
       <c r="A55" s="10">
         <v>43709</v>
       </c>
-      <c r="B55" s="15">
+      <c r="B55" s="14">
         <v>0.16626157407407408</v>
       </c>
       <c r="C55" s="9">
@@ -58710,7 +58710,7 @@
       <c r="A56" s="10">
         <v>43709</v>
       </c>
-      <c r="B56" s="15">
+      <c r="B56" s="14">
         <v>0.1732060185185185</v>
       </c>
       <c r="C56" s="9">
@@ -58724,7 +58724,7 @@
       <c r="A57" s="10">
         <v>43709</v>
       </c>
-      <c r="B57" s="15">
+      <c r="B57" s="14">
         <v>0.18015046296296297</v>
       </c>
       <c r="C57" s="9">
@@ -58738,7 +58738,7 @@
       <c r="A58" s="10">
         <v>43709</v>
       </c>
-      <c r="B58" s="15">
+      <c r="B58" s="14">
         <v>0.18709490740740742</v>
       </c>
       <c r="C58" s="9">
@@ -58752,7 +58752,7 @@
       <c r="A59" s="10">
         <v>43709</v>
       </c>
-      <c r="B59" s="15">
+      <c r="B59" s="14">
         <v>0.19403935185185184</v>
       </c>
       <c r="C59" s="9">
@@ -58766,7 +58766,7 @@
       <c r="A60" s="10">
         <v>43709</v>
       </c>
-      <c r="B60" s="15">
+      <c r="B60" s="14">
         <v>0.20098379629629629</v>
       </c>
       <c r="C60" s="9">
@@ -58780,7 +58780,7 @@
       <c r="A61" s="10">
         <v>43709</v>
       </c>
-      <c r="B61" s="15">
+      <c r="B61" s="14">
         <v>0.20792824074074076</v>
       </c>
       <c r="C61" s="9">
@@ -58794,7 +58794,7 @@
       <c r="A62" s="10">
         <v>43709</v>
       </c>
-      <c r="B62" s="15">
+      <c r="B62" s="14">
         <v>0.21487268518518518</v>
       </c>
       <c r="C62" s="9">
@@ -58808,7 +58808,7 @@
       <c r="A63" s="10">
         <v>43709</v>
       </c>
-      <c r="B63" s="15">
+      <c r="B63" s="14">
         <v>0.22181712962962963</v>
       </c>
       <c r="C63" s="9">
@@ -58822,7 +58822,7 @@
       <c r="A64" s="10">
         <v>43709</v>
       </c>
-      <c r="B64" s="15">
+      <c r="B64" s="14">
         <v>0.22876157407407408</v>
       </c>
       <c r="C64" s="9">
@@ -58836,7 +58836,7 @@
       <c r="A65" s="10">
         <v>43709</v>
       </c>
-      <c r="B65" s="15">
+      <c r="B65" s="14">
         <v>0.2357060185185185</v>
       </c>
       <c r="C65" s="9">
@@ -58850,7 +58850,7 @@
       <c r="A66" s="10">
         <v>43709</v>
       </c>
-      <c r="B66" s="15">
+      <c r="B66" s="14">
         <v>0.24265046296296297</v>
       </c>
       <c r="C66" s="9">
@@ -58864,7 +58864,7 @@
       <c r="A67" s="10">
         <v>43709</v>
       </c>
-      <c r="B67" s="15">
+      <c r="B67" s="14">
         <v>0.24959490740740742</v>
       </c>
       <c r="C67" s="9">
@@ -58878,7 +58878,7 @@
       <c r="A68" s="10">
         <v>43709</v>
       </c>
-      <c r="B68" s="15">
+      <c r="B68" s="14">
         <v>0.25653935185185184</v>
       </c>
       <c r="C68" s="9">
@@ -58892,7 +58892,7 @@
       <c r="A69" s="10">
         <v>43709</v>
       </c>
-      <c r="B69" s="15">
+      <c r="B69" s="14">
         <v>0.26348379629629631</v>
       </c>
       <c r="C69" s="9">
@@ -58906,7 +58906,7 @@
       <c r="A70" s="10">
         <v>43709</v>
       </c>
-      <c r="B70" s="15">
+      <c r="B70" s="14">
         <v>0.27042824074074073</v>
       </c>
       <c r="C70" s="9">
@@ -58920,7 +58920,7 @@
       <c r="A71" s="10">
         <v>43709</v>
       </c>
-      <c r="B71" s="15">
+      <c r="B71" s="14">
         <v>0.27737268518518515</v>
       </c>
       <c r="C71" s="9">
@@ -58934,7 +58934,7 @@
       <c r="A72" s="10">
         <v>43709</v>
       </c>
-      <c r="B72" s="15">
+      <c r="B72" s="14">
         <v>0.28431712962962963</v>
       </c>
       <c r="C72" s="9">
@@ -58948,7 +58948,7 @@
       <c r="A73" s="10">
         <v>43709</v>
       </c>
-      <c r="B73" s="15">
+      <c r="B73" s="14">
         <v>0.2912615740740741</v>
       </c>
       <c r="C73" s="9">
@@ -58962,7 +58962,7 @@
       <c r="A74" s="10">
         <v>43709</v>
       </c>
-      <c r="B74" s="15">
+      <c r="B74" s="14">
         <v>0.29820601851851852</v>
       </c>
       <c r="C74" s="9">
@@ -58976,7 +58976,7 @@
       <c r="A75" s="10">
         <v>43709</v>
       </c>
-      <c r="B75" s="15">
+      <c r="B75" s="14">
         <v>0.30515046296296294</v>
       </c>
       <c r="C75" s="9">
@@ -58990,7 +58990,7 @@
       <c r="A76" s="10">
         <v>43709</v>
       </c>
-      <c r="B76" s="15">
+      <c r="B76" s="14">
         <v>0.31209490740740742</v>
       </c>
       <c r="C76" s="9">
@@ -59004,7 +59004,7 @@
       <c r="A77" s="10">
         <v>43709</v>
       </c>
-      <c r="B77" s="15">
+      <c r="B77" s="14">
         <v>0.31903935185185184</v>
       </c>
       <c r="C77" s="9">
@@ -59018,7 +59018,7 @@
       <c r="A78" s="10">
         <v>43709</v>
       </c>
-      <c r="B78" s="15">
+      <c r="B78" s="14">
         <v>0.32598379629629631</v>
       </c>
       <c r="C78" s="9">
@@ -59032,7 +59032,7 @@
       <c r="A79" s="10">
         <v>43709</v>
       </c>
-      <c r="B79" s="15">
+      <c r="B79" s="14">
         <v>0.33292824074074073</v>
       </c>
       <c r="C79" s="9">
@@ -59046,7 +59046,7 @@
       <c r="A80" s="10">
         <v>43709</v>
       </c>
-      <c r="B80" s="15">
+      <c r="B80" s="14">
         <v>0.79820601851851858</v>
       </c>
       <c r="C80" s="9">
@@ -59060,7 +59060,7 @@
       <c r="A81" s="10">
         <v>43709</v>
       </c>
-      <c r="B81" s="15">
+      <c r="B81" s="14">
         <v>0.805150462962963</v>
       </c>
       <c r="C81" s="9">
@@ -59074,7 +59074,7 @@
       <c r="A82" s="10">
         <v>43709</v>
       </c>
-      <c r="B82" s="15">
+      <c r="B82" s="14">
         <v>0.81209490740740742</v>
       </c>
       <c r="C82" s="9">
@@ -59088,7 +59088,7 @@
       <c r="A83" s="10">
         <v>43709</v>
       </c>
-      <c r="B83" s="15">
+      <c r="B83" s="14">
         <v>0.81903935185185184</v>
       </c>
       <c r="C83" s="9">
@@ -59102,7 +59102,7 @@
       <c r="A84" s="10">
         <v>43709</v>
       </c>
-      <c r="B84" s="15">
+      <c r="B84" s="14">
         <v>0.82598379629629637</v>
       </c>
       <c r="C84" s="9">
@@ -59116,7 +59116,7 @@
       <c r="A85" s="10">
         <v>43709</v>
       </c>
-      <c r="B85" s="15">
+      <c r="B85" s="14">
         <v>0.83292824074074068</v>
       </c>
       <c r="C85" s="9">
@@ -59130,7 +59130,7 @@
       <c r="A86" s="10">
         <v>43709</v>
       </c>
-      <c r="B86" s="15">
+      <c r="B86" s="14">
         <v>0.83987268518518521</v>
       </c>
       <c r="C86" s="9">
@@ -59144,7 +59144,7 @@
       <c r="A87" s="10">
         <v>43709</v>
       </c>
-      <c r="B87" s="15">
+      <c r="B87" s="14">
         <v>0.84681712962962974</v>
       </c>
       <c r="C87" s="9">
@@ -59158,7 +59158,7 @@
       <c r="A88" s="10">
         <v>43709</v>
       </c>
-      <c r="B88" s="15">
+      <c r="B88" s="14">
         <v>0.85376157407407405</v>
       </c>
       <c r="C88" s="9">
@@ -59172,7 +59172,7 @@
       <c r="A89" s="10">
         <v>43709</v>
       </c>
-      <c r="B89" s="15">
+      <c r="B89" s="14">
         <v>0.86070601851851858</v>
       </c>
       <c r="C89" s="9">
@@ -59186,7 +59186,7 @@
       <c r="A90" s="10">
         <v>43709</v>
       </c>
-      <c r="B90" s="15">
+      <c r="B90" s="14">
         <v>0.867650462962963</v>
       </c>
       <c r="C90" s="9">
@@ -59200,7 +59200,7 @@
       <c r="A91" s="10">
         <v>43709</v>
       </c>
-      <c r="B91" s="15">
+      <c r="B91" s="14">
         <v>0.87459490740740742</v>
       </c>
       <c r="C91" s="9">
@@ -59214,7 +59214,7 @@
       <c r="A92" s="10">
         <v>43709</v>
       </c>
-      <c r="B92" s="15">
+      <c r="B92" s="14">
         <v>0.88153935185185184</v>
       </c>
       <c r="C92" s="9">
@@ -59228,7 +59228,7 @@
       <c r="A93" s="10">
         <v>43709</v>
       </c>
-      <c r="B93" s="15">
+      <c r="B93" s="14">
         <v>0.88848379629629637</v>
       </c>
       <c r="C93" s="9">
@@ -59242,7 +59242,7 @@
       <c r="A94" s="10">
         <v>43709</v>
       </c>
-      <c r="B94" s="15">
+      <c r="B94" s="14">
         <v>0.89542824074074068</v>
       </c>
       <c r="C94" s="9">
@@ -59256,7 +59256,7 @@
       <c r="A95" s="10">
         <v>43709</v>
       </c>
-      <c r="B95" s="15">
+      <c r="B95" s="14">
         <v>0.90237268518518521</v>
       </c>
       <c r="C95" s="9">
@@ -59270,7 +59270,7 @@
       <c r="A96" s="10">
         <v>43709</v>
       </c>
-      <c r="B96" s="15">
+      <c r="B96" s="14">
         <v>0.90931712962962974</v>
       </c>
       <c r="C96" s="9">
@@ -59284,7 +59284,7 @@
       <c r="A97" s="10">
         <v>43709</v>
       </c>
-      <c r="B97" s="15">
+      <c r="B97" s="14">
         <v>0.91626157407407405</v>
       </c>
       <c r="C97" s="9">
@@ -59298,7 +59298,7 @@
       <c r="A98" s="10">
         <v>43709</v>
       </c>
-      <c r="B98" s="15">
+      <c r="B98" s="14">
         <v>0.92320601851851858</v>
       </c>
       <c r="C98" s="9">
@@ -59312,7 +59312,7 @@
       <c r="A99" s="10">
         <v>43709</v>
       </c>
-      <c r="B99" s="15">
+      <c r="B99" s="14">
         <v>0.930150462962963</v>
       </c>
       <c r="C99" s="9">
@@ -59326,7 +59326,7 @@
       <c r="A100" s="10">
         <v>43709</v>
       </c>
-      <c r="B100" s="15">
+      <c r="B100" s="14">
         <v>0.93709490740740742</v>
       </c>
       <c r="C100" s="9">
@@ -59340,7 +59340,7 @@
       <c r="A101" s="10">
         <v>43709</v>
       </c>
-      <c r="B101" s="15">
+      <c r="B101" s="14">
         <v>0.94403935185185184</v>
       </c>
       <c r="C101" s="9">
@@ -59354,7 +59354,7 @@
       <c r="A102" s="10">
         <v>43709</v>
       </c>
-      <c r="B102" s="15">
+      <c r="B102" s="14">
         <v>0.95098379629629637</v>
       </c>
       <c r="C102" s="9">
@@ -59368,7 +59368,7 @@
       <c r="A103" s="10">
         <v>43709</v>
       </c>
-      <c r="B103" s="15">
+      <c r="B103" s="14">
         <v>0.95792824074074068</v>
       </c>
       <c r="C103" s="9">
@@ -59382,7 +59382,7 @@
       <c r="A104" s="10">
         <v>43709</v>
       </c>
-      <c r="B104" s="15">
+      <c r="B104" s="14">
         <v>0.96487268518518521</v>
       </c>
       <c r="C104" s="9">
@@ -59396,7 +59396,7 @@
       <c r="A105" s="10">
         <v>43709</v>
       </c>
-      <c r="B105" s="15">
+      <c r="B105" s="14">
         <v>0.97181712962962974</v>
       </c>
       <c r="C105" s="9">
@@ -59410,7 +59410,7 @@
       <c r="A106" s="10">
         <v>43709</v>
       </c>
-      <c r="B106" s="15">
+      <c r="B106" s="14">
         <v>0.97876157407407405</v>
       </c>
       <c r="C106" s="9">
@@ -59424,7 +59424,7 @@
       <c r="A107" s="10">
         <v>43709</v>
       </c>
-      <c r="B107" s="15">
+      <c r="B107" s="14">
         <v>0.98570601851851858</v>
       </c>
       <c r="C107" s="9">
@@ -59438,7 +59438,7 @@
       <c r="A108" s="10">
         <v>43709</v>
       </c>
-      <c r="B108" s="15">
+      <c r="B108" s="14">
         <v>0.992650462962963</v>
       </c>
       <c r="C108" s="9">
@@ -59452,7 +59452,7 @@
       <c r="A109" s="10">
         <v>43709</v>
       </c>
-      <c r="B109" s="15">
+      <c r="B109" s="14">
         <v>0.99959490740740742</v>
       </c>
       <c r="C109" s="9">
@@ -59466,7 +59466,7 @@
       <c r="A110" s="10">
         <v>43710</v>
       </c>
-      <c r="B110" s="15">
+      <c r="B110" s="14">
         <v>6.5393518518518517E-3</v>
       </c>
       <c r="C110" s="9">
@@ -59480,7 +59480,7 @@
       <c r="A111" s="10">
         <v>43710</v>
       </c>
-      <c r="B111" s="15">
+      <c r="B111" s="14">
         <v>1.3483796296296298E-2</v>
       </c>
       <c r="C111" s="9">
@@ -59494,7 +59494,7 @@
       <c r="A112" s="10">
         <v>43710</v>
       </c>
-      <c r="B112" s="15">
+      <c r="B112" s="14">
         <v>2.0428240740740743E-2</v>
       </c>
       <c r="C112" s="9">
@@ -59508,7 +59508,7 @@
       <c r="A113" s="10">
         <v>43710</v>
       </c>
-      <c r="B113" s="15">
+      <c r="B113" s="14">
         <v>2.7372685185185184E-2</v>
       </c>
       <c r="C113" s="9">
@@ -59522,7 +59522,7 @@
       <c r="A114" s="10">
         <v>43710</v>
       </c>
-      <c r="B114" s="15">
+      <c r="B114" s="14">
         <v>3.4317129629629628E-2</v>
       </c>
       <c r="C114" s="9">
@@ -59536,7 +59536,7 @@
       <c r="A115" s="10">
         <v>43710</v>
       </c>
-      <c r="B115" s="15">
+      <c r="B115" s="14">
         <v>4.1261574074074069E-2</v>
       </c>
       <c r="C115" s="9">
@@ -59550,7 +59550,7 @@
       <c r="A116" s="10">
         <v>43710</v>
       </c>
-      <c r="B116" s="15">
+      <c r="B116" s="14">
         <v>4.8206018518518523E-2</v>
       </c>
       <c r="C116" s="9">
@@ -59564,7 +59564,7 @@
       <c r="A117" s="10">
         <v>43710</v>
       </c>
-      <c r="B117" s="15">
+      <c r="B117" s="14">
         <v>5.5150462962962964E-2</v>
       </c>
       <c r="C117" s="9">
@@ -59578,7 +59578,7 @@
       <c r="A118" s="10">
         <v>43710</v>
       </c>
-      <c r="B118" s="15">
+      <c r="B118" s="14">
         <v>6.2094907407407411E-2</v>
       </c>
       <c r="C118" s="9">
@@ -59592,7 +59592,7 @@
       <c r="A119" s="10">
         <v>43710</v>
       </c>
-      <c r="B119" s="15">
+      <c r="B119" s="14">
         <v>6.9039351851851852E-2</v>
       </c>
       <c r="C119" s="9">
@@ -59606,7 +59606,7 @@
       <c r="A120" s="10">
         <v>43710</v>
       </c>
-      <c r="B120" s="15">
+      <c r="B120" s="14">
         <v>7.5983796296296299E-2</v>
       </c>
       <c r="C120" s="9">
@@ -59620,7 +59620,7 @@
       <c r="A121" s="10">
         <v>43710</v>
       </c>
-      <c r="B121" s="15">
+      <c r="B121" s="14">
         <v>8.2928240740740733E-2</v>
       </c>
       <c r="C121" s="9">
@@ -59634,7 +59634,7 @@
       <c r="A122" s="10">
         <v>43710</v>
       </c>
-      <c r="B122" s="15">
+      <c r="B122" s="14">
         <v>8.9872685185185194E-2</v>
       </c>
       <c r="C122" s="9">
@@ -59648,7 +59648,7 @@
       <c r="A123" s="10">
         <v>43710</v>
       </c>
-      <c r="B123" s="15">
+      <c r="B123" s="14">
         <v>9.6817129629629628E-2</v>
       </c>
       <c r="C123" s="9">
@@ -59662,7 +59662,7 @@
       <c r="A124" s="10">
         <v>43710</v>
       </c>
-      <c r="B124" s="15">
+      <c r="B124" s="14">
         <v>0.10376157407407409</v>
       </c>
       <c r="C124" s="9">
@@ -59676,7 +59676,7 @@
       <c r="A125" s="10">
         <v>43710</v>
       </c>
-      <c r="B125" s="15">
+      <c r="B125" s="14">
         <v>0.11070601851851852</v>
       </c>
       <c r="C125" s="9">
@@ -59690,7 +59690,7 @@
       <c r="A126" s="10">
         <v>43710</v>
       </c>
-      <c r="B126" s="15">
+      <c r="B126" s="14">
         <v>0.11765046296296296</v>
       </c>
       <c r="C126" s="9">
@@ -59704,7 +59704,7 @@
       <c r="A127" s="10">
         <v>43710</v>
       </c>
-      <c r="B127" s="15">
+      <c r="B127" s="14">
         <v>0.1245949074074074</v>
       </c>
       <c r="C127" s="9">
@@ -59718,7 +59718,7 @@
       <c r="A128" s="10">
         <v>43710</v>
       </c>
-      <c r="B128" s="15">
+      <c r="B128" s="14">
         <v>0.13153935185185187</v>
       </c>
       <c r="C128" s="9">
@@ -59732,7 +59732,7 @@
       <c r="A129" s="10">
         <v>43710</v>
       </c>
-      <c r="B129" s="15">
+      <c r="B129" s="14">
         <v>0.13848379629629629</v>
       </c>
       <c r="C129" s="9">
@@ -59746,7 +59746,7 @@
       <c r="A130" s="10">
         <v>43710</v>
       </c>
-      <c r="B130" s="15">
+      <c r="B130" s="14">
         <v>0.14542824074074076</v>
       </c>
       <c r="C130" s="9">
@@ -59760,7 +59760,7 @@
       <c r="A131" s="10">
         <v>43710</v>
       </c>
-      <c r="B131" s="15">
+      <c r="B131" s="14">
         <v>0.15237268518518518</v>
       </c>
       <c r="C131" s="9">
@@ -59774,7 +59774,7 @@
       <c r="A132" s="10">
         <v>43710</v>
       </c>
-      <c r="B132" s="15">
+      <c r="B132" s="14">
         <v>0.15931712962962963</v>
       </c>
       <c r="C132" s="9">
@@ -59788,7 +59788,7 @@
       <c r="A133" s="10">
         <v>43710</v>
       </c>
-      <c r="B133" s="15">
+      <c r="B133" s="14">
         <v>0.16626157407407408</v>
       </c>
       <c r="C133" s="9">
@@ -59802,7 +59802,7 @@
       <c r="A134" s="10">
         <v>43710</v>
       </c>
-      <c r="B134" s="15">
+      <c r="B134" s="14">
         <v>0.1732060185185185</v>
       </c>
       <c r="C134" s="9">
@@ -59816,7 +59816,7 @@
       <c r="A135" s="10">
         <v>43710</v>
       </c>
-      <c r="B135" s="15">
+      <c r="B135" s="14">
         <v>0.18015046296296297</v>
       </c>
       <c r="C135" s="9">
@@ -59830,7 +59830,7 @@
       <c r="A136" s="10">
         <v>43710</v>
       </c>
-      <c r="B136" s="15">
+      <c r="B136" s="14">
         <v>0.18709490740740742</v>
       </c>
       <c r="C136" s="9">
@@ -59844,7 +59844,7 @@
       <c r="A137" s="10">
         <v>43710</v>
       </c>
-      <c r="B137" s="15">
+      <c r="B137" s="14">
         <v>0.19403935185185184</v>
       </c>
       <c r="C137" s="9">
@@ -59858,7 +59858,7 @@
       <c r="A138" s="10">
         <v>43710</v>
       </c>
-      <c r="B138" s="15">
+      <c r="B138" s="14">
         <v>0.20098379629629629</v>
       </c>
       <c r="C138" s="9">
@@ -59872,7 +59872,7 @@
       <c r="A139" s="10">
         <v>43710</v>
       </c>
-      <c r="B139" s="15">
+      <c r="B139" s="14">
         <v>0.20792824074074076</v>
       </c>
       <c r="C139" s="9">
@@ -59886,7 +59886,7 @@
       <c r="A140" s="10">
         <v>43710</v>
       </c>
-      <c r="B140" s="15">
+      <c r="B140" s="14">
         <v>0.21487268518518518</v>
       </c>
       <c r="C140" s="9">
@@ -59900,7 +59900,7 @@
       <c r="A141" s="10">
         <v>43710</v>
       </c>
-      <c r="B141" s="15">
+      <c r="B141" s="14">
         <v>0.22181712962962963</v>
       </c>
       <c r="C141" s="9">
@@ -59914,7 +59914,7 @@
       <c r="A142" s="10">
         <v>43710</v>
       </c>
-      <c r="B142" s="15">
+      <c r="B142" s="14">
         <v>0.22876157407407408</v>
       </c>
       <c r="C142" s="9">
@@ -59928,7 +59928,7 @@
       <c r="A143" s="10">
         <v>43710</v>
       </c>
-      <c r="B143" s="15">
+      <c r="B143" s="14">
         <v>0.2357060185185185</v>
       </c>
       <c r="C143" s="9">
@@ -59942,7 +59942,7 @@
       <c r="A144" s="10">
         <v>43710</v>
       </c>
-      <c r="B144" s="15">
+      <c r="B144" s="14">
         <v>0.24265046296296297</v>
       </c>
       <c r="C144" s="9">
@@ -59956,7 +59956,7 @@
       <c r="A145" s="10">
         <v>43710</v>
       </c>
-      <c r="B145" s="15">
+      <c r="B145" s="14">
         <v>0.24959490740740742</v>
       </c>
       <c r="C145" s="9">
@@ -59970,7 +59970,7 @@
       <c r="A146" s="10">
         <v>43710</v>
       </c>
-      <c r="B146" s="15">
+      <c r="B146" s="14">
         <v>0.25653935185185184</v>
       </c>
       <c r="C146" s="9">
@@ -59984,7 +59984,7 @@
       <c r="A147" s="10">
         <v>43710</v>
       </c>
-      <c r="B147" s="15">
+      <c r="B147" s="14">
         <v>0.26348379629629631</v>
       </c>
       <c r="C147" s="9">
@@ -59998,7 +59998,7 @@
       <c r="A148" s="10">
         <v>43710</v>
       </c>
-      <c r="B148" s="15">
+      <c r="B148" s="14">
         <v>0.27042824074074073</v>
       </c>
       <c r="C148" s="9">
@@ -60012,7 +60012,7 @@
       <c r="A149" s="10">
         <v>43710</v>
       </c>
-      <c r="B149" s="15">
+      <c r="B149" s="14">
         <v>0.27737268518518515</v>
       </c>
       <c r="C149" s="9">
@@ -60026,7 +60026,7 @@
       <c r="A150" s="10">
         <v>43710</v>
       </c>
-      <c r="B150" s="15">
+      <c r="B150" s="14">
         <v>0.28431712962962963</v>
       </c>
       <c r="C150" s="9">
@@ -60040,7 +60040,7 @@
       <c r="A151" s="10">
         <v>43710</v>
       </c>
-      <c r="B151" s="15">
+      <c r="B151" s="14">
         <v>0.2912615740740741</v>
       </c>
       <c r="C151" s="9">
@@ -60054,7 +60054,7 @@
       <c r="A152" s="10">
         <v>43710</v>
       </c>
-      <c r="B152" s="15">
+      <c r="B152" s="14">
         <v>0.29820601851851852</v>
       </c>
       <c r="C152" s="9">
@@ -60068,7 +60068,7 @@
       <c r="A153" s="10">
         <v>43710</v>
       </c>
-      <c r="B153" s="15">
+      <c r="B153" s="14">
         <v>0.30515046296296294</v>
       </c>
       <c r="C153" s="9">
@@ -60082,7 +60082,7 @@
       <c r="A154" s="10">
         <v>43710</v>
       </c>
-      <c r="B154" s="15">
+      <c r="B154" s="14">
         <v>0.31209490740740742</v>
       </c>
       <c r="C154" s="9">
@@ -60096,7 +60096,7 @@
       <c r="A155" s="10">
         <v>43710</v>
       </c>
-      <c r="B155" s="15">
+      <c r="B155" s="14">
         <v>0.31903935185185184</v>
       </c>
       <c r="C155" s="9">
@@ -60110,7 +60110,7 @@
       <c r="A156" s="10">
         <v>43710</v>
       </c>
-      <c r="B156" s="15">
+      <c r="B156" s="14">
         <v>0.32598379629629631</v>
       </c>
       <c r="C156" s="9">
@@ -60124,7 +60124,7 @@
       <c r="A157" s="10">
         <v>43710</v>
       </c>
-      <c r="B157" s="15">
+      <c r="B157" s="14">
         <v>0.33292824074074073</v>
       </c>
       <c r="C157" s="9">
@@ -60138,7 +60138,7 @@
       <c r="A158" s="10">
         <v>43710</v>
       </c>
-      <c r="B158" s="15">
+      <c r="B158" s="14">
         <v>0.79820601851851858</v>
       </c>
       <c r="C158" s="9">
@@ -60152,7 +60152,7 @@
       <c r="A159" s="10">
         <v>43710</v>
       </c>
-      <c r="B159" s="15">
+      <c r="B159" s="14">
         <v>0.805150462962963</v>
       </c>
       <c r="C159" s="9">
@@ -60166,7 +60166,7 @@
       <c r="A160" s="10">
         <v>43710</v>
       </c>
-      <c r="B160" s="15">
+      <c r="B160" s="14">
         <v>0.81209490740740742</v>
       </c>
       <c r="C160" s="9">
@@ -60180,7 +60180,7 @@
       <c r="A161" s="10">
         <v>43710</v>
       </c>
-      <c r="B161" s="15">
+      <c r="B161" s="14">
         <v>0.81903935185185184</v>
       </c>
       <c r="C161" s="9">
@@ -60194,7 +60194,7 @@
       <c r="A162" s="10">
         <v>43710</v>
       </c>
-      <c r="B162" s="15">
+      <c r="B162" s="14">
         <v>0.82598379629629637</v>
       </c>
       <c r="C162" s="9">
@@ -60208,7 +60208,7 @@
       <c r="A163" s="10">
         <v>43710</v>
       </c>
-      <c r="B163" s="15">
+      <c r="B163" s="14">
         <v>0.83292824074074068</v>
       </c>
       <c r="C163" s="9">
@@ -60222,7 +60222,7 @@
       <c r="A164" s="10">
         <v>43710</v>
       </c>
-      <c r="B164" s="15">
+      <c r="B164" s="14">
         <v>0.83987268518518521</v>
       </c>
       <c r="C164" s="9">
@@ -60236,7 +60236,7 @@
       <c r="A165" s="10">
         <v>43710</v>
       </c>
-      <c r="B165" s="15">
+      <c r="B165" s="14">
         <v>0.84681712962962974</v>
       </c>
       <c r="C165" s="9">
@@ -60250,7 +60250,7 @@
       <c r="A166" s="10">
         <v>43710</v>
       </c>
-      <c r="B166" s="15">
+      <c r="B166" s="14">
         <v>0.85376157407407405</v>
       </c>
       <c r="C166" s="9">
@@ -60264,7 +60264,7 @@
       <c r="A167" s="10">
         <v>43710</v>
       </c>
-      <c r="B167" s="15">
+      <c r="B167" s="14">
         <v>0.86070601851851858</v>
       </c>
       <c r="C167" s="9">
@@ -60278,7 +60278,7 @@
       <c r="A168" s="10">
         <v>43710</v>
       </c>
-      <c r="B168" s="15">
+      <c r="B168" s="14">
         <v>0.867650462962963</v>
       </c>
       <c r="C168" s="9">
@@ -60292,7 +60292,7 @@
       <c r="A169" s="10">
         <v>43710</v>
       </c>
-      <c r="B169" s="15">
+      <c r="B169" s="14">
         <v>0.87459490740740742</v>
       </c>
       <c r="C169" s="9">
@@ -60306,7 +60306,7 @@
       <c r="A170" s="10">
         <v>43710</v>
       </c>
-      <c r="B170" s="15">
+      <c r="B170" s="14">
         <v>0.88153935185185184</v>
       </c>
       <c r="C170" s="9">
@@ -60320,7 +60320,7 @@
       <c r="A171" s="10">
         <v>43710</v>
       </c>
-      <c r="B171" s="15">
+      <c r="B171" s="14">
         <v>0.88848379629629637</v>
       </c>
       <c r="C171" s="9">
@@ -60334,7 +60334,7 @@
       <c r="A172" s="10">
         <v>43710</v>
       </c>
-      <c r="B172" s="15">
+      <c r="B172" s="14">
         <v>0.89542824074074068</v>
       </c>
       <c r="C172" s="9">
@@ -60348,7 +60348,7 @@
       <c r="A173" s="10">
         <v>43710</v>
       </c>
-      <c r="B173" s="15">
+      <c r="B173" s="14">
         <v>0.90237268518518521</v>
       </c>
       <c r="C173" s="9">
@@ -60362,7 +60362,7 @@
       <c r="A174" s="10">
         <v>43710</v>
       </c>
-      <c r="B174" s="15">
+      <c r="B174" s="14">
         <v>0.90931712962962974</v>
       </c>
       <c r="C174" s="9">
@@ -60376,7 +60376,7 @@
       <c r="A175" s="10">
         <v>43710</v>
       </c>
-      <c r="B175" s="15">
+      <c r="B175" s="14">
         <v>0.91626157407407405</v>
       </c>
       <c r="C175" s="9">
@@ -60390,7 +60390,7 @@
       <c r="A176" s="10">
         <v>43710</v>
       </c>
-      <c r="B176" s="15">
+      <c r="B176" s="14">
         <v>0.92320601851851858</v>
       </c>
       <c r="C176" s="9">
@@ -60404,7 +60404,7 @@
       <c r="A177" s="10">
         <v>43710</v>
       </c>
-      <c r="B177" s="15">
+      <c r="B177" s="14">
         <v>0.930150462962963</v>
       </c>
       <c r="C177" s="9">
@@ -60418,7 +60418,7 @@
       <c r="A178" s="10">
         <v>43710</v>
       </c>
-      <c r="B178" s="15">
+      <c r="B178" s="14">
         <v>0.93709490740740742</v>
       </c>
       <c r="C178" s="9">
@@ -60432,7 +60432,7 @@
       <c r="A179" s="10">
         <v>43710</v>
       </c>
-      <c r="B179" s="15">
+      <c r="B179" s="14">
         <v>0.94403935185185184</v>
       </c>
       <c r="C179" s="9">
@@ -60446,7 +60446,7 @@
       <c r="A180" s="10">
         <v>43710</v>
       </c>
-      <c r="B180" s="15">
+      <c r="B180" s="14">
         <v>0.95098379629629637</v>
       </c>
       <c r="C180" s="9">
@@ -60460,7 +60460,7 @@
       <c r="A181" s="10">
         <v>43710</v>
       </c>
-      <c r="B181" s="15">
+      <c r="B181" s="14">
         <v>0.95792824074074068</v>
       </c>
       <c r="C181" s="9">
@@ -60474,7 +60474,7 @@
       <c r="A182" s="10">
         <v>43710</v>
       </c>
-      <c r="B182" s="15">
+      <c r="B182" s="14">
         <v>0.96487268518518521</v>
       </c>
       <c r="C182" s="9">
@@ -60488,7 +60488,7 @@
       <c r="A183" s="10">
         <v>43710</v>
       </c>
-      <c r="B183" s="15">
+      <c r="B183" s="14">
         <v>0.97181712962962974</v>
       </c>
       <c r="C183" s="9">
@@ -60502,7 +60502,7 @@
       <c r="A184" s="10">
         <v>43710</v>
       </c>
-      <c r="B184" s="15">
+      <c r="B184" s="14">
         <v>0.97876157407407405</v>
       </c>
       <c r="C184" s="9">
@@ -60516,7 +60516,7 @@
       <c r="A185" s="10">
         <v>43710</v>
       </c>
-      <c r="B185" s="15">
+      <c r="B185" s="14">
         <v>0.98570601851851858</v>
       </c>
       <c r="C185" s="9">
@@ -60530,7 +60530,7 @@
       <c r="A186" s="10">
         <v>43710</v>
       </c>
-      <c r="B186" s="15">
+      <c r="B186" s="14">
         <v>0.992650462962963</v>
       </c>
       <c r="C186" s="9">
@@ -60544,7 +60544,7 @@
       <c r="A187" s="10">
         <v>43710</v>
       </c>
-      <c r="B187" s="15">
+      <c r="B187" s="14">
         <v>0.99959490740740742</v>
       </c>
       <c r="C187" s="9">
@@ -60558,7 +60558,7 @@
       <c r="A188" s="10">
         <v>43711</v>
       </c>
-      <c r="B188" s="15">
+      <c r="B188" s="14">
         <v>6.5393518518518517E-3</v>
       </c>
       <c r="C188" s="9">
@@ -60572,7 +60572,7 @@
       <c r="A189" s="10">
         <v>43711</v>
       </c>
-      <c r="B189" s="15">
+      <c r="B189" s="14">
         <v>1.3483796296296298E-2</v>
       </c>
       <c r="C189" s="9">
@@ -60586,7 +60586,7 @@
       <c r="A190" s="10">
         <v>43711</v>
       </c>
-      <c r="B190" s="15">
+      <c r="B190" s="14">
         <v>2.0428240740740743E-2</v>
       </c>
       <c r="C190" s="9">
@@ -60600,7 +60600,7 @@
       <c r="A191" s="10">
         <v>43711</v>
       </c>
-      <c r="B191" s="15">
+      <c r="B191" s="14">
         <v>2.7372685185185184E-2</v>
       </c>
       <c r="C191" s="9">
@@ -60614,7 +60614,7 @@
       <c r="A192" s="10">
         <v>43711</v>
       </c>
-      <c r="B192" s="15">
+      <c r="B192" s="14">
         <v>3.4317129629629628E-2</v>
       </c>
       <c r="C192" s="9">
@@ -60628,7 +60628,7 @@
       <c r="A193" s="10">
         <v>43711</v>
       </c>
-      <c r="B193" s="15">
+      <c r="B193" s="14">
         <v>4.1261574074074069E-2</v>
       </c>
       <c r="C193" s="9">
@@ -60642,7 +60642,7 @@
       <c r="A194" s="10">
         <v>43711</v>
       </c>
-      <c r="B194" s="15">
+      <c r="B194" s="14">
         <v>4.8206018518518523E-2</v>
       </c>
       <c r="C194" s="9">
@@ -60656,7 +60656,7 @@
       <c r="A195" s="10">
         <v>43711</v>
       </c>
-      <c r="B195" s="15">
+      <c r="B195" s="14">
         <v>5.5150462962962964E-2</v>
       </c>
       <c r="C195" s="9">
@@ -60670,7 +60670,7 @@
       <c r="A196" s="10">
         <v>43711</v>
       </c>
-      <c r="B196" s="15">
+      <c r="B196" s="14">
         <v>6.2094907407407411E-2</v>
       </c>
       <c r="C196" s="9">
@@ -60684,7 +60684,7 @@
       <c r="A197" s="10">
         <v>43711</v>
       </c>
-      <c r="B197" s="15">
+      <c r="B197" s="14">
         <v>6.9039351851851852E-2</v>
       </c>
       <c r="C197" s="9">
@@ -60698,7 +60698,7 @@
       <c r="A198" s="10">
         <v>43711</v>
       </c>
-      <c r="B198" s="15">
+      <c r="B198" s="14">
         <v>7.5983796296296299E-2</v>
       </c>
       <c r="C198" s="9">
@@ -60712,7 +60712,7 @@
       <c r="A199" s="10">
         <v>43711</v>
       </c>
-      <c r="B199" s="15">
+      <c r="B199" s="14">
         <v>8.2928240740740733E-2</v>
       </c>
       <c r="C199" s="9">
@@ -60726,7 +60726,7 @@
       <c r="A200" s="10">
         <v>43711</v>
       </c>
-      <c r="B200" s="15">
+      <c r="B200" s="14">
         <v>8.9872685185185194E-2</v>
       </c>
       <c r="C200" s="9">
@@ -60740,7 +60740,7 @@
       <c r="A201" s="10">
         <v>43711</v>
       </c>
-      <c r="B201" s="15">
+      <c r="B201" s="14">
         <v>9.6817129629629628E-2</v>
       </c>
       <c r="C201" s="9">
@@ -60754,7 +60754,7 @@
       <c r="A202" s="10">
         <v>43711</v>
       </c>
-      <c r="B202" s="15">
+      <c r="B202" s="14">
         <v>0.10376157407407409</v>
       </c>
       <c r="C202" s="9">
@@ -60768,7 +60768,7 @@
       <c r="A203" s="10">
         <v>43711</v>
       </c>
-      <c r="B203" s="15">
+      <c r="B203" s="14">
         <v>0.11070601851851852</v>
       </c>
       <c r="C203" s="9">
@@ -60782,7 +60782,7 @@
       <c r="A204" s="10">
         <v>43711</v>
       </c>
-      <c r="B204" s="15">
+      <c r="B204" s="14">
         <v>0.11765046296296296</v>
       </c>
       <c r="C204" s="9">
@@ -60796,7 +60796,7 @@
       <c r="A205" s="10">
         <v>43711</v>
       </c>
-      <c r="B205" s="15">
+      <c r="B205" s="14">
         <v>0.1245949074074074</v>
       </c>
       <c r="C205" s="9">
@@ -60810,7 +60810,7 @@
       <c r="A206" s="10">
         <v>43711</v>
       </c>
-      <c r="B206" s="15">
+      <c r="B206" s="14">
         <v>0.13153935185185187</v>
       </c>
       <c r="C206" s="9">
@@ -60824,7 +60824,7 @@
       <c r="A207" s="10">
         <v>43711</v>
       </c>
-      <c r="B207" s="15">
+      <c r="B207" s="14">
         <v>0.13848379629629629</v>
       </c>
       <c r="C207" s="9">
@@ -60838,7 +60838,7 @@
       <c r="A208" s="10">
         <v>43711</v>
       </c>
-      <c r="B208" s="15">
+      <c r="B208" s="14">
         <v>0.14542824074074076</v>
       </c>
       <c r="C208" s="9">
@@ -60852,7 +60852,7 @@
       <c r="A209" s="10">
         <v>43711</v>
       </c>
-      <c r="B209" s="15">
+      <c r="B209" s="14">
         <v>0.15237268518518518</v>
       </c>
       <c r="C209" s="9">
@@ -60866,7 +60866,7 @@
       <c r="A210" s="10">
         <v>43711</v>
       </c>
-      <c r="B210" s="15">
+      <c r="B210" s="14">
         <v>0.15931712962962963</v>
       </c>
       <c r="C210" s="9">
@@ -60880,7 +60880,7 @@
       <c r="A211" s="10">
         <v>43711</v>
       </c>
-      <c r="B211" s="15">
+      <c r="B211" s="14">
         <v>0.16626157407407408</v>
       </c>
       <c r="C211" s="9">
@@ -60894,7 +60894,7 @@
       <c r="A212" s="10">
         <v>43711</v>
       </c>
-      <c r="B212" s="15">
+      <c r="B212" s="14">
         <v>0.1732060185185185</v>
       </c>
       <c r="C212" s="9">
@@ -60908,7 +60908,7 @@
       <c r="A213" s="10">
         <v>43711</v>
       </c>
-      <c r="B213" s="15">
+      <c r="B213" s="14">
         <v>0.18015046296296297</v>
       </c>
       <c r="C213" s="9">
@@ -60922,7 +60922,7 @@
       <c r="A214" s="10">
         <v>43711</v>
       </c>
-      <c r="B214" s="15">
+      <c r="B214" s="14">
         <v>0.18709490740740742</v>
       </c>
       <c r="C214" s="9">
@@ -60936,7 +60936,7 @@
       <c r="A215" s="10">
         <v>43711</v>
       </c>
-      <c r="B215" s="15">
+      <c r="B215" s="14">
         <v>0.19403935185185184</v>
       </c>
       <c r="C215" s="9">
@@ -60950,7 +60950,7 @@
       <c r="A216" s="10">
         <v>43711</v>
       </c>
-      <c r="B216" s="15">
+      <c r="B216" s="14">
         <v>0.20098379629629629</v>
       </c>
       <c r="C216" s="9">
@@ -60964,7 +60964,7 @@
       <c r="A217" s="10">
         <v>43711</v>
       </c>
-      <c r="B217" s="15">
+      <c r="B217" s="14">
         <v>0.20792824074074076</v>
       </c>
       <c r="C217" s="9">
@@ -60978,7 +60978,7 @@
       <c r="A218" s="10">
         <v>43711</v>
       </c>
-      <c r="B218" s="15">
+      <c r="B218" s="14">
         <v>0.21487268518518518</v>
       </c>
       <c r="C218" s="9">
@@ -60992,7 +60992,7 @@
       <c r="A219" s="10">
         <v>43711</v>
       </c>
-      <c r="B219" s="15">
+      <c r="B219" s="14">
         <v>0.22181712962962963</v>
       </c>
       <c r="C219" s="9">
@@ -61006,7 +61006,7 @@
       <c r="A220" s="10">
         <v>43711</v>
       </c>
-      <c r="B220" s="15">
+      <c r="B220" s="14">
         <v>0.22876157407407408</v>
       </c>
       <c r="C220" s="9">
@@ -61020,7 +61020,7 @@
       <c r="A221" s="10">
         <v>43711</v>
       </c>
-      <c r="B221" s="15">
+      <c r="B221" s="14">
         <v>0.2357060185185185</v>
       </c>
       <c r="C221" s="9">
@@ -61034,7 +61034,7 @@
       <c r="A222" s="10">
         <v>43711</v>
       </c>
-      <c r="B222" s="15">
+      <c r="B222" s="14">
         <v>0.24265046296296297</v>
       </c>
       <c r="C222" s="9">
@@ -61048,7 +61048,7 @@
       <c r="A223" s="10">
         <v>43711</v>
       </c>
-      <c r="B223" s="15">
+      <c r="B223" s="14">
         <v>0.24959490740740742</v>
       </c>
       <c r="C223" s="9">
@@ -61062,7 +61062,7 @@
       <c r="A224" s="10">
         <v>43711</v>
       </c>
-      <c r="B224" s="15">
+      <c r="B224" s="14">
         <v>0.25653935185185184</v>
       </c>
       <c r="C224" s="9">
@@ -61076,7 +61076,7 @@
       <c r="A225" s="10">
         <v>43711</v>
       </c>
-      <c r="B225" s="15">
+      <c r="B225" s="14">
         <v>0.26348379629629631</v>
       </c>
       <c r="C225" s="9">
@@ -61090,7 +61090,7 @@
       <c r="A226" s="10">
         <v>43711</v>
       </c>
-      <c r="B226" s="15">
+      <c r="B226" s="14">
         <v>0.27042824074074073</v>
       </c>
       <c r="C226" s="9">
@@ -61104,7 +61104,7 @@
       <c r="A227" s="10">
         <v>43711</v>
       </c>
-      <c r="B227" s="15">
+      <c r="B227" s="14">
         <v>0.27737268518518515</v>
       </c>
       <c r="C227" s="9">
@@ -61118,7 +61118,7 @@
       <c r="A228" s="10">
         <v>43711</v>
       </c>
-      <c r="B228" s="15">
+      <c r="B228" s="14">
         <v>0.28431712962962963</v>
       </c>
       <c r="C228" s="9">
@@ -61132,7 +61132,7 @@
       <c r="A229" s="10">
         <v>43711</v>
       </c>
-      <c r="B229" s="15">
+      <c r="B229" s="14">
         <v>0.2912615740740741</v>
       </c>
       <c r="C229" s="9">
@@ -61146,7 +61146,7 @@
       <c r="A230" s="10">
         <v>43711</v>
       </c>
-      <c r="B230" s="15">
+      <c r="B230" s="14">
         <v>0.29820601851851852</v>
       </c>
       <c r="C230" s="9">
@@ -61160,7 +61160,7 @@
       <c r="A231" s="10">
         <v>43711</v>
       </c>
-      <c r="B231" s="15">
+      <c r="B231" s="14">
         <v>0.30515046296296294</v>
       </c>
       <c r="C231" s="9">
@@ -61174,7 +61174,7 @@
       <c r="A232" s="10">
         <v>43711</v>
       </c>
-      <c r="B232" s="15">
+      <c r="B232" s="14">
         <v>0.31209490740740742</v>
       </c>
       <c r="C232" s="9">
@@ -61188,7 +61188,7 @@
       <c r="A233" s="10">
         <v>43711</v>
       </c>
-      <c r="B233" s="15">
+      <c r="B233" s="14">
         <v>0.31903935185185184</v>
       </c>
       <c r="C233" s="9">
@@ -61202,7 +61202,7 @@
       <c r="A234" s="10">
         <v>43711</v>
       </c>
-      <c r="B234" s="15">
+      <c r="B234" s="14">
         <v>0.32598379629629631</v>
       </c>
       <c r="C234" s="9">
@@ -61216,7 +61216,7 @@
       <c r="A235" s="10">
         <v>43711</v>
       </c>
-      <c r="B235" s="15">
+      <c r="B235" s="14">
         <v>0.33292824074074073</v>
       </c>
       <c r="C235" s="9">
@@ -61230,7 +61230,7 @@
       <c r="A236" s="10">
         <v>43711</v>
       </c>
-      <c r="B236" s="15">
+      <c r="B236" s="14">
         <v>0.79820601851851858</v>
       </c>
       <c r="C236" s="9">
@@ -61244,7 +61244,7 @@
       <c r="A237" s="10">
         <v>43711</v>
       </c>
-      <c r="B237" s="15">
+      <c r="B237" s="14">
         <v>0.805150462962963</v>
       </c>
       <c r="C237" s="9">
@@ -61258,7 +61258,7 @@
       <c r="A238" s="10">
         <v>43711</v>
       </c>
-      <c r="B238" s="15">
+      <c r="B238" s="14">
         <v>0.81209490740740742</v>
       </c>
       <c r="C238" s="9">
@@ -61272,7 +61272,7 @@
       <c r="A239" s="10">
         <v>43711</v>
       </c>
-      <c r="B239" s="15">
+      <c r="B239" s="14">
         <v>0.81903935185185184</v>
       </c>
       <c r="C239" s="9">
@@ -61286,7 +61286,7 @@
       <c r="A240" s="10">
         <v>43711</v>
       </c>
-      <c r="B240" s="15">
+      <c r="B240" s="14">
         <v>0.82598379629629637</v>
       </c>
       <c r="C240" s="9">
@@ -61300,7 +61300,7 @@
       <c r="A241" s="10">
         <v>43711</v>
       </c>
-      <c r="B241" s="15">
+      <c r="B241" s="14">
         <v>0.83292824074074068</v>
       </c>
       <c r="C241" s="9">
@@ -61314,7 +61314,7 @@
       <c r="A242" s="10">
         <v>43711</v>
       </c>
-      <c r="B242" s="15">
+      <c r="B242" s="14">
         <v>0.83987268518518521</v>
       </c>
       <c r="C242" s="9">
@@ -61328,7 +61328,7 @@
       <c r="A243" s="10">
         <v>43711</v>
       </c>
-      <c r="B243" s="15">
+      <c r="B243" s="14">
         <v>0.84681712962962974</v>
       </c>
       <c r="C243" s="9">
@@ -61342,7 +61342,7 @@
       <c r="A244" s="10">
         <v>43711</v>
       </c>
-      <c r="B244" s="15">
+      <c r="B244" s="14">
         <v>0.85376157407407405</v>
       </c>
       <c r="C244" s="9">
@@ -61356,7 +61356,7 @@
       <c r="A245" s="10">
         <v>43711</v>
       </c>
-      <c r="B245" s="15">
+      <c r="B245" s="14">
         <v>0.86070601851851858</v>
       </c>
       <c r="C245" s="9">
@@ -61370,7 +61370,7 @@
       <c r="A246" s="10">
         <v>43711</v>
       </c>
-      <c r="B246" s="15">
+      <c r="B246" s="14">
         <v>0.867650462962963</v>
       </c>
       <c r="C246" s="9">
@@ -61384,7 +61384,7 @@
       <c r="A247" s="10">
         <v>43711</v>
       </c>
-      <c r="B247" s="15">
+      <c r="B247" s="14">
         <v>0.87459490740740742</v>
       </c>
       <c r="C247" s="9">
@@ -61398,7 +61398,7 @@
       <c r="A248" s="10">
         <v>43711</v>
       </c>
-      <c r="B248" s="15">
+      <c r="B248" s="14">
         <v>0.88153935185185184</v>
       </c>
       <c r="C248" s="9">
@@ -61412,7 +61412,7 @@
       <c r="A249" s="10">
         <v>43711</v>
       </c>
-      <c r="B249" s="15">
+      <c r="B249" s="14">
         <v>0.88848379629629637</v>
       </c>
       <c r="C249" s="9">
@@ -61426,7 +61426,7 @@
       <c r="A250" s="10">
         <v>43711</v>
       </c>
-      <c r="B250" s="15">
+      <c r="B250" s="14">
         <v>0.89542824074074068</v>
       </c>
       <c r="C250" s="9">
@@ -61440,7 +61440,7 @@
       <c r="A251" s="10">
         <v>43711</v>
       </c>
-      <c r="B251" s="15">
+      <c r="B251" s="14">
         <v>0.90237268518518521</v>
       </c>
       <c r="C251" s="9">
@@ -61454,7 +61454,7 @@
       <c r="A252" s="10">
         <v>43711</v>
       </c>
-      <c r="B252" s="15">
+      <c r="B252" s="14">
         <v>0.90931712962962974</v>
       </c>
       <c r="C252" s="9">
@@ -61468,7 +61468,7 @@
       <c r="A253" s="10">
         <v>43711</v>
       </c>
-      <c r="B253" s="15">
+      <c r="B253" s="14">
         <v>0.91626157407407405</v>
       </c>
       <c r="C253" s="9">
@@ -61482,7 +61482,7 @@
       <c r="A254" s="10">
         <v>43711</v>
       </c>
-      <c r="B254" s="15">
+      <c r="B254" s="14">
         <v>0.92320601851851858</v>
       </c>
       <c r="C254" s="9">
@@ -61496,7 +61496,7 @@
       <c r="A255" s="10">
         <v>43711</v>
       </c>
-      <c r="B255" s="15">
+      <c r="B255" s="14">
         <v>0.930150462962963</v>
       </c>
       <c r="C255" s="9">
@@ -61510,7 +61510,7 @@
       <c r="A256" s="10">
         <v>43711</v>
       </c>
-      <c r="B256" s="15">
+      <c r="B256" s="14">
         <v>0.93709490740740742</v>
       </c>
       <c r="C256" s="9">
@@ -61524,7 +61524,7 @@
       <c r="A257" s="10">
         <v>43711</v>
       </c>
-      <c r="B257" s="15">
+      <c r="B257" s="14">
         <v>0.94403935185185184</v>
       </c>
       <c r="C257" s="9">
@@ -61538,7 +61538,7 @@
       <c r="A258" s="10">
         <v>43711</v>
       </c>
-      <c r="B258" s="15">
+      <c r="B258" s="14">
         <v>0.95098379629629637</v>
       </c>
       <c r="C258" s="9">
@@ -61552,7 +61552,7 @@
       <c r="A259" s="10">
         <v>43711</v>
       </c>
-      <c r="B259" s="15">
+      <c r="B259" s="14">
         <v>0.95792824074074068</v>
       </c>
       <c r="C259" s="9">
@@ -61566,7 +61566,7 @@
       <c r="A260" s="10">
         <v>43711</v>
       </c>
-      <c r="B260" s="15">
+      <c r="B260" s="14">
         <v>0.96487268518518521</v>
       </c>
       <c r="C260" s="9">
@@ -61580,7 +61580,7 @@
       <c r="A261" s="10">
         <v>43711</v>
       </c>
-      <c r="B261" s="15">
+      <c r="B261" s="14">
         <v>0.97181712962962974</v>
       </c>
       <c r="C261" s="9">
@@ -61594,7 +61594,7 @@
       <c r="A262" s="10">
         <v>43711</v>
       </c>
-      <c r="B262" s="15">
+      <c r="B262" s="14">
         <v>0.97876157407407405</v>
       </c>
       <c r="C262" s="9">
@@ -61608,7 +61608,7 @@
       <c r="A263" s="10">
         <v>43711</v>
       </c>
-      <c r="B263" s="15">
+      <c r="B263" s="14">
         <v>0.98570601851851858</v>
       </c>
       <c r="C263" s="9">
@@ -61622,7 +61622,7 @@
       <c r="A264" s="10">
         <v>43711</v>
       </c>
-      <c r="B264" s="15">
+      <c r="B264" s="14">
         <v>0.992650462962963</v>
       </c>
       <c r="C264" s="9">
@@ -61636,7 +61636,7 @@
       <c r="A265" s="10">
         <v>43711</v>
       </c>
-      <c r="B265" s="15">
+      <c r="B265" s="14">
         <v>0.99959490740740742</v>
       </c>
       <c r="C265" s="9">
@@ -61650,7 +61650,7 @@
       <c r="A266" s="10">
         <v>43712</v>
       </c>
-      <c r="B266" s="15">
+      <c r="B266" s="14">
         <v>6.5393518518518517E-3</v>
       </c>
       <c r="C266" s="9">
@@ -61664,7 +61664,7 @@
       <c r="A267" s="10">
         <v>43712</v>
       </c>
-      <c r="B267" s="15">
+      <c r="B267" s="14">
         <v>1.3483796296296298E-2</v>
       </c>
       <c r="C267" s="9">
@@ -61678,7 +61678,7 @@
       <c r="A268" s="10">
         <v>43712</v>
       </c>
-      <c r="B268" s="15">
+      <c r="B268" s="14">
         <v>2.0428240740740743E-2</v>
       </c>
       <c r="C268" s="9">
@@ -61692,7 +61692,7 @@
       <c r="A269" s="10">
         <v>43712</v>
       </c>
-      <c r="B269" s="15">
+      <c r="B269" s="14">
         <v>2.7372685185185184E-2</v>
       </c>
       <c r="C269" s="9">
@@ -61706,7 +61706,7 @@
       <c r="A270" s="10">
         <v>43712</v>
       </c>
-      <c r="B270" s="15">
+      <c r="B270" s="14">
         <v>3.4317129629629628E-2</v>
       </c>
       <c r="C270" s="9">
@@ -61720,7 +61720,7 @@
       <c r="A271" s="10">
         <v>43712</v>
       </c>
-      <c r="B271" s="15">
+      <c r="B271" s="14">
         <v>4.1261574074074069E-2</v>
       </c>
       <c r="C271" s="9">
@@ -61734,7 +61734,7 @@
       <c r="A272" s="10">
         <v>43712</v>
       </c>
-      <c r="B272" s="15">
+      <c r="B272" s="14">
         <v>4.8206018518518523E-2</v>
       </c>
       <c r="C272" s="9">
@@ -61748,7 +61748,7 @@
       <c r="A273" s="10">
         <v>43712</v>
       </c>
-      <c r="B273" s="15">
+      <c r="B273" s="14">
         <v>5.5150462962962964E-2</v>
       </c>
       <c r="C273" s="9">
@@ -61762,7 +61762,7 @@
       <c r="A274" s="10">
         <v>43712</v>
       </c>
-      <c r="B274" s="15">
+      <c r="B274" s="14">
         <v>6.2094907407407411E-2</v>
       </c>
       <c r="C274" s="9">
@@ -61776,7 +61776,7 @@
       <c r="A275" s="10">
         <v>43712</v>
       </c>
-      <c r="B275" s="15">
+      <c r="B275" s="14">
         <v>6.9039351851851852E-2</v>
       </c>
       <c r="C275" s="9">
@@ -61790,7 +61790,7 @@
       <c r="A276" s="10">
         <v>43712</v>
       </c>
-      <c r="B276" s="15">
+      <c r="B276" s="14">
         <v>7.5983796296296299E-2</v>
       </c>
       <c r="C276" s="9">
@@ -61804,7 +61804,7 @@
       <c r="A277" s="10">
         <v>43712</v>
       </c>
-      <c r="B277" s="15">
+      <c r="B277" s="14">
         <v>8.2928240740740733E-2</v>
       </c>
       <c r="C277" s="9">
@@ -61818,7 +61818,7 @@
       <c r="A278" s="10">
         <v>43712</v>
       </c>
-      <c r="B278" s="15">
+      <c r="B278" s="14">
         <v>8.9872685185185194E-2</v>
       </c>
       <c r="C278" s="9">
@@ -61832,7 +61832,7 @@
       <c r="A279" s="10">
         <v>43712</v>
       </c>
-      <c r="B279" s="15">
+      <c r="B279" s="14">
         <v>9.6817129629629628E-2</v>
       </c>
       <c r="C279" s="9">
@@ -61846,7 +61846,7 @@
       <c r="A280" s="10">
         <v>43712</v>
       </c>
-      <c r="B280" s="15">
+      <c r="B280" s="14">
         <v>0.10376157407407409</v>
       </c>
       <c r="C280" s="9">
@@ -61860,7 +61860,7 @@
       <c r="A281" s="10">
         <v>43712</v>
       </c>
-      <c r="B281" s="15">
+      <c r="B281" s="14">
         <v>0.11070601851851852</v>
       </c>
       <c r="C281" s="9">
@@ -61874,7 +61874,7 @@
       <c r="A282" s="10">
         <v>43712</v>
       </c>
-      <c r="B282" s="15">
+      <c r="B282" s="14">
         <v>0.11765046296296296</v>
       </c>
       <c r="C282" s="9">
@@ -61888,7 +61888,7 @@
       <c r="A283" s="10">
         <v>43712</v>
       </c>
-      <c r="B283" s="15">
+      <c r="B283" s="14">
         <v>0.1245949074074074</v>
       </c>
       <c r="C283" s="9">
@@ -61902,7 +61902,7 @@
       <c r="A284" s="10">
         <v>43712</v>
       </c>
-      <c r="B284" s="15">
+      <c r="B284" s="14">
         <v>0.13153935185185187</v>
       </c>
       <c r="C284" s="9">
@@ -61916,7 +61916,7 @@
       <c r="A285" s="10">
         <v>43712</v>
       </c>
-      <c r="B285" s="15">
+      <c r="B285" s="14">
         <v>0.13848379629629629</v>
       </c>
       <c r="C285" s="9">
@@ -61930,7 +61930,7 @@
       <c r="A286" s="10">
         <v>43712</v>
       </c>
-      <c r="B286" s="15">
+      <c r="B286" s="14">
         <v>0.14542824074074076</v>
       </c>
       <c r="C286" s="9">
@@ -61944,7 +61944,7 @@
       <c r="A287" s="10">
         <v>43712</v>
       </c>
-      <c r="B287" s="15">
+      <c r="B287" s="14">
         <v>0.15237268518518518</v>
       </c>
       <c r="C287" s="9">
@@ -61958,7 +61958,7 @@
       <c r="A288" s="10">
         <v>43712</v>
       </c>
-      <c r="B288" s="15">
+      <c r="B288" s="14">
         <v>0.15931712962962963</v>
       </c>
       <c r="C288" s="9">
@@ -61972,7 +61972,7 @@
       <c r="A289" s="10">
         <v>43712</v>
       </c>
-      <c r="B289" s="15">
+      <c r="B289" s="14">
         <v>0.16626157407407408</v>
       </c>
       <c r="C289" s="9">
@@ -61986,7 +61986,7 @@
       <c r="A290" s="10">
         <v>43712</v>
       </c>
-      <c r="B290" s="15">
+      <c r="B290" s="14">
         <v>0.1732060185185185</v>
       </c>
       <c r="C290" s="9">
@@ -62000,7 +62000,7 @@
       <c r="A291" s="10">
         <v>43712</v>
       </c>
-      <c r="B291" s="15">
+      <c r="B291" s="14">
         <v>0.18015046296296297</v>
       </c>
       <c r="C291" s="9">
@@ -62014,7 +62014,7 @@
       <c r="A292" s="10">
         <v>43712</v>
       </c>
-      <c r="B292" s="15">
+      <c r="B292" s="14">
         <v>0.18709490740740742</v>
       </c>
       <c r="C292" s="9">
@@ -62028,7 +62028,7 @@
       <c r="A293" s="10">
         <v>43712</v>
       </c>
-      <c r="B293" s="15">
+      <c r="B293" s="14">
         <v>0.19403935185185184</v>
       </c>
       <c r="C293" s="9">
@@ -62042,7 +62042,7 @@
       <c r="A294" s="10">
         <v>43712</v>
       </c>
-      <c r="B294" s="15">
+      <c r="B294" s="14">
         <v>0.20098379629629629</v>
       </c>
       <c r="C294" s="9">
@@ -62056,7 +62056,7 @@
       <c r="A295" s="10">
         <v>43712</v>
       </c>
-      <c r="B295" s="15">
+      <c r="B295" s="14">
         <v>0.20792824074074076</v>
       </c>
       <c r="C295" s="9">
@@ -62070,7 +62070,7 @@
       <c r="A296" s="10">
         <v>43712</v>
       </c>
-      <c r="B296" s="15">
+      <c r="B296" s="14">
         <v>0.21487268518518518</v>
       </c>
       <c r="C296" s="9">
@@ -62084,7 +62084,7 @@
       <c r="A297" s="10">
         <v>43712</v>
       </c>
-      <c r="B297" s="15">
+      <c r="B297" s="14">
         <v>0.22181712962962963</v>
       </c>
       <c r="C297" s="9">
@@ -62098,7 +62098,7 @@
       <c r="A298" s="10">
         <v>43712</v>
       </c>
-      <c r="B298" s="15">
+      <c r="B298" s="14">
         <v>0.22876157407407408</v>
       </c>
       <c r="C298" s="9">
@@ -62112,7 +62112,7 @@
       <c r="A299" s="10">
         <v>43712</v>
       </c>
-      <c r="B299" s="15">
+      <c r="B299" s="14">
         <v>0.2357060185185185</v>
       </c>
       <c r="C299" s="9">
@@ -62126,7 +62126,7 @@
       <c r="A300" s="10">
         <v>43712</v>
       </c>
-      <c r="B300" s="15">
+      <c r="B300" s="14">
         <v>0.24265046296296297</v>
       </c>
       <c r="C300" s="9">
@@ -62140,7 +62140,7 @@
       <c r="A301" s="10">
         <v>43712</v>
       </c>
-      <c r="B301" s="15">
+      <c r="B301" s="14">
         <v>0.24959490740740742</v>
       </c>
       <c r="C301" s="9">
@@ -62154,7 +62154,7 @@
       <c r="A302" s="10">
         <v>43712</v>
       </c>
-      <c r="B302" s="15">
+      <c r="B302" s="14">
         <v>0.25653935185185184</v>
       </c>
       <c r="C302" s="9">
@@ -62168,7 +62168,7 @@
       <c r="A303" s="10">
         <v>43712</v>
       </c>
-      <c r="B303" s="15">
+      <c r="B303" s="14">
         <v>0.26348379629629631</v>
       </c>
       <c r="C303" s="9">
@@ -62182,7 +62182,7 @@
       <c r="A304" s="10">
         <v>43712</v>
       </c>
-      <c r="B304" s="15">
+      <c r="B304" s="14">
         <v>0.27042824074074073</v>
       </c>
       <c r="C304" s="9">
@@ -62196,7 +62196,7 @@
       <c r="A305" s="10">
         <v>43712</v>
       </c>
-      <c r="B305" s="15">
+      <c r="B305" s="14">
         <v>0.27737268518518515</v>
       </c>
       <c r="C305" s="9">
@@ -62210,7 +62210,7 @@
       <c r="A306" s="10">
         <v>43712</v>
       </c>
-      <c r="B306" s="15">
+      <c r="B306" s="14">
         <v>0.28431712962962963</v>
       </c>
       <c r="C306" s="9">
@@ -62224,7 +62224,7 @@
       <c r="A307" s="10">
         <v>43712</v>
       </c>
-      <c r="B307" s="15">
+      <c r="B307" s="14">
         <v>0.2912615740740741</v>
       </c>
       <c r="C307" s="9">
@@ -62238,7 +62238,7 @@
       <c r="A308" s="10">
         <v>43712</v>
       </c>
-      <c r="B308" s="15">
+      <c r="B308" s="14">
         <v>0.29820601851851852</v>
       </c>
       <c r="C308" s="9">
@@ -62252,7 +62252,7 @@
       <c r="A309" s="10">
         <v>43712</v>
       </c>
-      <c r="B309" s="15">
+      <c r="B309" s="14">
         <v>0.30515046296296294</v>
       </c>
       <c r="C309" s="9">
@@ -62266,7 +62266,7 @@
       <c r="A310" s="10">
         <v>43712</v>
       </c>
-      <c r="B310" s="15">
+      <c r="B310" s="14">
         <v>0.31209490740740742</v>
       </c>
       <c r="C310" s="9">
@@ -62280,7 +62280,7 @@
       <c r="A311" s="10">
         <v>43712</v>
       </c>
-      <c r="B311" s="15">
+      <c r="B311" s="14">
         <v>0.31903935185185184</v>
       </c>
       <c r="C311" s="9">
@@ -62294,7 +62294,7 @@
       <c r="A312" s="10">
         <v>43712</v>
       </c>
-      <c r="B312" s="15">
+      <c r="B312" s="14">
         <v>0.32598379629629631</v>
       </c>
       <c r="C312" s="9">
@@ -62308,7 +62308,7 @@
       <c r="A313" s="10">
         <v>43712</v>
       </c>
-      <c r="B313" s="15">
+      <c r="B313" s="14">
         <v>0.33292824074074073</v>
       </c>
       <c r="C313" s="9">
@@ -62322,7 +62322,7 @@
       <c r="A314" s="10">
         <v>43713</v>
       </c>
-      <c r="B314" s="15">
+      <c r="B314" s="14">
         <v>0.79820601851851858</v>
       </c>
       <c r="C314" s="9">
@@ -62336,7 +62336,7 @@
       <c r="A315" s="10">
         <v>43713</v>
       </c>
-      <c r="B315" s="15">
+      <c r="B315" s="14">
         <v>0.805150462962963</v>
       </c>
       <c r="C315" s="9">
@@ -62350,7 +62350,7 @@
       <c r="A316" s="10">
         <v>43713</v>
       </c>
-      <c r="B316" s="15">
+      <c r="B316" s="14">
         <v>0.81209490740740742</v>
       </c>
       <c r="C316" s="9">
@@ -62364,7 +62364,7 @@
       <c r="A317" s="10">
         <v>43713</v>
       </c>
-      <c r="B317" s="15">
+      <c r="B317" s="14">
         <v>0.81903935185185184</v>
       </c>
       <c r="C317" s="9">
@@ -62378,7 +62378,7 @@
       <c r="A318" s="10">
         <v>43713</v>
       </c>
-      <c r="B318" s="15">
+      <c r="B318" s="14">
         <v>0.82598379629629637</v>
       </c>
       <c r="C318" s="9">
@@ -62392,7 +62392,7 @@
       <c r="A319" s="10">
         <v>43713</v>
       </c>
-      <c r="B319" s="15">
+      <c r="B319" s="14">
         <v>0.83292824074074068</v>
       </c>
       <c r="C319" s="9">
@@ -62406,7 +62406,7 @@
       <c r="A320" s="10">
         <v>43713</v>
       </c>
-      <c r="B320" s="15">
+      <c r="B320" s="14">
         <v>0.83987268518518521</v>
       </c>
       <c r="C320" s="9">
@@ -62420,7 +62420,7 @@
       <c r="A321" s="10">
         <v>43713</v>
       </c>
-      <c r="B321" s="15">
+      <c r="B321" s="14">
         <v>0.84681712962962974</v>
       </c>
       <c r="C321" s="9">
@@ -62434,7 +62434,7 @@
       <c r="A322" s="10">
         <v>43713</v>
       </c>
-      <c r="B322" s="15">
+      <c r="B322" s="14">
         <v>0.85376157407407405</v>
       </c>
       <c r="C322" s="9">
@@ -62448,7 +62448,7 @@
       <c r="A323" s="10">
         <v>43713</v>
       </c>
-      <c r="B323" s="15">
+      <c r="B323" s="14">
         <v>0.86070601851851858</v>
       </c>
       <c r="C323" s="9">
@@ -62462,7 +62462,7 @@
       <c r="A324" s="10">
         <v>43713</v>
       </c>
-      <c r="B324" s="15">
+      <c r="B324" s="14">
         <v>0.867650462962963</v>
       </c>
       <c r="C324" s="9">
@@ -62476,7 +62476,7 @@
       <c r="A325" s="10">
         <v>43713</v>
       </c>
-      <c r="B325" s="15">
+      <c r="B325" s="14">
         <v>0.87459490740740742</v>
       </c>
       <c r="C325" s="9">
@@ -62490,7 +62490,7 @@
       <c r="A326" s="10">
         <v>43713</v>
       </c>
-      <c r="B326" s="15">
+      <c r="B326" s="14">
         <v>0.88153935185185184</v>
       </c>
       <c r="C326" s="9">
@@ -62504,7 +62504,7 @@
       <c r="A327" s="10">
         <v>43713</v>
       </c>
-      <c r="B327" s="15">
+      <c r="B327" s="14">
         <v>0.88848379629629637</v>
       </c>
       <c r="C327" s="9">
@@ -62518,7 +62518,7 @@
       <c r="A328" s="10">
         <v>43713</v>
       </c>
-      <c r="B328" s="15">
+      <c r="B328" s="14">
         <v>0.89542824074074068</v>
       </c>
       <c r="C328" s="9">
@@ -62532,7 +62532,7 @@
       <c r="A329" s="10">
         <v>43713</v>
       </c>
-      <c r="B329" s="15">
+      <c r="B329" s="14">
         <v>0.90237268518518521</v>
       </c>
       <c r="C329" s="9">
@@ -62546,7 +62546,7 @@
       <c r="A330" s="10">
         <v>43713</v>
       </c>
-      <c r="B330" s="15">
+      <c r="B330" s="14">
         <v>0.90931712962962974</v>
       </c>
       <c r="C330" s="9">
@@ -62560,7 +62560,7 @@
       <c r="A331" s="10">
         <v>43713</v>
       </c>
-      <c r="B331" s="15">
+      <c r="B331" s="14">
         <v>0.91626157407407405</v>
       </c>
       <c r="C331" s="9">
@@ -62574,7 +62574,7 @@
       <c r="A332" s="10">
         <v>43713</v>
       </c>
-      <c r="B332" s="15">
+      <c r="B332" s="14">
         <v>0.92320601851851858</v>
       </c>
       <c r="C332" s="9">
@@ -62588,7 +62588,7 @@
       <c r="A333" s="10">
         <v>43713</v>
       </c>
-      <c r="B333" s="15">
+      <c r="B333" s="14">
         <v>0.930150462962963</v>
       </c>
       <c r="C333" s="9">
@@ -62602,7 +62602,7 @@
       <c r="A334" s="10">
         <v>43713</v>
       </c>
-      <c r="B334" s="15">
+      <c r="B334" s="14">
         <v>0.93709490740740742</v>
       </c>
       <c r="C334" s="9">
@@ -62616,7 +62616,7 @@
       <c r="A335" s="10">
         <v>43713</v>
       </c>
-      <c r="B335" s="15">
+      <c r="B335" s="14">
         <v>0.94403935185185184</v>
       </c>
       <c r="C335" s="9">
@@ -62630,7 +62630,7 @@
       <c r="A336" s="10">
         <v>43713</v>
       </c>
-      <c r="B336" s="15">
+      <c r="B336" s="14">
         <v>0.95098379629629637</v>
       </c>
       <c r="C336" s="9">
@@ -62644,7 +62644,7 @@
       <c r="A337" s="10">
         <v>43713</v>
       </c>
-      <c r="B337" s="15">
+      <c r="B337" s="14">
         <v>0.95792824074074068</v>
       </c>
       <c r="C337" s="9">
@@ -62658,7 +62658,7 @@
       <c r="A338" s="10">
         <v>43713</v>
       </c>
-      <c r="B338" s="15">
+      <c r="B338" s="14">
         <v>0.96487268518518521</v>
       </c>
       <c r="C338" s="9">
@@ -62672,7 +62672,7 @@
       <c r="A339" s="10">
         <v>43713</v>
       </c>
-      <c r="B339" s="15">
+      <c r="B339" s="14">
         <v>0.97181712962962974</v>
       </c>
       <c r="C339" s="9">
@@ -62686,7 +62686,7 @@
       <c r="A340" s="10">
         <v>43713</v>
       </c>
-      <c r="B340" s="15">
+      <c r="B340" s="14">
         <v>0.97876157407407405</v>
       </c>
       <c r="C340" s="9">
@@ -62700,7 +62700,7 @@
       <c r="A341" s="10">
         <v>43713</v>
       </c>
-      <c r="B341" s="15">
+      <c r="B341" s="14">
         <v>0.98570601851851858</v>
       </c>
       <c r="C341" s="9">
@@ -62714,7 +62714,7 @@
       <c r="A342" s="10">
         <v>43713</v>
       </c>
-      <c r="B342" s="15">
+      <c r="B342" s="14">
         <v>0.992650462962963</v>
       </c>
       <c r="C342" s="9">
@@ -62728,7 +62728,7 @@
       <c r="A343" s="10">
         <v>43713</v>
       </c>
-      <c r="B343" s="15">
+      <c r="B343" s="14">
         <v>0.99959490740740742</v>
       </c>
       <c r="C343" s="9">
@@ -62742,7 +62742,7 @@
       <c r="A344" s="10">
         <v>43714</v>
       </c>
-      <c r="B344" s="15">
+      <c r="B344" s="14">
         <v>6.5393518518518517E-3</v>
       </c>
       <c r="C344" s="9">
@@ -62756,7 +62756,7 @@
       <c r="A345" s="10">
         <v>43714</v>
       </c>
-      <c r="B345" s="15">
+      <c r="B345" s="14">
         <v>1.3483796296296298E-2</v>
       </c>
       <c r="C345" s="9">
@@ -62770,7 +62770,7 @@
       <c r="A346" s="10">
         <v>43714</v>
       </c>
-      <c r="B346" s="15">
+      <c r="B346" s="14">
         <v>2.0428240740740743E-2</v>
       </c>
       <c r="C346" s="9">
@@ -62784,7 +62784,7 @@
       <c r="A347" s="10">
         <v>43714</v>
       </c>
-      <c r="B347" s="15">
+      <c r="B347" s="14">
         <v>2.7372685185185184E-2</v>
       </c>
       <c r="C347" s="9">
@@ -62798,7 +62798,7 @@
       <c r="A348" s="10">
         <v>43714</v>
       </c>
-      <c r="B348" s="15">
+      <c r="B348" s="14">
         <v>3.4317129629629628E-2</v>
       </c>
       <c r="C348" s="9">
@@ -62812,7 +62812,7 @@
       <c r="A349" s="10">
         <v>43714</v>
       </c>
-      <c r="B349" s="15">
+      <c r="B349" s="14">
         <v>4.1261574074074069E-2</v>
       </c>
       <c r="C349" s="9">
@@ -62826,7 +62826,7 @@
       <c r="A350" s="10">
         <v>43714</v>
       </c>
-      <c r="B350" s="15">
+      <c r="B350" s="14">
         <v>4.8206018518518523E-2</v>
       </c>
       <c r="C350" s="9">
@@ -62840,7 +62840,7 @@
       <c r="A351" s="10">
         <v>43714</v>
       </c>
-      <c r="B351" s="15">
+      <c r="B351" s="14">
         <v>5.5150462962962964E-2</v>
       </c>
       <c r="C351" s="9">
@@ -62854,7 +62854,7 @@
       <c r="A352" s="10">
         <v>43714</v>
       </c>
-      <c r="B352" s="15">
+      <c r="B352" s="14">
         <v>6.2094907407407411E-2</v>
       </c>
       <c r="C352" s="9">
@@ -62868,7 +62868,7 @@
       <c r="A353" s="10">
         <v>43714</v>
       </c>
-      <c r="B353" s="15">
+      <c r="B353" s="14">
         <v>6.9039351851851852E-2</v>
       </c>
       <c r="C353" s="9">
@@ -62882,7 +62882,7 @@
       <c r="A354" s="10">
         <v>43714</v>
       </c>
-      <c r="B354" s="15">
+      <c r="B354" s="14">
         <v>7.5983796296296299E-2</v>
       </c>
       <c r="C354" s="9">
@@ -62896,7 +62896,7 @@
       <c r="A355" s="10">
         <v>43714</v>
       </c>
-      <c r="B355" s="15">
+      <c r="B355" s="14">
         <v>8.2928240740740733E-2</v>
       </c>
       <c r="C355" s="9">
@@ -62910,7 +62910,7 @@
       <c r="A356" s="10">
         <v>43714</v>
       </c>
-      <c r="B356" s="15">
+      <c r="B356" s="14">
         <v>8.9872685185185194E-2</v>
       </c>
       <c r="C356" s="9">
@@ -62924,7 +62924,7 @@
       <c r="A357" s="10">
         <v>43714</v>
       </c>
-      <c r="B357" s="15">
+      <c r="B357" s="14">
         <v>9.6817129629629628E-2</v>
       </c>
       <c r="C357" s="9">
@@ -62938,7 +62938,7 @@
       <c r="A358" s="10">
         <v>43714</v>
       </c>
-      <c r="B358" s="15">
+      <c r="B358" s="14">
         <v>0.10376157407407409</v>
       </c>
       <c r="C358" s="9">
@@ -62952,7 +62952,7 @@
       <c r="A359" s="10">
         <v>43714</v>
       </c>
-      <c r="B359" s="15">
+      <c r="B359" s="14">
         <v>0.11070601851851852</v>
       </c>
       <c r="C359" s="9">
@@ -62966,7 +62966,7 @@
       <c r="A360" s="10">
         <v>43714</v>
       </c>
-      <c r="B360" s="15">
+      <c r="B360" s="14">
         <v>0.11765046296296296</v>
       </c>
       <c r="C360" s="9">
@@ -62980,7 +62980,7 @@
       <c r="A361" s="10">
         <v>43714</v>
       </c>
-      <c r="B361" s="15">
+      <c r="B361" s="14">
         <v>0.1245949074074074</v>
       </c>
       <c r="C361" s="9">
@@ -62994,7 +62994,7 @@
       <c r="A362" s="10">
         <v>43714</v>
       </c>
-      <c r="B362" s="15">
+      <c r="B362" s="14">
         <v>0.13153935185185187</v>
       </c>
       <c r="C362" s="9">
@@ -63008,7 +63008,7 @@
       <c r="A363" s="10">
         <v>43714</v>
       </c>
-      <c r="B363" s="15">
+      <c r="B363" s="14">
         <v>0.13848379629629629</v>
       </c>
       <c r="C363" s="9">
@@ -63022,7 +63022,7 @@
       <c r="A364" s="10">
         <v>43714</v>
       </c>
-      <c r="B364" s="15">
+      <c r="B364" s="14">
         <v>0.14542824074074076</v>
       </c>
       <c r="C364" s="9">
@@ -63036,7 +63036,7 @@
       <c r="A365" s="10">
         <v>43714</v>
       </c>
-      <c r="B365" s="15">
+      <c r="B365" s="14">
         <v>0.15237268518518518</v>
       </c>
       <c r="C365" s="9">
@@ -63050,7 +63050,7 @@
       <c r="A366" s="10">
         <v>43714</v>
       </c>
-      <c r="B366" s="15">
+      <c r="B366" s="14">
         <v>0.15931712962962963</v>
       </c>
       <c r="C366" s="9">
@@ -63064,7 +63064,7 @@
       <c r="A367" s="10">
         <v>43714</v>
       </c>
-      <c r="B367" s="15">
+      <c r="B367" s="14">
         <v>0.16626157407407408</v>
       </c>
       <c r="C367" s="9">
@@ -63078,7 +63078,7 @@
       <c r="A368" s="10">
         <v>43714</v>
       </c>
-      <c r="B368" s="15">
+      <c r="B368" s="14">
         <v>0.1732060185185185</v>
       </c>
       <c r="C368" s="9">
@@ -63092,7 +63092,7 @@
       <c r="A369" s="10">
         <v>43714</v>
       </c>
-      <c r="B369" s="15">
+      <c r="B369" s="14">
         <v>0.18015046296296297</v>
       </c>
       <c r="C369" s="9">
@@ -63106,7 +63106,7 @@
       <c r="A370" s="10">
         <v>43714</v>
       </c>
-      <c r="B370" s="15">
+      <c r="B370" s="14">
         <v>0.18709490740740742</v>
       </c>
       <c r="C370" s="9">
@@ -63120,7 +63120,7 @@
       <c r="A371" s="10">
         <v>43714</v>
       </c>
-      <c r="B371" s="15">
+      <c r="B371" s="14">
         <v>0.19403935185185184</v>
       </c>
       <c r="C371" s="9">
@@ -63134,7 +63134,7 @@
       <c r="A372" s="10">
         <v>43714</v>
       </c>
-      <c r="B372" s="15">
+      <c r="B372" s="14">
         <v>0.20098379629629629</v>
       </c>
       <c r="C372" s="9">
@@ -63148,7 +63148,7 @@
       <c r="A373" s="10">
         <v>43714</v>
       </c>
-      <c r="B373" s="15">
+      <c r="B373" s="14">
         <v>0.20792824074074076</v>
       </c>
       <c r="C373" s="9">
@@ -63162,7 +63162,7 @@
       <c r="A374" s="10">
         <v>43714</v>
       </c>
-      <c r="B374" s="15">
+      <c r="B374" s="14">
         <v>0.21487268518518518</v>
       </c>
       <c r="C374" s="9">
@@ -63176,7 +63176,7 @@
       <c r="A375" s="10">
         <v>43714</v>
       </c>
-      <c r="B375" s="15">
+      <c r="B375" s="14">
         <v>0.22181712962962963</v>
       </c>
       <c r="C375" s="9">
@@ -63190,7 +63190,7 @@
       <c r="A376" s="10">
         <v>43714</v>
       </c>
-      <c r="B376" s="15">
+      <c r="B376" s="14">
         <v>0.22876157407407408</v>
       </c>
       <c r="C376" s="9">
@@ -63204,7 +63204,7 @@
       <c r="A377" s="10">
         <v>43714</v>
       </c>
-      <c r="B377" s="15">
+      <c r="B377" s="14">
         <v>0.2357060185185185</v>
       </c>
       <c r="C377" s="9">
@@ -63218,7 +63218,7 @@
       <c r="A378" s="10">
         <v>43714</v>
       </c>
-      <c r="B378" s="15">
+      <c r="B378" s="14">
         <v>0.24265046296296297</v>
       </c>
       <c r="C378" s="9">
@@ -63232,7 +63232,7 @@
       <c r="A379" s="10">
         <v>43714</v>
       </c>
-      <c r="B379" s="15">
+      <c r="B379" s="14">
         <v>0.24959490740740742</v>
       </c>
       <c r="C379" s="9">
@@ -63246,7 +63246,7 @@
       <c r="A380" s="10">
         <v>43714</v>
       </c>
-      <c r="B380" s="15">
+      <c r="B380" s="14">
         <v>0.25653935185185184</v>
       </c>
       <c r="C380" s="9">
@@ -63260,7 +63260,7 @@
       <c r="A381" s="10">
         <v>43714</v>
       </c>
-      <c r="B381" s="15">
+      <c r="B381" s="14">
         <v>0.26348379629629631</v>
       </c>
       <c r="C381" s="9">
@@ -63274,7 +63274,7 @@
       <c r="A382" s="10">
         <v>43714</v>
       </c>
-      <c r="B382" s="15">
+      <c r="B382" s="14">
         <v>0.27042824074074073</v>
       </c>
       <c r="C382" s="9">
@@ -63288,7 +63288,7 @@
       <c r="A383" s="10">
         <v>43714</v>
       </c>
-      <c r="B383" s="15">
+      <c r="B383" s="14">
         <v>0.27737268518518515</v>
       </c>
       <c r="C383" s="9">
@@ -63302,7 +63302,7 @@
       <c r="A384" s="10">
         <v>43714</v>
       </c>
-      <c r="B384" s="15">
+      <c r="B384" s="14">
         <v>0.28431712962962963</v>
       </c>
       <c r="C384" s="9">
@@ -63316,7 +63316,7 @@
       <c r="A385" s="10">
         <v>43714</v>
       </c>
-      <c r="B385" s="15">
+      <c r="B385" s="14">
         <v>0.2912615740740741</v>
       </c>
       <c r="C385" s="9">
@@ -63330,7 +63330,7 @@
       <c r="A386" s="10">
         <v>43714</v>
       </c>
-      <c r="B386" s="15">
+      <c r="B386" s="14">
         <v>0.29820601851851852</v>
       </c>
       <c r="C386" s="9">
@@ -63344,7 +63344,7 @@
       <c r="A387" s="10">
         <v>43714</v>
       </c>
-      <c r="B387" s="15">
+      <c r="B387" s="14">
         <v>0.30515046296296294</v>
       </c>
       <c r="C387" s="9">
@@ -63358,7 +63358,7 @@
       <c r="A388" s="10">
         <v>43714</v>
       </c>
-      <c r="B388" s="15">
+      <c r="B388" s="14">
         <v>0.31209490740740742</v>
       </c>
       <c r="C388" s="9">
@@ -63372,7 +63372,7 @@
       <c r="A389" s="10">
         <v>43714</v>
       </c>
-      <c r="B389" s="15">
+      <c r="B389" s="14">
         <v>0.31903935185185184</v>
       </c>
       <c r="C389" s="9">
@@ -63386,7 +63386,7 @@
       <c r="A390" s="10">
         <v>43714</v>
       </c>
-      <c r="B390" s="15">
+      <c r="B390" s="14">
         <v>0.32598379629629631</v>
       </c>
       <c r="C390" s="9">
@@ -63400,7 +63400,7 @@
       <c r="A391" s="10">
         <v>43714</v>
       </c>
-      <c r="B391" s="15">
+      <c r="B391" s="14">
         <v>0.33292824074074073</v>
       </c>
       <c r="C391" s="9">
@@ -63414,7 +63414,7 @@
       <c r="A392" s="10">
         <v>43714</v>
       </c>
-      <c r="B392" s="15">
+      <c r="B392" s="14">
         <v>0.79820601851851858</v>
       </c>
       <c r="C392" s="9">
@@ -63428,7 +63428,7 @@
       <c r="A393" s="10">
         <v>43714</v>
       </c>
-      <c r="B393" s="15">
+      <c r="B393" s="14">
         <v>0.805150462962963</v>
       </c>
       <c r="C393" s="9">
@@ -63442,7 +63442,7 @@
       <c r="A394" s="10">
         <v>43714</v>
       </c>
-      <c r="B394" s="15">
+      <c r="B394" s="14">
         <v>0.81209490740740742</v>
       </c>
       <c r="C394" s="9">
@@ -63456,7 +63456,7 @@
       <c r="A395" s="10">
         <v>43714</v>
       </c>
-      <c r="B395" s="15">
+      <c r="B395" s="14">
         <v>0.81903935185185184</v>
       </c>
       <c r="C395" s="9">
@@ -63470,7 +63470,7 @@
       <c r="A396" s="10">
         <v>43714</v>
       </c>
-      <c r="B396" s="15">
+      <c r="B396" s="14">
         <v>0.82598379629629637</v>
       </c>
       <c r="C396" s="9">
@@ -63484,7 +63484,7 @@
       <c r="A397" s="10">
         <v>43714</v>
       </c>
-      <c r="B397" s="15">
+      <c r="B397" s="14">
         <v>0.83292824074074068</v>
       </c>
       <c r="C397" s="9">
@@ -63498,7 +63498,7 @@
       <c r="A398" s="10">
         <v>43714</v>
       </c>
-      <c r="B398" s="15">
+      <c r="B398" s="14">
         <v>0.83987268518518521</v>
       </c>
       <c r="C398" s="9">
@@ -63512,7 +63512,7 @@
       <c r="A399" s="10">
         <v>43714</v>
       </c>
-      <c r="B399" s="15">
+      <c r="B399" s="14">
         <v>0.84681712962962974</v>
       </c>
       <c r="C399" s="9">
@@ -63526,7 +63526,7 @@
       <c r="A400" s="10">
         <v>43714</v>
       </c>
-      <c r="B400" s="15">
+      <c r="B400" s="14">
         <v>0.85376157407407405</v>
       </c>
       <c r="C400" s="9">
@@ -63540,7 +63540,7 @@
       <c r="A401" s="10">
         <v>43714</v>
       </c>
-      <c r="B401" s="15">
+      <c r="B401" s="14">
         <v>0.86070601851851858</v>
       </c>
       <c r="C401" s="9">
@@ -63554,7 +63554,7 @@
       <c r="A402" s="10">
         <v>43714</v>
       </c>
-      <c r="B402" s="15">
+      <c r="B402" s="14">
         <v>0.867650462962963</v>
       </c>
       <c r="C402" s="9">
@@ -63568,7 +63568,7 @@
       <c r="A403" s="10">
         <v>43714</v>
       </c>
-      <c r="B403" s="15">
+      <c r="B403" s="14">
         <v>0.87459490740740742</v>
       </c>
       <c r="C403" s="9">
@@ -63582,7 +63582,7 @@
       <c r="A404" s="10">
         <v>43714</v>
       </c>
-      <c r="B404" s="15">
+      <c r="B404" s="14">
         <v>0.88153935185185184</v>
       </c>
       <c r="C404" s="9">
@@ -63596,7 +63596,7 @@
       <c r="A405" s="10">
         <v>43714</v>
       </c>
-      <c r="B405" s="15">
+      <c r="B405" s="14">
         <v>0.88848379629629637</v>
       </c>
       <c r="C405" s="9">
@@ -63610,7 +63610,7 @@
       <c r="A406" s="10">
         <v>43714</v>
       </c>
-      <c r="B406" s="15">
+      <c r="B406" s="14">
         <v>0.89542824074074068</v>
       </c>
       <c r="C406" s="9">
@@ -63624,7 +63624,7 @@
       <c r="A407" s="10">
         <v>43714</v>
       </c>
-      <c r="B407" s="15">
+      <c r="B407" s="14">
         <v>0.90237268518518521</v>
       </c>
       <c r="C407" s="9">
@@ -63638,7 +63638,7 @@
       <c r="A408" s="10">
         <v>43714</v>
       </c>
-      <c r="B408" s="15">
+      <c r="B408" s="14">
         <v>0.90931712962962974</v>
       </c>
       <c r="C408" s="9">
@@ -63652,7 +63652,7 @@
       <c r="A409" s="10">
         <v>43714</v>
       </c>
-      <c r="B409" s="15">
+      <c r="B409" s="14">
         <v>0.91626157407407405</v>
       </c>
       <c r="C409" s="9">
@@ -63666,7 +63666,7 @@
       <c r="A410" s="10">
         <v>43714</v>
       </c>
-      <c r="B410" s="15">
+      <c r="B410" s="14">
         <v>0.92320601851851858</v>
       </c>
       <c r="C410" s="9">
@@ -63680,7 +63680,7 @@
       <c r="A411" s="10">
         <v>43714</v>
       </c>
-      <c r="B411" s="15">
+      <c r="B411" s="14">
         <v>0.930150462962963</v>
       </c>
       <c r="C411" s="9">
@@ -63694,7 +63694,7 @@
       <c r="A412" s="10">
         <v>43714</v>
       </c>
-      <c r="B412" s="15">
+      <c r="B412" s="14">
         <v>0.93709490740740742</v>
       </c>
       <c r="C412" s="9">
@@ -63708,7 +63708,7 @@
       <c r="A413" s="10">
         <v>43714</v>
       </c>
-      <c r="B413" s="15">
+      <c r="B413" s="14">
         <v>0.94403935185185184</v>
       </c>
       <c r="C413" s="9">
@@ -63722,7 +63722,7 @@
       <c r="A414" s="10">
         <v>43714</v>
       </c>
-      <c r="B414" s="15">
+      <c r="B414" s="14">
         <v>0.95098379629629637</v>
       </c>
       <c r="C414" s="9">
@@ -63736,7 +63736,7 @@
       <c r="A415" s="10">
         <v>43714</v>
       </c>
-      <c r="B415" s="15">
+      <c r="B415" s="14">
         <v>0.95792824074074068</v>
       </c>
       <c r="C415" s="9">
@@ -63750,7 +63750,7 @@
       <c r="A416" s="10">
         <v>43714</v>
       </c>
-      <c r="B416" s="15">
+      <c r="B416" s="14">
         <v>0.96487268518518521</v>
       </c>
       <c r="C416" s="9">
@@ -63764,7 +63764,7 @@
       <c r="A417" s="10">
         <v>43714</v>
       </c>
-      <c r="B417" s="15">
+      <c r="B417" s="14">
         <v>0.97181712962962974</v>
       </c>
       <c r="C417" s="9">
@@ -63778,7 +63778,7 @@
       <c r="A418" s="10">
         <v>43714</v>
       </c>
-      <c r="B418" s="15">
+      <c r="B418" s="14">
         <v>0.97876157407407405</v>
       </c>
       <c r="C418" s="9">
@@ -63792,7 +63792,7 @@
       <c r="A419" s="10">
         <v>43714</v>
       </c>
-      <c r="B419" s="15">
+      <c r="B419" s="14">
         <v>0.98570601851851858</v>
       </c>
       <c r="C419" s="9">
@@ -63806,7 +63806,7 @@
       <c r="A420" s="10">
         <v>43714</v>
       </c>
-      <c r="B420" s="15">
+      <c r="B420" s="14">
         <v>0.992650462962963</v>
       </c>
       <c r="C420" s="9">
@@ -63820,7 +63820,7 @@
       <c r="A421" s="10">
         <v>43714</v>
       </c>
-      <c r="B421" s="15">
+      <c r="B421" s="14">
         <v>0.99959490740740742</v>
       </c>
       <c r="C421" s="9">
@@ -63834,7 +63834,7 @@
       <c r="A422" s="10">
         <v>43715</v>
       </c>
-      <c r="B422" s="15">
+      <c r="B422" s="14">
         <v>6.5393518518518517E-3</v>
       </c>
       <c r="C422" s="9">
@@ -63848,7 +63848,7 @@
       <c r="A423" s="10">
         <v>43715</v>
       </c>
-      <c r="B423" s="15">
+      <c r="B423" s="14">
         <v>1.3483796296296298E-2</v>
       </c>
       <c r="C423" s="9">
@@ -63862,7 +63862,7 @@
       <c r="A424" s="10">
         <v>43715</v>
       </c>
-      <c r="B424" s="15">
+      <c r="B424" s="14">
         <v>2.0428240740740743E-2</v>
       </c>
       <c r="C424" s="9">
@@ -63876,7 +63876,7 @@
       <c r="A425" s="10">
         <v>43715</v>
       </c>
-      <c r="B425" s="15">
+      <c r="B425" s="14">
         <v>2.7372685185185184E-2</v>
       </c>
       <c r="C425" s="9">
@@ -63890,7 +63890,7 @@
       <c r="A426" s="10">
         <v>43715</v>
       </c>
-      <c r="B426" s="15">
+      <c r="B426" s="14">
         <v>3.4317129629629628E-2</v>
       </c>
       <c r="C426" s="9">
@@ -63904,7 +63904,7 @@
       <c r="A427" s="10">
         <v>43715</v>
       </c>
-      <c r="B427" s="15">
+      <c r="B427" s="14">
         <v>4.1261574074074069E-2</v>
       </c>
       <c r="C427" s="9">
@@ -63918,7 +63918,7 @@
       <c r="A428" s="10">
         <v>43715</v>
       </c>
-      <c r="B428" s="15">
+      <c r="B428" s="14">
         <v>4.8206018518518523E-2</v>
       </c>
       <c r="C428" s="9">
@@ -63932,7 +63932,7 @@
       <c r="A429" s="10">
         <v>43715</v>
       </c>
-      <c r="B429" s="15">
+      <c r="B429" s="14">
         <v>5.5150462962962964E-2</v>
       </c>
       <c r="C429" s="9">
@@ -63946,7 +63946,7 @@
       <c r="A430" s="10">
         <v>43715</v>
       </c>
-      <c r="B430" s="15">
+      <c r="B430" s="14">
         <v>6.2094907407407411E-2</v>
       </c>
       <c r="C430" s="9">
@@ -63960,7 +63960,7 @@
       <c r="A431" s="10">
         <v>43715</v>
       </c>
-      <c r="B431" s="15">
+      <c r="B431" s="14">
         <v>6.9039351851851852E-2</v>
       </c>
       <c r="C431" s="9">
@@ -63974,7 +63974,7 @@
       <c r="A432" s="10">
         <v>43715</v>
       </c>
-      <c r="B432" s="15">
+      <c r="B432" s="14">
         <v>7.5983796296296299E-2</v>
       </c>
       <c r="C432" s="9">
@@ -63988,7 +63988,7 @@
       <c r="A433" s="10">
         <v>43715</v>
       </c>
-      <c r="B433" s="15">
+      <c r="B433" s="14">
         <v>8.2928240740740733E-2</v>
       </c>
       <c r="C433" s="9">
@@ -64002,7 +64002,7 @@
       <c r="A434" s="10">
         <v>43715</v>
       </c>
-      <c r="B434" s="15">
+      <c r="B434" s="14">
         <v>8.9872685185185194E-2</v>
       </c>
       <c r="C434" s="9">
@@ -64016,7 +64016,7 @@
       <c r="A435" s="10">
         <v>43715</v>
       </c>
-      <c r="B435" s="15">
+      <c r="B435" s="14">
         <v>9.6817129629629628E-2</v>
       </c>
       <c r="C435" s="9">
@@ -64030,7 +64030,7 @@
       <c r="A436" s="10">
         <v>43715</v>
       </c>
-      <c r="B436" s="15">
+      <c r="B436" s="14">
         <v>0.10376157407407409</v>
       </c>
       <c r="C436" s="9">
@@ -64044,7 +64044,7 @@
       <c r="A437" s="10">
         <v>43715</v>
       </c>
-      <c r="B437" s="15">
+      <c r="B437" s="14">
         <v>0.11070601851851852</v>
       </c>
       <c r="C437" s="9">
@@ -64058,7 +64058,7 @@
       <c r="A438" s="10">
         <v>43715</v>
       </c>
-      <c r="B438" s="15">
+      <c r="B438" s="14">
         <v>0.11765046296296296</v>
       </c>
       <c r="C438" s="9">
@@ -64072,7 +64072,7 @@
       <c r="A439" s="10">
         <v>43715</v>
       </c>
-      <c r="B439" s="15">
+      <c r="B439" s="14">
         <v>0.1245949074074074</v>
       </c>
       <c r="C439" s="9">
@@ -64086,7 +64086,7 @@
       <c r="A440" s="10">
         <v>43715</v>
       </c>
-      <c r="B440" s="15">
+      <c r="B440" s="14">
         <v>0.13153935185185187</v>
       </c>
       <c r="C440" s="9">
@@ -64100,7 +64100,7 @@
       <c r="A441" s="10">
         <v>43715</v>
       </c>
-      <c r="B441" s="15">
+      <c r="B441" s="14">
         <v>0.13848379629629629</v>
       </c>
       <c r="C441" s="9">
@@ -64114,7 +64114,7 @@
       <c r="A442" s="10">
         <v>43715</v>
       </c>
-      <c r="B442" s="15">
+      <c r="B442" s="14">
         <v>0.14542824074074076</v>
       </c>
       <c r="C442" s="9">
@@ -64128,7 +64128,7 @@
       <c r="A443" s="10">
         <v>43715</v>
       </c>
-      <c r="B443" s="15">
+      <c r="B443" s="14">
         <v>0.15237268518518518</v>
       </c>
       <c r="C443" s="9">
@@ -64142,7 +64142,7 @@
       <c r="A444" s="10">
         <v>43715</v>
       </c>
-      <c r="B444" s="15">
+      <c r="B444" s="14">
         <v>0.15931712962962963</v>
       </c>
       <c r="C444" s="9">
@@ -64156,7 +64156,7 @@
       <c r="A445" s="10">
         <v>43715</v>
       </c>
-      <c r="B445" s="15">
+      <c r="B445" s="14">
         <v>0.16626157407407408</v>
       </c>
       <c r="C445" s="9">
@@ -64170,7 +64170,7 @@
       <c r="A446" s="10">
         <v>43715</v>
       </c>
-      <c r="B446" s="15">
+      <c r="B446" s="14">
         <v>0.1732060185185185</v>
       </c>
       <c r="C446" s="9">
@@ -64184,7 +64184,7 @@
       <c r="A447" s="10">
         <v>43715</v>
       </c>
-      <c r="B447" s="15">
+      <c r="B447" s="14">
         <v>0.18015046296296297</v>
       </c>
       <c r="C447" s="9">
@@ -64198,7 +64198,7 @@
       <c r="A448" s="10">
         <v>43715</v>
       </c>
-      <c r="B448" s="15">
+      <c r="B448" s="14">
         <v>0.18709490740740742</v>
       </c>
       <c r="C448" s="9">
@@ -64212,7 +64212,7 @@
       <c r="A449" s="10">
         <v>43715</v>
       </c>
-      <c r="B449" s="15">
+      <c r="B449" s="14">
         <v>0.19403935185185184</v>
       </c>
       <c r="C449" s="9">
@@ -64226,7 +64226,7 @@
       <c r="A450" s="10">
         <v>43715</v>
       </c>
-      <c r="B450" s="15">
+      <c r="B450" s="14">
         <v>0.20098379629629629</v>
       </c>
       <c r="C450" s="9">
@@ -64240,7 +64240,7 @@
       <c r="A451" s="10">
         <v>43715</v>
       </c>
-      <c r="B451" s="15">
+      <c r="B451" s="14">
         <v>0.20792824074074076</v>
       </c>
       <c r="C451" s="9">
@@ -64254,7 +64254,7 @@
       <c r="A452" s="10">
         <v>43715</v>
       </c>
-      <c r="B452" s="15">
+      <c r="B452" s="14">
         <v>0.21487268518518518</v>
       </c>
       <c r="C452" s="9">
@@ -64268,7 +64268,7 @@
       <c r="A453" s="10">
         <v>43715</v>
       </c>
-      <c r="B453" s="15">
+      <c r="B453" s="14">
         <v>0.22181712962962963</v>
       </c>
       <c r="C453" s="9">
@@ -64282,7 +64282,7 @@
       <c r="A454" s="10">
         <v>43715</v>
       </c>
-      <c r="B454" s="15">
+      <c r="B454" s="14">
         <v>0.22876157407407408</v>
       </c>
       <c r="C454" s="9">
@@ -64296,7 +64296,7 @@
       <c r="A455" s="10">
         <v>43715</v>
       </c>
-      <c r="B455" s="15">
+      <c r="B455" s="14">
         <v>0.2357060185185185</v>
       </c>
       <c r="C455" s="9">
@@ -64310,7 +64310,7 @@
       <c r="A456" s="10">
         <v>43715</v>
       </c>
-      <c r="B456" s="15">
+      <c r="B456" s="14">
         <v>0.24265046296296297</v>
       </c>
       <c r="C456" s="9">
@@ -64324,7 +64324,7 @@
       <c r="A457" s="10">
         <v>43715</v>
       </c>
-      <c r="B457" s="15">
+      <c r="B457" s="14">
         <v>0.24959490740740742</v>
       </c>
       <c r="C457" s="9">
@@ -64338,7 +64338,7 @@
       <c r="A458" s="10">
         <v>43715</v>
       </c>
-      <c r="B458" s="15">
+      <c r="B458" s="14">
         <v>0.25653935185185184</v>
       </c>
       <c r="C458" s="9">
@@ -64352,7 +64352,7 @@
       <c r="A459" s="10">
         <v>43715</v>
       </c>
-      <c r="B459" s="15">
+      <c r="B459" s="14">
         <v>0.26348379629629631</v>
       </c>
       <c r="C459" s="9">
@@ -64366,7 +64366,7 @@
       <c r="A460" s="10">
         <v>43715</v>
       </c>
-      <c r="B460" s="15">
+      <c r="B460" s="14">
         <v>0.27042824074074073</v>
       </c>
       <c r="C460" s="9">
@@ -64380,7 +64380,7 @@
       <c r="A461" s="10">
         <v>43715</v>
       </c>
-      <c r="B461" s="15">
+      <c r="B461" s="14">
         <v>0.27737268518518515</v>
       </c>
       <c r="C461" s="9">
@@ -64394,7 +64394,7 @@
       <c r="A462" s="10">
         <v>43715</v>
       </c>
-      <c r="B462" s="15">
+      <c r="B462" s="14">
         <v>0.28431712962962963</v>
       </c>
       <c r="C462" s="9">
@@ -64408,7 +64408,7 @@
       <c r="A463" s="10">
         <v>43715</v>
       </c>
-      <c r="B463" s="15">
+      <c r="B463" s="14">
         <v>0.2912615740740741</v>
       </c>
       <c r="C463" s="9">
@@ -64422,7 +64422,7 @@
       <c r="A464" s="10">
         <v>43715</v>
       </c>
-      <c r="B464" s="15">
+      <c r="B464" s="14">
         <v>0.29820601851851852</v>
       </c>
       <c r="C464" s="9">
@@ -64436,7 +64436,7 @@
       <c r="A465" s="10">
         <v>43715</v>
       </c>
-      <c r="B465" s="15">
+      <c r="B465" s="14">
         <v>0.30515046296296294</v>
       </c>
       <c r="C465" s="9">
@@ -64450,7 +64450,7 @@
       <c r="A466" s="10">
         <v>43715</v>
       </c>
-      <c r="B466" s="15">
+      <c r="B466" s="14">
         <v>0.31209490740740742</v>
       </c>
       <c r="C466" s="9">
@@ -64481,10 +64481,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="15" t="s">
         <v>76</v>
       </c>
       <c r="C1" s="2" t="s">

</xml_diff>

<commit_message>
rest of videos hurry before iMac crashes again
</commit_message>
<xml_diff>
--- a/data/raw.xlsx
+++ b/data/raw.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/EcosystemRecoveryLab/github/Ritger-Corynactis-urchin-deterrence/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E7584CD-9A02-0F40-811D-F6C15D64ECDD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAD74ACD-35E7-2945-9387-67963A5FA7E0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1960" yWindow="10540" windowWidth="47980" windowHeight="16120" activeTab="2" xr2:uid="{58E670A5-634C-427F-960F-9DA76C64E810}"/>
+    <workbookView xWindow="3420" yWindow="7660" windowWidth="47980" windowHeight="16120" activeTab="2" xr2:uid="{58E670A5-634C-427F-960F-9DA76C64E810}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="3" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="117">
   <si>
     <t>Tank number</t>
   </si>
@@ -284,9 +284,6 @@
     <t>really good deterrence video</t>
   </si>
   <si>
-    <t>urchin tried crossing</t>
-  </si>
-  <si>
     <t>Time spent with Kelp (min)</t>
   </si>
   <si>
@@ -306,9 +303,6 @@
   </si>
   <si>
     <t>urchin lost kelp blade across Corynactis tile</t>
-  </si>
-  <si>
-    <t>5 hours video</t>
   </si>
   <si>
     <t>old urchin dropped on colony</t>
@@ -376,6 +370,18 @@
   <si>
     <t>4 hours video; urchin never moves</t>
   </si>
+  <si>
+    <t>urchin never moved</t>
+  </si>
+  <si>
+    <t>5 hours video; no movement</t>
+  </si>
+  <si>
+    <t>Polyp behavior obvious</t>
+  </si>
+  <si>
+    <t>Percent time with Kelp</t>
+  </si>
 </sst>
 </file>
 
@@ -414,7 +420,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -424,6 +430,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -440,7 +452,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -457,6 +469,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="21" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -792,10 +805,10 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="16"/>
+      <c r="B3" s="17"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
@@ -810,7 +823,7 @@
         <v>37</v>
       </c>
       <c r="B5" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -818,7 +831,7 @@
         <v>38</v>
       </c>
       <c r="B6" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -826,7 +839,7 @@
         <v>76</v>
       </c>
       <c r="B7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -882,7 +895,7 @@
         <v>5</v>
       </c>
       <c r="B14" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
@@ -890,7 +903,7 @@
         <v>51</v>
       </c>
       <c r="B15" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
@@ -898,7 +911,7 @@
         <v>50</v>
       </c>
       <c r="B16" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
@@ -906,7 +919,7 @@
         <v>77</v>
       </c>
       <c r="B17" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
@@ -954,7 +967,7 @@
         <v>68</v>
       </c>
       <c r="B23" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
@@ -977,10 +990,10 @@
       <c r="A26" s="2"/>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A27" s="16" t="s">
+      <c r="A27" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="B27" s="16"/>
+      <c r="B27" s="17"/>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
@@ -1008,10 +1021,10 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B31" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
@@ -1032,7 +1045,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>34</v>
@@ -1048,10 +1061,10 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B36" t="s">
         <v>99</v>
-      </c>
-      <c r="B36" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
@@ -1059,7 +1072,7 @@
         <v>56</v>
       </c>
       <c r="B37" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
@@ -1075,23 +1088,23 @@
         <v>57</v>
       </c>
       <c r="B39" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B40" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B41" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
@@ -54784,7 +54797,7 @@
         <v>yes</v>
       </c>
       <c r="V74" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="75" spans="1:22" x14ac:dyDescent="0.2">
@@ -54988,7 +55001,7 @@
         <v>yes</v>
       </c>
       <c r="V77" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -55002,12 +55015,12 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55F6BF2F-CBB2-4331-929A-D3F4AD694052}">
-  <dimension ref="A1:AB37"/>
+  <dimension ref="A1:AA37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="107" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="107" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="G1" sqref="G1"/>
-      <selection pane="bottomLeft" activeCell="T29" sqref="T29"/>
+      <selection pane="bottomLeft" activeCell="AA37" sqref="AA37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -55028,21 +55041,20 @@
     <col min="14" max="14" width="9.5" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="18.5" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="17.83203125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="19.1640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="19.33203125" customWidth="1"/>
-    <col min="21" max="21" width="21.6640625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="21" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="24.33203125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="23.5" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="9.5" customWidth="1"/>
-    <col min="27" max="27" width="30.1640625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="19.33203125" customWidth="1"/>
+    <col min="20" max="20" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="21" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="9.5" customWidth="1"/>
+    <col min="26" max="26" width="30.1640625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="10.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -55085,51 +55097,48 @@
       <c r="N1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="O1" s="2" t="s">
-        <v>86</v>
+      <c r="O1" s="16" t="s">
+        <v>85</v>
       </c>
       <c r="P1" s="2" t="s">
         <v>15</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>35</v>
+        <v>116</v>
       </c>
       <c r="R1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="W1" s="2" t="s">
         <v>87</v>
-      </c>
-      <c r="S1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="T1" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="U1" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="V1" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="W1" s="2" t="s">
-        <v>13</v>
       </c>
       <c r="X1" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="Y1" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="Z1" s="2" t="str">
+      <c r="Y1" s="2" t="str">
         <f>'Kelp consumption'!T1</f>
         <v>Kelp visibly consumed?</v>
       </c>
+      <c r="Z1" s="2" t="s">
+        <v>108</v>
+      </c>
       <c r="AA1" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="AB1" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -55189,43 +55198,39 @@
         <f>#REF!/O2</f>
         <v>#REF!</v>
       </c>
-      <c r="R2" t="e">
-        <f>#REF!/O2</f>
-        <v>#REF!</v>
+      <c r="R2">
+        <v>70</v>
       </c>
       <c r="S2">
-        <v>70</v>
-      </c>
-      <c r="T2">
         <f>127+(1208-1060)</f>
         <v>275</v>
       </c>
+      <c r="T2">
+        <v>6</v>
+      </c>
       <c r="U2">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="V2">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="W2">
-        <v>5</v>
+        <v>58</v>
       </c>
       <c r="X2">
-        <v>58</v>
-      </c>
-      <c r="Y2">
-        <f>(34+17+11+13)/(W2-1)</f>
+        <f>(34+17+11+13)/(V2-1)</f>
         <v>18.75</v>
       </c>
-      <c r="Z2" s="4" t="str">
+      <c r="Y2" s="4" t="str">
         <f>'Kelp consumption'!T2</f>
         <v>yes</v>
       </c>
-      <c r="AA2" s="4" t="str">
-        <f>IF(Z2="yes",IF(T2&gt;0,"kelp consumed during video","kelp consumed AFTER video"),"urchin never ate kelp")</f>
+      <c r="Z2" s="4" t="str">
+        <f>IF(Y2="yes",IF(S2&gt;0,"kelp consumed during video","kelp consumed AFTER video"),"urchin never ate kelp")</f>
         <v>kelp consumed during video</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -55285,29 +55290,25 @@
         <f>#REF!/O3</f>
         <v>#REF!</v>
       </c>
-      <c r="R3" t="e">
-        <f>#REF!/O3</f>
-        <v>#REF!</v>
+      <c r="T3">
+        <v>4</v>
       </c>
       <c r="U3">
         <v>4</v>
       </c>
       <c r="V3">
-        <v>4</v>
-      </c>
-      <c r="W3">
         <v>0</v>
       </c>
-      <c r="Z3" s="4" t="str">
+      <c r="Y3" s="4" t="str">
         <f>'Kelp consumption'!T3</f>
         <v>no</v>
       </c>
-      <c r="AA3" s="4" t="str">
-        <f t="shared" ref="AA3:AA37" si="2">IF(Z3="yes",IF(T3&gt;0,"kelp consumed during video","kelp consumed AFTER video"),"urchin never ate kelp")</f>
+      <c r="Z3" s="4" t="str">
+        <f t="shared" ref="Z3:Z37" si="2">IF(Y3="yes",IF(S3&gt;0,"kelp consumed during video","kelp consumed AFTER video"),"urchin never ate kelp")</f>
         <v>urchin never ate kelp</v>
       </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -55367,42 +55368,38 @@
         <f>#REF!/O4</f>
         <v>#REF!</v>
       </c>
-      <c r="R4" t="e">
-        <f>#REF!/O4</f>
-        <v>#REF!</v>
+      <c r="R4">
+        <v>7</v>
       </c>
       <c r="S4">
-        <v>7</v>
-      </c>
-      <c r="T4">
         <f>11999-11693</f>
         <v>306</v>
       </c>
+      <c r="T4">
+        <v>1</v>
+      </c>
       <c r="U4">
+        <v>0</v>
+      </c>
+      <c r="V4">
         <v>1</v>
       </c>
-      <c r="V4">
-        <v>0</v>
-      </c>
       <c r="W4">
-        <v>1</v>
-      </c>
-      <c r="X4">
         <v>3</v>
       </c>
-      <c r="Z4" s="4" t="str">
+      <c r="Y4" s="4" t="str">
         <f>'Kelp consumption'!T4</f>
         <v>yes</v>
       </c>
-      <c r="AA4" s="4" t="str">
+      <c r="Z4" s="4" t="str">
         <f t="shared" si="2"/>
         <v>kelp consumed during video</v>
       </c>
-      <c r="AB4" t="s">
+      <c r="AA4" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -55462,39 +55459,35 @@
         <f>#REF!/O5</f>
         <v>#REF!</v>
       </c>
-      <c r="R5" t="e">
-        <f>#REF!/O5</f>
-        <v>#REF!</v>
+      <c r="R5">
+        <v>41</v>
       </c>
       <c r="S5">
-        <v>41</v>
-      </c>
-      <c r="T5">
         <f>12873-12410</f>
         <v>463</v>
       </c>
+      <c r="T5">
+        <v>2</v>
+      </c>
       <c r="U5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="V5">
         <v>1</v>
       </c>
       <c r="W5">
-        <v>1</v>
-      </c>
-      <c r="X5">
         <v>15</v>
       </c>
-      <c r="Z5" s="4" t="str">
+      <c r="Y5" s="4" t="str">
         <f>'Kelp consumption'!T5</f>
         <v>yes</v>
       </c>
-      <c r="AA5" s="4" t="str">
+      <c r="Z5" s="4" t="str">
         <f t="shared" si="2"/>
         <v>kelp consumed during video</v>
       </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -55554,43 +55547,39 @@
         <f>#REF!/O6</f>
         <v>#REF!</v>
       </c>
-      <c r="R6" t="e">
-        <f>#REF!/O6</f>
-        <v>#REF!</v>
+      <c r="R6">
+        <v>32</v>
       </c>
       <c r="S6">
-        <v>32</v>
-      </c>
-      <c r="T6">
         <f>(12950-12811)+(12747-12463)</f>
         <v>423</v>
       </c>
+      <c r="T6">
+        <v>3</v>
+      </c>
       <c r="U6">
+        <v>0</v>
+      </c>
+      <c r="V6">
         <v>3</v>
       </c>
-      <c r="V6">
-        <v>0</v>
-      </c>
       <c r="W6">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="X6">
-        <v>11</v>
-      </c>
-      <c r="Y6">
-        <f>(20+14)/W6-1</f>
+        <f>(20+14)/V6-1</f>
         <v>10.333333333333334</v>
       </c>
-      <c r="Z6" s="4" t="str">
+      <c r="Y6" s="4" t="str">
         <f>'Kelp consumption'!T6</f>
         <v>yes</v>
       </c>
-      <c r="AA6" s="4" t="str">
+      <c r="Z6" s="4" t="str">
         <f t="shared" si="2"/>
         <v>kelp consumed during video</v>
       </c>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -55650,43 +55639,39 @@
         <f>#REF!/O7</f>
         <v>#REF!</v>
       </c>
-      <c r="R7" t="e">
-        <f>#REF!/O7</f>
-        <v>#REF!</v>
+      <c r="R7">
+        <v>39</v>
       </c>
       <c r="S7">
-        <v>39</v>
-      </c>
-      <c r="T7">
         <f>(2044-1738)</f>
         <v>306</v>
       </c>
+      <c r="T7">
+        <v>10</v>
+      </c>
       <c r="U7">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="V7">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="W7">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="X7">
-        <v>20</v>
-      </c>
-      <c r="Y7">
         <f>(12+13+9+12+8+11+8)/7</f>
         <v>10.428571428571429</v>
       </c>
-      <c r="Z7" s="4" t="str">
+      <c r="Y7" s="4" t="str">
         <f>'Kelp consumption'!T7</f>
         <v>yes</v>
       </c>
-      <c r="AA7" s="4" t="str">
+      <c r="Z7" s="4" t="str">
         <f t="shared" si="2"/>
         <v>kelp consumed during video</v>
       </c>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>15</v>
       </c>
@@ -55746,9 +55731,8 @@
         <f>#REF!/O8</f>
         <v>#REF!</v>
       </c>
-      <c r="R8" t="e">
-        <f>#REF!/O8</f>
-        <v>#REF!</v>
+      <c r="T8">
+        <v>0</v>
       </c>
       <c r="U8">
         <v>0</v>
@@ -55756,22 +55740,19 @@
       <c r="V8">
         <v>0</v>
       </c>
-      <c r="W8">
-        <v>0</v>
-      </c>
-      <c r="Z8" s="4" t="str">
+      <c r="Y8" s="4" t="str">
         <f>'Kelp consumption'!T16</f>
         <v>no</v>
       </c>
-      <c r="AA8" s="4" t="str">
+      <c r="Z8" s="4" t="str">
         <f t="shared" si="2"/>
         <v>urchin never ate kelp</v>
       </c>
-      <c r="AB8" t="s">
+      <c r="AA8" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>16</v>
       </c>
@@ -55831,39 +55812,35 @@
         <f>#REF!/O9</f>
         <v>#REF!</v>
       </c>
-      <c r="R9" t="e">
-        <f>#REF!/O9</f>
-        <v>#REF!</v>
+      <c r="R9">
+        <v>14</v>
       </c>
       <c r="S9">
-        <v>14</v>
-      </c>
-      <c r="T9">
         <f>12906-12389</f>
         <v>517</v>
       </c>
+      <c r="T9">
+        <v>1</v>
+      </c>
       <c r="U9">
+        <v>0</v>
+      </c>
+      <c r="V9">
         <v>1</v>
       </c>
-      <c r="V9">
-        <v>0</v>
-      </c>
       <c r="W9">
-        <v>1</v>
-      </c>
-      <c r="X9">
         <v>8</v>
       </c>
-      <c r="Z9" s="4" t="str">
+      <c r="Y9" s="4" t="str">
         <f>'Kelp consumption'!T17</f>
         <v>yes</v>
       </c>
-      <c r="AA9" s="4" t="str">
+      <c r="Z9" s="4" t="str">
         <f t="shared" si="2"/>
         <v>kelp consumed during video</v>
       </c>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>17</v>
       </c>
@@ -55923,46 +55900,42 @@
         <f>#REF!/O10</f>
         <v>#REF!</v>
       </c>
-      <c r="R10" t="e">
-        <f>#REF!/O10</f>
-        <v>#REF!</v>
+      <c r="R10">
+        <v>32</v>
       </c>
       <c r="S10">
-        <v>32</v>
-      </c>
-      <c r="T10">
         <f>26+32+(10817-10744)</f>
         <v>131</v>
       </c>
+      <c r="T10">
+        <v>9</v>
+      </c>
       <c r="U10">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="V10">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="W10">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="X10">
-        <v>23</v>
-      </c>
-      <c r="Y10">
         <f>(16+9+12+9+13)/5</f>
         <v>11.8</v>
       </c>
-      <c r="Z10" s="4" t="str">
+      <c r="Y10" s="4" t="str">
         <f>'Kelp consumption'!T18</f>
         <v>no</v>
       </c>
-      <c r="AA10" s="4" t="str">
+      <c r="Z10" s="4" t="str">
         <f t="shared" si="2"/>
         <v>urchin never ate kelp</v>
       </c>
-      <c r="AB10" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AA10" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="11" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>18</v>
       </c>
@@ -56022,9 +55995,8 @@
         <f>#REF!/O11</f>
         <v>#REF!</v>
       </c>
-      <c r="R11" t="e">
-        <f>#REF!/O11</f>
-        <v>#REF!</v>
+      <c r="T11">
+        <v>0</v>
       </c>
       <c r="U11">
         <v>0</v>
@@ -56032,22 +56004,19 @@
       <c r="V11">
         <v>0</v>
       </c>
-      <c r="W11">
-        <v>0</v>
-      </c>
-      <c r="Z11" s="4" t="str">
+      <c r="Y11" s="4" t="str">
         <f>'Kelp consumption'!T19</f>
         <v>no</v>
       </c>
-      <c r="AA11" s="4" t="str">
+      <c r="Z11" s="4" t="str">
         <f t="shared" si="2"/>
         <v>urchin never ate kelp</v>
       </c>
-      <c r="AB11" t="s">
+      <c r="AA11" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>19</v>
       </c>
@@ -56107,39 +56076,35 @@
         <f>#REF!/O12</f>
         <v>#REF!</v>
       </c>
-      <c r="R12" t="e">
-        <f>#REF!/O12</f>
-        <v>#REF!</v>
+      <c r="R12">
+        <v>15</v>
       </c>
       <c r="S12">
-        <v>15</v>
-      </c>
-      <c r="T12">
         <f>(12810-12513)+24+14</f>
         <v>335</v>
       </c>
+      <c r="T12">
+        <v>3</v>
+      </c>
       <c r="U12">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="V12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="W12">
-        <v>1</v>
-      </c>
-      <c r="X12">
         <v>8</v>
       </c>
-      <c r="Z12" s="4" t="str">
+      <c r="Y12" s="4" t="str">
         <f>'Kelp consumption'!T20</f>
         <v>yes</v>
       </c>
-      <c r="AA12" s="4" t="str">
+      <c r="Z12" s="4" t="str">
         <f t="shared" si="2"/>
         <v>kelp consumed during video</v>
       </c>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>20</v>
       </c>
@@ -56199,29 +56164,25 @@
         <f>#REF!/O13</f>
         <v>#REF!</v>
       </c>
-      <c r="R13" t="e">
-        <f>#REF!/O13</f>
-        <v>#REF!</v>
+      <c r="T13">
+        <v>3</v>
       </c>
       <c r="U13">
         <v>3</v>
       </c>
       <c r="V13">
-        <v>3</v>
-      </c>
-      <c r="W13">
         <v>0</v>
       </c>
-      <c r="Z13" s="4" t="str">
+      <c r="Y13" s="4" t="str">
         <f>'Kelp consumption'!T21</f>
         <v>no</v>
       </c>
-      <c r="AA13" s="4" t="str">
+      <c r="Z13" s="4" t="str">
         <f t="shared" si="2"/>
         <v>urchin never ate kelp</v>
       </c>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>29</v>
       </c>
@@ -56281,42 +56242,38 @@
         <f>#REF!/O14</f>
         <v>#REF!</v>
       </c>
-      <c r="R14" t="e">
-        <f>#REF!/O14</f>
-        <v>#REF!</v>
+      <c r="R14">
+        <v>15</v>
       </c>
       <c r="S14">
-        <v>15</v>
-      </c>
-      <c r="T14">
         <f>10346-10074</f>
         <v>272</v>
       </c>
+      <c r="T14">
+        <v>1</v>
+      </c>
       <c r="U14">
+        <v>0</v>
+      </c>
+      <c r="V14">
         <v>1</v>
       </c>
-      <c r="V14">
-        <v>0</v>
-      </c>
       <c r="W14">
-        <v>1</v>
-      </c>
-      <c r="X14">
         <v>7</v>
       </c>
-      <c r="Z14" s="4" t="str">
+      <c r="Y14" s="4" t="str">
         <f>'Kelp consumption'!T30</f>
         <v>yes</v>
       </c>
-      <c r="AA14" s="4" t="str">
+      <c r="Z14" s="4" t="str">
         <f t="shared" si="2"/>
         <v>kelp consumed during video</v>
       </c>
-      <c r="AB14" t="s">
+      <c r="AA14" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>30</v>
       </c>
@@ -56376,39 +56333,35 @@
         <f>#REF!/O15</f>
         <v>#REF!</v>
       </c>
-      <c r="R15" t="e">
-        <f>#REF!/O15</f>
-        <v>#REF!</v>
+      <c r="R15">
+        <v>32</v>
       </c>
       <c r="S15">
-        <v>32</v>
-      </c>
-      <c r="T15">
         <f>12283-11704</f>
         <v>579</v>
       </c>
+      <c r="T15">
+        <v>1</v>
+      </c>
       <c r="U15">
+        <v>0</v>
+      </c>
+      <c r="V15">
         <v>1</v>
       </c>
-      <c r="V15">
-        <v>0</v>
-      </c>
       <c r="W15">
-        <v>1</v>
-      </c>
-      <c r="X15">
         <v>23</v>
       </c>
-      <c r="Z15" s="4" t="str">
+      <c r="Y15" s="4" t="str">
         <f>'Kelp consumption'!T31</f>
         <v>yes</v>
       </c>
-      <c r="AA15" s="4" t="str">
+      <c r="Z15" s="4" t="str">
         <f t="shared" si="2"/>
         <v>kelp consumed during video</v>
       </c>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>31</v>
       </c>
@@ -56468,42 +56421,38 @@
         <f>#REF!/O16</f>
         <v>#REF!</v>
       </c>
-      <c r="R16" t="e">
-        <f>#REF!/O16</f>
-        <v>#REF!</v>
+      <c r="R16">
+        <v>25</v>
       </c>
       <c r="S16">
-        <v>25</v>
-      </c>
-      <c r="T16">
         <f>(12094-12041)+54+26+103+74</f>
         <v>310</v>
       </c>
+      <c r="T16">
+        <v>12</v>
+      </c>
       <c r="U16">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="V16">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="W16">
-        <v>1</v>
-      </c>
-      <c r="X16">
         <v>17</v>
       </c>
-      <c r="Z16" s="4" t="str">
+      <c r="Y16" s="4" t="str">
         <f>'Kelp consumption'!T32</f>
         <v>yes</v>
       </c>
-      <c r="AA16" s="4" t="str">
+      <c r="Z16" s="4" t="str">
         <f t="shared" si="2"/>
         <v>kelp consumed during video</v>
       </c>
-      <c r="AB16" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AA16" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="17" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>32</v>
       </c>
@@ -56563,9 +56512,8 @@
         <f>#REF!/O17</f>
         <v>#REF!</v>
       </c>
-      <c r="R17" t="e">
-        <f>#REF!/O17</f>
-        <v>#REF!</v>
+      <c r="T17">
+        <v>0</v>
       </c>
       <c r="U17">
         <v>0</v>
@@ -56573,22 +56521,19 @@
       <c r="V17">
         <v>0</v>
       </c>
-      <c r="W17">
-        <v>0</v>
-      </c>
-      <c r="Z17" s="4" t="str">
+      <c r="Y17" s="4" t="str">
         <f>'Kelp consumption'!T33</f>
         <v>no</v>
       </c>
-      <c r="AA17" s="4" t="str">
+      <c r="Z17" s="4" t="str">
         <f t="shared" si="2"/>
         <v>urchin never ate kelp</v>
       </c>
-      <c r="AB17" t="s">
+      <c r="AA17" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>33</v>
       </c>
@@ -56648,40 +56593,36 @@
         <f>#REF!/O18</f>
         <v>#REF!</v>
       </c>
-      <c r="R18" t="e">
-        <f>#REF!/O18</f>
-        <v>#REF!</v>
-      </c>
-      <c r="S18">
+      <c r="R18">
         <f>120+10+5</f>
         <v>135</v>
       </c>
-      <c r="T18">
+      <c r="S18">
         <f>11896-11421</f>
         <v>475</v>
       </c>
+      <c r="T18">
+        <v>1</v>
+      </c>
       <c r="U18">
+        <v>0</v>
+      </c>
+      <c r="V18">
         <v>1</v>
       </c>
-      <c r="V18">
-        <v>0</v>
-      </c>
       <c r="W18">
-        <v>1</v>
-      </c>
-      <c r="X18">
         <v>120</v>
       </c>
-      <c r="Z18" s="4" t="str">
+      <c r="Y18" s="4" t="str">
         <f>'Kelp consumption'!T34</f>
         <v>yes</v>
       </c>
-      <c r="AA18" s="4" t="str">
+      <c r="Z18" s="4" t="str">
         <f t="shared" si="2"/>
         <v>kelp consumed during video</v>
       </c>
     </row>
-    <row r="19" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>34</v>
       </c>
@@ -56741,42 +56682,38 @@
         <f>#REF!/O19</f>
         <v>#REF!</v>
       </c>
-      <c r="R19" t="e">
-        <f>#REF!/O19</f>
-        <v>#REF!</v>
+      <c r="R19">
+        <v>14</v>
       </c>
       <c r="S19">
-        <v>14</v>
-      </c>
-      <c r="T19">
         <f>12895-12338</f>
         <v>557</v>
       </c>
+      <c r="T19">
+        <v>3</v>
+      </c>
       <c r="U19">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="V19">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="W19">
-        <v>2</v>
-      </c>
-      <c r="X19">
         <v>10</v>
       </c>
-      <c r="Z19" s="4" t="str">
+      <c r="Y19" s="4" t="str">
         <f>'Kelp consumption'!T35</f>
         <v>no</v>
       </c>
-      <c r="AA19" s="4" t="str">
+      <c r="Z19" s="4" t="str">
         <f t="shared" si="2"/>
         <v>urchin never ate kelp</v>
       </c>
-      <c r="AB19" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="20" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AA19" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="20" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>43</v>
       </c>
@@ -56836,39 +56773,35 @@
         <f>#REF!/O20</f>
         <v>#REF!</v>
       </c>
-      <c r="R20" t="e">
-        <f>#REF!/O20</f>
-        <v>#REF!</v>
+      <c r="R20">
+        <v>43</v>
       </c>
       <c r="S20">
-        <v>43</v>
-      </c>
-      <c r="T20">
         <f>11882-11411</f>
         <v>471</v>
       </c>
+      <c r="T20">
+        <v>1</v>
+      </c>
       <c r="U20">
+        <v>0</v>
+      </c>
+      <c r="V20">
         <v>1</v>
       </c>
-      <c r="V20">
-        <v>0</v>
-      </c>
       <c r="W20">
-        <v>1</v>
-      </c>
-      <c r="X20">
         <v>32</v>
       </c>
-      <c r="Z20" s="4" t="str">
+      <c r="Y20" s="4" t="str">
         <f>'Kelp consumption'!T44</f>
         <v>yes</v>
       </c>
-      <c r="AA20" s="4" t="str">
+      <c r="Z20" s="4" t="str">
         <f t="shared" si="2"/>
         <v>kelp consumed during video</v>
       </c>
     </row>
-    <row r="21" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>44</v>
       </c>
@@ -56928,42 +56861,38 @@
         <f>#REF!/O21</f>
         <v>#REF!</v>
       </c>
-      <c r="R21" t="e">
-        <f>#REF!/O21</f>
-        <v>#REF!</v>
+      <c r="R21">
+        <v>46</v>
       </c>
       <c r="S21">
-        <v>46</v>
-      </c>
-      <c r="T21">
         <f>22+(12179-12048)</f>
         <v>153</v>
       </c>
+      <c r="T21">
+        <v>3</v>
+      </c>
       <c r="U21">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="V21">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="W21">
-        <v>2</v>
+        <v>36</v>
       </c>
       <c r="X21">
-        <v>36</v>
-      </c>
-      <c r="Y21">
         <v>20</v>
       </c>
-      <c r="Z21" s="4" t="str">
+      <c r="Y21" s="4" t="str">
         <f>'Kelp consumption'!T45</f>
         <v>yes</v>
       </c>
-      <c r="AA21" s="4" t="str">
+      <c r="Z21" s="4" t="str">
         <f t="shared" si="2"/>
         <v>kelp consumed during video</v>
       </c>
     </row>
-    <row r="22" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>45</v>
       </c>
@@ -57023,9 +56952,8 @@
         <f>#REF!/O22</f>
         <v>#REF!</v>
       </c>
-      <c r="R22" t="e">
-        <f>#REF!/O22</f>
-        <v>#REF!</v>
+      <c r="T22">
+        <v>0</v>
       </c>
       <c r="U22">
         <v>0</v>
@@ -57033,22 +56961,19 @@
       <c r="V22">
         <v>0</v>
       </c>
-      <c r="W22">
-        <v>0</v>
-      </c>
-      <c r="Z22" s="4" t="str">
+      <c r="Y22" s="4" t="str">
         <f>'Kelp consumption'!T46</f>
         <v>no</v>
       </c>
-      <c r="AA22" s="4" t="str">
+      <c r="Z22" s="4" t="str">
         <f t="shared" si="2"/>
         <v>urchin never ate kelp</v>
       </c>
-      <c r="AB22" t="s">
+      <c r="AA22" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="23" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>46</v>
       </c>
@@ -57130,22 +57055,19 @@
       <c r="X23" t="s">
         <v>60</v>
       </c>
-      <c r="Y23" t="s">
-        <v>60</v>
-      </c>
-      <c r="Z23" s="4" t="str">
+      <c r="Y23" s="4" t="str">
         <f>'Kelp consumption'!T47</f>
         <v>no</v>
       </c>
-      <c r="AA23" s="4" t="str">
+      <c r="Z23" s="4" t="str">
         <f t="shared" si="2"/>
         <v>urchin never ate kelp</v>
       </c>
-      <c r="AB23" t="s">
+      <c r="AA23" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="24" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>47</v>
       </c>
@@ -57205,42 +57127,38 @@
         <f>#REF!/O24</f>
         <v>#REF!</v>
       </c>
-      <c r="R24" t="e">
-        <f>#REF!/O24</f>
-        <v>#REF!</v>
+      <c r="R24">
+        <v>9</v>
       </c>
       <c r="S24">
-        <v>9</v>
-      </c>
-      <c r="T24">
         <f>10260-10148</f>
         <v>112</v>
       </c>
+      <c r="T24">
+        <v>1</v>
+      </c>
       <c r="U24">
+        <v>0</v>
+      </c>
+      <c r="V24">
         <v>1</v>
       </c>
-      <c r="V24">
-        <v>0</v>
-      </c>
       <c r="W24">
-        <v>1</v>
-      </c>
-      <c r="X24">
         <v>2</v>
       </c>
-      <c r="Z24" s="4" t="str">
+      <c r="Y24" s="4" t="str">
         <f>'Kelp consumption'!T48</f>
         <v>no</v>
       </c>
-      <c r="AA24" s="4" t="str">
+      <c r="Z24" s="4" t="str">
         <f t="shared" si="2"/>
         <v>urchin never ate kelp</v>
       </c>
-      <c r="AB24" t="s">
+      <c r="AA24" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="25" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>48</v>
       </c>
@@ -57300,9 +57218,8 @@
         <f>#REF!/O25</f>
         <v>#REF!</v>
       </c>
-      <c r="R25" t="e">
-        <f>#REF!/O25</f>
-        <v>#REF!</v>
+      <c r="T25">
+        <v>0</v>
       </c>
       <c r="U25">
         <v>0</v>
@@ -57310,22 +57227,19 @@
       <c r="V25">
         <v>0</v>
       </c>
-      <c r="W25">
-        <v>0</v>
-      </c>
-      <c r="Z25" s="4" t="str">
+      <c r="Y25" s="4" t="str">
         <f>'Kelp consumption'!T49</f>
         <v>no</v>
       </c>
-      <c r="AA25" s="4" t="str">
+      <c r="Z25" s="4" t="str">
         <f t="shared" si="2"/>
         <v>urchin never ate kelp</v>
       </c>
-      <c r="AB25" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="26" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AA25" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="26" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>65</v>
       </c>
@@ -57385,9 +57299,8 @@
         <f>#REF!/O26</f>
         <v>#REF!</v>
       </c>
-      <c r="R26" t="e">
-        <f>#REF!/O26</f>
-        <v>#REF!</v>
+      <c r="T26">
+        <v>0</v>
       </c>
       <c r="U26">
         <v>0</v>
@@ -57395,22 +57308,19 @@
       <c r="V26">
         <v>0</v>
       </c>
-      <c r="W26">
-        <v>0</v>
-      </c>
-      <c r="Z26" s="4" t="str">
+      <c r="Y26" s="4" t="str">
         <f>'Kelp consumption'!T66</f>
         <v>yes</v>
       </c>
-      <c r="AA26" s="4" t="str">
+      <c r="Z26" s="4" t="str">
         <f t="shared" si="2"/>
         <v>kelp consumed AFTER video</v>
       </c>
-      <c r="AB26" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="27" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AA26" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="27" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>66</v>
       </c>
@@ -57470,42 +57380,38 @@
         <f>#REF!/O27</f>
         <v>#REF!</v>
       </c>
-      <c r="R27" t="e">
-        <f>#REF!/O27</f>
-        <v>#REF!</v>
+      <c r="R27">
+        <v>21</v>
       </c>
       <c r="S27">
-        <v>21</v>
-      </c>
-      <c r="T27">
         <f>12924-12418</f>
         <v>506</v>
       </c>
+      <c r="T27">
+        <v>1</v>
+      </c>
       <c r="U27">
+        <v>0</v>
+      </c>
+      <c r="V27">
         <v>1</v>
       </c>
-      <c r="V27">
-        <v>0</v>
-      </c>
       <c r="W27">
-        <v>1</v>
-      </c>
-      <c r="X27">
         <v>14</v>
       </c>
-      <c r="Z27" s="4" t="str">
+      <c r="Y27" s="4" t="str">
         <f>'Kelp consumption'!T67</f>
         <v>yes</v>
       </c>
-      <c r="AA27" s="4" t="str">
+      <c r="Z27" s="4" t="str">
         <f t="shared" si="2"/>
         <v>kelp consumed during video</v>
       </c>
-      <c r="AB27" t="s">
+      <c r="AA27" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="28" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>67</v>
       </c>
@@ -57565,32 +57471,28 @@
         <f>#REF!/O28</f>
         <v>#REF!</v>
       </c>
-      <c r="R28" t="e">
-        <f>#REF!/O28</f>
-        <v>#REF!</v>
+      <c r="T28">
+        <v>12</v>
       </c>
       <c r="U28">
         <v>12</v>
       </c>
       <c r="V28">
-        <v>12</v>
-      </c>
-      <c r="W28">
         <v>0</v>
       </c>
-      <c r="Z28" s="4" t="str">
+      <c r="Y28" s="4" t="str">
         <f>'Kelp consumption'!T68</f>
         <v>no</v>
       </c>
-      <c r="AA28" s="4" t="str">
+      <c r="Z28" s="4" t="str">
         <f t="shared" si="2"/>
         <v>urchin never ate kelp</v>
       </c>
-      <c r="AB28" t="s">
+      <c r="AA28" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="29" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>68</v>
       </c>
@@ -57650,36 +57552,36 @@
         <f>#REF!/O29</f>
         <v>#REF!</v>
       </c>
-      <c r="R29" t="e">
-        <f>#REF!/O29</f>
-        <v>#REF!</v>
-      </c>
-      <c r="T29">
+      <c r="R29">
+        <f>11574-11520</f>
+        <v>54</v>
+      </c>
+      <c r="S29">
         <f>11894-11574</f>
         <v>320</v>
       </c>
+      <c r="T29">
+        <v>3</v>
+      </c>
       <c r="U29">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="V29">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="W29">
-        <v>1</v>
-      </c>
-      <c r="X29">
         <v>15</v>
       </c>
-      <c r="Z29" s="4" t="str">
+      <c r="Y29" s="4" t="str">
         <f>'Kelp consumption'!T69</f>
         <v>yes</v>
       </c>
-      <c r="AA29" s="4" t="str">
+      <c r="Z29" s="4" t="str">
         <f t="shared" si="2"/>
         <v>kelp consumed during video</v>
       </c>
     </row>
-    <row r="30" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>69</v>
       </c>
@@ -57739,23 +57641,22 @@
         <f>#REF!/O30</f>
         <v>#REF!</v>
       </c>
-      <c r="R30" t="e">
-        <f>#REF!/O30</f>
-        <v>#REF!</v>
-      </c>
-      <c r="W30">
+      <c r="V30">
         <v>0</v>
       </c>
-      <c r="Z30" s="4" t="str">
+      <c r="Y30" s="4" t="str">
         <f>'Kelp consumption'!T70</f>
         <v>no</v>
       </c>
-      <c r="AA30" s="4" t="str">
+      <c r="Z30" s="4" t="str">
         <f t="shared" si="2"/>
         <v>urchin never ate kelp</v>
       </c>
-    </row>
-    <row r="31" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AA30" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="31" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>70</v>
       </c>
@@ -57815,26 +57716,36 @@
         <f>#REF!/O31</f>
         <v>#REF!</v>
       </c>
-      <c r="R31" t="e">
-        <f>#REF!/O31</f>
-        <v>#REF!</v>
+      <c r="R31">
+        <f>11715-11685</f>
+        <v>30</v>
+      </c>
+      <c r="S31">
+        <f>(11963-11715)-1+(12267-12105)</f>
+        <v>409</v>
+      </c>
+      <c r="T31">
+        <v>2</v>
+      </c>
+      <c r="U31">
+        <v>1</v>
+      </c>
+      <c r="V31">
+        <v>1</v>
       </c>
       <c r="W31">
-        <v>1</v>
-      </c>
-      <c r="Z31" s="4" t="str">
+        <v>21</v>
+      </c>
+      <c r="Y31" s="4" t="str">
         <f>'Kelp consumption'!T71</f>
         <v>yes</v>
       </c>
-      <c r="AA31" s="4" t="str">
+      <c r="Z31" s="4" t="str">
         <f t="shared" si="2"/>
-        <v>kelp consumed AFTER video</v>
-      </c>
-      <c r="AB31" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="32" spans="1:28" x14ac:dyDescent="0.2">
+        <v>kelp consumed during video</v>
+      </c>
+    </row>
+    <row r="32" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>71</v>
       </c>
@@ -57894,26 +57805,28 @@
         <f>#REF!/O32</f>
         <v>#REF!</v>
       </c>
-      <c r="R32" t="e">
-        <f>#REF!/O32</f>
-        <v>#REF!</v>
-      </c>
-      <c r="W32">
+      <c r="T32">
         <v>0</v>
       </c>
-      <c r="Z32" s="4" t="str">
+      <c r="U32">
+        <v>0</v>
+      </c>
+      <c r="V32">
+        <v>0</v>
+      </c>
+      <c r="Y32" s="4" t="str">
         <f>'Kelp consumption'!T72</f>
         <v>yes</v>
       </c>
-      <c r="AA32" s="4" t="str">
+      <c r="Z32" s="4" t="str">
         <f t="shared" si="2"/>
         <v>kelp consumed AFTER video</v>
       </c>
-      <c r="AB32" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="33" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AA32" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="33" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>72</v>
       </c>
@@ -57973,23 +57886,25 @@
         <f>#REF!/O33</f>
         <v>#REF!</v>
       </c>
-      <c r="R33" t="e">
-        <f>#REF!/O33</f>
-        <v>#REF!</v>
-      </c>
-      <c r="W33">
+      <c r="T33">
+        <v>5</v>
+      </c>
+      <c r="U33">
+        <v>5</v>
+      </c>
+      <c r="V33">
         <v>0</v>
       </c>
-      <c r="Z33" s="4" t="str">
+      <c r="Y33" s="4" t="str">
         <f>'Kelp consumption'!T73</f>
         <v>yes</v>
       </c>
-      <c r="AA33" s="4" t="str">
+      <c r="Z33" s="4" t="str">
         <f t="shared" si="2"/>
         <v>kelp consumed AFTER video</v>
       </c>
     </row>
-    <row r="34" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>73</v>
       </c>
@@ -58049,23 +57964,39 @@
         <f>#REF!/O34</f>
         <v>#REF!</v>
       </c>
-      <c r="R34" t="e">
-        <f>#REF!/O34</f>
-        <v>#REF!</v>
+      <c r="R34">
+        <f>12455-12437</f>
+        <v>18</v>
+      </c>
+      <c r="S34">
+        <f>12872-12455</f>
+        <v>417</v>
+      </c>
+      <c r="T34">
+        <v>2</v>
+      </c>
+      <c r="U34">
+        <v>1</v>
+      </c>
+      <c r="V34">
+        <v>1</v>
       </c>
       <c r="W34">
-        <v>1</v>
-      </c>
-      <c r="Z34" s="4" t="str">
+        <v>13</v>
+      </c>
+      <c r="Y34" s="4" t="str">
         <f>'Kelp consumption'!T74</f>
         <v>yes</v>
       </c>
-      <c r="AA34" s="4" t="str">
+      <c r="Z34" s="4" t="str">
         <f t="shared" si="2"/>
-        <v>kelp consumed AFTER video</v>
-      </c>
-    </row>
-    <row r="35" spans="1:28" x14ac:dyDescent="0.2">
+        <v>kelp consumed during video</v>
+      </c>
+      <c r="AA34" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="35" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>74</v>
       </c>
@@ -58125,23 +58056,36 @@
         <f>#REF!/O35</f>
         <v>#REF!</v>
       </c>
-      <c r="R35" t="e">
-        <f>#REF!/O35</f>
-        <v>#REF!</v>
+      <c r="R35">
+        <f>12811-12793</f>
+        <v>18</v>
+      </c>
+      <c r="S35">
+        <f>12890-12811</f>
+        <v>79</v>
+      </c>
+      <c r="T35">
+        <v>1</v>
+      </c>
+      <c r="U35">
+        <v>0</v>
+      </c>
+      <c r="V35">
+        <v>1</v>
       </c>
       <c r="W35">
-        <v>1</v>
-      </c>
-      <c r="Z35" s="4" t="str">
+        <v>12</v>
+      </c>
+      <c r="Y35" s="4" t="str">
         <f>'Kelp consumption'!T75</f>
         <v>yes</v>
       </c>
-      <c r="AA35" s="4" t="str">
+      <c r="Z35" s="4" t="str">
         <f t="shared" si="2"/>
-        <v>kelp consumed AFTER video</v>
-      </c>
-    </row>
-    <row r="36" spans="1:28" x14ac:dyDescent="0.2">
+        <v>kelp consumed during video</v>
+      </c>
+    </row>
+    <row r="36" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>75</v>
       </c>
@@ -58201,23 +58145,39 @@
         <f>#REF!/O36</f>
         <v>#REF!</v>
       </c>
-      <c r="R36" t="e">
-        <f>#REF!/O36</f>
-        <v>#REF!</v>
+      <c r="R36">
+        <f>11697-11576</f>
+        <v>121</v>
+      </c>
+      <c r="S36">
+        <f>11777-11697</f>
+        <v>80</v>
+      </c>
+      <c r="T36">
+        <v>5</v>
+      </c>
+      <c r="U36">
+        <v>4</v>
+      </c>
+      <c r="V36">
+        <v>1</v>
       </c>
       <c r="W36">
-        <v>1</v>
-      </c>
-      <c r="Z36" s="4" t="str">
+        <v>12</v>
+      </c>
+      <c r="Y36" s="4" t="str">
         <f>'Kelp consumption'!T76</f>
         <v>yes</v>
       </c>
-      <c r="AA36" s="4" t="str">
+      <c r="Z36" s="4" t="str">
         <f t="shared" si="2"/>
-        <v>kelp consumed AFTER video</v>
-      </c>
-    </row>
-    <row r="37" spans="1:28" x14ac:dyDescent="0.2">
+        <v>kelp consumed during video</v>
+      </c>
+      <c r="AA36" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="37" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>76</v>
       </c>
@@ -58277,23 +58237,25 @@
         <f>#REF!/O37</f>
         <v>#REF!</v>
       </c>
-      <c r="R37" t="e">
-        <f>#REF!/O37</f>
-        <v>#REF!</v>
-      </c>
-      <c r="W37">
+      <c r="T37">
+        <v>3</v>
+      </c>
+      <c r="U37">
+        <v>3</v>
+      </c>
+      <c r="V37">
         <v>0</v>
       </c>
-      <c r="Z37" s="4" t="str">
+      <c r="Y37" s="4" t="str">
         <f>'Kelp consumption'!T77</f>
         <v>no</v>
       </c>
-      <c r="AA37" s="4" t="str">
+      <c r="Z37" s="4" t="str">
         <f t="shared" si="2"/>
         <v>urchin never ate kelp</v>
       </c>
-      <c r="AB37" t="s">
-        <v>93</v>
+      <c r="AA37" t="s">
+        <v>91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Post data input clean up
</commit_message>
<xml_diff>
--- a/data/raw.xlsx
+++ b/data/raw.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/EcosystemRecoveryLab/github/Ritger-Corynactis-urchin-deterrence/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAD74ACD-35E7-2945-9387-67963A5FA7E0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BD46EC3-06CC-1E4C-9378-68C27DC2EC00}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3420" yWindow="7660" windowWidth="47980" windowHeight="16120" activeTab="2" xr2:uid="{58E670A5-634C-427F-960F-9DA76C64E810}"/>
+    <workbookView xWindow="1460" yWindow="7680" windowWidth="47980" windowHeight="16120" activeTab="2" xr2:uid="{58E670A5-634C-427F-960F-9DA76C64E810}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="3" r:id="rId1"/>
@@ -20,7 +20,6 @@
     <sheet name="Balcony temp" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="119">
   <si>
     <t>Tank number</t>
   </si>
@@ -381,6 +380,12 @@
   </si>
   <si>
     <t>Percent time with Kelp</t>
+  </si>
+  <si>
+    <t>Was the urchin deterred during video?</t>
+  </si>
+  <si>
+    <t>Was the urchin sucessfully deterred during video?</t>
   </si>
 </sst>
 </file>
@@ -55015,12 +55020,12 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55F6BF2F-CBB2-4331-929A-D3F4AD694052}">
-  <dimension ref="A1:AA37"/>
+  <dimension ref="A1:AC37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="107" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="O1" zoomScale="107" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="G1" sqref="G1"/>
-      <selection pane="bottomLeft" activeCell="AA37" sqref="AA37"/>
+      <selection pane="bottomLeft" activeCell="AC36" sqref="AC36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -55051,10 +55056,11 @@
     <col min="24" max="24" width="23.5" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="9.5" customWidth="1"/>
     <col min="26" max="26" width="30.1640625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="27" max="28" width="30.1640625" customWidth="1"/>
+    <col min="29" max="29" width="10.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:29" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -55135,10 +55141,16 @@
         <v>108</v>
       </c>
       <c r="AA1" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="AB1" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="AC1" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -55229,8 +55241,16 @@
         <f>IF(Y2="yes",IF(S2&gt;0,"kelp consumed during video","kelp consumed AFTER video"),"urchin never ate kelp")</f>
         <v>kelp consumed during video</v>
       </c>
-    </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AA2" s="4" t="str">
+        <f>IF(T2=0, "urchin never tried",IF(U2&gt;0, "Yes", "No"))</f>
+        <v>Yes</v>
+      </c>
+      <c r="AB2" s="4" t="str">
+        <f>IF(AA2="yes",IF(S2&gt;0,"Corynactis was so close","Corynactis was a monster"),IF(T2&gt;0,"Urchin was a beast","Urchin didn't even try"))</f>
+        <v>Corynactis was so close</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -55307,8 +55327,16 @@
         <f t="shared" ref="Z3:Z37" si="2">IF(Y3="yes",IF(S3&gt;0,"kelp consumed during video","kelp consumed AFTER video"),"urchin never ate kelp")</f>
         <v>urchin never ate kelp</v>
       </c>
-    </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AA3" s="4" t="str">
+        <f t="shared" ref="AA3:AA37" si="3">IF(T3=0, "urchin never tried",IF(U3&gt;0, "Yes", "No"))</f>
+        <v>Yes</v>
+      </c>
+      <c r="AB3" s="4" t="str">
+        <f t="shared" ref="AB3:AB37" si="4">IF(AA3="yes",IF(S3&gt;0,"Corynactis was so close","Corynactis was a monster"),IF(T3&gt;0,"Urchin was a beast","Urchin didn't even try"))</f>
+        <v>Corynactis was a monster</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -55395,11 +55423,19 @@
         <f t="shared" si="2"/>
         <v>kelp consumed during video</v>
       </c>
-      <c r="AA4" t="s">
+      <c r="AA4" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v>No</v>
+      </c>
+      <c r="AB4" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>Urchin was a beast</v>
+      </c>
+      <c r="AC4" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -55486,8 +55522,16 @@
         <f t="shared" si="2"/>
         <v>kelp consumed during video</v>
       </c>
-    </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AA5" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v>Yes</v>
+      </c>
+      <c r="AB5" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>Corynactis was so close</v>
+      </c>
+    </row>
+    <row r="6" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -55578,8 +55622,16 @@
         <f t="shared" si="2"/>
         <v>kelp consumed during video</v>
       </c>
-    </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AA6" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v>No</v>
+      </c>
+      <c r="AB6" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>Urchin was a beast</v>
+      </c>
+    </row>
+    <row r="7" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -55670,8 +55722,16 @@
         <f t="shared" si="2"/>
         <v>kelp consumed during video</v>
       </c>
-    </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AA7" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v>Yes</v>
+      </c>
+      <c r="AB7" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>Corynactis was so close</v>
+      </c>
+    </row>
+    <row r="8" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>15</v>
       </c>
@@ -55748,11 +55808,19 @@
         <f t="shared" si="2"/>
         <v>urchin never ate kelp</v>
       </c>
-      <c r="AA8" t="s">
+      <c r="AA8" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v>urchin never tried</v>
+      </c>
+      <c r="AB8" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>Urchin didn't even try</v>
+      </c>
+      <c r="AC8" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>16</v>
       </c>
@@ -55839,8 +55907,16 @@
         <f t="shared" si="2"/>
         <v>kelp consumed during video</v>
       </c>
-    </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AA9" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v>No</v>
+      </c>
+      <c r="AB9" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>Urchin was a beast</v>
+      </c>
+    </row>
+    <row r="10" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>17</v>
       </c>
@@ -55931,11 +56007,19 @@
         <f t="shared" si="2"/>
         <v>urchin never ate kelp</v>
       </c>
-      <c r="AA10" t="s">
+      <c r="AA10" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v>Yes</v>
+      </c>
+      <c r="AB10" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>Corynactis was so close</v>
+      </c>
+      <c r="AC10" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>18</v>
       </c>
@@ -56012,11 +56096,19 @@
         <f t="shared" si="2"/>
         <v>urchin never ate kelp</v>
       </c>
-      <c r="AA11" t="s">
+      <c r="AA11" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v>urchin never tried</v>
+      </c>
+      <c r="AB11" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>Urchin didn't even try</v>
+      </c>
+      <c r="AC11" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>19</v>
       </c>
@@ -56103,8 +56195,16 @@
         <f t="shared" si="2"/>
         <v>kelp consumed during video</v>
       </c>
-    </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AA12" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v>Yes</v>
+      </c>
+      <c r="AB12" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>Corynactis was so close</v>
+      </c>
+    </row>
+    <row r="13" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>20</v>
       </c>
@@ -56181,8 +56281,16 @@
         <f t="shared" si="2"/>
         <v>urchin never ate kelp</v>
       </c>
-    </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AA13" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v>Yes</v>
+      </c>
+      <c r="AB13" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>Corynactis was a monster</v>
+      </c>
+    </row>
+    <row r="14" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>29</v>
       </c>
@@ -56269,11 +56377,19 @@
         <f t="shared" si="2"/>
         <v>kelp consumed during video</v>
       </c>
-      <c r="AA14" t="s">
+      <c r="AA14" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v>No</v>
+      </c>
+      <c r="AB14" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>Urchin was a beast</v>
+      </c>
+      <c r="AC14" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>30</v>
       </c>
@@ -56360,8 +56476,16 @@
         <f t="shared" si="2"/>
         <v>kelp consumed during video</v>
       </c>
-    </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AA15" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v>No</v>
+      </c>
+      <c r="AB15" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>Urchin was a beast</v>
+      </c>
+    </row>
+    <row r="16" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>31</v>
       </c>
@@ -56448,11 +56572,19 @@
         <f t="shared" si="2"/>
         <v>kelp consumed during video</v>
       </c>
-      <c r="AA16" t="s">
+      <c r="AA16" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v>Yes</v>
+      </c>
+      <c r="AB16" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>Corynactis was so close</v>
+      </c>
+      <c r="AC16" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>32</v>
       </c>
@@ -56529,11 +56661,19 @@
         <f t="shared" si="2"/>
         <v>urchin never ate kelp</v>
       </c>
-      <c r="AA17" t="s">
+      <c r="AA17" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v>urchin never tried</v>
+      </c>
+      <c r="AB17" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>Urchin didn't even try</v>
+      </c>
+      <c r="AC17" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="18" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>33</v>
       </c>
@@ -56621,8 +56761,16 @@
         <f t="shared" si="2"/>
         <v>kelp consumed during video</v>
       </c>
-    </row>
-    <row r="19" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AA18" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v>No</v>
+      </c>
+      <c r="AB18" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>Urchin was a beast</v>
+      </c>
+    </row>
+    <row r="19" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>34</v>
       </c>
@@ -56709,11 +56857,19 @@
         <f t="shared" si="2"/>
         <v>urchin never ate kelp</v>
       </c>
-      <c r="AA19" t="s">
+      <c r="AA19" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v>Yes</v>
+      </c>
+      <c r="AB19" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>Corynactis was so close</v>
+      </c>
+      <c r="AC19" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="20" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>43</v>
       </c>
@@ -56800,8 +56956,16 @@
         <f t="shared" si="2"/>
         <v>kelp consumed during video</v>
       </c>
-    </row>
-    <row r="21" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AA20" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v>No</v>
+      </c>
+      <c r="AB20" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>Urchin was a beast</v>
+      </c>
+    </row>
+    <row r="21" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>44</v>
       </c>
@@ -56891,8 +57055,16 @@
         <f t="shared" si="2"/>
         <v>kelp consumed during video</v>
       </c>
-    </row>
-    <row r="22" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AA21" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v>Yes</v>
+      </c>
+      <c r="AB21" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>Corynactis was so close</v>
+      </c>
+    </row>
+    <row r="22" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>45</v>
       </c>
@@ -56969,11 +57141,19 @@
         <f t="shared" si="2"/>
         <v>urchin never ate kelp</v>
       </c>
-      <c r="AA22" t="s">
+      <c r="AA22" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v>urchin never tried</v>
+      </c>
+      <c r="AB22" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>Urchin didn't even try</v>
+      </c>
+      <c r="AC22" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="23" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>46</v>
       </c>
@@ -57063,11 +57243,19 @@
         <f t="shared" si="2"/>
         <v>urchin never ate kelp</v>
       </c>
-      <c r="AA23" t="s">
+      <c r="AA23" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v>Yes</v>
+      </c>
+      <c r="AB23" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>Corynactis was so close</v>
+      </c>
+      <c r="AC23" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="24" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>47</v>
       </c>
@@ -57154,11 +57342,19 @@
         <f t="shared" si="2"/>
         <v>urchin never ate kelp</v>
       </c>
-      <c r="AA24" t="s">
+      <c r="AA24" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v>No</v>
+      </c>
+      <c r="AB24" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>Urchin was a beast</v>
+      </c>
+      <c r="AC24" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="25" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>48</v>
       </c>
@@ -57235,11 +57431,19 @@
         <f t="shared" si="2"/>
         <v>urchin never ate kelp</v>
       </c>
-      <c r="AA25" t="s">
+      <c r="AA25" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v>urchin never tried</v>
+      </c>
+      <c r="AB25" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>Urchin didn't even try</v>
+      </c>
+      <c r="AC25" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="26" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>65</v>
       </c>
@@ -57316,11 +57520,19 @@
         <f t="shared" si="2"/>
         <v>kelp consumed AFTER video</v>
       </c>
-      <c r="AA26" t="s">
+      <c r="AA26" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v>urchin never tried</v>
+      </c>
+      <c r="AB26" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>Urchin didn't even try</v>
+      </c>
+      <c r="AC26" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="27" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>66</v>
       </c>
@@ -57338,11 +57550,11 @@
         <v>42</v>
       </c>
       <c r="F27" t="str">
-        <f t="shared" ref="F27:F37" si="3">IF(H27&lt;=0, "Control", IF(H27&lt;=10, "Red", IF(H27&gt;=21, "Pink", "Orange")))</f>
+        <f t="shared" ref="F27:F37" si="5">IF(H27&lt;=0, "Control", IF(H27&lt;=10, "Red", IF(H27&gt;=21, "Pink", "Orange")))</f>
         <v>Orange</v>
       </c>
       <c r="G27">
-        <f t="shared" ref="G27:G37" si="4">IF(F27="Control", 1, IF(F27="Red", 2, IF(F27="Orange", 3, 4)))</f>
+        <f t="shared" ref="G27:G37" si="6">IF(F27="Control", 1, IF(F27="Red", 2, IF(F27="Orange", 3, 4)))</f>
         <v>3</v>
       </c>
       <c r="H27" s="7">
@@ -57407,11 +57619,19 @@
         <f t="shared" si="2"/>
         <v>kelp consumed during video</v>
       </c>
-      <c r="AA27" t="s">
+      <c r="AA27" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v>No</v>
+      </c>
+      <c r="AB27" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>Urchin was a beast</v>
+      </c>
+      <c r="AC27" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="28" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>67</v>
       </c>
@@ -57429,11 +57649,11 @@
         <v>42</v>
       </c>
       <c r="F28" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>Pink</v>
       </c>
       <c r="G28">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="H28" s="7">
@@ -57488,11 +57708,19 @@
         <f t="shared" si="2"/>
         <v>urchin never ate kelp</v>
       </c>
-      <c r="AA28" t="s">
+      <c r="AA28" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v>Yes</v>
+      </c>
+      <c r="AB28" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>Corynactis was a monster</v>
+      </c>
+      <c r="AC28" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="29" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>68</v>
       </c>
@@ -57510,11 +57738,11 @@
         <v>43</v>
       </c>
       <c r="F29" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>Pink</v>
       </c>
       <c r="G29">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="H29" s="7">
@@ -57580,8 +57808,16 @@
         <f t="shared" si="2"/>
         <v>kelp consumed during video</v>
       </c>
-    </row>
-    <row r="30" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AA29" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v>Yes</v>
+      </c>
+      <c r="AB29" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>Corynactis was so close</v>
+      </c>
+    </row>
+    <row r="30" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>69</v>
       </c>
@@ -57599,11 +57835,11 @@
         <v>43</v>
       </c>
       <c r="F30" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>Pink</v>
       </c>
       <c r="G30">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="H30" s="7">
@@ -57652,11 +57888,19 @@
         <f t="shared" si="2"/>
         <v>urchin never ate kelp</v>
       </c>
-      <c r="AA30" t="s">
+      <c r="AA30" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v>urchin never tried</v>
+      </c>
+      <c r="AB30" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>Urchin didn't even try</v>
+      </c>
+      <c r="AC30" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="31" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>70</v>
       </c>
@@ -57674,11 +57918,11 @@
         <v>42</v>
       </c>
       <c r="F31" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>Red</v>
       </c>
       <c r="G31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
       <c r="H31" s="7">
@@ -57744,8 +57988,16 @@
         <f t="shared" si="2"/>
         <v>kelp consumed during video</v>
       </c>
-    </row>
-    <row r="32" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AA31" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v>Yes</v>
+      </c>
+      <c r="AB31" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>Corynactis was so close</v>
+      </c>
+    </row>
+    <row r="32" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>71</v>
       </c>
@@ -57763,11 +58015,11 @@
         <v>42</v>
       </c>
       <c r="F32" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>Control</v>
       </c>
       <c r="G32">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="H32" s="7">
@@ -57822,11 +58074,19 @@
         <f t="shared" si="2"/>
         <v>kelp consumed AFTER video</v>
       </c>
-      <c r="AA32" t="s">
+      <c r="AA32" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v>urchin never tried</v>
+      </c>
+      <c r="AB32" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>Urchin didn't even try</v>
+      </c>
+      <c r="AC32" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="33" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>72</v>
       </c>
@@ -57844,11 +58104,11 @@
         <v>43</v>
       </c>
       <c r="F33" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>Pink</v>
       </c>
       <c r="G33">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="H33" s="7">
@@ -57903,8 +58163,16 @@
         <f t="shared" si="2"/>
         <v>kelp consumed AFTER video</v>
       </c>
-    </row>
-    <row r="34" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AA33" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v>Yes</v>
+      </c>
+      <c r="AB33" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>Corynactis was a monster</v>
+      </c>
+    </row>
+    <row r="34" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>73</v>
       </c>
@@ -57922,11 +58190,11 @@
         <v>43</v>
       </c>
       <c r="F34" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>Orange</v>
       </c>
       <c r="G34">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>3</v>
       </c>
       <c r="H34" s="7">
@@ -57992,11 +58260,19 @@
         <f t="shared" si="2"/>
         <v>kelp consumed during video</v>
       </c>
-      <c r="AA34" t="s">
+      <c r="AA34" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v>Yes</v>
+      </c>
+      <c r="AB34" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>Corynactis was so close</v>
+      </c>
+      <c r="AC34" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="35" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>74</v>
       </c>
@@ -58014,11 +58290,11 @@
         <v>43</v>
       </c>
       <c r="F35" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>Red</v>
       </c>
       <c r="G35">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
       <c r="H35" s="7">
@@ -58084,8 +58360,16 @@
         <f t="shared" si="2"/>
         <v>kelp consumed during video</v>
       </c>
-    </row>
-    <row r="36" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AA35" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v>No</v>
+      </c>
+      <c r="AB35" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>Urchin was a beast</v>
+      </c>
+    </row>
+    <row r="36" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>75</v>
       </c>
@@ -58103,11 +58387,11 @@
         <v>42</v>
       </c>
       <c r="F36" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>Pink</v>
       </c>
       <c r="G36">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="H36" s="7">
@@ -58173,11 +58457,19 @@
         <f t="shared" si="2"/>
         <v>kelp consumed during video</v>
       </c>
-      <c r="AA36" t="s">
+      <c r="AA36" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v>Yes</v>
+      </c>
+      <c r="AB36" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>Corynactis was so close</v>
+      </c>
+      <c r="AC36" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="37" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>76</v>
       </c>
@@ -58195,11 +58487,11 @@
         <v>42</v>
       </c>
       <c r="F37" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>Red</v>
       </c>
       <c r="G37">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
       <c r="H37" s="7">
@@ -58254,7 +58546,15 @@
         <f t="shared" si="2"/>
         <v>urchin never ate kelp</v>
       </c>
-      <c r="AA37" t="s">
+      <c r="AA37" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v>Yes</v>
+      </c>
+      <c r="AB37" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>Corynactis was a monster</v>
+      </c>
+      <c r="AC37" t="s">
         <v>91</v>
       </c>
     </row>

</xml_diff>

<commit_message>
now that I know tidyverse a bit better
</commit_message>
<xml_diff>
--- a/data/raw.xlsx
+++ b/data/raw.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Amelia\github\Ritger-Corynactis-urchin-deterrence\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{E4B58984-6CF9-48FC-8EF7-763CD8B03805}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21B72FDE-D41C-4E2E-A45A-FB1AC82BE96B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="708" yWindow="504" windowWidth="17280" windowHeight="11412" activeTab="1" xr2:uid="{58E670A5-634C-427F-960F-9DA76C64E810}"/>
+    <workbookView xWindow="2328" yWindow="432" windowWidth="17256" windowHeight="10836" xr2:uid="{58E670A5-634C-427F-960F-9DA76C64E810}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="3" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="114">
   <si>
     <t>Tank number</t>
   </si>
@@ -376,99 +376,6 @@
     <t>no video, GoPro error</t>
   </si>
   <si>
-    <t>Trial</t>
-  </si>
-  <si>
-    <t>Tank</t>
-  </si>
-  <si>
-    <t>Video</t>
-  </si>
-  <si>
-    <t>Temp</t>
-  </si>
-  <si>
-    <t>Kelp</t>
-  </si>
-  <si>
-    <t>Treatment_numb</t>
-  </si>
-  <si>
-    <t>Cory_numb</t>
-  </si>
-  <si>
-    <t>Percent</t>
-  </si>
-  <si>
-    <t>Urchin_size</t>
-  </si>
-  <si>
-    <t>Urchin_wt_b</t>
-  </si>
-  <si>
-    <t>Urchin_wt_a</t>
-  </si>
-  <si>
-    <t>Urchin_age</t>
-  </si>
-  <si>
-    <t>Urchin_starve</t>
-  </si>
-  <si>
-    <t>Start</t>
-  </si>
-  <si>
-    <t>Stop</t>
-  </si>
-  <si>
-    <t>Kelp_b</t>
-  </si>
-  <si>
-    <t>Kelp_a</t>
-  </si>
-  <si>
-    <t>Visible_consumption</t>
-  </si>
-  <si>
-    <t>Time_to_kelp</t>
-  </si>
-  <si>
-    <t>Time_with_kelp</t>
-  </si>
-  <si>
-    <t>Numb_contact</t>
-  </si>
-  <si>
-    <t>Numb_deter</t>
-  </si>
-  <si>
-    <t>Numb_cross</t>
-  </si>
-  <si>
-    <t>Time_cross_first</t>
-  </si>
-  <si>
-    <t>Time_cross_avg</t>
-  </si>
-  <si>
-    <t>Total_video</t>
-  </si>
-  <si>
-    <t>Percent_alone</t>
-  </si>
-  <si>
-    <t>Percent_kelp</t>
-  </si>
-  <si>
-    <t>When_consumption</t>
-  </si>
-  <si>
-    <t>Urchin_deter</t>
-  </si>
-  <si>
-    <t>Urchin_deter_success</t>
-  </si>
-  <si>
     <t>Urchin was beast</t>
   </si>
 </sst>
@@ -552,10 +459,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="21" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -872,8 +779,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{168F7463-EB05-46FE-9A95-7790352FDB02}">
   <dimension ref="A1:D16240"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A41" sqref="A41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
@@ -890,10 +797,10 @@
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="16"/>
+      <c r="B3" s="17"/>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="2" t="s">
@@ -1075,10 +982,10 @@
       <c r="A26" s="2"/>
     </row>
     <row r="27" spans="1:4">
-      <c r="A27" s="16" t="s">
+      <c r="A27" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="B27" s="16"/>
+      <c r="B27" s="17"/>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="2" t="s">
@@ -49813,11 +49720,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD5E687B-43EE-4B00-8604-7EB9984510DD}">
-  <dimension ref="A1:AK77"/>
+  <dimension ref="A1:AJ77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AC1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="AE1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AH4" sqref="AH4"/>
+      <selection pane="bottomLeft" activeCell="AH9" sqref="AH9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
@@ -49855,14 +49762,14 @@
     <col min="31" max="31" width="19.109375" style="5" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="30.44140625" style="5" customWidth="1"/>
     <col min="33" max="33" width="22.44140625" style="5" customWidth="1"/>
-    <col min="34" max="35" width="23" style="5" customWidth="1"/>
-    <col min="36" max="36" width="10.109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="37" max="16384" width="8.77734375" style="5"/>
+    <col min="34" max="34" width="23" style="5" customWidth="1"/>
+    <col min="35" max="35" width="10.109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="36" max="16384" width="8.77734375" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" s="6" customFormat="1">
-      <c r="A1" s="6" t="s">
-        <v>113</v>
+    <row r="1" spans="1:36" s="6" customFormat="1">
+      <c r="A1" s="2" t="s">
+        <v>1</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>30</v>
@@ -49870,111 +49777,111 @@
       <c r="C1" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="D1" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="G1" s="6" t="s">
+      <c r="D1" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="H1" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="I1" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="J1" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="K1" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="L1" s="6" t="s">
-        <v>122</v>
-      </c>
-      <c r="M1" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="N1" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="O1" s="6" t="s">
-        <v>125</v>
-      </c>
-      <c r="P1" s="6" t="s">
-        <v>126</v>
-      </c>
-      <c r="Q1" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="R1" s="6" t="s">
-        <v>128</v>
-      </c>
-      <c r="S1" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="T1" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="U1" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="V1" s="6" t="s">
-        <v>131</v>
-      </c>
-      <c r="W1" s="6" t="s">
-        <v>132</v>
-      </c>
-      <c r="X1" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="Y1" s="6" t="s">
-        <v>134</v>
-      </c>
-      <c r="Z1" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="AA1" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="AB1" s="6" t="s">
-        <v>137</v>
-      </c>
-      <c r="AC1" s="6" t="s">
-        <v>138</v>
-      </c>
-      <c r="AD1" s="6" t="s">
-        <v>139</v>
-      </c>
-      <c r="AE1" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="AF1" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="AG1" s="6" t="s">
-        <v>142</v>
-      </c>
-      <c r="AH1" s="6" t="s">
-        <v>143</v>
+      <c r="H1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="W1" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="X1" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="Y1" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="Z1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AA1" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="AB1" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="AC1" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="AD1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="AE1" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="AF1" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="AG1" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="AH1" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="AI1" s="6" t="s">
+        <v>111</v>
       </c>
       <c r="AJ1" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="AK1" s="6" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="2" spans="1:37">
+    <row r="2" spans="1:36">
       <c r="A2" s="5">
         <v>1</v>
       </c>
-      <c r="B2" s="17">
+      <c r="B2" s="16">
         <v>43708</v>
       </c>
       <c r="C2" s="5">
@@ -50079,19 +49986,15 @@
         <v>Yes</v>
       </c>
       <c r="AH2" s="5" t="str">
-        <f>IF(AG2="Yes", IF(T2="yes", "Cory was close", "Cory was beast"), IF(T2="yes", "Urchin was beast", "Urchin never moved"))</f>
+        <f t="shared" ref="AH2:AH7" si="5">IF(AG2="Yes", IF(T2="yes", "Cory was close", "Cory was beast"), IF(T2="yes", "Urchin was beast", "Urchin never moved"))</f>
         <v>Cory was close</v>
       </c>
-      <c r="AI2" s="5" t="str">
-        <f>G2</f>
-        <v>Orange</v>
-      </c>
-    </row>
-    <row r="3" spans="1:37">
+    </row>
+    <row r="3" spans="1:36">
       <c r="A3" s="5">
         <v>2</v>
       </c>
-      <c r="B3" s="17">
+      <c r="B3" s="16">
         <v>43708</v>
       </c>
       <c r="C3" s="5">
@@ -50108,11 +50011,11 @@
         <v>35</v>
       </c>
       <c r="G3" s="5" t="str">
-        <f t="shared" ref="G3:G57" si="5">IF(I3&lt;=0, "Control", IF(I3&lt;=10, "Red", IF(I3&gt;=21, "Pink", "Orange")))</f>
+        <f t="shared" ref="G3:G57" si="6">IF(I3&lt;=0, "Control", IF(I3&lt;=10, "Red", IF(I3&gt;=21, "Pink", "Orange")))</f>
         <v>Orange</v>
       </c>
       <c r="H3" s="5">
-        <f t="shared" ref="H3:H57" si="6">IF(G3="Control", 1, IF(G3="Red", 2, IF(G3="Orange", 3, 4)))</f>
+        <f t="shared" ref="H3:H57" si="7">IF(G3="Control", 1, IF(G3="Red", 2, IF(G3="Orange", 3, 4)))</f>
         <v>3</v>
       </c>
       <c r="I3" s="7">
@@ -50182,22 +50085,18 @@
         <v>Yes</v>
       </c>
       <c r="AH3" s="5" t="str">
-        <f>IF(AG3="Yes", IF(T3="yes", "Cory was close", "Cory was beast"), IF(T3="yes", "Urchin was beast", "Urchin never moved"))</f>
+        <f t="shared" si="5"/>
         <v>Cory was beast</v>
       </c>
-      <c r="AI3" s="5" t="str">
-        <f>G3</f>
-        <v>Orange</v>
-      </c>
-      <c r="AJ3" s="5" t="s">
+      <c r="AI3" s="5" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="4" spans="1:37">
+    <row r="4" spans="1:36">
       <c r="A4" s="5">
         <v>3</v>
       </c>
-      <c r="B4" s="17">
+      <c r="B4" s="16">
         <v>43708</v>
       </c>
       <c r="C4" s="5">
@@ -50214,11 +50113,11 @@
         <v>36</v>
       </c>
       <c r="G4" s="5" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>Control</v>
       </c>
       <c r="H4" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="I4" s="7">
@@ -50298,22 +50197,18 @@
         <v>No</v>
       </c>
       <c r="AH4" s="5" t="str">
-        <f>IF(AG4="Yes", IF(T4="yes", "Cory was close", "Cory was beast"), IF(T4="yes", "Urchin was beast", "Urchin never moved"))</f>
+        <f t="shared" si="5"/>
         <v>Urchin was beast</v>
       </c>
-      <c r="AI4" s="5" t="str">
-        <f t="shared" ref="AI4:AI67" si="7">G4</f>
-        <v>Control</v>
-      </c>
-      <c r="AK4" s="5" t="s">
+      <c r="AJ4" s="5" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:37">
+    <row r="5" spans="1:36">
       <c r="A5" s="5">
         <v>4</v>
       </c>
-      <c r="B5" s="17">
+      <c r="B5" s="16">
         <v>43708</v>
       </c>
       <c r="C5" s="5">
@@ -50330,11 +50225,11 @@
         <v>35</v>
       </c>
       <c r="G5" s="5" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>Red</v>
       </c>
       <c r="H5" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
       <c r="I5" s="7">
@@ -50415,19 +50310,15 @@
         <v>Yes</v>
       </c>
       <c r="AH5" s="5" t="str">
-        <f>IF(AG5="Yes", IF(T5="yes", "Cory was close", "Cory was beast"), IF(T5="yes", "Urchin was beast", "Urchin never moved"))</f>
+        <f t="shared" si="5"/>
         <v>Cory was close</v>
       </c>
-      <c r="AI5" s="5" t="str">
-        <f t="shared" si="7"/>
-        <v>Red</v>
-      </c>
-    </row>
-    <row r="6" spans="1:37">
+    </row>
+    <row r="6" spans="1:36">
       <c r="A6" s="5">
         <v>5</v>
       </c>
-      <c r="B6" s="17">
+      <c r="B6" s="16">
         <v>43708</v>
       </c>
       <c r="C6" s="5">
@@ -50444,11 +50335,11 @@
         <v>35</v>
       </c>
       <c r="G6" s="5" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>Pink</v>
       </c>
       <c r="H6" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="I6" s="7">
@@ -50532,22 +50423,18 @@
         <v>No</v>
       </c>
       <c r="AH6" s="5" t="str">
-        <f>IF(AG6="Yes", IF(T6="yes", "Cory was close", "Cory was beast"), IF(T6="yes", "Urchin was beast", "Urchin never moved"))</f>
+        <f t="shared" si="5"/>
         <v>Urchin was beast</v>
       </c>
-      <c r="AI6" s="5" t="str">
-        <f t="shared" si="7"/>
-        <v>Pink</v>
-      </c>
-      <c r="AJ6" s="5" t="s">
+      <c r="AI6" s="5" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="7" spans="1:37">
+    <row r="7" spans="1:36">
       <c r="A7" s="5">
         <v>6</v>
       </c>
-      <c r="B7" s="17">
+      <c r="B7" s="16">
         <v>43708</v>
       </c>
       <c r="C7" s="5">
@@ -50564,11 +50451,11 @@
         <v>35</v>
       </c>
       <c r="G7" s="5" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>Orange</v>
       </c>
       <c r="H7" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>3</v>
       </c>
       <c r="I7" s="7">
@@ -50653,19 +50540,15 @@
         <v>Yes</v>
       </c>
       <c r="AH7" s="5" t="str">
-        <f>IF(AG7="Yes", IF(T7="yes", "Cory was close", "Cory was beast"), IF(T7="yes", "Urchin was beast", "Urchin never moved"))</f>
+        <f t="shared" si="5"/>
         <v>Cory was close</v>
       </c>
-      <c r="AI7" s="5" t="str">
-        <f t="shared" si="7"/>
-        <v>Orange</v>
-      </c>
-    </row>
-    <row r="8" spans="1:37">
+    </row>
+    <row r="8" spans="1:36">
       <c r="A8" s="5">
         <v>7</v>
       </c>
-      <c r="B8" s="17">
+      <c r="B8" s="16">
         <v>43708</v>
       </c>
       <c r="C8" s="5">
@@ -50682,11 +50565,11 @@
         <v>35</v>
       </c>
       <c r="G8" s="5" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>Orange</v>
       </c>
       <c r="H8" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>3</v>
       </c>
       <c r="I8" s="5">
@@ -50727,16 +50610,12 @@
         <f t="shared" si="1"/>
         <v>no</v>
       </c>
-      <c r="AI8" s="5" t="str">
-        <f t="shared" si="7"/>
-        <v>Orange</v>
-      </c>
-    </row>
-    <row r="9" spans="1:37">
+    </row>
+    <row r="9" spans="1:36">
       <c r="A9" s="5">
         <v>8</v>
       </c>
-      <c r="B9" s="17">
+      <c r="B9" s="16">
         <v>43708</v>
       </c>
       <c r="C9" s="5">
@@ -50753,11 +50632,11 @@
         <v>36</v>
       </c>
       <c r="G9" s="5" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>Pink</v>
       </c>
       <c r="H9" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="I9" s="7">
@@ -50798,16 +50677,12 @@
         <f t="shared" si="1"/>
         <v>no</v>
       </c>
-      <c r="AI9" s="5" t="str">
-        <f t="shared" si="7"/>
-        <v>Pink</v>
-      </c>
-    </row>
-    <row r="10" spans="1:37">
+    </row>
+    <row r="10" spans="1:36">
       <c r="A10" s="5">
         <v>9</v>
       </c>
-      <c r="B10" s="17">
+      <c r="B10" s="16">
         <v>43708</v>
       </c>
       <c r="C10" s="5">
@@ -50824,11 +50699,11 @@
         <v>35</v>
       </c>
       <c r="G10" s="5" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>Red</v>
       </c>
       <c r="H10" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
       <c r="I10" s="5">
@@ -50869,19 +50744,15 @@
         <f t="shared" si="1"/>
         <v>no</v>
       </c>
-      <c r="AI10" s="5" t="str">
-        <f t="shared" si="7"/>
-        <v>Red</v>
-      </c>
-      <c r="AJ10" s="5" t="s">
+      <c r="AI10" s="5" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="11" spans="1:37">
+    <row r="11" spans="1:36">
       <c r="A11" s="5">
         <v>10</v>
       </c>
-      <c r="B11" s="17">
+      <c r="B11" s="16">
         <v>43708</v>
       </c>
       <c r="C11" s="5">
@@ -50898,11 +50769,11 @@
         <v>36</v>
       </c>
       <c r="G11" s="5" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>Red</v>
       </c>
       <c r="H11" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
       <c r="I11" s="5">
@@ -50943,19 +50814,15 @@
         <f t="shared" si="1"/>
         <v>no</v>
       </c>
-      <c r="AI11" s="5" t="str">
-        <f t="shared" si="7"/>
-        <v>Red</v>
-      </c>
-      <c r="AJ11" s="5" t="s">
+      <c r="AI11" s="5" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="12" spans="1:37">
+    <row r="12" spans="1:36">
       <c r="A12" s="5">
         <v>11</v>
       </c>
-      <c r="B12" s="17">
+      <c r="B12" s="16">
         <v>43708</v>
       </c>
       <c r="C12" s="5">
@@ -50972,11 +50839,11 @@
         <v>35</v>
       </c>
       <c r="G12" s="5" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>Control</v>
       </c>
       <c r="H12" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="I12" s="5">
@@ -51017,19 +50884,15 @@
         <f t="shared" si="1"/>
         <v>no</v>
       </c>
-      <c r="AI12" s="5" t="str">
-        <f t="shared" si="7"/>
-        <v>Control</v>
-      </c>
-      <c r="AJ12" s="5" t="s">
+      <c r="AI12" s="5" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="13" spans="1:37">
+    <row r="13" spans="1:36">
       <c r="A13" s="5">
         <v>12</v>
       </c>
-      <c r="B13" s="17">
+      <c r="B13" s="16">
         <v>43708</v>
       </c>
       <c r="C13" s="5">
@@ -51046,11 +50909,11 @@
         <v>35</v>
       </c>
       <c r="G13" s="5" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>Orange</v>
       </c>
       <c r="H13" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>3</v>
       </c>
       <c r="I13" s="5">
@@ -51091,19 +50954,15 @@
         <f t="shared" si="1"/>
         <v>no</v>
       </c>
-      <c r="AI13" s="5" t="str">
-        <f t="shared" si="7"/>
-        <v>Orange</v>
-      </c>
-      <c r="AJ13" s="5" t="s">
+      <c r="AI13" s="5" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="14" spans="1:37">
+    <row r="14" spans="1:36">
       <c r="A14" s="5">
         <v>13</v>
       </c>
-      <c r="B14" s="17">
+      <c r="B14" s="16">
         <v>43708</v>
       </c>
       <c r="C14" s="5">
@@ -51120,11 +50979,11 @@
         <v>36</v>
       </c>
       <c r="G14" s="5" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>Control</v>
       </c>
       <c r="H14" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="I14" s="5">
@@ -51165,19 +51024,15 @@
         <f t="shared" si="1"/>
         <v>no</v>
       </c>
-      <c r="AI14" s="5" t="str">
-        <f t="shared" si="7"/>
-        <v>Control</v>
-      </c>
-      <c r="AJ14" s="5" t="s">
+      <c r="AI14" s="5" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="15" spans="1:37">
+    <row r="15" spans="1:36">
       <c r="A15" s="5">
         <v>14</v>
       </c>
-      <c r="B15" s="17">
+      <c r="B15" s="16">
         <v>43708</v>
       </c>
       <c r="C15" s="5">
@@ -51194,11 +51049,11 @@
         <v>36</v>
       </c>
       <c r="G15" s="5" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>Pink</v>
       </c>
       <c r="H15" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="I15" s="5">
@@ -51239,19 +51094,15 @@
         <f t="shared" si="1"/>
         <v>no</v>
       </c>
-      <c r="AI15" s="5" t="str">
-        <f t="shared" si="7"/>
-        <v>Pink</v>
-      </c>
-      <c r="AJ15" s="5" t="s">
+      <c r="AI15" s="5" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="16" spans="1:37">
+    <row r="16" spans="1:36">
       <c r="A16" s="5">
         <v>15</v>
       </c>
-      <c r="B16" s="17">
+      <c r="B16" s="16">
         <v>43709</v>
       </c>
       <c r="C16" s="5">
@@ -51268,11 +51119,11 @@
         <v>35</v>
       </c>
       <c r="G16" s="5" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>Red</v>
       </c>
       <c r="H16" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
       <c r="I16" s="7">
@@ -51345,19 +51196,15 @@
         <f>IF(AG16="Yes", IF(T16="yes", "Cory was close", "Cory was beast"), IF(T16="yes", "Urchin was beast", "Urchin never moved"))</f>
         <v>Urchin never moved</v>
       </c>
-      <c r="AI16" s="5" t="str">
-        <f t="shared" si="7"/>
-        <v>Red</v>
-      </c>
-      <c r="AK16" s="5" t="s">
+      <c r="AJ16" s="5" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="17" spans="1:37">
+    <row r="17" spans="1:36">
       <c r="A17" s="5">
         <v>16</v>
       </c>
-      <c r="B17" s="17">
+      <c r="B17" s="16">
         <v>43709</v>
       </c>
       <c r="C17" s="5">
@@ -51374,11 +51221,11 @@
         <v>36</v>
       </c>
       <c r="G17" s="5" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>Orange</v>
       </c>
       <c r="H17" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>3</v>
       </c>
       <c r="I17" s="7">
@@ -51462,19 +51309,15 @@
         <f>IF(AG17="Yes", IF(T17="yes", "Cory was close", "Cory was beast"), IF(T17="yes", "Urchin was beast", "Urchin never moved"))</f>
         <v>Urchin was beast</v>
       </c>
-      <c r="AI17" s="5" t="str">
-        <f t="shared" si="7"/>
-        <v>Orange</v>
-      </c>
-      <c r="AJ17" s="5" t="s">
+      <c r="AI17" s="5" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="1:37">
+    <row r="18" spans="1:36">
       <c r="A18" s="5">
         <v>17</v>
       </c>
-      <c r="B18" s="17">
+      <c r="B18" s="16">
         <v>43709</v>
       </c>
       <c r="C18" s="5">
@@ -51491,11 +51334,11 @@
         <v>35</v>
       </c>
       <c r="G18" s="5" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>Orange</v>
       </c>
       <c r="H18" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>3</v>
       </c>
       <c r="I18" s="7">
@@ -51579,24 +51422,20 @@
         <v>Yes</v>
       </c>
       <c r="AH18" s="5" t="s">
-        <v>144</v>
-      </c>
-      <c r="AI18" s="5" t="str">
-        <f t="shared" si="7"/>
-        <v>Orange</v>
+        <v>113</v>
+      </c>
+      <c r="AI18" s="5" t="s">
+        <v>51</v>
       </c>
       <c r="AJ18" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="AK18" s="5" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="19" spans="1:37">
+    <row r="19" spans="1:36">
       <c r="A19" s="5">
         <v>18</v>
       </c>
-      <c r="B19" s="17">
+      <c r="B19" s="16">
         <v>43709</v>
       </c>
       <c r="C19" s="5">
@@ -51613,11 +51452,11 @@
         <v>36</v>
       </c>
       <c r="G19" s="5" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>Control</v>
       </c>
       <c r="H19" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="I19" s="7">
@@ -51690,19 +51529,15 @@
         <f>IF(AG19="Yes", IF(T19="yes", "Cory was close", "Cory was beast"), IF(T19="yes", "Urchin was beast", "Urchin never moved"))</f>
         <v>Urchin never moved</v>
       </c>
-      <c r="AI19" s="5" t="str">
-        <f t="shared" si="7"/>
-        <v>Control</v>
-      </c>
-      <c r="AK19" s="5" t="s">
+      <c r="AJ19" s="5" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="20" spans="1:37">
+    <row r="20" spans="1:36">
       <c r="A20" s="5">
         <v>19</v>
       </c>
-      <c r="B20" s="17">
+      <c r="B20" s="16">
         <v>43709</v>
       </c>
       <c r="C20" s="5">
@@ -51719,11 +51554,11 @@
         <v>35</v>
       </c>
       <c r="G20" s="5" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>Pink</v>
       </c>
       <c r="H20" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="I20" s="7">
@@ -51806,16 +51641,12 @@
         <f>IF(AG20="Yes", IF(T20="yes", "Cory was close", "Cory was beast"), IF(T20="yes", "Urchin was beast", "Urchin never moved"))</f>
         <v>Cory was close</v>
       </c>
-      <c r="AI20" s="5" t="str">
-        <f t="shared" si="7"/>
-        <v>Pink</v>
-      </c>
-    </row>
-    <row r="21" spans="1:37">
+    </row>
+    <row r="21" spans="1:36">
       <c r="A21" s="5">
         <v>20</v>
       </c>
-      <c r="B21" s="17">
+      <c r="B21" s="16">
         <v>43709</v>
       </c>
       <c r="C21" s="5">
@@ -51832,11 +51663,11 @@
         <v>35</v>
       </c>
       <c r="G21" s="5" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>Red</v>
       </c>
       <c r="H21" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
       <c r="I21" s="7">
@@ -51909,16 +51740,12 @@
         <f>IF(AG21="Yes", IF(T21="yes", "Cory was close", "Cory was beast"), IF(T21="yes", "Urchin was beast", "Urchin never moved"))</f>
         <v>Cory was beast</v>
       </c>
-      <c r="AI21" s="5" t="str">
-        <f t="shared" si="7"/>
-        <v>Red</v>
-      </c>
-    </row>
-    <row r="22" spans="1:37">
+    </row>
+    <row r="22" spans="1:36">
       <c r="A22" s="5">
         <v>21</v>
       </c>
-      <c r="B22" s="17">
+      <c r="B22" s="16">
         <v>43709</v>
       </c>
       <c r="C22" s="5">
@@ -51935,11 +51762,11 @@
         <v>35</v>
       </c>
       <c r="G22" s="5" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>Pink</v>
       </c>
       <c r="H22" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="I22" s="7">
@@ -51980,16 +51807,12 @@
         <f t="shared" si="1"/>
         <v>no</v>
       </c>
-      <c r="AI22" s="5" t="str">
-        <f t="shared" si="7"/>
-        <v>Pink</v>
-      </c>
-    </row>
-    <row r="23" spans="1:37">
+    </row>
+    <row r="23" spans="1:36">
       <c r="A23" s="5">
         <v>22</v>
       </c>
-      <c r="B23" s="17">
+      <c r="B23" s="16">
         <v>43709</v>
       </c>
       <c r="C23" s="5">
@@ -52006,11 +51829,11 @@
         <v>36</v>
       </c>
       <c r="G23" s="5" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>Red</v>
       </c>
       <c r="H23" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
       <c r="I23" s="7">
@@ -52051,16 +51874,12 @@
         <f t="shared" si="1"/>
         <v>no</v>
       </c>
-      <c r="AI23" s="5" t="str">
-        <f t="shared" si="7"/>
-        <v>Red</v>
-      </c>
-    </row>
-    <row r="24" spans="1:37">
+    </row>
+    <row r="24" spans="1:36">
       <c r="A24" s="5">
         <v>23</v>
       </c>
-      <c r="B24" s="17">
+      <c r="B24" s="16">
         <v>43709</v>
       </c>
       <c r="C24" s="5">
@@ -52077,11 +51896,11 @@
         <v>35</v>
       </c>
       <c r="G24" s="5" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>Red</v>
       </c>
       <c r="H24" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
       <c r="I24" s="7">
@@ -52122,16 +51941,12 @@
         <f t="shared" si="1"/>
         <v>no</v>
       </c>
-      <c r="AI24" s="5" t="str">
-        <f t="shared" si="7"/>
-        <v>Red</v>
-      </c>
-    </row>
-    <row r="25" spans="1:37">
+    </row>
+    <row r="25" spans="1:36">
       <c r="A25" s="5">
         <v>24</v>
       </c>
-      <c r="B25" s="17">
+      <c r="B25" s="16">
         <v>43709</v>
       </c>
       <c r="C25" s="5">
@@ -52148,11 +51963,11 @@
         <v>35</v>
       </c>
       <c r="G25" s="5" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>Red</v>
       </c>
       <c r="H25" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
       <c r="I25" s="7">
@@ -52193,16 +52008,12 @@
         <f t="shared" si="1"/>
         <v>no</v>
       </c>
-      <c r="AI25" s="5" t="str">
-        <f t="shared" si="7"/>
-        <v>Red</v>
-      </c>
-    </row>
-    <row r="26" spans="1:37">
+    </row>
+    <row r="26" spans="1:36">
       <c r="A26" s="5">
         <v>25</v>
       </c>
-      <c r="B26" s="17">
+      <c r="B26" s="16">
         <v>43709</v>
       </c>
       <c r="C26" s="5">
@@ -52219,11 +52030,11 @@
         <v>36</v>
       </c>
       <c r="G26" s="5" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>Control</v>
       </c>
       <c r="H26" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="I26" s="7">
@@ -52265,16 +52076,12 @@
         <f t="shared" si="1"/>
         <v>no</v>
       </c>
-      <c r="AI26" s="5" t="str">
-        <f t="shared" si="7"/>
-        <v>Control</v>
-      </c>
-    </row>
-    <row r="27" spans="1:37">
+    </row>
+    <row r="27" spans="1:36">
       <c r="A27" s="5">
         <v>26</v>
       </c>
-      <c r="B27" s="17">
+      <c r="B27" s="16">
         <v>43709</v>
       </c>
       <c r="C27" s="5">
@@ -52291,11 +52098,11 @@
         <v>35</v>
       </c>
       <c r="G27" s="5" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>Pink</v>
       </c>
       <c r="H27" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="I27" s="7">
@@ -52336,16 +52143,12 @@
         <f t="shared" si="1"/>
         <v>no</v>
       </c>
-      <c r="AI27" s="5" t="str">
-        <f t="shared" si="7"/>
-        <v>Pink</v>
-      </c>
-    </row>
-    <row r="28" spans="1:37">
+    </row>
+    <row r="28" spans="1:36">
       <c r="A28" s="5">
         <v>27</v>
       </c>
-      <c r="B28" s="17">
+      <c r="B28" s="16">
         <v>43709</v>
       </c>
       <c r="C28" s="5">
@@ -52362,11 +52165,11 @@
         <v>35</v>
       </c>
       <c r="G28" s="5" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>Orange</v>
       </c>
       <c r="H28" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>3</v>
       </c>
       <c r="I28" s="7">
@@ -52407,16 +52210,12 @@
         <f t="shared" si="1"/>
         <v>no</v>
       </c>
-      <c r="AI28" s="5" t="str">
-        <f t="shared" si="7"/>
-        <v>Orange</v>
-      </c>
-    </row>
-    <row r="29" spans="1:37">
+    </row>
+    <row r="29" spans="1:36">
       <c r="A29" s="5">
         <v>28</v>
       </c>
-      <c r="B29" s="17">
+      <c r="B29" s="16">
         <v>43709</v>
       </c>
       <c r="C29" s="5">
@@ -52433,11 +52232,11 @@
         <v>36</v>
       </c>
       <c r="G29" s="5" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>Control</v>
       </c>
       <c r="H29" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="I29" s="7">
@@ -52478,16 +52277,12 @@
         <f t="shared" si="1"/>
         <v>no</v>
       </c>
-      <c r="AI29" s="5" t="str">
-        <f t="shared" si="7"/>
-        <v>Control</v>
-      </c>
-    </row>
-    <row r="30" spans="1:37">
+    </row>
+    <row r="30" spans="1:36">
       <c r="A30" s="5">
         <v>29</v>
       </c>
-      <c r="B30" s="17">
+      <c r="B30" s="16">
         <v>43710</v>
       </c>
       <c r="C30" s="5">
@@ -52504,11 +52299,11 @@
         <v>36</v>
       </c>
       <c r="G30" s="5" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>Control</v>
       </c>
       <c r="H30" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="I30" s="7">
@@ -52592,19 +52387,15 @@
         <f>IF(AG30="Yes", IF(T30="yes", "Cory was close", "Cory was beast"), IF(T30="yes", "Urchin was beast", "Urchin never moved"))</f>
         <v>Urchin was beast</v>
       </c>
-      <c r="AI30" s="5" t="str">
-        <f t="shared" si="7"/>
-        <v>Control</v>
-      </c>
-      <c r="AK30" s="5" t="s">
+      <c r="AJ30" s="5" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="31" spans="1:37">
+    <row r="31" spans="1:36">
       <c r="A31" s="5">
         <v>30</v>
       </c>
-      <c r="B31" s="17">
+      <c r="B31" s="16">
         <v>43710</v>
       </c>
       <c r="C31" s="5">
@@ -52621,11 +52412,11 @@
         <v>36</v>
       </c>
       <c r="G31" s="5" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>Pink</v>
       </c>
       <c r="H31" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="I31" s="7">
@@ -52708,16 +52499,12 @@
         <f>IF(AG31="Yes", IF(T31="yes", "Cory was close", "Cory was beast"), IF(T31="yes", "Urchin was beast", "Urchin never moved"))</f>
         <v>Urchin was beast</v>
       </c>
-      <c r="AI31" s="5" t="str">
-        <f t="shared" si="7"/>
-        <v>Pink</v>
-      </c>
-    </row>
-    <row r="32" spans="1:37">
+    </row>
+    <row r="32" spans="1:36">
       <c r="A32" s="5">
         <v>31</v>
       </c>
-      <c r="B32" s="17">
+      <c r="B32" s="16">
         <v>43710</v>
       </c>
       <c r="C32" s="5">
@@ -52734,11 +52521,11 @@
         <v>36</v>
       </c>
       <c r="G32" s="5" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>Red</v>
       </c>
       <c r="H32" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
       <c r="I32" s="7">
@@ -52821,19 +52608,15 @@
         <f>IF(AG32="Yes", IF(T32="yes", "Cory was close", "Cory was beast"), IF(T32="yes", "Urchin was beast", "Urchin never moved"))</f>
         <v>Cory was close</v>
       </c>
-      <c r="AI32" s="5" t="str">
-        <f t="shared" si="7"/>
-        <v>Red</v>
-      </c>
-      <c r="AK32" s="5" t="s">
+      <c r="AJ32" s="5" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="33" spans="1:37">
+    <row r="33" spans="1:36">
       <c r="A33" s="5">
         <v>32</v>
       </c>
-      <c r="B33" s="17">
+      <c r="B33" s="16">
         <v>43710</v>
       </c>
       <c r="C33" s="5">
@@ -52850,11 +52633,11 @@
         <v>36</v>
       </c>
       <c r="G33" s="5" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>Orange</v>
       </c>
       <c r="H33" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>3</v>
       </c>
       <c r="I33" s="7">
@@ -52927,19 +52710,15 @@
         <f>IF(AG33="Yes", IF(T33="yes", "Cory was close", "Cory was beast"), IF(T33="yes", "Urchin was beast", "Urchin never moved"))</f>
         <v>Urchin never moved</v>
       </c>
-      <c r="AI33" s="5" t="str">
-        <f t="shared" si="7"/>
-        <v>Orange</v>
-      </c>
-      <c r="AK33" s="5" t="s">
+      <c r="AJ33" s="5" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="34" spans="1:37">
+    <row r="34" spans="1:36">
       <c r="A34" s="5">
         <v>33</v>
       </c>
-      <c r="B34" s="17">
+      <c r="B34" s="16">
         <v>43710</v>
       </c>
       <c r="C34" s="5">
@@ -52956,11 +52735,11 @@
         <v>35</v>
       </c>
       <c r="G34" s="5" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>Orange</v>
       </c>
       <c r="H34" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>3</v>
       </c>
       <c r="I34" s="7">
@@ -53045,16 +52824,12 @@
         <f>IF(AG34="Yes", IF(T34="yes", "Cory was close", "Cory was beast"), IF(T34="yes", "Urchin was beast", "Urchin never moved"))</f>
         <v>Urchin was beast</v>
       </c>
-      <c r="AI34" s="5" t="str">
-        <f t="shared" si="7"/>
-        <v>Orange</v>
-      </c>
-    </row>
-    <row r="35" spans="1:37">
+    </row>
+    <row r="35" spans="1:36">
       <c r="A35" s="5">
         <v>34</v>
       </c>
-      <c r="B35" s="17">
+      <c r="B35" s="16">
         <v>43710</v>
       </c>
       <c r="C35" s="5">
@@ -53071,11 +52846,11 @@
         <v>35</v>
       </c>
       <c r="G35" s="5" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>Red</v>
       </c>
       <c r="H35" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
       <c r="I35" s="7">
@@ -53155,21 +52930,17 @@
         <v>Yes</v>
       </c>
       <c r="AH35" s="5" t="s">
-        <v>144</v>
-      </c>
-      <c r="AI35" s="5" t="str">
-        <f t="shared" si="7"/>
-        <v>Red</v>
-      </c>
-      <c r="AK35" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="AJ35" s="5" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="36" spans="1:37">
+    <row r="36" spans="1:36">
       <c r="A36" s="5">
         <v>35</v>
       </c>
-      <c r="B36" s="17">
+      <c r="B36" s="16">
         <v>43710</v>
       </c>
       <c r="C36" s="5">
@@ -53186,11 +52957,11 @@
         <v>36</v>
       </c>
       <c r="G36" s="5" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>Control</v>
       </c>
       <c r="H36" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="I36" s="7">
@@ -53231,16 +53002,12 @@
         <f t="shared" si="1"/>
         <v>no</v>
       </c>
-      <c r="AI36" s="5" t="str">
-        <f t="shared" si="7"/>
-        <v>Control</v>
-      </c>
-    </row>
-    <row r="37" spans="1:37">
+    </row>
+    <row r="37" spans="1:36">
       <c r="A37" s="5">
         <v>36</v>
       </c>
-      <c r="B37" s="17">
+      <c r="B37" s="16">
         <v>43710</v>
       </c>
       <c r="C37" s="5">
@@ -53257,11 +53024,11 @@
         <v>36</v>
       </c>
       <c r="G37" s="5" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>Control</v>
       </c>
       <c r="H37" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="I37" s="7">
@@ -53302,16 +53069,12 @@
         <f t="shared" si="1"/>
         <v>no</v>
       </c>
-      <c r="AI37" s="5" t="str">
-        <f t="shared" si="7"/>
-        <v>Control</v>
-      </c>
-    </row>
-    <row r="38" spans="1:37">
+    </row>
+    <row r="38" spans="1:36">
       <c r="A38" s="5">
         <v>37</v>
       </c>
-      <c r="B38" s="17">
+      <c r="B38" s="16">
         <v>43710</v>
       </c>
       <c r="C38" s="5">
@@ -53328,11 +53091,11 @@
         <v>36</v>
       </c>
       <c r="G38" s="5" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>Orange</v>
       </c>
       <c r="H38" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>3</v>
       </c>
       <c r="I38" s="7">
@@ -53374,16 +53137,12 @@
         <f t="shared" si="1"/>
         <v>no</v>
       </c>
-      <c r="AI38" s="5" t="str">
-        <f t="shared" si="7"/>
-        <v>Orange</v>
-      </c>
-    </row>
-    <row r="39" spans="1:37">
+    </row>
+    <row r="39" spans="1:36">
       <c r="A39" s="5">
         <v>38</v>
       </c>
-      <c r="B39" s="17">
+      <c r="B39" s="16">
         <v>43710</v>
       </c>
       <c r="C39" s="5">
@@ -53400,11 +53159,11 @@
         <v>36</v>
       </c>
       <c r="G39" s="5" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>Orange</v>
       </c>
       <c r="H39" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>3</v>
       </c>
       <c r="I39" s="7">
@@ -53445,16 +53204,12 @@
         <f t="shared" si="1"/>
         <v>no</v>
       </c>
-      <c r="AI39" s="5" t="str">
-        <f t="shared" si="7"/>
-        <v>Orange</v>
-      </c>
-    </row>
-    <row r="40" spans="1:37">
+    </row>
+    <row r="40" spans="1:36">
       <c r="A40" s="5">
         <v>39</v>
       </c>
-      <c r="B40" s="17">
+      <c r="B40" s="16">
         <v>43710</v>
       </c>
       <c r="C40" s="5">
@@ -53471,11 +53226,11 @@
         <v>35</v>
       </c>
       <c r="G40" s="5" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>Pink</v>
       </c>
       <c r="H40" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="I40" s="7">
@@ -53516,16 +53271,12 @@
         <f t="shared" si="1"/>
         <v>no</v>
       </c>
-      <c r="AI40" s="5" t="str">
-        <f t="shared" si="7"/>
-        <v>Pink</v>
-      </c>
-    </row>
-    <row r="41" spans="1:37">
+    </row>
+    <row r="41" spans="1:36">
       <c r="A41" s="5">
         <v>40</v>
       </c>
-      <c r="B41" s="17">
+      <c r="B41" s="16">
         <v>43710</v>
       </c>
       <c r="C41" s="5">
@@ -53542,11 +53293,11 @@
         <v>35</v>
       </c>
       <c r="G41" s="5" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>Red</v>
       </c>
       <c r="H41" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
       <c r="I41" s="7">
@@ -53588,16 +53339,12 @@
         <f t="shared" si="1"/>
         <v>no</v>
       </c>
-      <c r="AI41" s="5" t="str">
-        <f t="shared" si="7"/>
-        <v>Red</v>
-      </c>
-    </row>
-    <row r="42" spans="1:37">
+    </row>
+    <row r="42" spans="1:36">
       <c r="A42" s="5">
         <v>41</v>
       </c>
-      <c r="B42" s="17">
+      <c r="B42" s="16">
         <v>43710</v>
       </c>
       <c r="C42" s="5">
@@ -53614,11 +53361,11 @@
         <v>36</v>
       </c>
       <c r="G42" s="5" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>Pink</v>
       </c>
       <c r="H42" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="I42" s="7">
@@ -53659,16 +53406,12 @@
         <f t="shared" si="1"/>
         <v>no</v>
       </c>
-      <c r="AI42" s="5" t="str">
-        <f t="shared" si="7"/>
-        <v>Pink</v>
-      </c>
-    </row>
-    <row r="43" spans="1:37">
+    </row>
+    <row r="43" spans="1:36">
       <c r="A43" s="5">
         <v>42</v>
       </c>
-      <c r="B43" s="17">
+      <c r="B43" s="16">
         <v>43710</v>
       </c>
       <c r="C43" s="5">
@@ -53685,11 +53428,11 @@
         <v>35</v>
       </c>
       <c r="G43" s="5" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>Orange</v>
       </c>
       <c r="H43" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>3</v>
       </c>
       <c r="I43" s="7">
@@ -53730,19 +53473,15 @@
         <f t="shared" si="1"/>
         <v>no</v>
       </c>
-      <c r="AI43" s="5" t="str">
-        <f t="shared" si="7"/>
-        <v>Orange</v>
-      </c>
-      <c r="AJ43" s="5" t="s">
+      <c r="AI43" s="5" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="44" spans="1:37">
+    <row r="44" spans="1:36">
       <c r="A44" s="5">
         <v>43</v>
       </c>
-      <c r="B44" s="17">
+      <c r="B44" s="16">
         <v>43711</v>
       </c>
       <c r="C44" s="5">
@@ -53759,11 +53498,11 @@
         <v>36</v>
       </c>
       <c r="G44" s="5" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>Red</v>
       </c>
       <c r="H44" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
       <c r="I44" s="7">
@@ -53845,16 +53584,12 @@
         <f>IF(AG44="Yes", IF(T44="yes", "Cory was close", "Cory was beast"), IF(T44="yes", "Urchin was beast", "Urchin never moved"))</f>
         <v>Urchin was beast</v>
       </c>
-      <c r="AI44" s="5" t="str">
-        <f t="shared" si="7"/>
-        <v>Red</v>
-      </c>
-    </row>
-    <row r="45" spans="1:37">
+    </row>
+    <row r="45" spans="1:36">
       <c r="A45" s="5">
         <v>44</v>
       </c>
-      <c r="B45" s="17">
+      <c r="B45" s="16">
         <v>43711</v>
       </c>
       <c r="C45" s="5">
@@ -53871,11 +53606,11 @@
         <v>35</v>
       </c>
       <c r="G45" s="5" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>Pink</v>
       </c>
       <c r="H45" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="I45" s="7">
@@ -53961,16 +53696,12 @@
         <f>IF(AG45="Yes", IF(T45="yes", "Cory was close", "Cory was beast"), IF(T45="yes", "Urchin was beast", "Urchin never moved"))</f>
         <v>Cory was close</v>
       </c>
-      <c r="AI45" s="5" t="str">
-        <f t="shared" si="7"/>
-        <v>Pink</v>
-      </c>
-    </row>
-    <row r="46" spans="1:37">
+    </row>
+    <row r="46" spans="1:36">
       <c r="A46" s="5">
         <v>45</v>
       </c>
-      <c r="B46" s="17">
+      <c r="B46" s="16">
         <v>43711</v>
       </c>
       <c r="C46" s="5">
@@ -53987,11 +53718,11 @@
         <v>35</v>
       </c>
       <c r="G46" s="5" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>Red</v>
       </c>
       <c r="H46" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
       <c r="I46" s="7">
@@ -54063,19 +53794,15 @@
         <f>IF(AG46="Yes", IF(T46="yes", "Cory was close", "Cory was beast"), IF(T46="yes", "Urchin was beast", "Urchin never moved"))</f>
         <v>Urchin never moved</v>
       </c>
-      <c r="AI46" s="5" t="str">
-        <f t="shared" si="7"/>
-        <v>Red</v>
-      </c>
-      <c r="AK46" s="5" t="s">
+      <c r="AJ46" s="5" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="47" spans="1:37">
+    <row r="47" spans="1:36">
       <c r="A47" s="5">
         <v>46</v>
       </c>
-      <c r="B47" s="17">
+      <c r="B47" s="16">
         <v>43711</v>
       </c>
       <c r="C47" s="5">
@@ -54092,11 +53819,11 @@
         <v>36</v>
       </c>
       <c r="G47" s="5" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>Orange</v>
       </c>
       <c r="H47" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>3</v>
       </c>
       <c r="I47" s="7">
@@ -54140,19 +53867,15 @@
         <f>IF(AG47="Yes", IF(T47="yes", "Cory was close", "Cory was beast"), IF(T47="yes", "Urchin was beast", "Urchin never moved"))</f>
         <v>Urchin never moved</v>
       </c>
-      <c r="AI47" s="5" t="str">
-        <f t="shared" si="7"/>
-        <v>Orange</v>
-      </c>
-      <c r="AJ47" s="5" t="s">
+      <c r="AI47" s="5" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="48" spans="1:37">
+    <row r="48" spans="1:36">
       <c r="A48" s="5">
         <v>47</v>
       </c>
-      <c r="B48" s="17">
+      <c r="B48" s="16">
         <v>43711</v>
       </c>
       <c r="C48" s="5">
@@ -54169,11 +53892,11 @@
         <v>35</v>
       </c>
       <c r="G48" s="5" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>Control</v>
       </c>
       <c r="H48" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="I48" s="7">
@@ -54253,24 +53976,20 @@
         <v>No</v>
       </c>
       <c r="AH48" s="5" t="s">
-        <v>144</v>
-      </c>
-      <c r="AI48" s="5" t="str">
-        <f t="shared" si="7"/>
-        <v>Control</v>
+        <v>113</v>
+      </c>
+      <c r="AI48" s="5" t="s">
+        <v>69</v>
       </c>
       <c r="AJ48" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="AK48" s="5" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="49" spans="1:37">
+    <row r="49" spans="1:36">
       <c r="A49" s="5">
         <v>48</v>
       </c>
-      <c r="B49" s="17">
+      <c r="B49" s="16">
         <v>43711</v>
       </c>
       <c r="C49" s="5">
@@ -54287,11 +54006,11 @@
         <v>35</v>
       </c>
       <c r="G49" s="5" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>Pink</v>
       </c>
       <c r="H49" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="I49" s="7">
@@ -54363,19 +54082,15 @@
         <f>IF(AG49="Yes", IF(T49="yes", "Cory was close", "Cory was beast"), IF(T49="yes", "Urchin was beast", "Urchin never moved"))</f>
         <v>Urchin never moved</v>
       </c>
-      <c r="AI49" s="5" t="str">
-        <f t="shared" si="7"/>
-        <v>Pink</v>
-      </c>
-      <c r="AK49" s="5" t="s">
+      <c r="AJ49" s="5" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="50" spans="1:37">
+    <row r="50" spans="1:36">
       <c r="A50" s="5">
         <v>49</v>
       </c>
-      <c r="B50" s="17">
+      <c r="B50" s="16">
         <v>43711</v>
       </c>
       <c r="C50" s="5">
@@ -54392,11 +54107,11 @@
         <v>35</v>
       </c>
       <c r="G50" s="5" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>Pink</v>
       </c>
       <c r="H50" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="I50" s="7">
@@ -54437,19 +54152,15 @@
         <f t="shared" si="18"/>
         <v>no</v>
       </c>
-      <c r="AI50" s="5" t="str">
-        <f t="shared" si="7"/>
-        <v>Pink</v>
-      </c>
-      <c r="AJ50" s="5" t="s">
+      <c r="AI50" s="5" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="51" spans="1:37">
+    <row r="51" spans="1:36">
       <c r="A51" s="5">
         <v>50</v>
       </c>
-      <c r="B51" s="17">
+      <c r="B51" s="16">
         <v>43711</v>
       </c>
       <c r="C51" s="5">
@@ -54466,11 +54177,11 @@
         <v>36</v>
       </c>
       <c r="G51" s="5" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>Pink</v>
       </c>
       <c r="H51" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="I51" s="7">
@@ -54510,16 +54221,12 @@
         <f t="shared" si="18"/>
         <v>no</v>
       </c>
-      <c r="AI51" s="5" t="str">
-        <f t="shared" si="7"/>
-        <v>Pink</v>
-      </c>
-    </row>
-    <row r="52" spans="1:37">
+    </row>
+    <row r="52" spans="1:36">
       <c r="A52" s="5">
         <v>51</v>
       </c>
-      <c r="B52" s="17">
+      <c r="B52" s="16">
         <v>43711</v>
       </c>
       <c r="C52" s="5">
@@ -54536,11 +54243,11 @@
         <v>35</v>
       </c>
       <c r="G52" s="5" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>Orange</v>
       </c>
       <c r="H52" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>3</v>
       </c>
       <c r="I52" s="7">
@@ -54581,16 +54288,12 @@
         <f t="shared" si="18"/>
         <v>no</v>
       </c>
-      <c r="AI52" s="5" t="str">
-        <f t="shared" si="7"/>
-        <v>Orange</v>
-      </c>
-    </row>
-    <row r="53" spans="1:37">
+    </row>
+    <row r="53" spans="1:36">
       <c r="A53" s="5">
         <v>52</v>
       </c>
-      <c r="B53" s="17">
+      <c r="B53" s="16">
         <v>43711</v>
       </c>
       <c r="C53" s="5">
@@ -54607,11 +54310,11 @@
         <v>36</v>
       </c>
       <c r="G53" s="5" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>Orange</v>
       </c>
       <c r="H53" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>3</v>
       </c>
       <c r="I53" s="7">
@@ -54652,16 +54355,12 @@
         <f t="shared" si="18"/>
         <v>no</v>
       </c>
-      <c r="AI53" s="5" t="str">
-        <f t="shared" si="7"/>
-        <v>Orange</v>
-      </c>
-    </row>
-    <row r="54" spans="1:37">
+    </row>
+    <row r="54" spans="1:36">
       <c r="A54" s="5">
         <v>53</v>
       </c>
-      <c r="B54" s="17">
+      <c r="B54" s="16">
         <v>43711</v>
       </c>
       <c r="C54" s="5">
@@ -54678,11 +54377,11 @@
         <v>35</v>
       </c>
       <c r="G54" s="5" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>Pink</v>
       </c>
       <c r="H54" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="I54" s="7">
@@ -54723,16 +54422,12 @@
         <f t="shared" si="18"/>
         <v>no</v>
       </c>
-      <c r="AI54" s="5" t="str">
-        <f t="shared" si="7"/>
-        <v>Pink</v>
-      </c>
-    </row>
-    <row r="55" spans="1:37">
+    </row>
+    <row r="55" spans="1:36">
       <c r="A55" s="5">
         <v>54</v>
       </c>
-      <c r="B55" s="17">
+      <c r="B55" s="16">
         <v>43711</v>
       </c>
       <c r="C55" s="5">
@@ -54749,11 +54444,11 @@
         <v>35</v>
       </c>
       <c r="G55" s="5" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>Control</v>
       </c>
       <c r="H55" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="I55" s="7">
@@ -54793,16 +54488,12 @@
         <f t="shared" si="18"/>
         <v>no</v>
       </c>
-      <c r="AI55" s="5" t="str">
-        <f t="shared" si="7"/>
-        <v>Control</v>
-      </c>
-    </row>
-    <row r="56" spans="1:37">
+    </row>
+    <row r="56" spans="1:36">
       <c r="A56" s="5">
         <v>55</v>
       </c>
-      <c r="B56" s="17">
+      <c r="B56" s="16">
         <v>43711</v>
       </c>
       <c r="C56" s="5">
@@ -54819,11 +54510,11 @@
         <v>35</v>
       </c>
       <c r="G56" s="5" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>Control</v>
       </c>
       <c r="H56" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="I56" s="7">
@@ -54864,16 +54555,12 @@
         <f t="shared" si="18"/>
         <v>no</v>
       </c>
-      <c r="AI56" s="5" t="str">
-        <f t="shared" si="7"/>
-        <v>Control</v>
-      </c>
-    </row>
-    <row r="57" spans="1:37">
+    </row>
+    <row r="57" spans="1:36">
       <c r="A57" s="5">
         <v>56</v>
       </c>
-      <c r="B57" s="17">
+      <c r="B57" s="16">
         <v>43711</v>
       </c>
       <c r="C57" s="5">
@@ -54890,11 +54577,11 @@
         <v>35</v>
       </c>
       <c r="G57" s="5" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>Red</v>
       </c>
       <c r="H57" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
       <c r="I57" s="7">
@@ -54935,16 +54622,12 @@
         <f t="shared" si="18"/>
         <v>no</v>
       </c>
-      <c r="AI57" s="5" t="str">
-        <f t="shared" si="7"/>
-        <v>Red</v>
-      </c>
-    </row>
-    <row r="58" spans="1:37">
+    </row>
+    <row r="58" spans="1:36">
       <c r="A58" s="5">
         <v>57</v>
       </c>
-      <c r="B58" s="17">
+      <c r="B58" s="16">
         <v>43712</v>
       </c>
       <c r="C58" s="5">
@@ -55006,16 +54689,12 @@
         <f t="shared" si="18"/>
         <v>no</v>
       </c>
-      <c r="AI58" s="5" t="str">
-        <f t="shared" si="7"/>
-        <v>Red</v>
-      </c>
-    </row>
-    <row r="59" spans="1:37">
+    </row>
+    <row r="59" spans="1:36">
       <c r="A59" s="5">
         <v>58</v>
       </c>
-      <c r="B59" s="17">
+      <c r="B59" s="16">
         <v>43712</v>
       </c>
       <c r="C59" s="5">
@@ -55078,16 +54757,12 @@
         <f t="shared" si="18"/>
         <v>no</v>
       </c>
-      <c r="AI59" s="5" t="str">
-        <f t="shared" si="7"/>
-        <v>Control</v>
-      </c>
-    </row>
-    <row r="60" spans="1:37">
+    </row>
+    <row r="60" spans="1:36">
       <c r="A60" s="5">
         <v>59</v>
       </c>
-      <c r="B60" s="17">
+      <c r="B60" s="16">
         <v>43712</v>
       </c>
       <c r="C60" s="5">
@@ -55149,16 +54824,12 @@
         <f t="shared" si="18"/>
         <v>no</v>
       </c>
-      <c r="AI60" s="5" t="str">
-        <f t="shared" si="7"/>
-        <v>Pink</v>
-      </c>
-    </row>
-    <row r="61" spans="1:37">
+    </row>
+    <row r="61" spans="1:36">
       <c r="A61" s="5">
         <v>60</v>
       </c>
-      <c r="B61" s="17">
+      <c r="B61" s="16">
         <v>43712</v>
       </c>
       <c r="C61" s="5">
@@ -55220,16 +54891,12 @@
         <f t="shared" si="18"/>
         <v>no</v>
       </c>
-      <c r="AI61" s="5" t="str">
-        <f t="shared" si="7"/>
-        <v>Red</v>
-      </c>
-    </row>
-    <row r="62" spans="1:37">
+    </row>
+    <row r="62" spans="1:36">
       <c r="A62" s="5">
         <v>61</v>
       </c>
-      <c r="B62" s="17">
+      <c r="B62" s="16">
         <v>43712</v>
       </c>
       <c r="C62" s="5">
@@ -55292,16 +54959,12 @@
         <f t="shared" si="18"/>
         <v>no</v>
       </c>
-      <c r="AI62" s="5" t="str">
-        <f t="shared" si="7"/>
-        <v>Orange</v>
-      </c>
-    </row>
-    <row r="63" spans="1:37">
+    </row>
+    <row r="63" spans="1:36">
       <c r="A63" s="5">
         <v>62</v>
       </c>
-      <c r="B63" s="17">
+      <c r="B63" s="16">
         <v>43712</v>
       </c>
       <c r="C63" s="5">
@@ -55364,16 +55027,12 @@
         <f t="shared" si="18"/>
         <v>no</v>
       </c>
-      <c r="AI63" s="5" t="str">
-        <f t="shared" si="7"/>
-        <v>Orange</v>
-      </c>
-    </row>
-    <row r="64" spans="1:37">
+    </row>
+    <row r="64" spans="1:36">
       <c r="A64" s="5">
         <v>63</v>
       </c>
-      <c r="B64" s="17">
+      <c r="B64" s="16">
         <v>43712</v>
       </c>
       <c r="C64" s="5">
@@ -55436,16 +55095,12 @@
         <f t="shared" si="18"/>
         <v>no</v>
       </c>
-      <c r="AI64" s="5" t="str">
-        <f t="shared" si="7"/>
-        <v>Control</v>
-      </c>
-    </row>
-    <row r="65" spans="1:37">
+    </row>
+    <row r="65" spans="1:36">
       <c r="A65" s="5">
         <v>64</v>
       </c>
-      <c r="B65" s="17">
+      <c r="B65" s="16">
         <v>43712</v>
       </c>
       <c r="C65" s="5">
@@ -55507,19 +55162,15 @@
         <f t="shared" si="18"/>
         <v>no</v>
       </c>
-      <c r="AI65" s="5" t="str">
-        <f t="shared" si="7"/>
-        <v>Red</v>
-      </c>
-      <c r="AJ65" s="5" t="s">
+      <c r="AI65" s="5" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="66" spans="1:37">
+    <row r="66" spans="1:36">
       <c r="A66" s="5">
         <v>65</v>
       </c>
-      <c r="B66" s="17">
+      <c r="B66" s="16">
         <v>43713</v>
       </c>
       <c r="C66" s="5">
@@ -55614,19 +55265,15 @@
         <f>IF(AG66="Yes", IF(T66="yes", "Cory was close", "Cory was beast"), IF(T66="yes", "Urchin was beast", "Urchin never moved"))</f>
         <v>Urchin was beast</v>
       </c>
-      <c r="AI66" s="5" t="str">
-        <f t="shared" si="7"/>
-        <v>Control</v>
-      </c>
-      <c r="AK66" s="5" t="s">
+      <c r="AJ66" s="5" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="67" spans="1:37">
+    <row r="67" spans="1:36">
       <c r="A67" s="5">
         <v>66</v>
       </c>
-      <c r="B67" s="17">
+      <c r="B67" s="16">
         <v>43713</v>
       </c>
       <c r="C67" s="5">
@@ -55730,19 +55377,15 @@
         <f t="shared" ref="AH67:AH77" si="26">IF(AG67="Yes", IF(T67="yes", "Cory was close", "Cory was beast"), IF(T67="yes", "Urchin was beast", "Urchin never moved"))</f>
         <v>Urchin was beast</v>
       </c>
-      <c r="AI67" s="5" t="str">
-        <f t="shared" si="7"/>
-        <v>Orange</v>
-      </c>
-      <c r="AK67" s="5" t="s">
+      <c r="AJ67" s="5" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="68" spans="1:37">
+    <row r="68" spans="1:36">
       <c r="A68" s="5">
         <v>67</v>
       </c>
-      <c r="B68" s="17">
+      <c r="B68" s="16">
         <v>43713</v>
       </c>
       <c r="C68" s="5">
@@ -55836,22 +55479,18 @@
         <f t="shared" si="26"/>
         <v>Cory was beast</v>
       </c>
-      <c r="AI68" s="5" t="str">
-        <f t="shared" ref="AI68:AI77" si="27">G68</f>
-        <v>Pink</v>
+      <c r="AI68" s="5" t="s">
+        <v>68</v>
       </c>
       <c r="AJ68" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="AK68" s="5" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="69" spans="1:37">
+    <row r="69" spans="1:36">
       <c r="A69" s="5">
         <v>68</v>
       </c>
-      <c r="B69" s="17">
+      <c r="B69" s="16">
         <v>43713</v>
       </c>
       <c r="C69" s="5">
@@ -55956,16 +55595,12 @@
         <f t="shared" si="26"/>
         <v>Cory was close</v>
       </c>
-      <c r="AI69" s="5" t="str">
-        <f t="shared" si="27"/>
-        <v>Pink</v>
-      </c>
-    </row>
-    <row r="70" spans="1:37">
+    </row>
+    <row r="70" spans="1:36">
       <c r="A70" s="5">
         <v>69</v>
       </c>
-      <c r="B70" s="17">
+      <c r="B70" s="16">
         <v>43713</v>
       </c>
       <c r="C70" s="5">
@@ -56059,19 +55694,15 @@
         <f t="shared" si="26"/>
         <v>Urchin never moved</v>
       </c>
-      <c r="AI70" s="5" t="str">
-        <f t="shared" si="27"/>
-        <v>Pink</v>
-      </c>
-      <c r="AK70" s="5" t="s">
+      <c r="AJ70" s="5" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="71" spans="1:37">
+    <row r="71" spans="1:36">
       <c r="A71" s="5">
         <v>70</v>
       </c>
-      <c r="B71" s="17">
+      <c r="B71" s="16">
         <v>43713</v>
       </c>
       <c r="C71" s="5">
@@ -56176,16 +55807,12 @@
         <f t="shared" si="26"/>
         <v>Cory was close</v>
       </c>
-      <c r="AI71" s="5" t="str">
-        <f t="shared" si="27"/>
-        <v>Red</v>
-      </c>
-    </row>
-    <row r="72" spans="1:37">
+    </row>
+    <row r="72" spans="1:36">
       <c r="A72" s="5">
         <v>71</v>
       </c>
-      <c r="B72" s="17">
+      <c r="B72" s="16">
         <v>43714</v>
       </c>
       <c r="C72" s="5">
@@ -56202,11 +55829,11 @@
         <v>35</v>
       </c>
       <c r="G72" s="5" t="str">
-        <f t="shared" ref="G72:G77" si="28">IF(I72&lt;=0, "Control", IF(I72&lt;=10, "Red", IF(I72&gt;=21, "Pink", "Orange")))</f>
+        <f t="shared" ref="G72:G77" si="27">IF(I72&lt;=0, "Control", IF(I72&lt;=10, "Red", IF(I72&gt;=21, "Pink", "Orange")))</f>
         <v>Control</v>
       </c>
       <c r="H72" s="5">
-        <f t="shared" ref="H72:H77" si="29">IF(G72="Control", 1, IF(G72="Red", 2, IF(G72="Orange", 3, 4)))</f>
+        <f t="shared" ref="H72:H77" si="28">IF(G72="Control", 1, IF(G72="Red", 2, IF(G72="Orange", 3, 4)))</f>
         <v>1</v>
       </c>
       <c r="I72" s="7">
@@ -56280,19 +55907,15 @@
         <f t="shared" si="26"/>
         <v>Urchin was beast</v>
       </c>
-      <c r="AI72" s="5" t="str">
-        <f t="shared" si="27"/>
-        <v>Control</v>
-      </c>
-      <c r="AK72" s="5" t="s">
+      <c r="AJ72" s="5" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="73" spans="1:37">
+    <row r="73" spans="1:36">
       <c r="A73" s="5">
         <v>72</v>
       </c>
-      <c r="B73" s="17">
+      <c r="B73" s="16">
         <v>43714</v>
       </c>
       <c r="C73" s="5">
@@ -56309,11 +55932,11 @@
         <v>36</v>
       </c>
       <c r="G73" s="5" t="str">
+        <f t="shared" si="27"/>
+        <v>Pink</v>
+      </c>
+      <c r="H73" s="5">
         <f t="shared" si="28"/>
-        <v>Pink</v>
-      </c>
-      <c r="H73" s="5">
-        <f t="shared" si="29"/>
         <v>4</v>
       </c>
       <c r="I73" s="7">
@@ -56387,16 +56010,12 @@
         <f t="shared" si="26"/>
         <v>Cory was close</v>
       </c>
-      <c r="AI73" s="5" t="str">
-        <f t="shared" si="27"/>
-        <v>Pink</v>
-      </c>
-    </row>
-    <row r="74" spans="1:37">
+    </row>
+    <row r="74" spans="1:36">
       <c r="A74" s="5">
         <v>73</v>
       </c>
-      <c r="B74" s="17">
+      <c r="B74" s="16">
         <v>43714</v>
       </c>
       <c r="C74" s="5">
@@ -56413,11 +56032,11 @@
         <v>36</v>
       </c>
       <c r="G74" s="5" t="str">
+        <f t="shared" si="27"/>
+        <v>Orange</v>
+      </c>
+      <c r="H74" s="5">
         <f t="shared" si="28"/>
-        <v>Orange</v>
-      </c>
-      <c r="H74" s="5">
-        <f t="shared" si="29"/>
         <v>3</v>
       </c>
       <c r="I74" s="7">
@@ -56501,22 +56120,18 @@
         <f t="shared" si="26"/>
         <v>Cory was close</v>
       </c>
-      <c r="AI74" s="5" t="str">
-        <f t="shared" si="27"/>
-        <v>Orange</v>
+      <c r="AI74" s="5" t="s">
+        <v>77</v>
       </c>
       <c r="AJ74" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="AK74" s="5" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="75" spans="1:37">
+    <row r="75" spans="1:36">
       <c r="A75" s="5">
         <v>74</v>
       </c>
-      <c r="B75" s="17">
+      <c r="B75" s="16">
         <v>43714</v>
       </c>
       <c r="C75" s="5">
@@ -56533,11 +56148,11 @@
         <v>36</v>
       </c>
       <c r="G75" s="5" t="str">
+        <f t="shared" si="27"/>
+        <v>Red</v>
+      </c>
+      <c r="H75" s="5">
         <f t="shared" si="28"/>
-        <v>Red</v>
-      </c>
-      <c r="H75" s="5">
-        <f t="shared" si="29"/>
         <v>2</v>
       </c>
       <c r="I75" s="7">
@@ -56621,16 +56236,12 @@
         <f t="shared" si="26"/>
         <v>Urchin was beast</v>
       </c>
-      <c r="AI75" s="5" t="str">
-        <f t="shared" si="27"/>
-        <v>Red</v>
-      </c>
-    </row>
-    <row r="76" spans="1:37">
+    </row>
+    <row r="76" spans="1:36">
       <c r="A76" s="5">
         <v>75</v>
       </c>
-      <c r="B76" s="17">
+      <c r="B76" s="16">
         <v>43714</v>
       </c>
       <c r="C76" s="5">
@@ -56647,11 +56258,11 @@
         <v>35</v>
       </c>
       <c r="G76" s="5" t="str">
+        <f t="shared" si="27"/>
+        <v>Pink</v>
+      </c>
+      <c r="H76" s="5">
         <f t="shared" si="28"/>
-        <v>Pink</v>
-      </c>
-      <c r="H76" s="5">
-        <f t="shared" si="29"/>
         <v>4</v>
       </c>
       <c r="I76" s="7">
@@ -56735,19 +56346,15 @@
         <f t="shared" si="26"/>
         <v>Cory was close</v>
       </c>
-      <c r="AI76" s="5" t="str">
-        <f t="shared" si="27"/>
-        <v>Pink</v>
-      </c>
-      <c r="AK76" s="5" t="s">
+      <c r="AJ76" s="5" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="77" spans="1:37">
+    <row r="77" spans="1:36">
       <c r="A77" s="5">
         <v>76</v>
       </c>
-      <c r="B77" s="17">
+      <c r="B77" s="16">
         <v>43714</v>
       </c>
       <c r="C77" s="5">
@@ -56764,11 +56371,11 @@
         <v>35</v>
       </c>
       <c r="G77" s="5" t="str">
+        <f t="shared" si="27"/>
+        <v>Red</v>
+      </c>
+      <c r="H77" s="5">
         <f t="shared" si="28"/>
-        <v>Red</v>
-      </c>
-      <c r="H77" s="5">
-        <f t="shared" si="29"/>
         <v>2</v>
       </c>
       <c r="I77" s="7">
@@ -56841,14 +56448,10 @@
         <f t="shared" si="26"/>
         <v>Cory was beast</v>
       </c>
-      <c r="AI77" s="5" t="str">
-        <f t="shared" si="27"/>
-        <v>Red</v>
+      <c r="AI77" s="5" t="s">
+        <v>76</v>
       </c>
       <c r="AJ77" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="AK77" s="5" t="s">
         <v>78</v>
       </c>
     </row>
@@ -56978,7 +56581,7 @@
       </c>
       <c r="Y1" s="2" t="str">
         <f>raw!T1</f>
-        <v>Visible_consumption</v>
+        <v>Kelp visibly consumed?</v>
       </c>
       <c r="Z1" s="2" t="s">
         <v>95</v>

</xml_diff>

<commit_message>
Made data accessible to janitor package
</commit_message>
<xml_diff>
--- a/data/raw.xlsx
+++ b/data/raw.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Amelia\github\Ritger-Corynactis-urchin-deterrence\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Amelia\github\Ritger-2019-Corynactis-urchin-deterrence\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21B72FDE-D41C-4E2E-A45A-FB1AC82BE96B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB3B0211-10FC-4CAF-963E-F81CD0C86CA5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2328" yWindow="432" windowWidth="17256" windowHeight="10836" xr2:uid="{58E670A5-634C-427F-960F-9DA76C64E810}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{58E670A5-634C-427F-960F-9DA76C64E810}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="3" r:id="rId1"/>
@@ -779,7 +779,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{168F7463-EB05-46FE-9A95-7790352FDB02}">
   <dimension ref="A1:D16240"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
@@ -49722,9 +49722,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD5E687B-43EE-4B00-8604-7EB9984510DD}">
   <dimension ref="A1:AJ77"/>
   <sheetViews>
-    <sheetView topLeftCell="AE1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AH9" sqref="AH9"/>
+      <selection pane="bottomLeft" activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>

</xml_diff>